<commit_message>
Updated with some corrections
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E709647-4DD1-4EDF-821C-5FA6596C715E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E996C71-E3FB-4905-B417-775788BAF33F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-45" yWindow="120" windowWidth="25815" windowHeight="15975" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3326" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3330" uniqueCount="1152">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3474,6 +3474,21 @@
   </si>
   <si>
     <t>gov.gsa.conformancelib.tests.CMSTests</t>
+  </si>
+  <si>
+    <t>extended key usage (extKeyUsage) asserts id-PIV-content-signing.</t>
+  </si>
+  <si>
+    <t>Certificate Policy and Extended Key Usage</t>
+  </si>
+  <si>
+    <t>11.7.2.4.1</t>
+  </si>
+  <si>
+    <t>11.7.2.4.2</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -3724,7 +3739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3909,7 +3924,6 @@
     <xf numFmtId="49" fontId="14" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3922,6 +3936,8 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8004,9 +8020,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:G445"/>
+  <dimension ref="A1:G446"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A325" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C436" sqref="C436"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
@@ -8016,11 +8034,12 @@
     <col min="4" max="4" width="13.5" style="4" customWidth="1"/>
     <col min="5" max="5" width="24.125" style="53" customWidth="1"/>
     <col min="6" max="6" width="84.625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9" style="67"/>
     <col min="8" max="1026" width="8.5" style="28" customWidth="1"/>
     <col min="1027" max="16384" width="9" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="63" customFormat="1" ht="18.75">
+    <row r="1" spans="1:7" s="62" customFormat="1" ht="18.75">
       <c r="A1" s="52" t="s">
         <v>52</v>
       </c>
@@ -8039,14 +8058,14 @@
       <c r="F1" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="62"/>
+      <c r="G1" s="66"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="2">
-        <v>8</v>
+      <c r="B2" s="2" t="s">
+        <v>1151</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
@@ -8069,7 +8088,7 @@
       <c r="E3" s="58"/>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="31.5">
       <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
@@ -8087,7 +8106,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="31.5">
       <c r="A5" s="3" t="s">
         <v>58</v>
       </c>
@@ -8119,7 +8138,7 @@
       <c r="E6" s="55"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="31.5">
       <c r="A7" s="3" t="s">
         <v>58</v>
       </c>
@@ -8135,7 +8154,7 @@
       <c r="E7" s="55"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="31.5">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
@@ -8167,7 +8186,7 @@
       <c r="E9" s="55"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="31.5">
       <c r="A10" s="3" t="s">
         <v>58</v>
       </c>
@@ -8183,7 +8202,7 @@
       <c r="E10" s="55"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="31.5">
+    <row r="11" spans="1:7" ht="47.25">
       <c r="A11" s="3" t="s">
         <v>58</v>
       </c>
@@ -8199,7 +8218,7 @@
       <c r="E11" s="55"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="31.5">
       <c r="A12" s="3" t="s">
         <v>58</v>
       </c>
@@ -8215,7 +8234,7 @@
       <c r="E12" s="55"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="31.5">
       <c r="A13" s="3" t="s">
         <v>58</v>
       </c>
@@ -8279,7 +8298,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" ht="31.5">
       <c r="A17" s="3" t="s">
         <v>58</v>
       </c>
@@ -8311,7 +8330,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" ht="31.5">
       <c r="A19" s="3" t="s">
         <v>58</v>
       </c>
@@ -8343,7 +8362,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" ht="31.5">
       <c r="A21" s="3" t="s">
         <v>58</v>
       </c>
@@ -8359,7 +8378,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" ht="31.5">
       <c r="A22" s="3" t="s">
         <v>58</v>
       </c>
@@ -8375,7 +8394,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" ht="31.5">
       <c r="A23" s="3" t="s">
         <v>58</v>
       </c>
@@ -8391,7 +8410,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" ht="31.5">
       <c r="A24" s="3" t="s">
         <v>58</v>
       </c>
@@ -8407,7 +8426,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" ht="47.25">
       <c r="A25" s="3" t="s">
         <v>58</v>
       </c>
@@ -8423,7 +8442,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" ht="31.5">
       <c r="A26" s="3" t="s">
         <v>58</v>
       </c>
@@ -8471,7 +8490,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" ht="31.5">
+    <row r="29" spans="1:6" ht="47.25">
       <c r="A29" s="3" t="s">
         <v>58</v>
       </c>
@@ -8533,7 +8552,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="10"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" ht="31.5">
       <c r="A33" s="3" t="s">
         <v>58</v>
       </c>
@@ -8551,7 +8570,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" ht="31.5">
       <c r="A34" s="3" t="s">
         <v>58</v>
       </c>
@@ -8583,7 +8602,7 @@
       <c r="E35" s="55"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" ht="31.5">
       <c r="A36" s="3" t="s">
         <v>58</v>
       </c>
@@ -8631,7 +8650,7 @@
       <c r="E38" s="55"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" ht="31.5">
       <c r="A39" s="3" t="s">
         <v>58</v>
       </c>
@@ -8647,7 +8666,7 @@
       <c r="E39" s="55"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" ht="31.5">
       <c r="A40" s="3" t="s">
         <v>58</v>
       </c>
@@ -8663,7 +8682,7 @@
       <c r="E40" s="55"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" ht="31.5">
       <c r="A41" s="3" t="s">
         <v>58</v>
       </c>
@@ -8709,7 +8728,7 @@
       <c r="E43" s="55"/>
       <c r="F43" s="10"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" ht="31.5">
       <c r="A44" s="3" t="s">
         <v>58</v>
       </c>
@@ -8727,7 +8746,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" ht="31.5">
       <c r="A45" s="3" t="s">
         <v>58</v>
       </c>
@@ -8759,7 +8778,7 @@
       <c r="E46" s="55"/>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" ht="31.5">
       <c r="A47" s="3" t="s">
         <v>58</v>
       </c>
@@ -8791,7 +8810,7 @@
       <c r="E48" s="55"/>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" ht="31.5">
       <c r="A49" s="3" t="s">
         <v>58</v>
       </c>
@@ -8807,7 +8826,7 @@
       <c r="E49" s="55"/>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" ht="31.5">
       <c r="A50" s="3" t="s">
         <v>58</v>
       </c>
@@ -8823,7 +8842,7 @@
       <c r="E50" s="55"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" ht="31.5">
       <c r="A51" s="3" t="s">
         <v>58</v>
       </c>
@@ -8869,7 +8888,7 @@
       <c r="E53" s="55"/>
       <c r="F53" s="10"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" ht="31.5">
       <c r="A54" s="3" t="s">
         <v>58</v>
       </c>
@@ -8887,7 +8906,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" ht="31.5">
       <c r="A55" s="3" t="s">
         <v>58</v>
       </c>
@@ -8919,7 +8938,7 @@
       <c r="E56" s="55"/>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" ht="31.5">
       <c r="A57" s="3" t="s">
         <v>58</v>
       </c>
@@ -8948,12 +8967,12 @@
       <c r="D58" s="41" t="s">
         <v>175</v>
       </c>
-      <c r="E58" s="65" t="s">
+      <c r="E58" s="64" t="s">
         <v>175</v>
       </c>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" ht="31.5">
       <c r="A59" s="3" t="s">
         <v>58</v>
       </c>
@@ -8969,7 +8988,7 @@
       <c r="E59" s="55"/>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" ht="31.5">
       <c r="A60" s="3" t="s">
         <v>58</v>
       </c>
@@ -8985,7 +9004,7 @@
       <c r="E60" s="55"/>
       <c r="F60" s="3"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" ht="31.5">
       <c r="A61" s="3" t="s">
         <v>58</v>
       </c>
@@ -9001,7 +9020,7 @@
       <c r="E61" s="55"/>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" ht="31.5">
       <c r="A62" s="3" t="s">
         <v>58</v>
       </c>
@@ -9047,7 +9066,7 @@
       <c r="E64" s="55"/>
       <c r="F64" s="10"/>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" ht="31.5">
       <c r="A65" s="3" t="s">
         <v>58</v>
       </c>
@@ -9065,7 +9084,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" ht="31.5">
       <c r="A66" s="3" t="s">
         <v>58</v>
       </c>
@@ -9097,7 +9116,7 @@
       <c r="E67" s="55"/>
       <c r="F67" s="3"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" ht="31.5">
       <c r="A68" s="3" t="s">
         <v>58</v>
       </c>
@@ -9113,7 +9132,7 @@
       <c r="E68" s="55"/>
       <c r="F68" s="3"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" ht="31.5">
       <c r="A69" s="3" t="s">
         <v>58</v>
       </c>
@@ -9129,7 +9148,7 @@
       <c r="E69" s="55"/>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" ht="31.5">
       <c r="A70" s="3" t="s">
         <v>58</v>
       </c>
@@ -9191,7 +9210,7 @@
       <c r="E73" s="55"/>
       <c r="F73" s="10"/>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" ht="31.5">
       <c r="A74" s="3" t="s">
         <v>58</v>
       </c>
@@ -9209,7 +9228,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" ht="31.5">
       <c r="A75" s="3" t="s">
         <v>58</v>
       </c>
@@ -9241,7 +9260,7 @@
       <c r="E76" s="55"/>
       <c r="F76" s="3"/>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" ht="31.5">
       <c r="A77" s="3" t="s">
         <v>58</v>
       </c>
@@ -9289,7 +9308,7 @@
       <c r="E79" s="55"/>
       <c r="F79" s="3"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" ht="31.5">
       <c r="A80" s="3" t="s">
         <v>58</v>
       </c>
@@ -9305,7 +9324,7 @@
       <c r="E80" s="55"/>
       <c r="F80" s="3"/>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" ht="31.5">
       <c r="A81" s="3" t="s">
         <v>58</v>
       </c>
@@ -9321,7 +9340,7 @@
       <c r="E81" s="55"/>
       <c r="F81" s="3"/>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" ht="31.5">
       <c r="A82" s="3" t="s">
         <v>58</v>
       </c>
@@ -9367,7 +9386,7 @@
       <c r="E84" s="55"/>
       <c r="F84" s="10"/>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" ht="31.5">
       <c r="A85" s="3" t="s">
         <v>58</v>
       </c>
@@ -9385,7 +9404,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" ht="31.5">
       <c r="A86" s="3" t="s">
         <v>58</v>
       </c>
@@ -9417,7 +9436,7 @@
       <c r="E87" s="55"/>
       <c r="F87" s="3"/>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" ht="31.5">
       <c r="A88" s="3" t="s">
         <v>58</v>
       </c>
@@ -9465,7 +9484,7 @@
       <c r="E90" s="55"/>
       <c r="F90" s="3"/>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" ht="31.5">
       <c r="A91" s="3" t="s">
         <v>58</v>
       </c>
@@ -9481,7 +9500,7 @@
       <c r="E91" s="55"/>
       <c r="F91" s="3"/>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" ht="31.5">
       <c r="A92" s="3" t="s">
         <v>58</v>
       </c>
@@ -9497,7 +9516,7 @@
       <c r="E92" s="55"/>
       <c r="F92" s="3"/>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" ht="31.5">
       <c r="A93" s="3" t="s">
         <v>58</v>
       </c>
@@ -9543,7 +9562,7 @@
       <c r="E95" s="55"/>
       <c r="F95" s="10"/>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" ht="31.5">
       <c r="A96" s="3" t="s">
         <v>58</v>
       </c>
@@ -9561,7 +9580,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:6" ht="31.5">
       <c r="A97" s="3" t="s">
         <v>58</v>
       </c>
@@ -9593,7 +9612,7 @@
       <c r="E98" s="55"/>
       <c r="F98" s="3"/>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:6" ht="31.5">
       <c r="A99" s="3" t="s">
         <v>58</v>
       </c>
@@ -9641,7 +9660,7 @@
       <c r="E101" s="55"/>
       <c r="F101" s="3"/>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:6" ht="31.5">
       <c r="A102" s="3" t="s">
         <v>58</v>
       </c>
@@ -9657,7 +9676,7 @@
       <c r="E102" s="55"/>
       <c r="F102" s="3"/>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" ht="31.5">
       <c r="A103" s="3" t="s">
         <v>58</v>
       </c>
@@ -9673,7 +9692,7 @@
       <c r="E103" s="55"/>
       <c r="F103" s="3"/>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" ht="31.5">
       <c r="A104" s="3" t="s">
         <v>58</v>
       </c>
@@ -9719,7 +9738,7 @@
       <c r="E106" s="55"/>
       <c r="F106" s="10"/>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:6" ht="31.5">
       <c r="A107" s="3" t="s">
         <v>58</v>
       </c>
@@ -9737,7 +9756,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:6" ht="31.5">
       <c r="A108" s="3" t="s">
         <v>58</v>
       </c>
@@ -9769,7 +9788,7 @@
       <c r="E109" s="55"/>
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:6" ht="31.5">
       <c r="A110" s="3" t="s">
         <v>58</v>
       </c>
@@ -9833,7 +9852,7 @@
       <c r="E113" s="55"/>
       <c r="F113" s="3"/>
     </row>
-    <row r="114" spans="1:6" ht="31.5">
+    <row r="114" spans="1:6" ht="47.25">
       <c r="A114" s="3" t="s">
         <v>58</v>
       </c>
@@ -9863,7 +9882,7 @@
       <c r="E115" s="55"/>
       <c r="F115" s="10"/>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:6" ht="28.5">
       <c r="A116" s="3" t="s">
         <v>58</v>
       </c>
@@ -9883,7 +9902,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="117" spans="1:6">
+    <row r="117" spans="1:6" ht="28.5">
       <c r="A117" s="3" t="s">
         <v>58</v>
       </c>
@@ -9919,7 +9938,7 @@
       </c>
       <c r="F118" s="11"/>
     </row>
-    <row r="119" spans="1:6">
+    <row r="119" spans="1:6" ht="28.5">
       <c r="A119" s="3" t="s">
         <v>58</v>
       </c>
@@ -9955,7 +9974,7 @@
       </c>
       <c r="F120" s="11"/>
     </row>
-    <row r="121" spans="1:6" ht="31.5">
+    <row r="121" spans="1:6" ht="47.25">
       <c r="A121" s="3" t="s">
         <v>58</v>
       </c>
@@ -9973,7 +9992,7 @@
       </c>
       <c r="F121" s="3"/>
     </row>
-    <row r="122" spans="1:6">
+    <row r="122" spans="1:6" ht="31.5">
       <c r="A122" s="3" t="s">
         <v>58</v>
       </c>
@@ -9991,7 +10010,7 @@
       </c>
       <c r="F122" s="3"/>
     </row>
-    <row r="123" spans="1:6" ht="47.25">
+    <row r="123" spans="1:6" ht="78.75">
       <c r="A123" s="3" t="s">
         <v>58</v>
       </c>
@@ -10223,7 +10242,7 @@
       <c r="E136" s="55"/>
       <c r="F136" s="18"/>
     </row>
-    <row r="137" spans="1:6">
+    <row r="137" spans="1:6" ht="31.5">
       <c r="A137" s="3" t="s">
         <v>58</v>
       </c>
@@ -10303,7 +10322,7 @@
       <c r="E141" s="55"/>
       <c r="F141" s="18"/>
     </row>
-    <row r="142" spans="1:6">
+    <row r="142" spans="1:6" ht="31.5">
       <c r="A142" s="3" t="s">
         <v>58</v>
       </c>
@@ -10321,7 +10340,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="143" spans="1:6">
+    <row r="143" spans="1:6" ht="31.5">
       <c r="A143" s="3" t="s">
         <v>58</v>
       </c>
@@ -10337,7 +10356,7 @@
       <c r="E143" s="55"/>
       <c r="F143" s="3"/>
     </row>
-    <row r="144" spans="1:6" ht="31.5">
+    <row r="144" spans="1:6" ht="47.25">
       <c r="A144" s="3" t="s">
         <v>58</v>
       </c>
@@ -10371,7 +10390,7 @@
       </c>
       <c r="F145" s="3"/>
     </row>
-    <row r="146" spans="1:6" ht="31.5">
+    <row r="146" spans="1:6" ht="47.25">
       <c r="A146" s="3" t="s">
         <v>58</v>
       </c>
@@ -10387,7 +10406,7 @@
       <c r="E146" s="55"/>
       <c r="F146" s="3"/>
     </row>
-    <row r="147" spans="1:6">
+    <row r="147" spans="1:6" ht="31.5">
       <c r="A147" s="3" t="s">
         <v>58</v>
       </c>
@@ -10403,7 +10422,7 @@
       <c r="E147" s="55"/>
       <c r="F147" s="3"/>
     </row>
-    <row r="148" spans="1:6">
+    <row r="148" spans="1:6" ht="31.5">
       <c r="A148" s="3" t="s">
         <v>58</v>
       </c>
@@ -10421,7 +10440,7 @@
       </c>
       <c r="F148" s="3"/>
     </row>
-    <row r="149" spans="1:6" ht="31.5">
+    <row r="149" spans="1:6" ht="63">
       <c r="A149" s="3" t="s">
         <v>58</v>
       </c>
@@ -10457,7 +10476,7 @@
       </c>
       <c r="F150" s="40"/>
     </row>
-    <row r="151" spans="1:6" ht="31.5">
+    <row r="151" spans="1:6" ht="78.75">
       <c r="A151" s="3" t="s">
         <v>58</v>
       </c>
@@ -10473,7 +10492,7 @@
       <c r="E151" s="55"/>
       <c r="F151" s="3"/>
     </row>
-    <row r="152" spans="1:6" ht="31.5">
+    <row r="152" spans="1:6" ht="47.25">
       <c r="A152" s="3" t="s">
         <v>58</v>
       </c>
@@ -10489,7 +10508,7 @@
       <c r="E152" s="55"/>
       <c r="F152" s="3"/>
     </row>
-    <row r="153" spans="1:6">
+    <row r="153" spans="1:6" ht="31.5">
       <c r="A153" s="3" t="s">
         <v>58</v>
       </c>
@@ -10533,7 +10552,7 @@
       <c r="E155" s="55"/>
       <c r="F155" s="18"/>
     </row>
-    <row r="156" spans="1:6">
+    <row r="156" spans="1:6" ht="31.5">
       <c r="A156" s="3" t="s">
         <v>58</v>
       </c>
@@ -10613,7 +10632,7 @@
       <c r="E160" s="55"/>
       <c r="F160" s="18"/>
     </row>
-    <row r="161" spans="1:6">
+    <row r="161" spans="1:6" ht="31.5">
       <c r="A161" s="3" t="s">
         <v>58</v>
       </c>
@@ -10631,7 +10650,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="162" spans="1:6">
+    <row r="162" spans="1:6" ht="31.5">
       <c r="A162" s="3" t="s">
         <v>58</v>
       </c>
@@ -10647,7 +10666,7 @@
       <c r="E162" s="55"/>
       <c r="F162" s="3"/>
     </row>
-    <row r="163" spans="1:6" ht="31.5">
+    <row r="163" spans="1:6" ht="47.25">
       <c r="A163" s="3" t="s">
         <v>58</v>
       </c>
@@ -10681,7 +10700,7 @@
       </c>
       <c r="F164" s="3"/>
     </row>
-    <row r="165" spans="1:6" ht="31.5">
+    <row r="165" spans="1:6" ht="47.25">
       <c r="A165" s="3" t="s">
         <v>58</v>
       </c>
@@ -10697,7 +10716,7 @@
       <c r="E165" s="55"/>
       <c r="F165" s="3"/>
     </row>
-    <row r="166" spans="1:6">
+    <row r="166" spans="1:6" ht="31.5">
       <c r="A166" s="3" t="s">
         <v>58</v>
       </c>
@@ -10713,7 +10732,7 @@
       <c r="E166" s="55"/>
       <c r="F166" s="3"/>
     </row>
-    <row r="167" spans="1:6">
+    <row r="167" spans="1:6" ht="31.5">
       <c r="A167" s="3" t="s">
         <v>58</v>
       </c>
@@ -10731,7 +10750,7 @@
       </c>
       <c r="F167" s="3"/>
     </row>
-    <row r="168" spans="1:6" ht="31.5">
+    <row r="168" spans="1:6" ht="47.25">
       <c r="A168" s="3" t="s">
         <v>58</v>
       </c>
@@ -10767,7 +10786,7 @@
       </c>
       <c r="F169" s="3"/>
     </row>
-    <row r="170" spans="1:6" ht="31.5">
+    <row r="170" spans="1:6" ht="78.75">
       <c r="A170" s="3" t="s">
         <v>58</v>
       </c>
@@ -10783,7 +10802,7 @@
       <c r="E170" s="55"/>
       <c r="F170" s="3"/>
     </row>
-    <row r="171" spans="1:6" ht="31.5">
+    <row r="171" spans="1:6" ht="47.25">
       <c r="A171" s="3" t="s">
         <v>58</v>
       </c>
@@ -10799,7 +10818,7 @@
       <c r="E171" s="55"/>
       <c r="F171" s="3"/>
     </row>
-    <row r="172" spans="1:6">
+    <row r="172" spans="1:6" ht="31.5">
       <c r="A172" s="3" t="s">
         <v>58</v>
       </c>
@@ -10843,7 +10862,7 @@
       <c r="E174" s="55"/>
       <c r="F174" s="18"/>
     </row>
-    <row r="175" spans="1:6">
+    <row r="175" spans="1:6" ht="31.5">
       <c r="A175" s="3" t="s">
         <v>58</v>
       </c>
@@ -10939,7 +10958,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="181" spans="1:6">
+    <row r="181" spans="1:6" ht="31.5">
       <c r="A181" s="3" t="s">
         <v>58</v>
       </c>
@@ -10989,7 +11008,7 @@
       </c>
       <c r="F183" s="3"/>
     </row>
-    <row r="184" spans="1:6" ht="31.5">
+    <row r="184" spans="1:6" ht="47.25">
       <c r="A184" s="3" t="s">
         <v>58</v>
       </c>
@@ -11005,7 +11024,7 @@
       <c r="E184" s="55"/>
       <c r="F184" s="3"/>
     </row>
-    <row r="185" spans="1:6">
+    <row r="185" spans="1:6" ht="31.5">
       <c r="A185" s="3" t="s">
         <v>58</v>
       </c>
@@ -11021,7 +11040,7 @@
       <c r="E185" s="55"/>
       <c r="F185" s="3"/>
     </row>
-    <row r="186" spans="1:6">
+    <row r="186" spans="1:6" ht="31.5">
       <c r="A186" s="3" t="s">
         <v>58</v>
       </c>
@@ -11039,7 +11058,7 @@
       </c>
       <c r="F186" s="3"/>
     </row>
-    <row r="187" spans="1:6" ht="31.5">
+    <row r="187" spans="1:6" ht="47.25">
       <c r="A187" s="3" t="s">
         <v>58</v>
       </c>
@@ -11075,7 +11094,7 @@
       </c>
       <c r="F188" s="3"/>
     </row>
-    <row r="189" spans="1:6" ht="31.5">
+    <row r="189" spans="1:6" ht="78.75">
       <c r="A189" s="3" t="s">
         <v>58</v>
       </c>
@@ -11091,7 +11110,7 @@
       <c r="E189" s="55"/>
       <c r="F189" s="3"/>
     </row>
-    <row r="190" spans="1:6" ht="31.5">
+    <row r="190" spans="1:6" ht="47.25">
       <c r="A190" s="3" t="s">
         <v>58</v>
       </c>
@@ -11107,7 +11126,7 @@
       <c r="E190" s="55"/>
       <c r="F190" s="3"/>
     </row>
-    <row r="191" spans="1:6">
+    <row r="191" spans="1:6" ht="31.5">
       <c r="A191" s="3" t="s">
         <v>58</v>
       </c>
@@ -11151,7 +11170,7 @@
       <c r="E193" s="55"/>
       <c r="F193" s="18"/>
     </row>
-    <row r="194" spans="1:6">
+    <row r="194" spans="1:6" ht="31.5">
       <c r="A194" s="3" t="s">
         <v>58</v>
       </c>
@@ -11169,7 +11188,7 @@
         <v>1120</v>
       </c>
     </row>
-    <row r="195" spans="1:6">
+    <row r="195" spans="1:6" ht="31.5">
       <c r="A195" s="3" t="s">
         <v>58</v>
       </c>
@@ -11185,7 +11204,7 @@
       <c r="E195" s="55"/>
       <c r="F195" s="3"/>
     </row>
-    <row r="196" spans="1:6">
+    <row r="196" spans="1:6" ht="31.5">
       <c r="A196" s="3" t="s">
         <v>58</v>
       </c>
@@ -11201,7 +11220,7 @@
       <c r="E196" s="55"/>
       <c r="F196" s="3"/>
     </row>
-    <row r="197" spans="1:6" ht="31.5">
+    <row r="197" spans="1:6" ht="63">
       <c r="A197" s="3" t="s">
         <v>58</v>
       </c>
@@ -11217,7 +11236,7 @@
       <c r="E197" s="55"/>
       <c r="F197" s="3"/>
     </row>
-    <row r="198" spans="1:6" ht="31.5">
+    <row r="198" spans="1:6" ht="63">
       <c r="A198" s="3" t="s">
         <v>58</v>
       </c>
@@ -11233,7 +11252,7 @@
       <c r="E198" s="55"/>
       <c r="F198" s="3"/>
     </row>
-    <row r="199" spans="1:6">
+    <row r="199" spans="1:6" ht="31.5">
       <c r="A199" s="3" t="s">
         <v>58</v>
       </c>
@@ -11267,7 +11286,7 @@
       <c r="E200" s="55"/>
       <c r="F200" s="3"/>
     </row>
-    <row r="201" spans="1:6">
+    <row r="201" spans="1:6" ht="31.5">
       <c r="A201" s="3" t="s">
         <v>58</v>
       </c>
@@ -11399,7 +11418,7 @@
       <c r="E208" s="55"/>
       <c r="F208" s="3"/>
     </row>
-    <row r="209" spans="1:6">
+    <row r="209" spans="1:6" ht="31.5">
       <c r="A209" s="3" t="s">
         <v>58</v>
       </c>
@@ -11431,7 +11450,7 @@
       <c r="E210" s="55"/>
       <c r="F210" s="3"/>
     </row>
-    <row r="211" spans="1:6">
+    <row r="211" spans="1:6" ht="31.5">
       <c r="A211" s="3" t="s">
         <v>58</v>
       </c>
@@ -11444,7 +11463,7 @@
       <c r="D211" s="46" t="s">
         <v>989</v>
       </c>
-      <c r="E211" s="66" t="s">
+      <c r="E211" s="65" t="s">
         <v>1139</v>
       </c>
       <c r="F211" s="3"/>
@@ -11481,7 +11500,7 @@
       <c r="E213" s="55"/>
       <c r="F213" s="3"/>
     </row>
-    <row r="214" spans="1:6">
+    <row r="214" spans="1:6" ht="31.5">
       <c r="A214" s="3" t="s">
         <v>58</v>
       </c>
@@ -11607,7 +11626,7 @@
       <c r="E221" s="55"/>
       <c r="F221" s="19"/>
     </row>
-    <row r="222" spans="1:6">
+    <row r="222" spans="1:6" ht="31.5">
       <c r="A222" s="3" t="s">
         <v>58</v>
       </c>
@@ -11757,7 +11776,7 @@
       <c r="E231" s="55"/>
       <c r="F231" s="21"/>
     </row>
-    <row r="232" spans="1:6" ht="31.5">
+    <row r="232" spans="1:6" ht="63">
       <c r="A232" s="3" t="s">
         <v>58</v>
       </c>
@@ -11775,7 +11794,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="233" spans="1:6">
+    <row r="233" spans="1:6" ht="31.5">
       <c r="A233" s="3" t="s">
         <v>58</v>
       </c>
@@ -11791,7 +11810,7 @@
       <c r="E233" s="55"/>
       <c r="F233" s="5"/>
     </row>
-    <row r="234" spans="1:6">
+    <row r="234" spans="1:6" ht="31.5">
       <c r="A234" s="3" t="s">
         <v>58</v>
       </c>
@@ -11807,7 +11826,7 @@
       <c r="E234" s="55"/>
       <c r="F234" s="5"/>
     </row>
-    <row r="235" spans="1:6" ht="31.5">
+    <row r="235" spans="1:6" ht="47.25">
       <c r="A235" s="3" t="s">
         <v>58</v>
       </c>
@@ -11839,7 +11858,7 @@
       <c r="E236" s="55"/>
       <c r="F236" s="5"/>
     </row>
-    <row r="237" spans="1:6">
+    <row r="237" spans="1:6" ht="31.5">
       <c r="A237" s="3" t="s">
         <v>58</v>
       </c>
@@ -11855,7 +11874,7 @@
       <c r="E237" s="55"/>
       <c r="F237" s="5"/>
     </row>
-    <row r="238" spans="1:6" ht="31.5">
+    <row r="238" spans="1:6" ht="63">
       <c r="A238" s="3" t="s">
         <v>58</v>
       </c>
@@ -11871,7 +11890,7 @@
       <c r="E238" s="55"/>
       <c r="F238" s="5"/>
     </row>
-    <row r="239" spans="1:6" ht="31.5">
+    <row r="239" spans="1:6" ht="63">
       <c r="A239" s="3" t="s">
         <v>58</v>
       </c>
@@ -11887,7 +11906,7 @@
       <c r="E239" s="55"/>
       <c r="F239" s="5"/>
     </row>
-    <row r="240" spans="1:6" ht="47.25">
+    <row r="240" spans="1:6" ht="94.5">
       <c r="A240" s="3" t="s">
         <v>58</v>
       </c>
@@ -11903,7 +11922,7 @@
       <c r="E240" s="55"/>
       <c r="F240" s="5"/>
     </row>
-    <row r="241" spans="1:6" ht="31.5">
+    <row r="241" spans="1:6" ht="78.75">
       <c r="A241" s="3" t="s">
         <v>58</v>
       </c>
@@ -11919,7 +11938,7 @@
       <c r="E241" s="55"/>
       <c r="F241" s="5"/>
     </row>
-    <row r="242" spans="1:6" ht="47.25">
+    <row r="242" spans="1:6" ht="94.5">
       <c r="A242" s="3" t="s">
         <v>58</v>
       </c>
@@ -11935,7 +11954,7 @@
       <c r="E242" s="55"/>
       <c r="F242" s="5"/>
     </row>
-    <row r="243" spans="1:6">
+    <row r="243" spans="1:6" ht="31.5">
       <c r="A243" s="3" t="s">
         <v>58</v>
       </c>
@@ -11979,7 +11998,7 @@
       <c r="E245" s="55"/>
       <c r="F245" s="21"/>
     </row>
-    <row r="246" spans="1:6" ht="31.5">
+    <row r="246" spans="1:6" ht="63">
       <c r="A246" s="3" t="s">
         <v>58</v>
       </c>
@@ -12013,7 +12032,7 @@
       <c r="E247" s="55"/>
       <c r="F247" s="5"/>
     </row>
-    <row r="248" spans="1:6">
+    <row r="248" spans="1:6" ht="31.5">
       <c r="A248" s="3" t="s">
         <v>58</v>
       </c>
@@ -12029,7 +12048,7 @@
       <c r="E248" s="55"/>
       <c r="F248" s="5"/>
     </row>
-    <row r="249" spans="1:6" ht="31.5">
+    <row r="249" spans="1:6" ht="47.25">
       <c r="A249" s="3" t="s">
         <v>58</v>
       </c>
@@ -12061,7 +12080,7 @@
       <c r="E250" s="55"/>
       <c r="F250" s="5"/>
     </row>
-    <row r="251" spans="1:6">
+    <row r="251" spans="1:6" ht="31.5">
       <c r="A251" s="3" t="s">
         <v>58</v>
       </c>
@@ -12093,7 +12112,7 @@
       <c r="E252" s="55"/>
       <c r="F252" s="5"/>
     </row>
-    <row r="253" spans="1:6">
+    <row r="253" spans="1:6" ht="31.5">
       <c r="A253" s="3" t="s">
         <v>58</v>
       </c>
@@ -12109,7 +12128,7 @@
       <c r="E253" s="55"/>
       <c r="F253" s="5"/>
     </row>
-    <row r="254" spans="1:6">
+    <row r="254" spans="1:6" ht="31.5">
       <c r="A254" s="3" t="s">
         <v>58</v>
       </c>
@@ -12125,7 +12144,7 @@
       <c r="E254" s="55"/>
       <c r="F254" s="5"/>
     </row>
-    <row r="255" spans="1:6" ht="31.5">
+    <row r="255" spans="1:6" ht="47.25">
       <c r="A255" s="3" t="s">
         <v>58</v>
       </c>
@@ -12141,7 +12160,7 @@
       <c r="E255" s="55"/>
       <c r="F255" s="5"/>
     </row>
-    <row r="256" spans="1:6" ht="31.5">
+    <row r="256" spans="1:6" ht="47.25">
       <c r="A256" s="3" t="s">
         <v>58</v>
       </c>
@@ -12157,7 +12176,7 @@
       <c r="E256" s="55"/>
       <c r="F256" s="5"/>
     </row>
-    <row r="257" spans="1:6" ht="31.5">
+    <row r="257" spans="1:6" ht="78.75">
       <c r="A257" s="3" t="s">
         <v>58</v>
       </c>
@@ -12173,7 +12192,7 @@
       <c r="E257" s="55"/>
       <c r="F257" s="3"/>
     </row>
-    <row r="258" spans="1:6" ht="47.25">
+    <row r="258" spans="1:6" ht="78.75">
       <c r="A258" s="3" t="s">
         <v>58</v>
       </c>
@@ -12189,7 +12208,7 @@
       <c r="E258" s="55"/>
       <c r="F258" s="5"/>
     </row>
-    <row r="259" spans="1:6" ht="47.25">
+    <row r="259" spans="1:6" ht="94.5">
       <c r="A259" s="3" t="s">
         <v>58</v>
       </c>
@@ -12205,7 +12224,7 @@
       <c r="E259" s="55"/>
       <c r="F259" s="3"/>
     </row>
-    <row r="260" spans="1:6" ht="47.25">
+    <row r="260" spans="1:6" ht="94.5">
       <c r="A260" s="3" t="s">
         <v>58</v>
       </c>
@@ -12221,7 +12240,7 @@
       <c r="E260" s="55"/>
       <c r="F260" s="5"/>
     </row>
-    <row r="261" spans="1:6" ht="31.5">
+    <row r="261" spans="1:6" ht="63">
       <c r="A261" s="3" t="s">
         <v>58</v>
       </c>
@@ -12265,7 +12284,7 @@
       <c r="E263" s="55"/>
       <c r="F263" s="13"/>
     </row>
-    <row r="264" spans="1:6" ht="31.5">
+    <row r="264" spans="1:6" ht="63">
       <c r="A264" s="3" t="s">
         <v>58</v>
       </c>
@@ -12299,7 +12318,7 @@
       <c r="E265" s="55"/>
       <c r="F265" s="5"/>
     </row>
-    <row r="266" spans="1:6">
+    <row r="266" spans="1:6" ht="31.5">
       <c r="A266" s="3" t="s">
         <v>58</v>
       </c>
@@ -12315,7 +12334,7 @@
       <c r="E266" s="55"/>
       <c r="F266" s="5"/>
     </row>
-    <row r="267" spans="1:6" ht="31.5">
+    <row r="267" spans="1:6" ht="47.25">
       <c r="A267" s="3" t="s">
         <v>58</v>
       </c>
@@ -12347,7 +12366,7 @@
       <c r="E268" s="55"/>
       <c r="F268" s="5"/>
     </row>
-    <row r="269" spans="1:6">
+    <row r="269" spans="1:6" ht="31.5">
       <c r="A269" s="3" t="s">
         <v>58</v>
       </c>
@@ -12379,7 +12398,7 @@
       <c r="E270" s="55"/>
       <c r="F270" s="5"/>
     </row>
-    <row r="271" spans="1:6">
+    <row r="271" spans="1:6" ht="31.5">
       <c r="A271" s="3" t="s">
         <v>58</v>
       </c>
@@ -12395,7 +12414,7 @@
       <c r="E271" s="55"/>
       <c r="F271" s="5"/>
     </row>
-    <row r="272" spans="1:6">
+    <row r="272" spans="1:6" ht="31.5">
       <c r="A272" s="3" t="s">
         <v>58</v>
       </c>
@@ -12411,7 +12430,7 @@
       <c r="E272" s="55"/>
       <c r="F272" s="5"/>
     </row>
-    <row r="273" spans="1:6" ht="31.5">
+    <row r="273" spans="1:6" ht="47.25">
       <c r="A273" s="3" t="s">
         <v>58</v>
       </c>
@@ -12427,7 +12446,7 @@
       <c r="E273" s="55"/>
       <c r="F273" s="5"/>
     </row>
-    <row r="274" spans="1:6" ht="31.5">
+    <row r="274" spans="1:6" ht="47.25">
       <c r="A274" s="3" t="s">
         <v>58</v>
       </c>
@@ -12443,7 +12462,7 @@
       <c r="E274" s="55"/>
       <c r="F274" s="5"/>
     </row>
-    <row r="275" spans="1:6" ht="31.5">
+    <row r="275" spans="1:6" ht="78.75">
       <c r="A275" s="3" t="s">
         <v>58</v>
       </c>
@@ -12459,7 +12478,7 @@
       <c r="E275" s="55"/>
       <c r="F275" s="3"/>
     </row>
-    <row r="276" spans="1:6" ht="47.25">
+    <row r="276" spans="1:6" ht="78.75">
       <c r="A276" s="3" t="s">
         <v>58</v>
       </c>
@@ -12475,7 +12494,7 @@
       <c r="E276" s="55"/>
       <c r="F276" s="5"/>
     </row>
-    <row r="277" spans="1:6" ht="47.25">
+    <row r="277" spans="1:6" ht="94.5">
       <c r="A277" s="3" t="s">
         <v>58</v>
       </c>
@@ -12491,7 +12510,7 @@
       <c r="E277" s="55"/>
       <c r="F277" s="3"/>
     </row>
-    <row r="278" spans="1:6" ht="47.25">
+    <row r="278" spans="1:6" ht="94.5">
       <c r="A278" s="3" t="s">
         <v>58</v>
       </c>
@@ -12507,7 +12526,7 @@
       <c r="E278" s="55"/>
       <c r="F278" s="5"/>
     </row>
-    <row r="279" spans="1:6" ht="31.5">
+    <row r="279" spans="1:6" ht="63">
       <c r="A279" s="3" t="s">
         <v>58</v>
       </c>
@@ -12551,7 +12570,7 @@
       <c r="E281" s="55"/>
       <c r="F281" s="18"/>
     </row>
-    <row r="282" spans="1:6" ht="31.5">
+    <row r="282" spans="1:6" ht="47.25">
       <c r="A282" s="3" t="s">
         <v>58</v>
       </c>
@@ -12583,7 +12602,7 @@
       <c r="E283" s="55"/>
       <c r="F283" s="18"/>
     </row>
-    <row r="284" spans="1:6" ht="31.5">
+    <row r="284" spans="1:6" ht="47.25">
       <c r="A284" s="3" t="s">
         <v>58</v>
       </c>
@@ -12633,7 +12652,7 @@
       <c r="E286" s="55"/>
       <c r="F286" s="5"/>
     </row>
-    <row r="287" spans="1:6" ht="31.5">
+    <row r="287" spans="1:6" ht="47.25">
       <c r="A287" s="3" t="s">
         <v>58</v>
       </c>
@@ -12649,7 +12668,7 @@
       <c r="E287" s="55"/>
       <c r="F287" s="5"/>
     </row>
-    <row r="288" spans="1:6">
+    <row r="288" spans="1:6" ht="31.5">
       <c r="A288" s="3" t="s">
         <v>58</v>
       </c>
@@ -12681,7 +12700,7 @@
       <c r="E289" s="55"/>
       <c r="F289" s="5"/>
     </row>
-    <row r="290" spans="1:6" ht="47.25">
+    <row r="290" spans="1:6" ht="94.5">
       <c r="A290" s="3" t="s">
         <v>58</v>
       </c>
@@ -12725,7 +12744,7 @@
       <c r="E292" s="55"/>
       <c r="F292" s="25"/>
     </row>
-    <row r="293" spans="1:6" ht="31.5">
+    <row r="293" spans="1:6" ht="63">
       <c r="A293" s="3" t="s">
         <v>58</v>
       </c>
@@ -12759,7 +12778,7 @@
       <c r="E294" s="55"/>
       <c r="F294" s="3"/>
     </row>
-    <row r="295" spans="1:6">
+    <row r="295" spans="1:6" ht="31.5">
       <c r="A295" s="3" t="s">
         <v>58</v>
       </c>
@@ -12775,7 +12794,7 @@
       <c r="E295" s="55"/>
       <c r="F295" s="3"/>
     </row>
-    <row r="296" spans="1:6" ht="31.5">
+    <row r="296" spans="1:6" ht="47.25">
       <c r="A296" s="3" t="s">
         <v>58</v>
       </c>
@@ -12807,7 +12826,7 @@
       <c r="E297" s="55"/>
       <c r="F297" s="3"/>
     </row>
-    <row r="298" spans="1:6">
+    <row r="298" spans="1:6" ht="31.5">
       <c r="A298" s="3" t="s">
         <v>58</v>
       </c>
@@ -12839,7 +12858,7 @@
       <c r="E299" s="55"/>
       <c r="F299" s="3"/>
     </row>
-    <row r="300" spans="1:6">
+    <row r="300" spans="1:6" ht="31.5">
       <c r="A300" s="3" t="s">
         <v>58</v>
       </c>
@@ -12855,7 +12874,7 @@
       <c r="E300" s="55"/>
       <c r="F300" s="3"/>
     </row>
-    <row r="301" spans="1:6">
+    <row r="301" spans="1:6" ht="31.5">
       <c r="A301" s="3" t="s">
         <v>58</v>
       </c>
@@ -12871,7 +12890,7 @@
       <c r="E301" s="55"/>
       <c r="F301" s="3"/>
     </row>
-    <row r="302" spans="1:6" ht="31.5">
+    <row r="302" spans="1:6" ht="47.25">
       <c r="A302" s="3" t="s">
         <v>58</v>
       </c>
@@ -12887,7 +12906,7 @@
       <c r="E302" s="55"/>
       <c r="F302" s="3"/>
     </row>
-    <row r="303" spans="1:6" ht="31.5">
+    <row r="303" spans="1:6" ht="47.25">
       <c r="A303" s="3" t="s">
         <v>58</v>
       </c>
@@ -12903,7 +12922,7 @@
       <c r="E303" s="55"/>
       <c r="F303" s="3"/>
     </row>
-    <row r="304" spans="1:6" ht="31.5">
+    <row r="304" spans="1:6" ht="78.75">
       <c r="A304" s="3" t="s">
         <v>58</v>
       </c>
@@ -12919,7 +12938,7 @@
       <c r="E304" s="55"/>
       <c r="F304" s="3"/>
     </row>
-    <row r="305" spans="1:6" ht="47.25">
+    <row r="305" spans="1:6" ht="78.75">
       <c r="A305" s="3" t="s">
         <v>58</v>
       </c>
@@ -12935,7 +12954,7 @@
       <c r="E305" s="55"/>
       <c r="F305" s="3"/>
     </row>
-    <row r="306" spans="1:6" ht="47.25">
+    <row r="306" spans="1:6" ht="94.5">
       <c r="A306" s="3" t="s">
         <v>58</v>
       </c>
@@ -12951,7 +12970,7 @@
       <c r="E306" s="55"/>
       <c r="F306" s="3"/>
     </row>
-    <row r="307" spans="1:6" ht="47.25">
+    <row r="307" spans="1:6" ht="94.5">
       <c r="A307" s="3" t="s">
         <v>58</v>
       </c>
@@ -12967,7 +12986,7 @@
       <c r="E307" s="55"/>
       <c r="F307" s="3"/>
     </row>
-    <row r="308" spans="1:6" ht="31.5">
+    <row r="308" spans="1:6" ht="63">
       <c r="A308" s="3" t="s">
         <v>58</v>
       </c>
@@ -13025,7 +13044,7 @@
       <c r="E311" s="55"/>
       <c r="F311" s="25"/>
     </row>
-    <row r="312" spans="1:6" ht="63">
+    <row r="312" spans="1:6" ht="110.25">
       <c r="A312" s="3" t="s">
         <v>58</v>
       </c>
@@ -13043,7 +13062,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="313" spans="1:6">
+    <row r="313" spans="1:6" ht="31.5">
       <c r="A313" s="3" t="s">
         <v>58</v>
       </c>
@@ -13059,7 +13078,7 @@
       <c r="E313" s="55"/>
       <c r="F313" s="5"/>
     </row>
-    <row r="314" spans="1:6">
+    <row r="314" spans="1:6" ht="31.5">
       <c r="A314" s="3" t="s">
         <v>58</v>
       </c>
@@ -13134,7 +13153,7 @@
       </c>
       <c r="F318" s="3"/>
     </row>
-    <row r="319" spans="1:6">
+    <row r="319" spans="1:6" ht="31.5">
       <c r="A319" s="3" t="s">
         <v>58</v>
       </c>
@@ -13224,7 +13243,7 @@
       </c>
       <c r="F324" s="5"/>
     </row>
-    <row r="325" spans="1:6">
+    <row r="325" spans="1:6" ht="47.25">
       <c r="A325" s="3" t="s">
         <v>58</v>
       </c>
@@ -13252,7 +13271,7 @@
       <c r="D326" s="3"/>
       <c r="F326" s="18"/>
     </row>
-    <row r="327" spans="1:6" ht="47.25">
+    <row r="327" spans="1:6" ht="78.75">
       <c r="A327" s="3" t="s">
         <v>58</v>
       </c>
@@ -13272,7 +13291,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="328" spans="1:6" ht="31.5">
+    <row r="328" spans="1:6" ht="63">
       <c r="A328" s="3" t="s">
         <v>58</v>
       </c>
@@ -13290,7 +13309,7 @@
       </c>
       <c r="F328" s="5"/>
     </row>
-    <row r="329" spans="1:6">
+    <row r="329" spans="1:6" ht="31.5">
       <c r="A329" s="3" t="s">
         <v>58</v>
       </c>
@@ -13306,7 +13325,7 @@
       <c r="E329" s="55"/>
       <c r="F329" s="3"/>
     </row>
-    <row r="330" spans="1:6" ht="31.5">
+    <row r="330" spans="1:6" ht="47.25">
       <c r="A330" s="3" t="s">
         <v>58</v>
       </c>
@@ -13324,7 +13343,7 @@
       </c>
       <c r="F330" s="26"/>
     </row>
-    <row r="331" spans="1:6">
+    <row r="331" spans="1:6" ht="31.5">
       <c r="A331" s="3" t="s">
         <v>58</v>
       </c>
@@ -13422,7 +13441,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="337" spans="1:6">
+    <row r="337" spans="1:6" ht="31.5">
       <c r="A337" s="3" t="s">
         <v>58</v>
       </c>
@@ -13438,7 +13457,7 @@
       <c r="E337" s="60"/>
       <c r="F337" s="5"/>
     </row>
-    <row r="338" spans="1:6">
+    <row r="338" spans="1:6" ht="31.5">
       <c r="A338" s="3" t="s">
         <v>58</v>
       </c>
@@ -13470,7 +13489,7 @@
       <c r="E339" s="55"/>
       <c r="F339" s="26"/>
     </row>
-    <row r="340" spans="1:6">
+    <row r="340" spans="1:6" ht="31.5">
       <c r="A340" s="3" t="s">
         <v>58</v>
       </c>
@@ -13516,7 +13535,7 @@
       <c r="E342" s="55"/>
       <c r="F342" s="18"/>
     </row>
-    <row r="343" spans="1:6" ht="63">
+    <row r="343" spans="1:6" ht="110.25">
       <c r="A343" s="3" t="s">
         <v>58</v>
       </c>
@@ -13536,7 +13555,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="344" spans="1:6">
+    <row r="344" spans="1:6" ht="31.5">
       <c r="A344" s="3" t="s">
         <v>58</v>
       </c>
@@ -13554,7 +13573,7 @@
       </c>
       <c r="F344" s="5"/>
     </row>
-    <row r="345" spans="1:6">
+    <row r="345" spans="1:6" ht="31.5">
       <c r="A345" s="3" t="s">
         <v>58</v>
       </c>
@@ -13616,7 +13635,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="349" spans="1:6">
+    <row r="349" spans="1:6" ht="31.5">
       <c r="A349" s="3" t="s">
         <v>58</v>
       </c>
@@ -13632,7 +13651,7 @@
       <c r="E349" s="55"/>
       <c r="F349" s="5"/>
     </row>
-    <row r="350" spans="1:6" ht="31.5">
+    <row r="350" spans="1:6" ht="47.25">
       <c r="A350" s="3" t="s">
         <v>58</v>
       </c>
@@ -13648,7 +13667,7 @@
       <c r="E350" s="55"/>
       <c r="F350" s="5"/>
     </row>
-    <row r="351" spans="1:6" ht="31.5">
+    <row r="351" spans="1:6" ht="47.25">
       <c r="A351" s="3" t="s">
         <v>58</v>
       </c>
@@ -13666,7 +13685,7 @@
       </c>
       <c r="F351" s="5"/>
     </row>
-    <row r="352" spans="1:6">
+    <row r="352" spans="1:6" ht="31.5">
       <c r="A352" s="3" t="s">
         <v>58</v>
       </c>
@@ -13682,7 +13701,7 @@
       <c r="E352" s="55"/>
       <c r="F352" s="5"/>
     </row>
-    <row r="353" spans="1:6" ht="31.5">
+    <row r="353" spans="1:6" ht="47.25">
       <c r="A353" s="3" t="s">
         <v>58</v>
       </c>
@@ -13780,7 +13799,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="359" spans="1:6">
+    <row r="359" spans="1:6" ht="31.5">
       <c r="A359" s="3" t="s">
         <v>58</v>
       </c>
@@ -13796,7 +13815,7 @@
       <c r="E359" s="60"/>
       <c r="F359" s="26"/>
     </row>
-    <row r="360" spans="1:6">
+    <row r="360" spans="1:6" ht="31.5">
       <c r="A360" s="3" t="s">
         <v>58</v>
       </c>
@@ -13828,7 +13847,7 @@
       <c r="E361" s="55"/>
       <c r="F361" s="7"/>
     </row>
-    <row r="362" spans="1:6">
+    <row r="362" spans="1:6" ht="31.5">
       <c r="A362" s="3" t="s">
         <v>58</v>
       </c>
@@ -13874,7 +13893,7 @@
       <c r="E364" s="55"/>
       <c r="F364" s="21"/>
     </row>
-    <row r="365" spans="1:6" ht="47.25">
+    <row r="365" spans="1:6" ht="94.5">
       <c r="A365" s="3" t="s">
         <v>58</v>
       </c>
@@ -13892,7 +13911,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="366" spans="1:6">
+    <row r="366" spans="1:6" ht="31.5">
       <c r="A366" s="3" t="s">
         <v>58</v>
       </c>
@@ -13908,7 +13927,7 @@
       <c r="E366" s="55"/>
       <c r="F366" s="7"/>
     </row>
-    <row r="367" spans="1:6">
+    <row r="367" spans="1:6" ht="31.5">
       <c r="A367" s="3" t="s">
         <v>58</v>
       </c>
@@ -13952,7 +13971,7 @@
       <c r="E369" s="55"/>
       <c r="F369" s="21"/>
     </row>
-    <row r="370" spans="1:6">
+    <row r="370" spans="1:6" ht="47.25">
       <c r="A370" s="3" t="s">
         <v>58</v>
       </c>
@@ -13970,7 +13989,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="371" spans="1:6">
+    <row r="371" spans="1:6" ht="31.5">
       <c r="A371" s="3" t="s">
         <v>58</v>
       </c>
@@ -14002,7 +14021,7 @@
       <c r="E372" s="55"/>
       <c r="F372" s="26"/>
     </row>
-    <row r="373" spans="1:6" ht="31.5">
+    <row r="373" spans="1:6" ht="47.25">
       <c r="A373" s="3" t="s">
         <v>58</v>
       </c>
@@ -14018,7 +14037,7 @@
       <c r="E373" s="55"/>
       <c r="F373" s="26"/>
     </row>
-    <row r="374" spans="1:6">
+    <row r="374" spans="1:6" ht="31.5">
       <c r="A374" s="3" t="s">
         <v>58</v>
       </c>
@@ -14034,7 +14053,7 @@
       <c r="E374" s="55"/>
       <c r="F374" s="26"/>
     </row>
-    <row r="375" spans="1:6" ht="31.5">
+    <row r="375" spans="1:6" ht="47.25">
       <c r="A375" s="3" t="s">
         <v>58</v>
       </c>
@@ -14132,7 +14151,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="381" spans="1:6">
+    <row r="381" spans="1:6" ht="31.5">
       <c r="A381" s="3" t="s">
         <v>58</v>
       </c>
@@ -14148,7 +14167,7 @@
       <c r="E381" s="60"/>
       <c r="F381" s="26"/>
     </row>
-    <row r="382" spans="1:6">
+    <row r="382" spans="1:6" ht="31.5">
       <c r="A382" s="3" t="s">
         <v>58</v>
       </c>
@@ -14180,7 +14199,7 @@
       <c r="E383" s="55"/>
       <c r="F383" s="7"/>
     </row>
-    <row r="384" spans="1:6">
+    <row r="384" spans="1:6" ht="31.5">
       <c r="A384" s="3" t="s">
         <v>58</v>
       </c>
@@ -14226,7 +14245,7 @@
       <c r="E386" s="55"/>
       <c r="F386" s="21"/>
     </row>
-    <row r="387" spans="1:6" ht="47.25">
+    <row r="387" spans="1:6" ht="94.5">
       <c r="A387" s="3" t="s">
         <v>58</v>
       </c>
@@ -14244,7 +14263,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="388" spans="1:6">
+    <row r="388" spans="1:6" ht="31.5">
       <c r="A388" s="3" t="s">
         <v>58</v>
       </c>
@@ -14260,7 +14279,7 @@
       <c r="E388" s="55"/>
       <c r="F388" s="26"/>
     </row>
-    <row r="389" spans="1:6">
+    <row r="389" spans="1:6" ht="31.5">
       <c r="A389" s="3" t="s">
         <v>58</v>
       </c>
@@ -14354,7 +14373,7 @@
       <c r="E394" s="55"/>
       <c r="F394" s="26"/>
     </row>
-    <row r="395" spans="1:6">
+    <row r="395" spans="1:6" ht="31.5">
       <c r="A395" s="3" t="s">
         <v>58</v>
       </c>
@@ -14384,7 +14403,7 @@
       <c r="E396" s="55"/>
       <c r="F396" s="21"/>
     </row>
-    <row r="397" spans="1:6">
+    <row r="397" spans="1:6" ht="31.5">
       <c r="A397" s="3" t="s">
         <v>58</v>
       </c>
@@ -14402,7 +14421,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="398" spans="1:6">
+    <row r="398" spans="1:6" ht="31.5">
       <c r="A398" s="3" t="s">
         <v>58</v>
       </c>
@@ -14420,7 +14439,7 @@
       </c>
       <c r="F398" s="7"/>
     </row>
-    <row r="399" spans="1:6">
+    <row r="399" spans="1:6" ht="31.5">
       <c r="A399" s="3" t="s">
         <v>58</v>
       </c>
@@ -14486,7 +14505,7 @@
       <c r="E402" s="55"/>
       <c r="F402" s="5"/>
     </row>
-    <row r="403" spans="1:6">
+    <row r="403" spans="1:6" ht="31.5">
       <c r="A403" s="3" t="s">
         <v>58</v>
       </c>
@@ -14534,7 +14553,7 @@
       <c r="E405" s="55"/>
       <c r="F405" s="5"/>
     </row>
-    <row r="406" spans="1:6" ht="31.5">
+    <row r="406" spans="1:6" ht="47.25">
       <c r="A406" s="3" t="s">
         <v>58</v>
       </c>
@@ -14564,7 +14583,7 @@
       <c r="E407" s="55"/>
       <c r="F407" s="21"/>
     </row>
-    <row r="408" spans="1:6" ht="47.25">
+    <row r="408" spans="1:6" ht="78.75">
       <c r="A408" s="3" t="s">
         <v>58</v>
       </c>
@@ -14584,7 +14603,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="409" spans="1:6" ht="31.5">
+    <row r="409" spans="1:6" ht="63">
       <c r="A409" s="3" t="s">
         <v>58</v>
       </c>
@@ -14622,7 +14641,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="411" spans="1:6">
+    <row r="411" spans="1:6" ht="31.5">
       <c r="A411" s="3" t="s">
         <v>58</v>
       </c>
@@ -14702,7 +14721,7 @@
       <c r="E415" s="55"/>
       <c r="F415" s="21"/>
     </row>
-    <row r="416" spans="1:6">
+    <row r="416" spans="1:6" ht="31.5">
       <c r="A416" s="3" t="s">
         <v>58</v>
       </c>
@@ -14856,7 +14875,7 @@
       <c r="E425" s="55"/>
       <c r="F425" s="21"/>
     </row>
-    <row r="426" spans="1:6" ht="47.25">
+    <row r="426" spans="1:6" ht="94.5">
       <c r="A426" s="3" t="s">
         <v>58</v>
       </c>
@@ -14874,7 +14893,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="427" spans="1:6">
+    <row r="427" spans="1:6" ht="31.5">
       <c r="A427" s="3" t="s">
         <v>58</v>
       </c>
@@ -14890,7 +14909,7 @@
       <c r="E427" s="55"/>
       <c r="F427" s="26"/>
     </row>
-    <row r="428" spans="1:6">
+    <row r="428" spans="1:6" ht="31.5">
       <c r="A428" s="3" t="s">
         <v>58</v>
       </c>
@@ -14934,7 +14953,7 @@
       <c r="E430" s="55"/>
       <c r="F430" s="21"/>
     </row>
-    <row r="431" spans="1:6">
+    <row r="431" spans="1:6" ht="31.5">
       <c r="A431" s="3" t="s">
         <v>58</v>
       </c>
@@ -14984,7 +15003,7 @@
       <c r="E433" s="55"/>
       <c r="F433" s="7"/>
     </row>
-    <row r="434" spans="1:6">
+    <row r="434" spans="1:6" ht="31.5">
       <c r="A434" s="3" t="s">
         <v>58</v>
       </c>
@@ -15000,187 +15019,204 @@
       <c r="E434" s="55"/>
       <c r="F434" s="7"/>
     </row>
-    <row r="435" spans="1:6" ht="31.5">
+    <row r="435" spans="1:6">
       <c r="A435" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B435" s="3" t="s">
+      <c r="B435" s="40" t="s">
         <v>774</v>
       </c>
-      <c r="C435" s="3" t="s">
-        <v>775</v>
-      </c>
-      <c r="D435" s="3" t="s">
-        <v>589</v>
-      </c>
+      <c r="C435" s="40" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D435" s="3"/>
       <c r="E435" s="55"/>
       <c r="F435" s="7"/>
     </row>
-    <row r="436" spans="1:6">
+    <row r="436" spans="1:6" ht="63">
       <c r="A436" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B436" s="3" t="s">
-        <v>774</v>
+      <c r="B436" s="40" t="s">
+        <v>1149</v>
       </c>
       <c r="C436" s="3" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D436" s="3" t="s">
-        <v>728</v>
+        <v>589</v>
       </c>
       <c r="E436" s="55"/>
       <c r="F436" s="7"/>
     </row>
-    <row r="437" spans="1:6">
+    <row r="437" spans="1:6" ht="31.5">
       <c r="A437" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B437" s="3" t="s">
-        <v>777</v>
-      </c>
-      <c r="C437" s="13" t="s">
-        <v>624</v>
-      </c>
-      <c r="D437" s="3"/>
+      <c r="B437" s="40" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C437" s="40" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D437" s="3" t="s">
+        <v>728</v>
+      </c>
       <c r="E437" s="55"/>
-      <c r="F437" s="21"/>
+      <c r="F437" s="7"/>
     </row>
     <row r="438" spans="1:6">
       <c r="A438" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>778</v>
-      </c>
-      <c r="C438" s="5" t="s">
-        <v>626</v>
-      </c>
-      <c r="D438" s="3" t="s">
-        <v>600</v>
-      </c>
+        <v>777</v>
+      </c>
+      <c r="C438" s="13" t="s">
+        <v>624</v>
+      </c>
+      <c r="D438" s="3"/>
       <c r="E438" s="55"/>
-      <c r="F438" s="26" t="s">
-        <v>1123</v>
-      </c>
+      <c r="F438" s="21"/>
     </row>
     <row r="439" spans="1:6">
       <c r="A439" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>779</v>
-      </c>
-      <c r="C439" s="45" t="s">
-        <v>628</v>
-      </c>
-      <c r="D439" s="41" t="s">
-        <v>1122</v>
-      </c>
-      <c r="E439" s="54" t="s">
-        <v>1122</v>
-      </c>
-      <c r="F439" s="7"/>
+        <v>778</v>
+      </c>
+      <c r="C439" s="5" t="s">
+        <v>626</v>
+      </c>
+      <c r="D439" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="E439" s="55"/>
+      <c r="F439" s="26" t="s">
+        <v>1123</v>
+      </c>
     </row>
     <row r="440" spans="1:6">
       <c r="A440" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>780</v>
-      </c>
-      <c r="C440" s="13" t="s">
-        <v>630</v>
-      </c>
-      <c r="D440" s="3"/>
-      <c r="E440" s="55"/>
-      <c r="F440" s="21"/>
+        <v>779</v>
+      </c>
+      <c r="C440" s="45" t="s">
+        <v>628</v>
+      </c>
+      <c r="D440" s="41" t="s">
+        <v>1122</v>
+      </c>
+      <c r="E440" s="54" t="s">
+        <v>1122</v>
+      </c>
+      <c r="F440" s="7"/>
     </row>
     <row r="441" spans="1:6">
       <c r="A441" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>781</v>
-      </c>
-      <c r="C441" s="5" t="s">
-        <v>593</v>
-      </c>
-      <c r="D441" s="3" t="s">
-        <v>594</v>
-      </c>
+        <v>780</v>
+      </c>
+      <c r="C441" s="13" t="s">
+        <v>630</v>
+      </c>
+      <c r="D441" s="3"/>
       <c r="E441" s="55"/>
-      <c r="F441" s="8" t="s">
-        <v>1124</v>
-      </c>
+      <c r="F441" s="21"/>
     </row>
     <row r="442" spans="1:6">
       <c r="A442" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B442" s="3" t="s">
+        <v>781</v>
+      </c>
+      <c r="C442" s="5" t="s">
+        <v>593</v>
+      </c>
+      <c r="D442" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="E442" s="55"/>
+      <c r="F442" s="8" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" ht="31.5">
+      <c r="A443" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B443" s="3" t="s">
         <v>782</v>
       </c>
-      <c r="C442" s="5" t="s">
+      <c r="C443" s="5" t="s">
         <v>670</v>
       </c>
-      <c r="D442" s="3" t="s">
+      <c r="D443" s="3" t="s">
         <v>597</v>
-      </c>
-      <c r="E442" s="55"/>
-      <c r="F442" s="5"/>
-    </row>
-    <row r="443" spans="1:6">
-      <c r="A443" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B443" s="3" t="s">
-        <v>783</v>
-      </c>
-      <c r="C443" s="5" t="s">
-        <v>635</v>
-      </c>
-      <c r="D443" s="3" t="s">
-        <v>600</v>
       </c>
       <c r="E443" s="55"/>
       <c r="F443" s="5"/>
     </row>
-    <row r="444" spans="1:6">
+    <row r="444" spans="1:6" ht="31.5">
       <c r="A444" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>784</v>
-      </c>
-      <c r="C444" s="3" t="s">
-        <v>637</v>
+        <v>783</v>
+      </c>
+      <c r="C444" s="5" t="s">
+        <v>635</v>
       </c>
       <c r="D444" s="3" t="s">
-        <v>1128</v>
+        <v>600</v>
       </c>
       <c r="E444" s="55"/>
-      <c r="F444" s="3"/>
+      <c r="F444" s="5"/>
     </row>
     <row r="445" spans="1:6">
       <c r="A445" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>785</v>
-      </c>
-      <c r="C445" s="45" t="s">
-        <v>639</v>
-      </c>
-      <c r="D445" s="40" t="s">
-        <v>1125</v>
+        <v>784</v>
+      </c>
+      <c r="C445" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="D445" s="3" t="s">
+        <v>1128</v>
       </c>
       <c r="E445" s="55"/>
       <c r="F445" s="3"/>
+    </row>
+    <row r="446" spans="1:6" ht="31.5">
+      <c r="A446" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B446" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="C446" s="45" t="s">
+        <v>639</v>
+      </c>
+      <c r="D446" s="40" t="s">
+        <v>1125</v>
+      </c>
+      <c r="E446" s="55"/>
+      <c r="F446" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -15189,7 +15225,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AMK6"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
@@ -15336,7 +15374,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AMK43"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
@@ -16189,7 +16227,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:IV49"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
@@ -18643,7 +18681,7 @@
       <c r="F7" s="31" t="s">
         <v>794</v>
       </c>
-      <c r="G7" s="64" t="s">
+      <c r="G7" s="63" t="s">
         <v>1143</v>
       </c>
     </row>
@@ -18883,7 +18921,7 @@
       <c r="F19" s="31" t="s">
         <v>794</v>
       </c>
-      <c r="G19" s="64" t="s">
+      <c r="G19" s="63" t="s">
         <v>1144</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update spreadsheet/database with additional container OIDs
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\git\piv-conformance\conformancelib\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\gsa-devel\piv-conformance-swing\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1B1AA2-B6A1-4265-8875-474FBBF42034}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECEB31A-809D-4D5A-A1B9-ED5DC9B307A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3592" uniqueCount="1262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3644" uniqueCount="1262">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -4667,13 +4667,13 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="13.75" style="4" customWidth="1"/>
-    <col min="2" max="2" width="57.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="57.35546875" style="4" customWidth="1"/>
     <col min="3" max="5" width="10.5" style="4" customWidth="1"/>
-    <col min="6" max="256" width="8.83203125" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.83203125" style="27" customWidth="1"/>
+    <col min="6" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="27" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="27"/>
   </cols>
   <sheetData>
@@ -5330,7 +5330,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="31">
+    <row r="74" spans="1:5" ht="31.75">
       <c r="A74" s="3" t="s">
         <v>205</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="31">
+    <row r="85" spans="1:2" ht="31.75">
       <c r="A85" s="3" t="s">
         <v>217</v>
       </c>
@@ -5506,7 +5506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="31">
+    <row r="96" spans="1:2" ht="31.75">
       <c r="A96" s="3" t="s">
         <v>229</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="31">
+    <row r="114" spans="1:2" ht="31.75">
       <c r="A114" s="3" t="s">
         <v>255</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="28">
+    <row r="116" spans="1:2" ht="28.3">
       <c r="A116" s="3" t="s">
         <v>258</v>
       </c>
@@ -5706,7 +5706,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="46.5">
+    <row r="121" spans="1:2" ht="47.6">
       <c r="A121" s="3" t="s">
         <v>267</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="62">
+    <row r="123" spans="1:2" ht="63.45">
       <c r="A123" s="3" t="s">
         <v>272</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="31">
+    <row r="142" spans="1:2" ht="31.75">
       <c r="A142" s="3" t="s">
         <v>296</v>
       </c>
@@ -5890,7 +5890,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="31">
+    <row r="144" spans="1:2" ht="31.75">
       <c r="A144" s="3" t="s">
         <v>301</v>
       </c>
@@ -5898,7 +5898,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="46.5">
+    <row r="145" spans="1:2" ht="31.75">
       <c r="A145" s="3" t="s">
         <v>303</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="46.5">
+    <row r="146" spans="1:2" ht="47.6">
       <c r="A146" s="3" t="s">
         <v>305</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="46.5">
+    <row r="149" spans="1:2" ht="47.6">
       <c r="A149" s="3" t="s">
         <v>311</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="62">
+    <row r="151" spans="1:2" ht="47.6">
       <c r="A151" s="3" t="s">
         <v>315</v>
       </c>
@@ -5954,7 +5954,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="31">
+    <row r="152" spans="1:2" ht="31.75">
       <c r="A152" s="3" t="s">
         <v>317</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="31">
+    <row r="153" spans="1:2" ht="31.75">
       <c r="A153" s="3" t="s">
         <v>319</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="31">
+    <row r="161" spans="1:2" ht="31.75">
       <c r="A161" s="3" t="s">
         <v>327</v>
       </c>
@@ -6042,7 +6042,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="31">
+    <row r="163" spans="1:2" ht="31.75">
       <c r="A163" s="3" t="s">
         <v>329</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="31">
+    <row r="164" spans="1:2" ht="31.75">
       <c r="A164" s="3" t="s">
         <v>330</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="46.5">
+    <row r="165" spans="1:2" ht="47.6">
       <c r="A165" s="3" t="s">
         <v>332</v>
       </c>
@@ -6082,7 +6082,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="31">
+    <row r="168" spans="1:2" ht="31.75">
       <c r="A168" s="3" t="s">
         <v>336</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="62">
+    <row r="170" spans="1:2" ht="47.6">
       <c r="A170" s="3" t="s">
         <v>340</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="31">
+    <row r="171" spans="1:2" ht="31.75">
       <c r="A171" s="3" t="s">
         <v>341</v>
       </c>
@@ -6114,7 +6114,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="31">
+    <row r="172" spans="1:2" ht="31.75">
       <c r="A172" s="3" t="s">
         <v>342</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="46.5">
+    <row r="184" spans="1:2" ht="47.6">
       <c r="A184" s="3" t="s">
         <v>332</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="31">
+    <row r="187" spans="1:2" ht="31.75">
       <c r="A187" s="3" t="s">
         <v>360</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="62">
+    <row r="189" spans="1:2" ht="47.6">
       <c r="A189" s="3" t="s">
         <v>363</v>
       </c>
@@ -6258,7 +6258,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="31">
+    <row r="190" spans="1:2" ht="31.75">
       <c r="A190" s="3" t="s">
         <v>364</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="31">
+    <row r="191" spans="1:2" ht="31.75">
       <c r="A191" s="3" t="s">
         <v>365</v>
       </c>
@@ -6314,7 +6314,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="46.5">
+    <row r="197" spans="1:2" ht="47.6">
       <c r="A197" s="3" t="s">
         <v>375</v>
       </c>
@@ -6322,7 +6322,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="46.5">
+    <row r="198" spans="1:2" ht="47.6">
       <c r="A198" s="3" t="s">
         <v>377</v>
       </c>
@@ -6346,7 +6346,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="31">
+    <row r="201" spans="1:2" ht="31.75">
       <c r="A201" s="3" t="s">
         <v>382</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="31">
+    <row r="202" spans="1:2" ht="31.75">
       <c r="A202" s="3" t="s">
         <v>384</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="31">
+    <row r="215" spans="1:2" ht="31.75">
       <c r="A215" s="3" t="s">
         <v>409</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="46.5">
+    <row r="233" spans="1:2" ht="47.6">
       <c r="A233" s="3" t="s">
         <v>432</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="31">
+    <row r="235" spans="1:2" ht="31.75">
       <c r="A235" s="3" t="s">
         <v>439</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="31">
+    <row r="236" spans="1:2" ht="31.75">
       <c r="A236" s="3" t="s">
         <v>442</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="46.5">
+    <row r="239" spans="1:2" ht="47.6">
       <c r="A239" s="3" t="s">
         <v>451</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="46.5">
+    <row r="240" spans="1:2" ht="47.6">
       <c r="A240" s="3" t="s">
         <v>454</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="77.5">
+    <row r="241" spans="1:2" ht="79.3">
       <c r="A241" s="3" t="s">
         <v>457</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="46.5">
+    <row r="242" spans="1:2" ht="47.6">
       <c r="A242" s="3" t="s">
         <v>460</v>
       </c>
@@ -6682,7 +6682,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="77.5">
+    <row r="243" spans="1:2" ht="79.3">
       <c r="A243" s="3" t="s">
         <v>463</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="31">
+    <row r="244" spans="1:2" ht="31.75">
       <c r="A244" s="3" t="s">
         <v>466</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="46.5">
+    <row r="247" spans="1:2" ht="47.6">
       <c r="A247" s="3" t="s">
         <v>471</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="31">
+    <row r="249" spans="1:2" ht="31.75">
       <c r="A249" s="3" t="s">
         <v>476</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="31">
+    <row r="250" spans="1:2" ht="31.75">
       <c r="A250" s="3" t="s">
         <v>478</v>
       </c>
@@ -6770,7 +6770,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="31">
+    <row r="254" spans="1:2" ht="31.75">
       <c r="A254" s="3" t="s">
         <v>484</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="31">
+    <row r="255" spans="1:2" ht="31.75">
       <c r="A255" s="3" t="s">
         <v>486</v>
       </c>
@@ -6786,7 +6786,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="31">
+    <row r="256" spans="1:2" ht="31.75">
       <c r="A256" s="3" t="s">
         <v>489</v>
       </c>
@@ -6794,7 +6794,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="46.5">
+    <row r="257" spans="1:2" ht="47.6">
       <c r="A257" s="3" t="s">
         <v>491</v>
       </c>
@@ -6802,7 +6802,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="46.5">
+    <row r="258" spans="1:2" ht="47.6">
       <c r="A258" s="3" t="s">
         <v>494</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="62">
+    <row r="259" spans="1:2" ht="63.45">
       <c r="A259" s="3" t="s">
         <v>496</v>
       </c>
@@ -6818,7 +6818,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="77.5">
+    <row r="260" spans="1:2" ht="79.3">
       <c r="A260" s="3" t="s">
         <v>498</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="77.5">
+    <row r="261" spans="1:2" ht="79.3">
       <c r="A261" s="3" t="s">
         <v>500</v>
       </c>
@@ -6834,7 +6834,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="46.5">
+    <row r="262" spans="1:2" ht="47.6">
       <c r="A262" s="3" t="s">
         <v>503</v>
       </c>
@@ -6858,7 +6858,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="265" spans="1:2" ht="46.5">
+    <row r="265" spans="1:2" ht="47.6">
       <c r="A265" s="3" t="s">
         <v>507</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="31">
+    <row r="267" spans="1:2" ht="31.75">
       <c r="A267" s="3" t="s">
         <v>509</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="31">
+    <row r="268" spans="1:2" ht="31.75">
       <c r="A268" s="3" t="s">
         <v>510</v>
       </c>
@@ -6914,7 +6914,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="272" spans="1:2" ht="31">
+    <row r="272" spans="1:2" ht="31.75">
       <c r="A272" s="3" t="s">
         <v>514</v>
       </c>
@@ -6922,7 +6922,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="273" spans="1:2" ht="31">
+    <row r="273" spans="1:2" ht="31.75">
       <c r="A273" s="3" t="s">
         <v>515</v>
       </c>
@@ -6930,7 +6930,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="274" spans="1:2" ht="31">
+    <row r="274" spans="1:2" ht="31.75">
       <c r="A274" s="3" t="s">
         <v>516</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="275" spans="1:2" ht="46.5">
+    <row r="275" spans="1:2" ht="47.6">
       <c r="A275" s="3" t="s">
         <v>517</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="276" spans="1:2" ht="46.5">
+    <row r="276" spans="1:2" ht="47.6">
       <c r="A276" s="3" t="s">
         <v>518</v>
       </c>
@@ -6954,7 +6954,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="277" spans="1:2" ht="62">
+    <row r="277" spans="1:2" ht="63.45">
       <c r="A277" s="3" t="s">
         <v>519</v>
       </c>
@@ -6962,7 +6962,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="77.5">
+    <row r="278" spans="1:2" ht="79.3">
       <c r="A278" s="3" t="s">
         <v>520</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="279" spans="1:2" ht="77.5">
+    <row r="279" spans="1:2" ht="79.3">
       <c r="A279" s="3" t="s">
         <v>521</v>
       </c>
@@ -6978,7 +6978,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="280" spans="1:2" ht="46.5">
+    <row r="280" spans="1:2" ht="47.6">
       <c r="A280" s="3" t="s">
         <v>522</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="283" spans="1:2" ht="31">
+    <row r="283" spans="1:2" ht="31.75">
       <c r="A283" s="3" t="s">
         <v>524</v>
       </c>
@@ -7018,7 +7018,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="31">
+    <row r="285" spans="1:2" ht="31.75">
       <c r="A285" s="3" t="s">
         <v>528</v>
       </c>
@@ -7042,7 +7042,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="46.5">
+    <row r="288" spans="1:2" ht="47.6">
       <c r="A288" s="3" t="s">
         <v>537</v>
       </c>
@@ -7066,7 +7066,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="77.5">
+    <row r="291" spans="1:2" ht="79.3">
       <c r="A291" s="3" t="s">
         <v>545</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="46.5">
+    <row r="294" spans="1:2" ht="47.6">
       <c r="A294" s="3" t="s">
         <v>549</v>
       </c>
@@ -7106,7 +7106,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="31">
+    <row r="296" spans="1:2" ht="31.75">
       <c r="A296" s="3" t="s">
         <v>551</v>
       </c>
@@ -7114,7 +7114,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="31">
+    <row r="297" spans="1:2" ht="31.75">
       <c r="A297" s="3" t="s">
         <v>552</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="31">
+    <row r="301" spans="1:2" ht="31.75">
       <c r="A301" s="3" t="s">
         <v>556</v>
       </c>
@@ -7154,7 +7154,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="31">
+    <row r="302" spans="1:2" ht="31.75">
       <c r="A302" s="3" t="s">
         <v>557</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="31">
+    <row r="303" spans="1:2" ht="31.75">
       <c r="A303" s="3" t="s">
         <v>558</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="304" spans="1:2" ht="46.5">
+    <row r="304" spans="1:2" ht="47.6">
       <c r="A304" s="3" t="s">
         <v>559</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="305" spans="1:2" ht="46.5">
+    <row r="305" spans="1:2" ht="47.6">
       <c r="A305" s="3" t="s">
         <v>560</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="306" spans="1:2" ht="62">
+    <row r="306" spans="1:2" ht="63.45">
       <c r="A306" s="3" t="s">
         <v>561</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="307" spans="1:2" ht="77.5">
+    <row r="307" spans="1:2" ht="79.3">
       <c r="A307" s="3" t="s">
         <v>562</v>
       </c>
@@ -7202,7 +7202,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="308" spans="1:2" ht="77.5">
+    <row r="308" spans="1:2" ht="79.3">
       <c r="A308" s="3" t="s">
         <v>563</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="46.5">
+    <row r="309" spans="1:2" ht="47.6">
       <c r="A309" s="3" t="s">
         <v>564</v>
       </c>
@@ -7242,7 +7242,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="313" spans="1:2" ht="93">
+    <row r="313" spans="1:2" ht="95.15">
       <c r="A313" s="3" t="s">
         <v>566</v>
       </c>
@@ -7250,7 +7250,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="31">
+    <row r="314" spans="1:2" ht="31.75">
       <c r="A314" s="3" t="s">
         <v>569</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="31">
+    <row r="320" spans="1:2" ht="31.75">
       <c r="A320" s="3" t="s">
         <v>584</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="31">
+    <row r="324" spans="1:2" ht="31.75">
       <c r="A324" s="3" t="s">
         <v>595</v>
       </c>
@@ -7346,7 +7346,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="326" spans="1:2" ht="31">
+    <row r="326" spans="1:2" ht="31.75">
       <c r="A326" s="3" t="s">
         <v>601</v>
       </c>
@@ -7362,7 +7362,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="328" spans="1:2" ht="62">
+    <row r="328" spans="1:2" ht="63.45">
       <c r="A328" s="3" t="s">
         <v>607</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="329" spans="1:2" ht="46.5">
+    <row r="329" spans="1:2" ht="47.6">
       <c r="A329" s="3" t="s">
         <v>609</v>
       </c>
@@ -7386,7 +7386,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="331" spans="1:2" ht="31">
+    <row r="331" spans="1:2" ht="31.75">
       <c r="A331" s="3" t="s">
         <v>613</v>
       </c>
@@ -7394,7 +7394,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="332" spans="1:2" ht="31">
+    <row r="332" spans="1:2" ht="31.75">
       <c r="A332" s="3" t="s">
         <v>616</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="339" spans="1:2" ht="31">
+    <row r="339" spans="1:2" ht="31.75">
       <c r="A339" s="3" t="s">
         <v>630</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="344" spans="1:2" ht="93">
+    <row r="344" spans="1:2" ht="95.15">
       <c r="A344" s="3" t="s">
         <v>638</v>
       </c>
@@ -7498,7 +7498,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="31">
+    <row r="345" spans="1:2" ht="31.75">
       <c r="A345" s="3" t="s">
         <v>639</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="31">
+    <row r="351" spans="1:2" ht="31.75">
       <c r="A351" s="3" t="s">
         <v>652</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="352" spans="1:2" ht="31">
+    <row r="352" spans="1:2" ht="31.75">
       <c r="A352" s="3" t="s">
         <v>654</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="353" spans="1:2" ht="31">
+    <row r="353" spans="1:2" ht="31.75">
       <c r="A353" s="3" t="s">
         <v>656</v>
       </c>
@@ -7570,7 +7570,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="354" spans="1:2" ht="46.5">
+    <row r="354" spans="1:2" ht="47.6">
       <c r="A354" s="3" t="s">
         <v>658</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="361" spans="1:2" ht="31">
+    <row r="361" spans="1:2" ht="31.75">
       <c r="A361" s="3" t="s">
         <v>667</v>
       </c>
@@ -7666,7 +7666,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="77.5">
+    <row r="366" spans="1:2" ht="79.3">
       <c r="A366" s="3" t="s">
         <v>671</v>
       </c>
@@ -7674,7 +7674,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="367" spans="1:2" ht="31">
+    <row r="367" spans="1:2" ht="31.75">
       <c r="A367" s="3" t="s">
         <v>673</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="371" spans="1:2" ht="31">
+    <row r="371" spans="1:2" ht="31.75">
       <c r="A371" s="3" t="s">
         <v>679</v>
       </c>
@@ -7714,7 +7714,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="372" spans="1:2" ht="31">
+    <row r="372" spans="1:2" ht="31.75">
       <c r="A372" s="3" t="s">
         <v>682</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="31">
+    <row r="374" spans="1:2" ht="31.75">
       <c r="A374" s="3" t="s">
         <v>687</v>
       </c>
@@ -7738,7 +7738,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="31">
+    <row r="375" spans="1:2" ht="31.75">
       <c r="A375" s="3" t="s">
         <v>689</v>
       </c>
@@ -7746,7 +7746,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="376" spans="1:2" ht="46.5">
+    <row r="376" spans="1:2" ht="47.6">
       <c r="A376" s="3" t="s">
         <v>691</v>
       </c>
@@ -7802,7 +7802,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="383" spans="1:2" ht="31">
+    <row r="383" spans="1:2" ht="31.75">
       <c r="A383" s="3" t="s">
         <v>698</v>
       </c>
@@ -7842,7 +7842,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="388" spans="1:2" ht="77.5">
+    <row r="388" spans="1:2" ht="79.3">
       <c r="A388" s="3" t="s">
         <v>702</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="389" spans="1:2" ht="31">
+    <row r="389" spans="1:2" ht="31.75">
       <c r="A389" s="3" t="s">
         <v>703</v>
       </c>
@@ -7906,7 +7906,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="396" spans="1:2" ht="31">
+    <row r="396" spans="1:2" ht="31.75">
       <c r="A396" s="3" t="s">
         <v>714</v>
       </c>
@@ -7930,7 +7930,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="399" spans="1:2" ht="31">
+    <row r="399" spans="1:2" ht="31.75">
       <c r="A399" s="3" t="s">
         <v>722</v>
       </c>
@@ -7970,7 +7970,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="404" spans="1:2" ht="31">
+    <row r="404" spans="1:2" ht="31.75">
       <c r="A404" s="3" t="s">
         <v>732</v>
       </c>
@@ -7994,7 +7994,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="407" spans="1:2" ht="31">
+    <row r="407" spans="1:2" ht="31.75">
       <c r="A407" s="3" t="s">
         <v>735</v>
       </c>
@@ -8010,7 +8010,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="62">
+    <row r="409" spans="1:2" ht="63.45">
       <c r="A409" s="3" t="s">
         <v>737</v>
       </c>
@@ -8018,7 +8018,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="410" spans="1:2" ht="46.5">
+    <row r="410" spans="1:2" ht="47.6">
       <c r="A410" s="3" t="s">
         <v>739</v>
       </c>
@@ -8034,7 +8034,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="412" spans="1:2" ht="31">
+    <row r="412" spans="1:2" ht="31.75">
       <c r="A412" s="3" t="s">
         <v>742</v>
       </c>
@@ -8090,7 +8090,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="419" spans="1:2" ht="31">
+    <row r="419" spans="1:2" ht="31.75">
       <c r="A419" s="3" t="s">
         <v>749</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="431" spans="1:2" ht="77.5">
+    <row r="431" spans="1:2" ht="79.3">
       <c r="A431" s="3" t="s">
         <v>758</v>
       </c>
@@ -8194,7 +8194,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="432" spans="1:2" ht="31">
+    <row r="432" spans="1:2" ht="31.75">
       <c r="A432" s="3" t="s">
         <v>759</v>
       </c>
@@ -8250,7 +8250,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="439" spans="1:2" ht="31">
+    <row r="439" spans="1:2" ht="31.75">
       <c r="A439" s="3" t="s">
         <v>768</v>
       </c>
@@ -8258,7 +8258,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="440" spans="1:2" ht="46.5">
+    <row r="440" spans="1:2" ht="47.6">
       <c r="A440" s="3" t="s">
         <v>770</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="448" spans="1:2" ht="31">
+    <row r="448" spans="1:2" ht="31.75">
       <c r="A448" s="3" t="s">
         <v>779</v>
       </c>
@@ -8361,25 +8361,25 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H459"/>
   <sheetViews>
-    <sheetView topLeftCell="A210" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D219" sqref="D219"/>
+    <sheetView tabSelected="1" topLeftCell="C190" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F190" sqref="F190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="14.25" style="4" customWidth="1"/>
+    <col min="1" max="1" width="14.2109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="12" style="4" customWidth="1"/>
-    <col min="3" max="3" width="43.75" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.83203125" style="52" customWidth="1"/>
-    <col min="6" max="6" width="67.58203125" style="52" customWidth="1"/>
-    <col min="7" max="7" width="84.58203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="43.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20.35546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="52" customWidth="1"/>
+    <col min="6" max="6" width="67.5703125" style="52" customWidth="1"/>
+    <col min="7" max="7" width="84.5703125" style="4" customWidth="1"/>
     <col min="8" max="8" width="9" style="64"/>
     <col min="9" max="1027" width="8.5" style="27" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="60" customFormat="1" ht="18.5">
+    <row r="1" spans="1:8" s="60" customFormat="1" ht="18.45">
       <c r="A1" s="51" t="s">
         <v>52</v>
       </c>
@@ -8433,7 +8433,7 @@
       <c r="F3" s="56"/>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:8" ht="31">
+    <row r="4" spans="1:8" ht="31.75">
       <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
@@ -8454,7 +8454,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="31">
+    <row r="5" spans="1:8" ht="31.75">
       <c r="A5" s="3" t="s">
         <v>58</v>
       </c>
@@ -8492,7 +8492,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:8" ht="31">
+    <row r="7" spans="1:8" ht="31.75">
       <c r="A7" s="3" t="s">
         <v>58</v>
       </c>
@@ -8511,7 +8511,7 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="31">
+    <row r="8" spans="1:8" ht="31.75">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
@@ -8549,7 +8549,7 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:8" ht="31">
+    <row r="10" spans="1:8" ht="31.75">
       <c r="A10" s="3" t="s">
         <v>58</v>
       </c>
@@ -8568,7 +8568,7 @@
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:8" ht="46.5">
+    <row r="11" spans="1:8" ht="47.6">
       <c r="A11" s="3" t="s">
         <v>58</v>
       </c>
@@ -8587,7 +8587,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="31">
+    <row r="12" spans="1:8" ht="31.75">
       <c r="A12" s="3" t="s">
         <v>58</v>
       </c>
@@ -8606,7 +8606,7 @@
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="31">
+    <row r="13" spans="1:8" ht="31.75">
       <c r="A13" s="3" t="s">
         <v>58</v>
       </c>
@@ -8659,7 +8659,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="10"/>
     </row>
-    <row r="16" spans="1:8" ht="31">
+    <row r="16" spans="1:8" ht="31.75">
       <c r="A16" s="3" t="s">
         <v>58</v>
       </c>
@@ -8680,7 +8680,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="31">
+    <row r="17" spans="1:7" ht="31.75">
       <c r="A17" s="3" t="s">
         <v>58</v>
       </c>
@@ -8718,7 +8718,7 @@
       </c>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="31">
+    <row r="19" spans="1:7" ht="31.75">
       <c r="A19" s="3" t="s">
         <v>58</v>
       </c>
@@ -8775,7 +8775,7 @@
       </c>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="31">
+    <row r="22" spans="1:7" ht="31.75">
       <c r="A22" s="65" t="s">
         <v>58</v>
       </c>
@@ -8794,7 +8794,7 @@
       </c>
       <c r="G22" s="65"/>
     </row>
-    <row r="23" spans="1:7" ht="31">
+    <row r="23" spans="1:7" ht="31.75">
       <c r="A23" s="3" t="s">
         <v>58</v>
       </c>
@@ -8925,7 +8925,7 @@
       </c>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" ht="31">
+    <row r="30" spans="1:7" ht="47.6">
       <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
@@ -9020,7 +9020,7 @@
       </c>
       <c r="G34" s="65"/>
     </row>
-    <row r="35" spans="1:7" ht="31">
+    <row r="35" spans="1:7" ht="31.75">
       <c r="A35" s="3" t="s">
         <v>58</v>
       </c>
@@ -9077,7 +9077,7 @@
       </c>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" ht="46.5">
+    <row r="38" spans="1:7" ht="47.6">
       <c r="A38" s="3" t="s">
         <v>58</v>
       </c>
@@ -9149,7 +9149,7 @@
       <c r="F41" s="3"/>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" spans="1:7" ht="31">
+    <row r="42" spans="1:7" ht="31.75">
       <c r="A42" s="3" t="s">
         <v>58</v>
       </c>
@@ -9170,7 +9170,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="31">
+    <row r="43" spans="1:7" ht="31.75">
       <c r="A43" s="3" t="s">
         <v>58</v>
       </c>
@@ -9208,7 +9208,7 @@
       </c>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" ht="31">
+    <row r="45" spans="1:7" ht="31.75">
       <c r="A45" s="3" t="s">
         <v>58</v>
       </c>
@@ -9265,7 +9265,7 @@
       </c>
       <c r="G47" s="3"/>
     </row>
-    <row r="48" spans="1:7" ht="31">
+    <row r="48" spans="1:7" ht="31.75">
       <c r="A48" s="3" t="s">
         <v>58</v>
       </c>
@@ -9284,7 +9284,7 @@
       </c>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:7" ht="31">
+    <row r="49" spans="1:7" ht="31.75">
       <c r="A49" s="3" t="s">
         <v>58</v>
       </c>
@@ -9303,7 +9303,7 @@
       </c>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="1:7" ht="31">
+    <row r="50" spans="1:7" ht="31.75">
       <c r="A50" s="3" t="s">
         <v>58</v>
       </c>
@@ -9356,7 +9356,7 @@
       <c r="F52" s="53"/>
       <c r="G52" s="10"/>
     </row>
-    <row r="53" spans="1:7" ht="31">
+    <row r="53" spans="1:7" ht="31.75">
       <c r="A53" s="3" t="s">
         <v>58</v>
       </c>
@@ -9377,7 +9377,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="31">
+    <row r="54" spans="1:7" ht="31.75">
       <c r="A54" s="3" t="s">
         <v>58</v>
       </c>
@@ -9415,7 +9415,7 @@
       </c>
       <c r="G55" s="3"/>
     </row>
-    <row r="56" spans="1:7" ht="31">
+    <row r="56" spans="1:7" ht="31.75">
       <c r="A56" s="3" t="s">
         <v>58</v>
       </c>
@@ -9453,7 +9453,7 @@
       </c>
       <c r="G57" s="3"/>
     </row>
-    <row r="58" spans="1:7" ht="31">
+    <row r="58" spans="1:7" ht="31.75">
       <c r="A58" s="3" t="s">
         <v>58</v>
       </c>
@@ -9472,7 +9472,7 @@
       </c>
       <c r="G58" s="3"/>
     </row>
-    <row r="59" spans="1:7" ht="31">
+    <row r="59" spans="1:7" ht="31.75">
       <c r="A59" s="3" t="s">
         <v>58</v>
       </c>
@@ -9491,7 +9491,7 @@
       </c>
       <c r="G59" s="3"/>
     </row>
-    <row r="60" spans="1:7" ht="31">
+    <row r="60" spans="1:7" ht="31.75">
       <c r="A60" s="3" t="s">
         <v>58</v>
       </c>
@@ -9544,7 +9544,7 @@
       <c r="F62" s="53"/>
       <c r="G62" s="10"/>
     </row>
-    <row r="63" spans="1:7" ht="31">
+    <row r="63" spans="1:7" ht="31.75">
       <c r="A63" s="3" t="s">
         <v>58</v>
       </c>
@@ -9565,7 +9565,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="31">
+    <row r="64" spans="1:7" ht="31.75">
       <c r="A64" s="3" t="s">
         <v>58</v>
       </c>
@@ -9603,7 +9603,7 @@
       </c>
       <c r="G65" s="3"/>
     </row>
-    <row r="66" spans="1:7" ht="31">
+    <row r="66" spans="1:7" ht="31.75">
       <c r="A66" s="3" t="s">
         <v>58</v>
       </c>
@@ -9641,7 +9641,7 @@
       </c>
       <c r="G67" s="3"/>
     </row>
-    <row r="68" spans="1:7" ht="31">
+    <row r="68" spans="1:7" ht="31.75">
       <c r="A68" s="3" t="s">
         <v>58</v>
       </c>
@@ -9698,7 +9698,7 @@
       </c>
       <c r="G70" s="65"/>
     </row>
-    <row r="71" spans="1:7" ht="31">
+    <row r="71" spans="1:7" ht="31.75">
       <c r="A71" s="3" t="s">
         <v>58</v>
       </c>
@@ -9717,7 +9717,7 @@
       </c>
       <c r="G71" s="3"/>
     </row>
-    <row r="72" spans="1:7" ht="31">
+    <row r="72" spans="1:7" ht="31.75">
       <c r="A72" s="3" t="s">
         <v>58</v>
       </c>
@@ -9736,7 +9736,7 @@
       </c>
       <c r="G72" s="3"/>
     </row>
-    <row r="73" spans="1:7" ht="31">
+    <row r="73" spans="1:7" ht="31.75">
       <c r="A73" s="3" t="s">
         <v>58</v>
       </c>
@@ -9789,7 +9789,7 @@
       <c r="F75" s="53"/>
       <c r="G75" s="10"/>
     </row>
-    <row r="76" spans="1:7" ht="31">
+    <row r="76" spans="1:7" ht="31.75">
       <c r="A76" s="3" t="s">
         <v>58</v>
       </c>
@@ -9810,7 +9810,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="31">
+    <row r="77" spans="1:7" ht="31.75">
       <c r="A77" s="3" t="s">
         <v>58</v>
       </c>
@@ -9848,7 +9848,7 @@
       </c>
       <c r="G78" s="3"/>
     </row>
-    <row r="79" spans="1:7" ht="31">
+    <row r="79" spans="1:7" ht="31.75">
       <c r="A79" s="3" t="s">
         <v>58</v>
       </c>
@@ -9867,7 +9867,7 @@
       </c>
       <c r="G79" s="3"/>
     </row>
-    <row r="80" spans="1:7" ht="31">
+    <row r="80" spans="1:7" ht="31.75">
       <c r="A80" s="3" t="s">
         <v>58</v>
       </c>
@@ -9886,7 +9886,7 @@
       </c>
       <c r="G80" s="3"/>
     </row>
-    <row r="81" spans="1:7" ht="31">
+    <row r="81" spans="1:7" ht="31.75">
       <c r="A81" s="3" t="s">
         <v>58</v>
       </c>
@@ -9958,7 +9958,7 @@
       <c r="F84" s="53"/>
       <c r="G84" s="10"/>
     </row>
-    <row r="85" spans="1:7" ht="31">
+    <row r="85" spans="1:7" ht="31.75">
       <c r="A85" s="3" t="s">
         <v>58</v>
       </c>
@@ -9979,7 +9979,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="31">
+    <row r="86" spans="1:7" ht="31.75">
       <c r="A86" s="3" t="s">
         <v>58</v>
       </c>
@@ -10017,7 +10017,7 @@
       </c>
       <c r="G87" s="3"/>
     </row>
-    <row r="88" spans="1:7" ht="31">
+    <row r="88" spans="1:7" ht="31.75">
       <c r="A88" s="3" t="s">
         <v>58</v>
       </c>
@@ -10074,7 +10074,7 @@
       </c>
       <c r="G90" s="3"/>
     </row>
-    <row r="91" spans="1:7" ht="31">
+    <row r="91" spans="1:7" ht="31.75">
       <c r="A91" s="3" t="s">
         <v>58</v>
       </c>
@@ -10093,7 +10093,7 @@
       </c>
       <c r="G91" s="3"/>
     </row>
-    <row r="92" spans="1:7" ht="31">
+    <row r="92" spans="1:7" ht="31.75">
       <c r="A92" s="3" t="s">
         <v>58</v>
       </c>
@@ -10112,7 +10112,7 @@
       </c>
       <c r="G92" s="3"/>
     </row>
-    <row r="93" spans="1:7" ht="31">
+    <row r="93" spans="1:7" ht="31.75">
       <c r="A93" s="3" t="s">
         <v>58</v>
       </c>
@@ -10165,7 +10165,7 @@
       <c r="F95" s="53"/>
       <c r="G95" s="10"/>
     </row>
-    <row r="96" spans="1:7" ht="31">
+    <row r="96" spans="1:7" ht="31.75">
       <c r="A96" s="3" t="s">
         <v>58</v>
       </c>
@@ -10186,7 +10186,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="31">
+    <row r="97" spans="1:7" ht="31.75">
       <c r="A97" s="3" t="s">
         <v>58</v>
       </c>
@@ -10224,7 +10224,7 @@
       </c>
       <c r="G98" s="3"/>
     </row>
-    <row r="99" spans="1:7" ht="31">
+    <row r="99" spans="1:7" ht="31.75">
       <c r="A99" s="3" t="s">
         <v>58</v>
       </c>
@@ -10281,7 +10281,7 @@
       </c>
       <c r="G101" s="3"/>
     </row>
-    <row r="102" spans="1:7" ht="31">
+    <row r="102" spans="1:7" ht="31.75">
       <c r="A102" s="3" t="s">
         <v>58</v>
       </c>
@@ -10300,7 +10300,7 @@
       </c>
       <c r="G102" s="3"/>
     </row>
-    <row r="103" spans="1:7" ht="31">
+    <row r="103" spans="1:7" ht="31.75">
       <c r="A103" s="3" t="s">
         <v>58</v>
       </c>
@@ -10319,7 +10319,7 @@
       </c>
       <c r="G103" s="3"/>
     </row>
-    <row r="104" spans="1:7" ht="31">
+    <row r="104" spans="1:7" ht="31.75">
       <c r="A104" s="3" t="s">
         <v>58</v>
       </c>
@@ -10372,7 +10372,7 @@
       <c r="F106" s="53"/>
       <c r="G106" s="10"/>
     </row>
-    <row r="107" spans="1:7" ht="31">
+    <row r="107" spans="1:7" ht="31.75">
       <c r="A107" s="3" t="s">
         <v>58</v>
       </c>
@@ -10393,7 +10393,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="31">
+    <row r="108" spans="1:7" ht="31.75">
       <c r="A108" s="3" t="s">
         <v>58</v>
       </c>
@@ -10431,7 +10431,7 @@
       </c>
       <c r="G109" s="3"/>
     </row>
-    <row r="110" spans="1:7" ht="31">
+    <row r="110" spans="1:7" ht="31.75">
       <c r="A110" s="3" t="s">
         <v>58</v>
       </c>
@@ -10488,7 +10488,7 @@
       </c>
       <c r="G112" s="3"/>
     </row>
-    <row r="113" spans="1:7" ht="31">
+    <row r="113" spans="1:7" ht="31.75">
       <c r="A113" s="3" t="s">
         <v>58</v>
       </c>
@@ -10507,7 +10507,7 @@
       </c>
       <c r="G113" s="3"/>
     </row>
-    <row r="114" spans="1:7" ht="31">
+    <row r="114" spans="1:7" ht="31.75">
       <c r="A114" s="3" t="s">
         <v>58</v>
       </c>
@@ -10526,7 +10526,7 @@
       </c>
       <c r="G114" s="3"/>
     </row>
-    <row r="115" spans="1:7" ht="31">
+    <row r="115" spans="1:7" ht="31.75">
       <c r="A115" s="3" t="s">
         <v>58</v>
       </c>
@@ -10579,7 +10579,7 @@
       <c r="F117" s="53"/>
       <c r="G117" s="10"/>
     </row>
-    <row r="118" spans="1:7" ht="31">
+    <row r="118" spans="1:7" ht="31.75">
       <c r="A118" s="3" t="s">
         <v>58</v>
       </c>
@@ -10600,7 +10600,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="31">
+    <row r="119" spans="1:7" ht="31.75">
       <c r="A119" s="3" t="s">
         <v>58</v>
       </c>
@@ -10638,7 +10638,7 @@
       </c>
       <c r="G120" s="3"/>
     </row>
-    <row r="121" spans="1:7" ht="31">
+    <row r="121" spans="1:7" ht="31.75">
       <c r="A121" s="3" t="s">
         <v>58</v>
       </c>
@@ -10733,7 +10733,7 @@
       </c>
       <c r="G125" s="3"/>
     </row>
-    <row r="126" spans="1:7" ht="46.5">
+    <row r="126" spans="1:7" ht="47.6">
       <c r="A126" s="3" t="s">
         <v>58</v>
       </c>
@@ -10767,7 +10767,7 @@
       <c r="F127" s="53"/>
       <c r="G127" s="10"/>
     </row>
-    <row r="128" spans="1:7" ht="28">
+    <row r="128" spans="1:7" ht="28.3">
       <c r="A128" s="3" t="s">
         <v>58</v>
       </c>
@@ -10790,7 +10790,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="28">
+    <row r="129" spans="1:7" ht="28.3">
       <c r="A129" s="3" t="s">
         <v>58</v>
       </c>
@@ -10832,7 +10832,7 @@
       </c>
       <c r="G130" s="11"/>
     </row>
-    <row r="131" spans="1:7" ht="28">
+    <row r="131" spans="1:7" ht="28.3">
       <c r="A131" s="3" t="s">
         <v>58</v>
       </c>
@@ -10895,7 +10895,7 @@
       </c>
       <c r="G133" s="3"/>
     </row>
-    <row r="134" spans="1:7" ht="31">
+    <row r="134" spans="1:7" ht="31.75">
       <c r="A134" s="65" t="s">
         <v>58</v>
       </c>
@@ -10914,7 +10914,7 @@
       </c>
       <c r="G134" s="65"/>
     </row>
-    <row r="135" spans="1:7" ht="31">
+    <row r="135" spans="1:7" ht="31.75">
       <c r="A135" s="3" t="s">
         <v>58</v>
       </c>
@@ -10935,7 +10935,7 @@
       </c>
       <c r="G135" s="3"/>
     </row>
-    <row r="136" spans="1:7" ht="77.5">
+    <row r="136" spans="1:7" ht="79.3">
       <c r="A136" s="3" t="s">
         <v>58</v>
       </c>
@@ -10956,7 +10956,7 @@
       </c>
       <c r="G136" s="3"/>
     </row>
-    <row r="137" spans="1:7" ht="31">
+    <row r="137" spans="1:7" ht="31.75">
       <c r="A137" s="3" t="s">
         <v>131</v>
       </c>
@@ -11030,7 +11030,7 @@
       <c r="F140" s="53"/>
       <c r="G140" s="10"/>
     </row>
-    <row r="141" spans="1:7" ht="31">
+    <row r="141" spans="1:7" ht="31.75">
       <c r="A141" s="3" t="s">
         <v>58</v>
       </c>
@@ -11051,7 +11051,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="31">
+    <row r="142" spans="1:7" ht="31.75">
       <c r="A142" s="3" t="s">
         <v>58</v>
       </c>
@@ -11072,7 +11072,7 @@
         <v>1140</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="31">
+    <row r="143" spans="1:7" ht="31.75">
       <c r="A143" s="3" t="s">
         <v>58</v>
       </c>
@@ -11189,7 +11189,7 @@
       <c r="F149" s="53"/>
       <c r="G149" s="18"/>
     </row>
-    <row r="150" spans="1:7" ht="31">
+    <row r="150" spans="1:7" ht="31.75">
       <c r="A150" s="3" t="s">
         <v>58</v>
       </c>
@@ -11274,7 +11274,7 @@
       <c r="F154" s="53"/>
       <c r="G154" s="18"/>
     </row>
-    <row r="155" spans="1:7" ht="31">
+    <row r="155" spans="1:7" ht="31.75">
       <c r="A155" s="3" t="s">
         <v>58</v>
       </c>
@@ -11293,7 +11293,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="31">
+    <row r="156" spans="1:7" ht="31.75">
       <c r="A156" s="3" t="s">
         <v>58</v>
       </c>
@@ -11310,7 +11310,7 @@
       <c r="F156" s="53"/>
       <c r="G156" s="3"/>
     </row>
-    <row r="157" spans="1:7" ht="46.5">
+    <row r="157" spans="1:7" ht="47.6">
       <c r="A157" s="3" t="s">
         <v>58</v>
       </c>
@@ -11344,7 +11344,7 @@
       <c r="F158" s="62"/>
       <c r="G158" s="3"/>
     </row>
-    <row r="159" spans="1:7" ht="46.5">
+    <row r="159" spans="1:7" ht="47.6">
       <c r="A159" s="3" t="s">
         <v>58</v>
       </c>
@@ -11361,7 +11361,7 @@
       <c r="F159" s="62"/>
       <c r="G159" s="3"/>
     </row>
-    <row r="160" spans="1:7" ht="31">
+    <row r="160" spans="1:7" ht="31.75">
       <c r="A160" s="3" t="s">
         <v>58</v>
       </c>
@@ -11378,7 +11378,7 @@
       <c r="F160" s="62"/>
       <c r="G160" s="3"/>
     </row>
-    <row r="161" spans="1:7" ht="31">
+    <row r="161" spans="1:7" ht="31.75">
       <c r="A161" s="3" t="s">
         <v>58</v>
       </c>
@@ -11395,7 +11395,7 @@
       <c r="F161" s="62"/>
       <c r="G161" s="3"/>
     </row>
-    <row r="162" spans="1:7" ht="62">
+    <row r="162" spans="1:7" ht="63.45">
       <c r="A162" s="3" t="s">
         <v>58</v>
       </c>
@@ -11429,7 +11429,7 @@
       <c r="F163" s="62"/>
       <c r="G163" s="39"/>
     </row>
-    <row r="164" spans="1:7" ht="77.5">
+    <row r="164" spans="1:7" ht="63.45">
       <c r="A164" s="3" t="s">
         <v>58</v>
       </c>
@@ -11446,7 +11446,7 @@
       <c r="F164" s="53"/>
       <c r="G164" s="3"/>
     </row>
-    <row r="165" spans="1:7" ht="46.5">
+    <row r="165" spans="1:7" ht="47.6">
       <c r="A165" s="3" t="s">
         <v>58</v>
       </c>
@@ -11463,7 +11463,7 @@
       <c r="F165" s="53"/>
       <c r="G165" s="3"/>
     </row>
-    <row r="166" spans="1:7" ht="31">
+    <row r="166" spans="1:7" ht="31.75">
       <c r="A166" s="3" t="s">
         <v>58</v>
       </c>
@@ -11510,7 +11510,7 @@
       <c r="F168" s="53"/>
       <c r="G168" s="18"/>
     </row>
-    <row r="169" spans="1:7" ht="31">
+    <row r="169" spans="1:7" ht="31.75">
       <c r="A169" s="3" t="s">
         <v>58</v>
       </c>
@@ -11595,7 +11595,7 @@
       <c r="F173" s="53"/>
       <c r="G173" s="18"/>
     </row>
-    <row r="174" spans="1:7" ht="31">
+    <row r="174" spans="1:7" ht="31.75">
       <c r="A174" s="3" t="s">
         <v>58</v>
       </c>
@@ -11614,7 +11614,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="175" spans="1:7" ht="31">
+    <row r="175" spans="1:7" ht="31.75">
       <c r="A175" s="3" t="s">
         <v>58</v>
       </c>
@@ -11631,7 +11631,7 @@
       <c r="F175" s="53"/>
       <c r="G175" s="3"/>
     </row>
-    <row r="176" spans="1:7" ht="46.5">
+    <row r="176" spans="1:7" ht="47.6">
       <c r="A176" s="3" t="s">
         <v>58</v>
       </c>
@@ -11665,7 +11665,7 @@
       <c r="F177" s="62"/>
       <c r="G177" s="3"/>
     </row>
-    <row r="178" spans="1:7" ht="46.5">
+    <row r="178" spans="1:7" ht="47.6">
       <c r="A178" s="3" t="s">
         <v>58</v>
       </c>
@@ -11682,7 +11682,7 @@
       <c r="F178" s="62"/>
       <c r="G178" s="3"/>
     </row>
-    <row r="179" spans="1:7" ht="31">
+    <row r="179" spans="1:7" ht="31.75">
       <c r="A179" s="3" t="s">
         <v>58</v>
       </c>
@@ -11699,7 +11699,7 @@
       <c r="F179" s="62"/>
       <c r="G179" s="3"/>
     </row>
-    <row r="180" spans="1:7" ht="31">
+    <row r="180" spans="1:7">
       <c r="A180" s="3" t="s">
         <v>58</v>
       </c>
@@ -11716,7 +11716,7 @@
       <c r="F180" s="62"/>
       <c r="G180" s="3"/>
     </row>
-    <row r="181" spans="1:7" ht="46.5">
+    <row r="181" spans="1:7" ht="47.6">
       <c r="A181" s="3" t="s">
         <v>58</v>
       </c>
@@ -11750,7 +11750,7 @@
       <c r="F182" s="62"/>
       <c r="G182" s="3"/>
     </row>
-    <row r="183" spans="1:7" ht="77.5">
+    <row r="183" spans="1:7" ht="63.45">
       <c r="A183" s="3" t="s">
         <v>58</v>
       </c>
@@ -11767,7 +11767,7 @@
       <c r="F183" s="53"/>
       <c r="G183" s="3"/>
     </row>
-    <row r="184" spans="1:7" ht="46.5">
+    <row r="184" spans="1:7" ht="47.6">
       <c r="A184" s="3" t="s">
         <v>58</v>
       </c>
@@ -11784,7 +11784,7 @@
       <c r="F184" s="53"/>
       <c r="G184" s="3"/>
     </row>
-    <row r="185" spans="1:7" ht="31">
+    <row r="185" spans="1:7" ht="31.75">
       <c r="A185" s="3" t="s">
         <v>58</v>
       </c>
@@ -11831,7 +11831,7 @@
       <c r="F187" s="53"/>
       <c r="G187" s="18"/>
     </row>
-    <row r="188" spans="1:7" ht="31">
+    <row r="188" spans="1:7" ht="31.75">
       <c r="A188" s="3" t="s">
         <v>58</v>
       </c>
@@ -11935,7 +11935,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="194" spans="1:7" ht="31">
+    <row r="194" spans="1:7" ht="31.75">
       <c r="A194" s="3" t="s">
         <v>58</v>
       </c>
@@ -11986,7 +11986,7 @@
       <c r="F196" s="62"/>
       <c r="G196" s="3"/>
     </row>
-    <row r="197" spans="1:7" ht="46.5">
+    <row r="197" spans="1:7" ht="47.6">
       <c r="A197" s="3" t="s">
         <v>58</v>
       </c>
@@ -12003,7 +12003,7 @@
       <c r="F197" s="62"/>
       <c r="G197" s="3"/>
     </row>
-    <row r="198" spans="1:7" ht="31">
+    <row r="198" spans="1:7" ht="31.75">
       <c r="A198" s="3" t="s">
         <v>58</v>
       </c>
@@ -12020,7 +12020,7 @@
       <c r="F198" s="62"/>
       <c r="G198" s="3"/>
     </row>
-    <row r="199" spans="1:7" ht="31">
+    <row r="199" spans="1:7" ht="31.75">
       <c r="A199" s="3" t="s">
         <v>58</v>
       </c>
@@ -12037,7 +12037,7 @@
       <c r="F199" s="62"/>
       <c r="G199" s="3"/>
     </row>
-    <row r="200" spans="1:7" ht="46.5">
+    <row r="200" spans="1:7" ht="47.6">
       <c r="A200" s="3" t="s">
         <v>58</v>
       </c>
@@ -12071,7 +12071,7 @@
       <c r="F201" s="62"/>
       <c r="G201" s="3"/>
     </row>
-    <row r="202" spans="1:7" ht="77.5">
+    <row r="202" spans="1:7" ht="63.45">
       <c r="A202" s="3" t="s">
         <v>58</v>
       </c>
@@ -12088,7 +12088,7 @@
       <c r="F202" s="53"/>
       <c r="G202" s="3"/>
     </row>
-    <row r="203" spans="1:7" ht="46.5">
+    <row r="203" spans="1:7" ht="47.6">
       <c r="A203" s="3" t="s">
         <v>58</v>
       </c>
@@ -12105,7 +12105,7 @@
       <c r="F203" s="53"/>
       <c r="G203" s="3"/>
     </row>
-    <row r="204" spans="1:7" ht="31">
+    <row r="204" spans="1:7" ht="31.75">
       <c r="A204" s="3" t="s">
         <v>58</v>
       </c>
@@ -12152,7 +12152,7 @@
       <c r="F206" s="53"/>
       <c r="G206" s="18"/>
     </row>
-    <row r="207" spans="1:7" ht="31">
+    <row r="207" spans="1:7" ht="31.75">
       <c r="A207" s="3" t="s">
         <v>58</v>
       </c>
@@ -12171,7 +12171,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="208" spans="1:7" ht="31">
+    <row r="208" spans="1:7" ht="31.75">
       <c r="A208" s="3" t="s">
         <v>58</v>
       </c>
@@ -12188,7 +12188,7 @@
       <c r="F208" s="53"/>
       <c r="G208" s="3"/>
     </row>
-    <row r="209" spans="1:7" ht="31">
+    <row r="209" spans="1:7" ht="31.75">
       <c r="A209" s="3" t="s">
         <v>58</v>
       </c>
@@ -12205,7 +12205,7 @@
       <c r="F209" s="53"/>
       <c r="G209" s="3"/>
     </row>
-    <row r="210" spans="1:7" ht="62">
+    <row r="210" spans="1:7" ht="63.45">
       <c r="A210" s="3" t="s">
         <v>58</v>
       </c>
@@ -12222,7 +12222,7 @@
       <c r="F210" s="53"/>
       <c r="G210" s="3"/>
     </row>
-    <row r="211" spans="1:7" ht="62">
+    <row r="211" spans="1:7" ht="63.45">
       <c r="A211" s="3" t="s">
         <v>58</v>
       </c>
@@ -12239,7 +12239,7 @@
       <c r="F211" s="53"/>
       <c r="G211" s="3"/>
     </row>
-    <row r="212" spans="1:7" ht="31">
+    <row r="212" spans="1:7" ht="31.75">
       <c r="A212" s="3" t="s">
         <v>58</v>
       </c>
@@ -12273,7 +12273,7 @@
       <c r="F213" s="53"/>
       <c r="G213" s="3"/>
     </row>
-    <row r="214" spans="1:7" ht="31">
+    <row r="214" spans="1:7" ht="31.75">
       <c r="A214" s="3" t="s">
         <v>58</v>
       </c>
@@ -12292,7 +12292,7 @@
       <c r="F214" s="53"/>
       <c r="G214" s="39"/>
     </row>
-    <row r="215" spans="1:7" ht="31">
+    <row r="215" spans="1:7" ht="31.75">
       <c r="A215" s="3" t="s">
         <v>58</v>
       </c>
@@ -12413,7 +12413,7 @@
       <c r="F221" s="53"/>
       <c r="G221" s="3"/>
     </row>
-    <row r="222" spans="1:7" ht="31">
+    <row r="222" spans="1:7" ht="31.75">
       <c r="A222" s="3" t="s">
         <v>58</v>
       </c>
@@ -12447,7 +12447,7 @@
       <c r="F223" s="53"/>
       <c r="G223" s="3"/>
     </row>
-    <row r="224" spans="1:7" ht="31">
+    <row r="224" spans="1:7" ht="31.75">
       <c r="A224" s="3" t="s">
         <v>58</v>
       </c>
@@ -12500,7 +12500,7 @@
       <c r="F226" s="53"/>
       <c r="G226" s="3"/>
     </row>
-    <row r="227" spans="1:7" ht="31">
+    <row r="227" spans="1:7" ht="31.75">
       <c r="A227" s="3" t="s">
         <v>58</v>
       </c>
@@ -12634,7 +12634,7 @@
       <c r="F234" s="53"/>
       <c r="G234" s="19"/>
     </row>
-    <row r="235" spans="1:7" ht="31">
+    <row r="235" spans="1:7" ht="31.75">
       <c r="A235" s="3" t="s">
         <v>58</v>
       </c>
@@ -12794,7 +12794,7 @@
       <c r="F244" s="53"/>
       <c r="G244" s="21"/>
     </row>
-    <row r="245" spans="1:7" ht="62">
+    <row r="245" spans="1:7" ht="63.45">
       <c r="A245" s="3" t="s">
         <v>58</v>
       </c>
@@ -12808,12 +12808,14 @@
         <v>435</v>
       </c>
       <c r="E245" s="53"/>
-      <c r="F245" s="53"/>
+      <c r="F245" s="3" t="s">
+        <v>1153</v>
+      </c>
       <c r="G245" s="5" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="31">
+    <row r="246" spans="1:7">
       <c r="A246" s="3" t="s">
         <v>58</v>
       </c>
@@ -12827,10 +12829,12 @@
         <v>438</v>
       </c>
       <c r="E246" s="53"/>
-      <c r="F246" s="53"/>
+      <c r="F246" s="3" t="s">
+        <v>1153</v>
+      </c>
       <c r="G246" s="5"/>
     </row>
-    <row r="247" spans="1:7" ht="31">
+    <row r="247" spans="1:7" ht="31.75">
       <c r="A247" s="3" t="s">
         <v>58</v>
       </c>
@@ -12844,10 +12848,12 @@
         <v>441</v>
       </c>
       <c r="E247" s="53"/>
-      <c r="F247" s="53"/>
+      <c r="F247" s="3" t="s">
+        <v>1153</v>
+      </c>
       <c r="G247" s="5"/>
     </row>
-    <row r="248" spans="1:7" ht="46.5">
+    <row r="248" spans="1:7" ht="47.6">
       <c r="A248" s="3" t="s">
         <v>58</v>
       </c>
@@ -12861,7 +12867,9 @@
         <v>444</v>
       </c>
       <c r="E248" s="53"/>
-      <c r="F248" s="53"/>
+      <c r="F248" s="3" t="s">
+        <v>1153</v>
+      </c>
       <c r="G248" s="5"/>
     </row>
     <row r="249" spans="1:7">
@@ -12878,10 +12886,12 @@
         <v>447</v>
       </c>
       <c r="E249" s="53"/>
-      <c r="F249" s="53"/>
+      <c r="F249" s="3" t="s">
+        <v>1153</v>
+      </c>
       <c r="G249" s="5"/>
     </row>
-    <row r="250" spans="1:7" ht="31">
+    <row r="250" spans="1:7" ht="31.75">
       <c r="A250" s="3" t="s">
         <v>58</v>
       </c>
@@ -12895,10 +12905,12 @@
         <v>450</v>
       </c>
       <c r="E250" s="53"/>
-      <c r="F250" s="53"/>
+      <c r="F250" s="3" t="s">
+        <v>1153</v>
+      </c>
       <c r="G250" s="5"/>
     </row>
-    <row r="251" spans="1:7" ht="62">
+    <row r="251" spans="1:7" ht="63.45">
       <c r="A251" s="3" t="s">
         <v>58</v>
       </c>
@@ -12912,10 +12924,12 @@
         <v>453</v>
       </c>
       <c r="E251" s="53"/>
-      <c r="F251" s="53"/>
+      <c r="F251" s="3" t="s">
+        <v>1153</v>
+      </c>
       <c r="G251" s="5"/>
     </row>
-    <row r="252" spans="1:7" ht="62">
+    <row r="252" spans="1:7" ht="63.45">
       <c r="A252" s="3" t="s">
         <v>58</v>
       </c>
@@ -12929,10 +12943,12 @@
         <v>456</v>
       </c>
       <c r="E252" s="53"/>
-      <c r="F252" s="53"/>
+      <c r="F252" s="3" t="s">
+        <v>1153</v>
+      </c>
       <c r="G252" s="5"/>
     </row>
-    <row r="253" spans="1:7" ht="93">
+    <row r="253" spans="1:7" ht="95.15">
       <c r="A253" s="3" t="s">
         <v>58</v>
       </c>
@@ -12946,10 +12962,12 @@
         <v>459</v>
       </c>
       <c r="E253" s="53"/>
-      <c r="F253" s="53"/>
+      <c r="F253" s="3" t="s">
+        <v>1153</v>
+      </c>
       <c r="G253" s="5"/>
     </row>
-    <row r="254" spans="1:7" ht="62">
+    <row r="254" spans="1:7" ht="63.45">
       <c r="A254" s="3" t="s">
         <v>58</v>
       </c>
@@ -12963,10 +12981,12 @@
         <v>462</v>
       </c>
       <c r="E254" s="53"/>
-      <c r="F254" s="53"/>
+      <c r="F254" s="3" t="s">
+        <v>1153</v>
+      </c>
       <c r="G254" s="5"/>
     </row>
-    <row r="255" spans="1:7" ht="93">
+    <row r="255" spans="1:7" ht="95.15">
       <c r="A255" s="3" t="s">
         <v>58</v>
       </c>
@@ -12980,10 +13000,12 @@
         <v>465</v>
       </c>
       <c r="E255" s="53"/>
-      <c r="F255" s="53"/>
+      <c r="F255" s="3" t="s">
+        <v>1153</v>
+      </c>
       <c r="G255" s="5"/>
     </row>
-    <row r="256" spans="1:7" ht="31">
+    <row r="256" spans="1:7" ht="31.75">
       <c r="A256" s="3" t="s">
         <v>58</v>
       </c>
@@ -12997,7 +13019,9 @@
         <v>468</v>
       </c>
       <c r="E256" s="53"/>
-      <c r="F256" s="53"/>
+      <c r="F256" s="3" t="s">
+        <v>1153</v>
+      </c>
       <c r="G256" s="5"/>
     </row>
     <row r="257" spans="1:7">
@@ -13030,7 +13054,7 @@
       <c r="F258" s="53"/>
       <c r="G258" s="21"/>
     </row>
-    <row r="259" spans="1:7" ht="62">
+    <row r="259" spans="1:7" ht="63.45">
       <c r="A259" s="3" t="s">
         <v>58</v>
       </c>
@@ -13044,7 +13068,9 @@
         <v>435</v>
       </c>
       <c r="E259" s="53"/>
-      <c r="F259" s="53"/>
+      <c r="F259" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G259" s="5" t="s">
         <v>473</v>
       </c>
@@ -13063,10 +13089,12 @@
         <v>438</v>
       </c>
       <c r="E260" s="53"/>
-      <c r="F260" s="53"/>
+      <c r="F260" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G260" s="5"/>
     </row>
-    <row r="261" spans="1:7" ht="31">
+    <row r="261" spans="1:7" ht="31.75">
       <c r="A261" s="3" t="s">
         <v>58</v>
       </c>
@@ -13080,10 +13108,12 @@
         <v>456</v>
       </c>
       <c r="E261" s="53"/>
-      <c r="F261" s="53"/>
+      <c r="F261" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G261" s="5"/>
     </row>
-    <row r="262" spans="1:7" ht="46.5">
+    <row r="262" spans="1:7" ht="47.6">
       <c r="A262" s="3" t="s">
         <v>58</v>
       </c>
@@ -13097,7 +13127,9 @@
         <v>444</v>
       </c>
       <c r="E262" s="53"/>
-      <c r="F262" s="53"/>
+      <c r="F262" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G262" s="5"/>
     </row>
     <row r="263" spans="1:7">
@@ -13114,10 +13146,12 @@
         <v>447</v>
       </c>
       <c r="E263" s="53"/>
-      <c r="F263" s="53"/>
+      <c r="F263" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G263" s="5"/>
     </row>
-    <row r="264" spans="1:7" ht="31">
+    <row r="264" spans="1:7" ht="31.75">
       <c r="A264" s="3" t="s">
         <v>58</v>
       </c>
@@ -13131,7 +13165,9 @@
         <v>450</v>
       </c>
       <c r="E264" s="53"/>
-      <c r="F264" s="53"/>
+      <c r="F264" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G264" s="5"/>
     </row>
     <row r="265" spans="1:7">
@@ -13148,10 +13184,12 @@
         <v>453</v>
       </c>
       <c r="E265" s="53"/>
-      <c r="F265" s="53"/>
+      <c r="F265" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G265" s="5"/>
     </row>
-    <row r="266" spans="1:7" ht="31">
+    <row r="266" spans="1:7" ht="31.75">
       <c r="A266" s="3" t="s">
         <v>58</v>
       </c>
@@ -13165,10 +13203,12 @@
         <v>459</v>
       </c>
       <c r="E266" s="53"/>
-      <c r="F266" s="53"/>
+      <c r="F266" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G266" s="5"/>
     </row>
-    <row r="267" spans="1:7" ht="31">
+    <row r="267" spans="1:7" ht="31.75">
       <c r="A267" s="3" t="s">
         <v>58</v>
       </c>
@@ -13182,10 +13222,12 @@
         <v>488</v>
       </c>
       <c r="E267" s="53"/>
-      <c r="F267" s="53"/>
+      <c r="F267" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G267" s="5"/>
     </row>
-    <row r="268" spans="1:7" ht="46.5">
+    <row r="268" spans="1:7" ht="47.6">
       <c r="A268" s="3" t="s">
         <v>58</v>
       </c>
@@ -13199,10 +13241,12 @@
         <v>78.3</v>
       </c>
       <c r="E268" s="53"/>
-      <c r="F268" s="53"/>
+      <c r="F268" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G268" s="5"/>
     </row>
-    <row r="269" spans="1:7" ht="46.5">
+    <row r="269" spans="1:7" ht="47.6">
       <c r="A269" s="3" t="s">
         <v>58</v>
       </c>
@@ -13216,10 +13260,12 @@
         <v>493</v>
       </c>
       <c r="E269" s="53"/>
-      <c r="F269" s="53"/>
+      <c r="F269" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G269" s="5"/>
     </row>
-    <row r="270" spans="1:7" ht="62">
+    <row r="270" spans="1:7" ht="63.45">
       <c r="A270" s="3" t="s">
         <v>58</v>
       </c>
@@ -13233,10 +13279,12 @@
         <v>462</v>
       </c>
       <c r="E270" s="53"/>
-      <c r="F270" s="53"/>
+      <c r="F270" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G270" s="3"/>
     </row>
-    <row r="271" spans="1:7" ht="77.5">
+    <row r="271" spans="1:7" ht="79.3">
       <c r="A271" s="3" t="s">
         <v>58</v>
       </c>
@@ -13250,10 +13298,12 @@
         <v>465</v>
       </c>
       <c r="E271" s="53"/>
-      <c r="F271" s="53"/>
+      <c r="F271" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G271" s="5"/>
     </row>
-    <row r="272" spans="1:7" ht="93">
+    <row r="272" spans="1:7" ht="95.15">
       <c r="A272" s="3" t="s">
         <v>58</v>
       </c>
@@ -13267,10 +13317,12 @@
         <v>468</v>
       </c>
       <c r="E272" s="53"/>
-      <c r="F272" s="53"/>
+      <c r="F272" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G272" s="3"/>
     </row>
-    <row r="273" spans="1:7" ht="93">
+    <row r="273" spans="1:7" ht="95.15">
       <c r="A273" s="3" t="s">
         <v>58</v>
       </c>
@@ -13284,10 +13336,12 @@
         <v>502</v>
       </c>
       <c r="E273" s="53"/>
-      <c r="F273" s="53"/>
+      <c r="F273" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G273" s="5"/>
     </row>
-    <row r="274" spans="1:7" ht="62">
+    <row r="274" spans="1:7" ht="63.45">
       <c r="A274" s="3" t="s">
         <v>58</v>
       </c>
@@ -13301,7 +13355,9 @@
         <v>505</v>
       </c>
       <c r="E274" s="53"/>
-      <c r="F274" s="53"/>
+      <c r="F274" s="53" t="s">
+        <v>1155</v>
+      </c>
       <c r="G274" s="5"/>
     </row>
     <row r="275" spans="1:7">
@@ -13334,7 +13390,7 @@
       <c r="F276" s="53"/>
       <c r="G276" s="13"/>
     </row>
-    <row r="277" spans="1:7" ht="62">
+    <row r="277" spans="1:7" ht="63.45">
       <c r="A277" s="3" t="s">
         <v>58</v>
       </c>
@@ -13348,7 +13404,9 @@
         <v>435</v>
       </c>
       <c r="E277" s="53"/>
-      <c r="F277" s="53"/>
+      <c r="F277" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G277" s="5" t="s">
         <v>473</v>
       </c>
@@ -13367,10 +13425,12 @@
         <v>438</v>
       </c>
       <c r="E278" s="53"/>
-      <c r="F278" s="53"/>
+      <c r="F278" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G278" s="5"/>
     </row>
-    <row r="279" spans="1:7" ht="31">
+    <row r="279" spans="1:7" ht="31.75">
       <c r="A279" s="3" t="s">
         <v>58</v>
       </c>
@@ -13384,10 +13444,12 @@
         <v>456</v>
       </c>
       <c r="E279" s="53"/>
-      <c r="F279" s="53"/>
+      <c r="F279" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G279" s="5"/>
     </row>
-    <row r="280" spans="1:7" ht="46.5">
+    <row r="280" spans="1:7" ht="47.6">
       <c r="A280" s="3" t="s">
         <v>58</v>
       </c>
@@ -13401,7 +13463,9 @@
         <v>444</v>
       </c>
       <c r="E280" s="53"/>
-      <c r="F280" s="53"/>
+      <c r="F280" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G280" s="5"/>
     </row>
     <row r="281" spans="1:7">
@@ -13418,10 +13482,12 @@
         <v>447</v>
       </c>
       <c r="E281" s="53"/>
-      <c r="F281" s="53"/>
+      <c r="F281" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G281" s="5"/>
     </row>
-    <row r="282" spans="1:7" ht="31">
+    <row r="282" spans="1:7" ht="31.75">
       <c r="A282" s="3" t="s">
         <v>58</v>
       </c>
@@ -13435,7 +13501,9 @@
         <v>450</v>
       </c>
       <c r="E282" s="53"/>
-      <c r="F282" s="53"/>
+      <c r="F282" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G282" s="5"/>
     </row>
     <row r="283" spans="1:7">
@@ -13452,10 +13520,12 @@
         <v>453</v>
       </c>
       <c r="E283" s="53"/>
-      <c r="F283" s="53"/>
+      <c r="F283" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G283" s="5"/>
     </row>
-    <row r="284" spans="1:7" ht="31">
+    <row r="284" spans="1:7" ht="31.75">
       <c r="A284" s="3" t="s">
         <v>58</v>
       </c>
@@ -13469,10 +13539,12 @@
         <v>459</v>
       </c>
       <c r="E284" s="53"/>
-      <c r="F284" s="53"/>
+      <c r="F284" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G284" s="5"/>
     </row>
-    <row r="285" spans="1:7" ht="31">
+    <row r="285" spans="1:7" ht="31.75">
       <c r="A285" s="3" t="s">
         <v>58</v>
       </c>
@@ -13486,10 +13558,12 @@
         <v>488</v>
       </c>
       <c r="E285" s="53"/>
-      <c r="F285" s="53"/>
+      <c r="F285" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G285" s="5"/>
     </row>
-    <row r="286" spans="1:7" ht="46.5">
+    <row r="286" spans="1:7" ht="47.6">
       <c r="A286" s="3" t="s">
         <v>58</v>
       </c>
@@ -13503,10 +13577,12 @@
         <v>78.3</v>
       </c>
       <c r="E286" s="53"/>
-      <c r="F286" s="53"/>
+      <c r="F286" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G286" s="5"/>
     </row>
-    <row r="287" spans="1:7" ht="46.5">
+    <row r="287" spans="1:7" ht="47.6">
       <c r="A287" s="3" t="s">
         <v>58</v>
       </c>
@@ -13520,10 +13596,12 @@
         <v>493</v>
       </c>
       <c r="E287" s="53"/>
-      <c r="F287" s="53"/>
+      <c r="F287" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G287" s="5"/>
     </row>
-    <row r="288" spans="1:7" ht="62">
+    <row r="288" spans="1:7" ht="63.45">
       <c r="A288" s="3" t="s">
         <v>58</v>
       </c>
@@ -13537,10 +13615,12 @@
         <v>462</v>
       </c>
       <c r="E288" s="53"/>
-      <c r="F288" s="53"/>
+      <c r="F288" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G288" s="3"/>
     </row>
-    <row r="289" spans="1:7" ht="77.5">
+    <row r="289" spans="1:7" ht="79.3">
       <c r="A289" s="3" t="s">
         <v>58</v>
       </c>
@@ -13554,10 +13634,12 @@
         <v>465</v>
       </c>
       <c r="E289" s="53"/>
-      <c r="F289" s="53"/>
+      <c r="F289" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G289" s="5"/>
     </row>
-    <row r="290" spans="1:7" ht="93">
+    <row r="290" spans="1:7" ht="95.15">
       <c r="A290" s="3" t="s">
         <v>58</v>
       </c>
@@ -13571,10 +13653,12 @@
         <v>468</v>
       </c>
       <c r="E290" s="53"/>
-      <c r="F290" s="53"/>
+      <c r="F290" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G290" s="3"/>
     </row>
-    <row r="291" spans="1:7" ht="93">
+    <row r="291" spans="1:7" ht="95.15">
       <c r="A291" s="3" t="s">
         <v>58</v>
       </c>
@@ -13588,10 +13672,12 @@
         <v>502</v>
       </c>
       <c r="E291" s="53"/>
-      <c r="F291" s="53"/>
+      <c r="F291" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G291" s="5"/>
     </row>
-    <row r="292" spans="1:7" ht="62">
+    <row r="292" spans="1:7" ht="63.45">
       <c r="A292" s="3" t="s">
         <v>58</v>
       </c>
@@ -13605,7 +13691,9 @@
         <v>505</v>
       </c>
       <c r="E292" s="53"/>
-      <c r="F292" s="53"/>
+      <c r="F292" s="53" t="s">
+        <v>1157</v>
+      </c>
       <c r="G292" s="5"/>
     </row>
     <row r="293" spans="1:7">
@@ -13638,7 +13726,7 @@
       <c r="F294" s="53"/>
       <c r="G294" s="18"/>
     </row>
-    <row r="295" spans="1:7" ht="46.5">
+    <row r="295" spans="1:7" ht="47.6">
       <c r="A295" s="3" t="s">
         <v>58</v>
       </c>
@@ -13652,7 +13740,9 @@
         <v>526</v>
       </c>
       <c r="E295" s="53"/>
-      <c r="F295" s="53"/>
+      <c r="F295" s="53" t="s">
+        <v>1161</v>
+      </c>
       <c r="G295" s="5"/>
     </row>
     <row r="296" spans="1:7">
@@ -13670,7 +13760,7 @@
       <c r="F296" s="53"/>
       <c r="G296" s="18"/>
     </row>
-    <row r="297" spans="1:7" ht="46.5">
+    <row r="297" spans="1:7" ht="47.6">
       <c r="A297" s="3" t="s">
         <v>58</v>
       </c>
@@ -13684,7 +13774,9 @@
         <v>435</v>
       </c>
       <c r="E297" s="58"/>
-      <c r="F297" s="58"/>
+      <c r="F297" s="53" t="s">
+        <v>1161</v>
+      </c>
       <c r="G297" s="3" t="s">
         <v>530</v>
       </c>
@@ -13703,7 +13795,9 @@
         <v>533</v>
       </c>
       <c r="E298" s="53"/>
-      <c r="F298" s="53"/>
+      <c r="F298" s="53" t="s">
+        <v>1161</v>
+      </c>
       <c r="G298" s="5"/>
     </row>
     <row r="299" spans="1:7">
@@ -13720,10 +13814,12 @@
         <v>536</v>
       </c>
       <c r="E299" s="53"/>
-      <c r="F299" s="53"/>
+      <c r="F299" s="53" t="s">
+        <v>1161</v>
+      </c>
       <c r="G299" s="5"/>
     </row>
-    <row r="300" spans="1:7" ht="46.5">
+    <row r="300" spans="1:7" ht="47.6">
       <c r="A300" s="3" t="s">
         <v>58</v>
       </c>
@@ -13737,10 +13833,12 @@
         <v>539</v>
       </c>
       <c r="E300" s="53"/>
-      <c r="F300" s="53"/>
+      <c r="F300" s="53" t="s">
+        <v>1161</v>
+      </c>
       <c r="G300" s="5"/>
     </row>
-    <row r="301" spans="1:7" ht="31">
+    <row r="301" spans="1:7" ht="31.75">
       <c r="A301" s="3" t="s">
         <v>58</v>
       </c>
@@ -13754,7 +13852,9 @@
         <v>542</v>
       </c>
       <c r="E301" s="53"/>
-      <c r="F301" s="53"/>
+      <c r="F301" s="53" t="s">
+        <v>1161</v>
+      </c>
       <c r="G301" s="5"/>
     </row>
     <row r="302" spans="1:7">
@@ -13771,10 +13871,12 @@
         <v>488</v>
       </c>
       <c r="E302" s="53"/>
-      <c r="F302" s="53"/>
+      <c r="F302" s="53" t="s">
+        <v>1161</v>
+      </c>
       <c r="G302" s="5"/>
     </row>
-    <row r="303" spans="1:7" ht="93">
+    <row r="303" spans="1:7" ht="95.15">
       <c r="A303" s="3" t="s">
         <v>58</v>
       </c>
@@ -13788,7 +13890,9 @@
         <v>547</v>
       </c>
       <c r="E303" s="53"/>
-      <c r="F303" s="53"/>
+      <c r="F303" s="53" t="s">
+        <v>1161</v>
+      </c>
       <c r="G303" s="5"/>
     </row>
     <row r="304" spans="1:7">
@@ -13821,7 +13925,7 @@
       <c r="F305" s="53"/>
       <c r="G305" s="24"/>
     </row>
-    <row r="306" spans="1:7" ht="62">
+    <row r="306" spans="1:7" ht="63.45">
       <c r="A306" s="3" t="s">
         <v>58</v>
       </c>
@@ -13857,7 +13961,7 @@
       <c r="F307" s="53"/>
       <c r="G307" s="3"/>
     </row>
-    <row r="308" spans="1:7" ht="31">
+    <row r="308" spans="1:7" ht="31.75">
       <c r="A308" s="3" t="s">
         <v>58</v>
       </c>
@@ -13874,7 +13978,7 @@
       <c r="F308" s="53"/>
       <c r="G308" s="3"/>
     </row>
-    <row r="309" spans="1:7" ht="46.5">
+    <row r="309" spans="1:7" ht="47.6">
       <c r="A309" s="3" t="s">
         <v>58</v>
       </c>
@@ -13908,7 +14012,7 @@
       <c r="F310" s="53"/>
       <c r="G310" s="3"/>
     </row>
-    <row r="311" spans="1:7" ht="31">
+    <row r="311" spans="1:7" ht="31.75">
       <c r="A311" s="3" t="s">
         <v>58</v>
       </c>
@@ -13942,7 +14046,7 @@
       <c r="F312" s="53"/>
       <c r="G312" s="3"/>
     </row>
-    <row r="313" spans="1:7" ht="31">
+    <row r="313" spans="1:7" ht="31.75">
       <c r="A313" s="3" t="s">
         <v>58</v>
       </c>
@@ -13959,7 +14063,7 @@
       <c r="F313" s="53"/>
       <c r="G313" s="3"/>
     </row>
-    <row r="314" spans="1:7" ht="31">
+    <row r="314" spans="1:7" ht="31.75">
       <c r="A314" s="3" t="s">
         <v>58</v>
       </c>
@@ -13976,7 +14080,7 @@
       <c r="F314" s="53"/>
       <c r="G314" s="3"/>
     </row>
-    <row r="315" spans="1:7" ht="46.5">
+    <row r="315" spans="1:7" ht="47.6">
       <c r="A315" s="3" t="s">
         <v>58</v>
       </c>
@@ -13993,7 +14097,7 @@
       <c r="F315" s="53"/>
       <c r="G315" s="3"/>
     </row>
-    <row r="316" spans="1:7" ht="46.5">
+    <row r="316" spans="1:7" ht="47.6">
       <c r="A316" s="3" t="s">
         <v>58</v>
       </c>
@@ -14010,7 +14114,7 @@
       <c r="F316" s="53"/>
       <c r="G316" s="3"/>
     </row>
-    <row r="317" spans="1:7" ht="62">
+    <row r="317" spans="1:7" ht="63.45">
       <c r="A317" s="3" t="s">
         <v>58</v>
       </c>
@@ -14027,7 +14131,7 @@
       <c r="F317" s="53"/>
       <c r="G317" s="3"/>
     </row>
-    <row r="318" spans="1:7" ht="77.5">
+    <row r="318" spans="1:7" ht="79.3">
       <c r="A318" s="3" t="s">
         <v>58</v>
       </c>
@@ -14044,7 +14148,7 @@
       <c r="F318" s="53"/>
       <c r="G318" s="3"/>
     </row>
-    <row r="319" spans="1:7" ht="93">
+    <row r="319" spans="1:7" ht="95.15">
       <c r="A319" s="3" t="s">
         <v>58</v>
       </c>
@@ -14061,7 +14165,7 @@
       <c r="F319" s="53"/>
       <c r="G319" s="3"/>
     </row>
-    <row r="320" spans="1:7" ht="93">
+    <row r="320" spans="1:7" ht="95.15">
       <c r="A320" s="3" t="s">
         <v>58</v>
       </c>
@@ -14078,7 +14182,7 @@
       <c r="F320" s="53"/>
       <c r="G320" s="3"/>
     </row>
-    <row r="321" spans="1:7" ht="62">
+    <row r="321" spans="1:7" ht="63.45">
       <c r="A321" s="3" t="s">
         <v>58</v>
       </c>
@@ -14140,7 +14244,7 @@
       <c r="F324" s="53"/>
       <c r="G324" s="24"/>
     </row>
-    <row r="325" spans="1:7" ht="108.5">
+    <row r="325" spans="1:7" ht="111">
       <c r="A325" s="3" t="s">
         <v>58</v>
       </c>
@@ -14159,7 +14263,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="326" spans="1:7" ht="31">
+    <row r="326" spans="1:7" ht="31.75">
       <c r="A326" s="3" t="s">
         <v>58</v>
       </c>
@@ -14176,7 +14280,7 @@
       <c r="F326" s="53"/>
       <c r="G326" s="5"/>
     </row>
-    <row r="327" spans="1:7" ht="31">
+    <row r="327" spans="1:7" ht="31.75">
       <c r="A327" s="3" t="s">
         <v>58</v>
       </c>
@@ -14251,7 +14355,7 @@
       </c>
       <c r="G331" s="3"/>
     </row>
-    <row r="332" spans="1:7" ht="31">
+    <row r="332" spans="1:7" ht="31.75">
       <c r="A332" s="3" t="s">
         <v>58</v>
       </c>
@@ -14341,7 +14445,7 @@
       </c>
       <c r="G337" s="5"/>
     </row>
-    <row r="338" spans="1:7" ht="46.5">
+    <row r="338" spans="1:7" ht="31.75">
       <c r="A338" s="3" t="s">
         <v>58</v>
       </c>
@@ -14369,7 +14473,7 @@
       <c r="D339" s="39"/>
       <c r="G339" s="18"/>
     </row>
-    <row r="340" spans="1:7" ht="77.5">
+    <row r="340" spans="1:7" ht="79.3">
       <c r="A340" s="3" t="s">
         <v>58</v>
       </c>
@@ -14388,7 +14492,7 @@
         <v>1142</v>
       </c>
     </row>
-    <row r="341" spans="1:7" ht="62">
+    <row r="341" spans="1:7" ht="63.45">
       <c r="A341" s="3" t="s">
         <v>58</v>
       </c>
@@ -14405,7 +14509,7 @@
       <c r="F341" s="62"/>
       <c r="G341" s="5"/>
     </row>
-    <row r="342" spans="1:7" ht="31">
+    <row r="342" spans="1:7" ht="31.75">
       <c r="A342" s="3" t="s">
         <v>58</v>
       </c>
@@ -14422,7 +14526,7 @@
       <c r="F342" s="62"/>
       <c r="G342" s="3"/>
     </row>
-    <row r="343" spans="1:7" ht="46.5">
+    <row r="343" spans="1:7" ht="47.6">
       <c r="A343" s="3" t="s">
         <v>58</v>
       </c>
@@ -14439,7 +14543,7 @@
       <c r="F343" s="62"/>
       <c r="G343" s="25"/>
     </row>
-    <row r="344" spans="1:7" ht="31">
+    <row r="344" spans="1:7" ht="31.75">
       <c r="A344" s="3" t="s">
         <v>58</v>
       </c>
@@ -14541,7 +14645,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="350" spans="1:7" ht="31">
+    <row r="350" spans="1:7" ht="31.75">
       <c r="A350" s="3" t="s">
         <v>58</v>
       </c>
@@ -14558,7 +14662,7 @@
       <c r="F350" s="58"/>
       <c r="G350" s="5"/>
     </row>
-    <row r="351" spans="1:7" ht="31">
+    <row r="351" spans="1:7" ht="31.75">
       <c r="A351" s="3" t="s">
         <v>58</v>
       </c>
@@ -14592,7 +14696,7 @@
       <c r="F352" s="53"/>
       <c r="G352" s="25"/>
     </row>
-    <row r="353" spans="1:7" ht="31">
+    <row r="353" spans="1:7" ht="31.75">
       <c r="A353" s="3" t="s">
         <v>58</v>
       </c>
@@ -14641,7 +14745,7 @@
       <c r="F355" s="53"/>
       <c r="G355" s="18"/>
     </row>
-    <row r="356" spans="1:7" ht="108.5">
+    <row r="356" spans="1:7" ht="111">
       <c r="A356" s="3" t="s">
         <v>58</v>
       </c>
@@ -14660,7 +14764,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="357" spans="1:7" ht="31">
+    <row r="357" spans="1:7" ht="31.75">
       <c r="A357" s="3" t="s">
         <v>58</v>
       </c>
@@ -14677,7 +14781,7 @@
       <c r="F357" s="62"/>
       <c r="G357" s="5"/>
     </row>
-    <row r="358" spans="1:7" ht="31">
+    <row r="358" spans="1:7" ht="31.75">
       <c r="A358" s="3" t="s">
         <v>58</v>
       </c>
@@ -14743,7 +14847,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="362" spans="1:7" ht="31">
+    <row r="362" spans="1:7" ht="31.75">
       <c r="A362" s="3" t="s">
         <v>58</v>
       </c>
@@ -14760,7 +14864,7 @@
       <c r="F362" s="53"/>
       <c r="G362" s="5"/>
     </row>
-    <row r="363" spans="1:7" ht="46.5">
+    <row r="363" spans="1:7" ht="47.6">
       <c r="A363" s="3" t="s">
         <v>58</v>
       </c>
@@ -14777,7 +14881,7 @@
       <c r="F363" s="53"/>
       <c r="G363" s="5"/>
     </row>
-    <row r="364" spans="1:7" ht="46.5">
+    <row r="364" spans="1:7" ht="47.6">
       <c r="A364" s="3" t="s">
         <v>58</v>
       </c>
@@ -14794,7 +14898,7 @@
       <c r="F364" s="44"/>
       <c r="G364" s="5"/>
     </row>
-    <row r="365" spans="1:7" ht="31">
+    <row r="365" spans="1:7" ht="31.75">
       <c r="A365" s="3" t="s">
         <v>58</v>
       </c>
@@ -14811,7 +14915,7 @@
       <c r="F365" s="53"/>
       <c r="G365" s="5"/>
     </row>
-    <row r="366" spans="1:7" ht="46.5">
+    <row r="366" spans="1:7" ht="47.6">
       <c r="A366" s="3" t="s">
         <v>58</v>
       </c>
@@ -14915,7 +15019,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="372" spans="1:7" ht="31">
+    <row r="372" spans="1:7" ht="31.75">
       <c r="A372" s="3" t="s">
         <v>58</v>
       </c>
@@ -14932,7 +15036,7 @@
       <c r="F372" s="58"/>
       <c r="G372" s="25"/>
     </row>
-    <row r="373" spans="1:7" ht="31">
+    <row r="373" spans="1:7" ht="31.75">
       <c r="A373" s="3" t="s">
         <v>58</v>
       </c>
@@ -14966,7 +15070,7 @@
       <c r="F374" s="53"/>
       <c r="G374" s="7"/>
     </row>
-    <row r="375" spans="1:7" ht="31">
+    <row r="375" spans="1:7" ht="31.75">
       <c r="A375" s="3" t="s">
         <v>58</v>
       </c>
@@ -15015,7 +15119,7 @@
       <c r="F377" s="53"/>
       <c r="G377" s="21"/>
     </row>
-    <row r="378" spans="1:7" ht="93">
+    <row r="378" spans="1:7" ht="95.15">
       <c r="A378" s="3" t="s">
         <v>58</v>
       </c>
@@ -15034,7 +15138,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="379" spans="1:7" ht="31">
+    <row r="379" spans="1:7" ht="31.75">
       <c r="A379" s="3" t="s">
         <v>58</v>
       </c>
@@ -15051,7 +15155,7 @@
       <c r="F379" s="53"/>
       <c r="G379" s="7"/>
     </row>
-    <row r="380" spans="1:7" ht="31">
+    <row r="380" spans="1:7" ht="31.75">
       <c r="A380" s="3" t="s">
         <v>58</v>
       </c>
@@ -15098,7 +15202,7 @@
       <c r="F382" s="53"/>
       <c r="G382" s="21"/>
     </row>
-    <row r="383" spans="1:7" ht="46.5">
+    <row r="383" spans="1:7" ht="47.6">
       <c r="A383" s="3" t="s">
         <v>58</v>
       </c>
@@ -15117,7 +15221,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="384" spans="1:7" ht="31">
+    <row r="384" spans="1:7" ht="31.75">
       <c r="A384" s="3" t="s">
         <v>58</v>
       </c>
@@ -15151,7 +15255,7 @@
       <c r="F385" s="53"/>
       <c r="G385" s="25"/>
     </row>
-    <row r="386" spans="1:7" ht="46.5">
+    <row r="386" spans="1:7" ht="47.6">
       <c r="A386" s="3" t="s">
         <v>58</v>
       </c>
@@ -15168,7 +15272,7 @@
       <c r="F386" s="53"/>
       <c r="G386" s="25"/>
     </row>
-    <row r="387" spans="1:7" ht="31">
+    <row r="387" spans="1:7" ht="31.75">
       <c r="A387" s="3" t="s">
         <v>58</v>
       </c>
@@ -15185,7 +15289,7 @@
       <c r="F387" s="53"/>
       <c r="G387" s="25"/>
     </row>
-    <row r="388" spans="1:7" ht="46.5">
+    <row r="388" spans="1:7" ht="47.6">
       <c r="A388" s="3" t="s">
         <v>58</v>
       </c>
@@ -15289,7 +15393,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="394" spans="1:7" ht="31">
+    <row r="394" spans="1:7" ht="31.75">
       <c r="A394" s="3" t="s">
         <v>58</v>
       </c>
@@ -15306,7 +15410,7 @@
       <c r="F394" s="58"/>
       <c r="G394" s="25"/>
     </row>
-    <row r="395" spans="1:7" ht="31">
+    <row r="395" spans="1:7" ht="31.75">
       <c r="A395" s="3" t="s">
         <v>58</v>
       </c>
@@ -15340,7 +15444,7 @@
       <c r="F396" s="53"/>
       <c r="G396" s="7"/>
     </row>
-    <row r="397" spans="1:7" ht="31">
+    <row r="397" spans="1:7" ht="31.75">
       <c r="A397" s="3" t="s">
         <v>58</v>
       </c>
@@ -15389,7 +15493,7 @@
       <c r="F399" s="53"/>
       <c r="G399" s="21"/>
     </row>
-    <row r="400" spans="1:7" ht="93">
+    <row r="400" spans="1:7" ht="95.15">
       <c r="A400" s="3" t="s">
         <v>58</v>
       </c>
@@ -15408,7 +15512,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="401" spans="1:7" ht="31">
+    <row r="401" spans="1:7" ht="31.75">
       <c r="A401" s="3" t="s">
         <v>58</v>
       </c>
@@ -15425,7 +15529,7 @@
       <c r="F401" s="53"/>
       <c r="G401" s="25"/>
     </row>
-    <row r="402" spans="1:7" ht="31">
+    <row r="402" spans="1:7" ht="31.75">
       <c r="A402" s="3" t="s">
         <v>58</v>
       </c>
@@ -15525,7 +15629,7 @@
       <c r="F407" s="53"/>
       <c r="G407" s="25"/>
     </row>
-    <row r="408" spans="1:7" ht="31">
+    <row r="408" spans="1:7" ht="31.75">
       <c r="A408" s="3" t="s">
         <v>58</v>
       </c>
@@ -15557,7 +15661,7 @@
       <c r="F409" s="53"/>
       <c r="G409" s="21"/>
     </row>
-    <row r="410" spans="1:7" ht="31">
+    <row r="410" spans="1:7" ht="31.75">
       <c r="A410" s="3" t="s">
         <v>58</v>
       </c>
@@ -15576,7 +15680,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="411" spans="1:7" ht="31">
+    <row r="411" spans="1:7" ht="31.75">
       <c r="A411" s="3" t="s">
         <v>58</v>
       </c>
@@ -15593,7 +15697,7 @@
       <c r="F411" s="62"/>
       <c r="G411" s="7"/>
     </row>
-    <row r="412" spans="1:7" ht="31">
+    <row r="412" spans="1:7" ht="31.75">
       <c r="A412" s="3" t="s">
         <v>58</v>
       </c>
@@ -15661,7 +15765,7 @@
       <c r="F415" s="62"/>
       <c r="G415" s="5"/>
     </row>
-    <row r="416" spans="1:7" ht="31">
+    <row r="416" spans="1:7" ht="31.75">
       <c r="A416" s="3" t="s">
         <v>58</v>
       </c>
@@ -15712,7 +15816,7 @@
       <c r="F418" s="62"/>
       <c r="G418" s="5"/>
     </row>
-    <row r="419" spans="1:7" ht="46.5">
+    <row r="419" spans="1:7" ht="47.6">
       <c r="A419" s="3" t="s">
         <v>58</v>
       </c>
@@ -15744,7 +15848,7 @@
       <c r="F420" s="62"/>
       <c r="G420" s="21"/>
     </row>
-    <row r="421" spans="1:7" ht="77.5">
+    <row r="421" spans="1:7" ht="79.3">
       <c r="A421" s="3" t="s">
         <v>58</v>
       </c>
@@ -15763,7 +15867,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="422" spans="1:7" ht="62">
+    <row r="422" spans="1:7" ht="63.45">
       <c r="A422" s="3" t="s">
         <v>58</v>
       </c>
@@ -15780,7 +15884,7 @@
       <c r="F422" s="62"/>
       <c r="G422" s="25"/>
     </row>
-    <row r="423" spans="1:7" ht="31">
+    <row r="423" spans="1:7" ht="31.75">
       <c r="A423" s="3" t="s">
         <v>58</v>
       </c>
@@ -15799,7 +15903,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="424" spans="1:7" ht="31">
+    <row r="424" spans="1:7" ht="31.75">
       <c r="A424" s="3" t="s">
         <v>58</v>
       </c>
@@ -15884,7 +15988,7 @@
       <c r="F428" s="53"/>
       <c r="G428" s="21"/>
     </row>
-    <row r="429" spans="1:7" ht="31">
+    <row r="429" spans="1:7" ht="31.75">
       <c r="A429" s="3" t="s">
         <v>58</v>
       </c>
@@ -16048,7 +16152,7 @@
       <c r="F438" s="53"/>
       <c r="G438" s="21"/>
     </row>
-    <row r="439" spans="1:7" ht="93">
+    <row r="439" spans="1:7" ht="95.15">
       <c r="A439" s="3" t="s">
         <v>58</v>
       </c>
@@ -16067,7 +16171,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="440" spans="1:7" ht="31">
+    <row r="440" spans="1:7" ht="31.75">
       <c r="A440" s="3" t="s">
         <v>58</v>
       </c>
@@ -16084,7 +16188,7 @@
       <c r="F440" s="53"/>
       <c r="G440" s="25"/>
     </row>
-    <row r="441" spans="1:7" ht="31">
+    <row r="441" spans="1:7" ht="31.75">
       <c r="A441" s="3" t="s">
         <v>58</v>
       </c>
@@ -16131,7 +16235,7 @@
       <c r="F443" s="53"/>
       <c r="G443" s="21"/>
     </row>
-    <row r="444" spans="1:7" ht="31">
+    <row r="444" spans="1:7" ht="31.75">
       <c r="A444" s="3" t="s">
         <v>58</v>
       </c>
@@ -16184,7 +16288,7 @@
       <c r="F446" s="53"/>
       <c r="G446" s="7"/>
     </row>
-    <row r="447" spans="1:7" ht="31">
+    <row r="447" spans="1:7" ht="31.75">
       <c r="A447" s="3" t="s">
         <v>58</v>
       </c>
@@ -16216,7 +16320,7 @@
       <c r="F448" s="53"/>
       <c r="G448" s="7"/>
     </row>
-    <row r="449" spans="1:7" ht="62">
+    <row r="449" spans="1:7" ht="63.45">
       <c r="A449" s="3" t="s">
         <v>58</v>
       </c>
@@ -16233,7 +16337,7 @@
       <c r="F449" s="53"/>
       <c r="G449" s="7"/>
     </row>
-    <row r="450" spans="1:7" ht="31">
+    <row r="450" spans="1:7" ht="31.75">
       <c r="A450" s="3" t="s">
         <v>58</v>
       </c>
@@ -16335,7 +16439,7 @@
         <v>1112</v>
       </c>
     </row>
-    <row r="456" spans="1:7" ht="31">
+    <row r="456" spans="1:7" ht="31.75">
       <c r="A456" s="3" t="s">
         <v>58</v>
       </c>
@@ -16352,7 +16456,7 @@
       <c r="F456" s="53"/>
       <c r="G456" s="5"/>
     </row>
-    <row r="457" spans="1:7" ht="31">
+    <row r="457" spans="1:7" ht="31.75">
       <c r="A457" s="3" t="s">
         <v>58</v>
       </c>
@@ -16386,7 +16490,7 @@
       <c r="F458" s="53"/>
       <c r="G458" s="3"/>
     </row>
-    <row r="459" spans="1:7" ht="31">
+    <row r="459" spans="1:7" ht="31.75">
       <c r="A459" s="3" t="s">
         <v>58</v>
       </c>
@@ -16421,14 +16525,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="45.08203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.58203125" style="4" customWidth="1"/>
-    <col min="4" max="5" width="81.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="45.0703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="4" customWidth="1"/>
+    <col min="4" max="5" width="81.35546875" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="1025" width="8.83203125" style="4" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="4" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="27"/>
   </cols>
   <sheetData>
@@ -16512,7 +16616,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="139.5">
+    <row r="5" spans="1:7" ht="126.9">
       <c r="A5" s="3" t="s">
         <v>71</v>
       </c>
@@ -16568,20 +16672,20 @@
       <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="68.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="100" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.08203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.0703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="20" style="4" customWidth="1"/>
-    <col min="8" max="1025" width="8.83203125" style="4" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="4" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="31">
+    <row r="1" spans="1:7" ht="31.75">
       <c r="A1" s="8" t="s">
         <v>782</v>
       </c>
@@ -16889,7 +16993,7 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="46.5">
+    <row r="17" spans="1:7" ht="47.6">
       <c r="A17" s="3" t="s">
         <v>125</v>
       </c>
@@ -17271,7 +17375,7 @@
       </c>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="62">
+    <row r="37" spans="1:7" ht="63.45">
       <c r="A37" s="3" t="s">
         <v>257</v>
       </c>
@@ -17292,7 +17396,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="31">
+    <row r="38" spans="1:7" ht="31.75">
       <c r="A38" s="3" t="s">
         <v>526</v>
       </c>
@@ -17368,7 +17472,7 @@
       </c>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7" ht="46.5">
+    <row r="42" spans="1:7" ht="47.6">
       <c r="A42" s="3" t="s">
         <v>274</v>
       </c>
@@ -17652,15 +17756,15 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="41" customWidth="1"/>
-    <col min="2" max="2" width="47.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="4" customWidth="1"/>
-    <col min="4" max="5" width="80.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="41" customWidth="1"/>
+    <col min="2" max="2" width="47.35546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="4" customWidth="1"/>
+    <col min="4" max="5" width="80.85546875" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.83203125" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.83203125" style="27" customWidth="1"/>
+    <col min="8" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="27" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="27"/>
   </cols>
   <sheetData>
@@ -18819,7 +18923,7 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
-    <row r="49" spans="1:256" s="49" customFormat="1" ht="31">
+    <row r="49" spans="1:256" s="49" customFormat="1" ht="31.75">
       <c r="A49" s="40" t="s">
         <v>981</v>
       </c>
@@ -19099,21 +19203,21 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:IV30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="33.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.58203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.58203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="44.35546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="41.35546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" style="4" customWidth="1"/>
     <col min="7" max="7" width="29" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.83203125" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.83203125" style="27" customWidth="1"/>
+    <col min="8" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="27" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="27"/>
   </cols>
   <sheetData>
@@ -19568,7 +19672,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" ht="31">
+    <row r="24" spans="1:7" ht="31.75">
       <c r="A24" s="65" t="s">
         <v>1163</v>
       </c>
@@ -19585,7 +19689,7 @@
       <c r="F24" s="65"/>
       <c r="G24" s="65"/>
     </row>
-    <row r="25" spans="1:7" ht="31">
+    <row r="25" spans="1:7" ht="31.75">
       <c r="A25" s="65" t="s">
         <v>1167</v>
       </c>
@@ -19602,7 +19706,7 @@
       <c r="F25" s="65"/>
       <c r="G25" s="65"/>
     </row>
-    <row r="26" spans="1:7" ht="31">
+    <row r="26" spans="1:7" ht="31.75">
       <c r="A26" s="65" t="s">
         <v>1170</v>
       </c>
@@ -19619,7 +19723,7 @@
       <c r="F26" s="65"/>
       <c r="G26" s="65"/>
     </row>
-    <row r="27" spans="1:7" ht="46.5">
+    <row r="27" spans="1:7" ht="47.6">
       <c r="A27" s="65" t="s">
         <v>1173</v>
       </c>
@@ -19636,7 +19740,7 @@
       <c r="F27" s="65"/>
       <c r="G27" s="65"/>
     </row>
-    <row r="28" spans="1:7" ht="46.5">
+    <row r="28" spans="1:7" ht="31.75">
       <c r="A28" s="65" t="s">
         <v>1176</v>
       </c>
@@ -19653,7 +19757,7 @@
       <c r="F28" s="65"/>
       <c r="G28" s="65"/>
     </row>
-    <row r="29" spans="1:7" ht="31">
+    <row r="29" spans="1:7" ht="31.75">
       <c r="A29" s="65" t="s">
         <v>1179</v>
       </c>
@@ -19670,7 +19774,7 @@
       <c r="F29" s="65"/>
       <c r="G29" s="65"/>
     </row>
-    <row r="30" spans="1:7" ht="46.5">
+    <row r="30" spans="1:7" ht="47.6">
       <c r="A30" s="65" t="s">
         <v>1182</v>
       </c>
@@ -19705,15 +19809,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="54.58203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="4" customWidth="1"/>
-    <col min="4" max="5" width="75.58203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="54.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="4" customWidth="1"/>
+    <col min="4" max="5" width="75.5703125" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.83203125" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.83203125" style="27" customWidth="1"/>
+    <col min="8" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="27" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="27"/>
   </cols>
   <sheetData>
@@ -19821,17 +19925,17 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="35" customWidth="1"/>
-    <col min="2" max="2" width="53.33203125" style="28" customWidth="1"/>
+    <col min="2" max="2" width="53.35546875" style="28" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="28" customWidth="1"/>
     <col min="4" max="4" width="44.5" style="28" customWidth="1"/>
-    <col min="5" max="5" width="31.83203125" style="28" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" style="28" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="28" customWidth="1"/>
     <col min="7" max="7" width="44.5" style="28" customWidth="1"/>
-    <col min="8" max="256" width="8.83203125" style="28" customWidth="1"/>
-    <col min="257" max="1025" width="8.83203125" style="29" customWidth="1"/>
+    <col min="8" max="256" width="8.85546875" style="28" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="29" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="29"/>
   </cols>
   <sheetData>
@@ -20530,7 +20634,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="31">
+    <row r="23" spans="1:7" ht="31.75">
       <c r="A23" s="47" t="s">
         <v>1118</v>
       </c>
@@ -20581,7 +20685,7 @@
       <c r="F25" s="47"/>
       <c r="G25" s="47"/>
     </row>
-    <row r="26" spans="1:7" ht="31">
+    <row r="26" spans="1:7" ht="31.75">
       <c r="A26" s="47" t="s">
         <v>1113</v>
       </c>
@@ -20633,16 +20737,16 @@
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="19" style="32" customWidth="1"/>
-    <col min="2" max="2" width="53.33203125" style="27" customWidth="1"/>
+    <col min="2" max="2" width="53.35546875" style="27" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="27" customWidth="1"/>
     <col min="4" max="4" width="25" style="27" customWidth="1"/>
     <col min="5" max="5" width="46" style="27" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" style="27" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="27" customWidth="1"/>
     <col min="7" max="7" width="44.5" style="27" customWidth="1"/>
-    <col min="8" max="1025" width="8.83203125" style="27" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="27" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="27"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Generate sheet with prod oids off the most recent version
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\conformancelib\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\gsa-devel\piv-conformance-swing\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7BEA43-F2B3-495E-A23A-137500F1D6D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87D595A-DBDD-42C6-85EB-1D796A0520F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-180" yWindow="165" windowWidth="30570" windowHeight="16830" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="18472" windowHeight="11623" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -4727,17 +4727,17 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="13.75" style="4" customWidth="1"/>
-    <col min="2" max="2" width="57.375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="57.35546875" style="4" customWidth="1"/>
     <col min="3" max="5" width="10.5" style="4" customWidth="1"/>
-    <col min="6" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="19" customWidth="1"/>
+    <col min="6" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>53</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A2" s="2">
         <v>8</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A3" s="3">
         <v>8.1</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>59</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>63</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>66</v>
       </c>
@@ -4785,7 +4785,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>69</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>72</v>
       </c>
@@ -4801,7 +4801,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="9" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>75</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>78</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>81</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>84</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="13" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>87</v>
       </c>
@@ -4841,7 +4841,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>90</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A15" s="3">
         <v>8.1999999999999993</v>
       </c>
@@ -4857,7 +4857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="16" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>93</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="17" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>96</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="18" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>97</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>98</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>99</v>
       </c>
@@ -4897,7 +4897,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A21" s="3" t="s">
         <v>102</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="22" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A22" s="3" t="s">
         <v>105</v>
       </c>
@@ -4913,7 +4913,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A23" s="3" t="s">
         <v>108</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A24" s="3" t="s">
         <v>111</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A25" s="3" t="s">
         <v>114</v>
       </c>
@@ -4937,7 +4937,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A26" s="3" t="s">
         <v>117</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A27" s="3" t="s">
         <v>120</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A28" s="3" t="s">
         <v>123</v>
       </c>
@@ -4961,7 +4961,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="29" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A29" s="3" t="s">
         <v>126</v>
       </c>
@@ -4969,7 +4969,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A30" s="3" t="s">
         <v>128</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>132</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="1:2" ht="17.149999999999999" customHeight="1">
       <c r="A32" s="3">
         <v>8.3000000000000007</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A33" s="3" t="s">
         <v>134</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A34" s="3" t="s">
         <v>137</v>
       </c>
@@ -5009,7 +5009,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="35" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A35" s="3" t="s">
         <v>138</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="36" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A36" s="3" t="s">
         <v>139</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="37" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A37" s="3" t="s">
         <v>140</v>
       </c>
@@ -5033,7 +5033,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="38" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A38" s="3" t="s">
         <v>143</v>
       </c>
@@ -5041,7 +5041,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="39" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A39" s="3" t="s">
         <v>146</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="40" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A40" s="3" t="s">
         <v>149</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="41" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A41" s="3" t="s">
         <v>152</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A42" s="3" t="s">
         <v>155</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="43" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A43" s="3">
         <v>8.4</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="44" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A44" s="3" t="s">
         <v>156</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="45" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A45" s="3" t="s">
         <v>159</v>
       </c>
@@ -5097,7 +5097,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="46" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A46" s="3" t="s">
         <v>160</v>
       </c>
@@ -5105,7 +5105,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="47" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A47" s="3" t="s">
         <v>161</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="48" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A48" s="3" t="s">
         <v>162</v>
       </c>
@@ -5124,7 +5124,7 @@
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
     </row>
-    <row r="49" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="49" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A49" s="3" t="s">
         <v>163</v>
       </c>
@@ -5135,7 +5135,7 @@
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
     </row>
-    <row r="50" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="50" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A50" s="3" t="s">
         <v>164</v>
       </c>
@@ -5146,7 +5146,7 @@
       <c r="D50" s="18"/>
       <c r="E50" s="18"/>
     </row>
-    <row r="51" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="51" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A51" s="3" t="s">
         <v>165</v>
       </c>
@@ -5157,7 +5157,7 @@
       <c r="D51" s="18"/>
       <c r="E51" s="18"/>
     </row>
-    <row r="52" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="52" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A52" s="3" t="s">
         <v>166</v>
       </c>
@@ -5168,7 +5168,7 @@
       <c r="D52" s="18"/>
       <c r="E52" s="18"/>
     </row>
-    <row r="53" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="53" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A53" s="3">
         <v>8.5</v>
       </c>
@@ -5179,7 +5179,7 @@
       <c r="D53" s="18"/>
       <c r="E53" s="18"/>
     </row>
-    <row r="54" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="54" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A54" s="3" t="s">
         <v>167</v>
       </c>
@@ -5190,7 +5190,7 @@
       <c r="D54" s="18"/>
       <c r="E54" s="18"/>
     </row>
-    <row r="55" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="55" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A55" s="3" t="s">
         <v>170</v>
       </c>
@@ -5201,7 +5201,7 @@
       <c r="D55" s="18"/>
       <c r="E55" s="18"/>
     </row>
-    <row r="56" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="56" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A56" s="3" t="s">
         <v>171</v>
       </c>
@@ -5212,7 +5212,7 @@
       <c r="D56" s="18"/>
       <c r="E56" s="18"/>
     </row>
-    <row r="57" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="57" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A57" s="3" t="s">
         <v>172</v>
       </c>
@@ -5223,7 +5223,7 @@
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
     </row>
-    <row r="58" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="58" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A58" s="3" t="s">
         <v>173</v>
       </c>
@@ -5234,7 +5234,7 @@
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
     </row>
-    <row r="59" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="59" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A59" s="3" t="s">
         <v>176</v>
       </c>
@@ -5245,7 +5245,7 @@
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
     </row>
-    <row r="60" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="60" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A60" s="3" t="s">
         <v>179</v>
       </c>
@@ -5256,7 +5256,7 @@
       <c r="D60" s="18"/>
       <c r="E60" s="18"/>
     </row>
-    <row r="61" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="61" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A61" s="3" t="s">
         <v>182</v>
       </c>
@@ -5267,7 +5267,7 @@
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
     </row>
-    <row r="62" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="62" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A62" s="3" t="s">
         <v>185</v>
       </c>
@@ -5278,7 +5278,7 @@
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
     </row>
-    <row r="63" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="63" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A63" s="3" t="s">
         <v>188</v>
       </c>
@@ -5289,7 +5289,7 @@
       <c r="D63" s="18"/>
       <c r="E63" s="18"/>
     </row>
-    <row r="64" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="64" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A64" s="3">
         <v>8.6</v>
       </c>
@@ -5300,7 +5300,7 @@
       <c r="D64" s="18"/>
       <c r="E64" s="18"/>
     </row>
-    <row r="65" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="65" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A65" s="3" t="s">
         <v>189</v>
       </c>
@@ -5311,7 +5311,7 @@
       <c r="D65" s="18"/>
       <c r="E65" s="18"/>
     </row>
-    <row r="66" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="66" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A66" s="3" t="s">
         <v>192</v>
       </c>
@@ -5322,7 +5322,7 @@
       <c r="D66" s="18"/>
       <c r="E66" s="18"/>
     </row>
-    <row r="67" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="67" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A67" s="3" t="s">
         <v>193</v>
       </c>
@@ -5333,7 +5333,7 @@
       <c r="D67" s="18"/>
       <c r="E67" s="18"/>
     </row>
-    <row r="68" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="68" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A68" s="3" t="s">
         <v>194</v>
       </c>
@@ -5344,7 +5344,7 @@
       <c r="D68" s="18"/>
       <c r="E68" s="18"/>
     </row>
-    <row r="69" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="69" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A69" s="3" t="s">
         <v>195</v>
       </c>
@@ -5355,7 +5355,7 @@
       <c r="D69" s="18"/>
       <c r="E69" s="18"/>
     </row>
-    <row r="70" spans="1:5" ht="17.100000000000001" customHeight="1">
+    <row r="70" spans="1:5" ht="17.149999999999999" customHeight="1">
       <c r="A70" s="3" t="s">
         <v>198</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="31.5">
+    <row r="74" spans="1:5" ht="31.75">
       <c r="A74" s="3" t="s">
         <v>205</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="31.5">
+    <row r="85" spans="1:2" ht="31.75">
       <c r="A85" s="3" t="s">
         <v>217</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="31.5">
+    <row r="96" spans="1:2" ht="31.75">
       <c r="A96" s="3" t="s">
         <v>229</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="31.5">
+    <row r="114" spans="1:2" ht="31.75">
       <c r="A114" s="3" t="s">
         <v>255</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="28.5">
+    <row r="116" spans="1:2" ht="28.3">
       <c r="A116" s="3" t="s">
         <v>258</v>
       </c>
@@ -5766,7 +5766,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="47.25">
+    <row r="121" spans="1:2" ht="47.6">
       <c r="A121" s="3" t="s">
         <v>267</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="63">
+    <row r="123" spans="1:2" ht="63.45">
       <c r="A123" s="3" t="s">
         <v>272</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="31.5">
+    <row r="142" spans="1:2" ht="31.75">
       <c r="A142" s="3" t="s">
         <v>296</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="31.5">
+    <row r="144" spans="1:2" ht="31.75">
       <c r="A144" s="3" t="s">
         <v>301</v>
       </c>
@@ -5958,7 +5958,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="47.25">
+    <row r="145" spans="1:2" ht="31.75">
       <c r="A145" s="3" t="s">
         <v>303</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="47.25">
+    <row r="146" spans="1:2" ht="47.6">
       <c r="A146" s="3" t="s">
         <v>305</v>
       </c>
@@ -5990,7 +5990,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="47.25">
+    <row r="149" spans="1:2" ht="47.6">
       <c r="A149" s="3" t="s">
         <v>311</v>
       </c>
@@ -6006,7 +6006,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="63">
+    <row r="151" spans="1:2" ht="47.6">
       <c r="A151" s="3" t="s">
         <v>315</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="31.5">
+    <row r="152" spans="1:2" ht="31.75">
       <c r="A152" s="3" t="s">
         <v>317</v>
       </c>
@@ -6022,7 +6022,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="31.5">
+    <row r="153" spans="1:2" ht="31.75">
       <c r="A153" s="3" t="s">
         <v>319</v>
       </c>
@@ -6086,7 +6086,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="31.5">
+    <row r="161" spans="1:2" ht="31.75">
       <c r="A161" s="3" t="s">
         <v>327</v>
       </c>
@@ -6102,7 +6102,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="31.5">
+    <row r="163" spans="1:2" ht="31.75">
       <c r="A163" s="3" t="s">
         <v>329</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="31.5">
+    <row r="164" spans="1:2" ht="31.75">
       <c r="A164" s="3" t="s">
         <v>330</v>
       </c>
@@ -6118,7 +6118,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="47.25">
+    <row r="165" spans="1:2" ht="47.6">
       <c r="A165" s="3" t="s">
         <v>332</v>
       </c>
@@ -6142,7 +6142,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="31.5">
+    <row r="168" spans="1:2" ht="31.75">
       <c r="A168" s="3" t="s">
         <v>336</v>
       </c>
@@ -6158,7 +6158,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="63">
+    <row r="170" spans="1:2" ht="47.6">
       <c r="A170" s="3" t="s">
         <v>340</v>
       </c>
@@ -6166,7 +6166,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="31.5">
+    <row r="171" spans="1:2" ht="31.75">
       <c r="A171" s="3" t="s">
         <v>341</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="31.5">
+    <row r="172" spans="1:2" ht="31.75">
       <c r="A172" s="3" t="s">
         <v>342</v>
       </c>
@@ -6270,7 +6270,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="47.25">
+    <row r="184" spans="1:2" ht="47.6">
       <c r="A184" s="3" t="s">
         <v>332</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="31.5">
+    <row r="187" spans="1:2" ht="31.75">
       <c r="A187" s="3" t="s">
         <v>360</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="63">
+    <row r="189" spans="1:2" ht="47.6">
       <c r="A189" s="3" t="s">
         <v>363</v>
       </c>
@@ -6318,7 +6318,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="31.5">
+    <row r="190" spans="1:2" ht="31.75">
       <c r="A190" s="3" t="s">
         <v>364</v>
       </c>
@@ -6326,7 +6326,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="31.5">
+    <row r="191" spans="1:2" ht="31.75">
       <c r="A191" s="3" t="s">
         <v>365</v>
       </c>
@@ -6374,7 +6374,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="47.25">
+    <row r="197" spans="1:2" ht="47.6">
       <c r="A197" s="3" t="s">
         <v>375</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="47.25">
+    <row r="198" spans="1:2" ht="47.6">
       <c r="A198" s="3" t="s">
         <v>377</v>
       </c>
@@ -6406,7 +6406,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="31.5">
+    <row r="201" spans="1:2" ht="31.75">
       <c r="A201" s="3" t="s">
         <v>382</v>
       </c>
@@ -6414,7 +6414,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="31.5">
+    <row r="202" spans="1:2" ht="31.75">
       <c r="A202" s="3" t="s">
         <v>384</v>
       </c>
@@ -6518,7 +6518,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="31.5">
+    <row r="215" spans="1:2" ht="31.75">
       <c r="A215" s="3" t="s">
         <v>409</v>
       </c>
@@ -6662,7 +6662,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="47.25">
+    <row r="233" spans="1:2" ht="47.6">
       <c r="A233" s="3" t="s">
         <v>432</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="31.5">
+    <row r="235" spans="1:2" ht="31.75">
       <c r="A235" s="3" t="s">
         <v>439</v>
       </c>
@@ -6686,7 +6686,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="31.5">
+    <row r="236" spans="1:2" ht="31.75">
       <c r="A236" s="3" t="s">
         <v>442</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="47.25">
+    <row r="239" spans="1:2" ht="47.6">
       <c r="A239" s="3" t="s">
         <v>451</v>
       </c>
@@ -6718,7 +6718,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="47.25">
+    <row r="240" spans="1:2" ht="47.6">
       <c r="A240" s="3" t="s">
         <v>454</v>
       </c>
@@ -6726,7 +6726,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="78.75">
+    <row r="241" spans="1:2" ht="79.3">
       <c r="A241" s="3" t="s">
         <v>457</v>
       </c>
@@ -6734,7 +6734,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="47.25">
+    <row r="242" spans="1:2" ht="47.6">
       <c r="A242" s="3" t="s">
         <v>460</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="78.75">
+    <row r="243" spans="1:2" ht="79.3">
       <c r="A243" s="3" t="s">
         <v>463</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="31.5">
+    <row r="244" spans="1:2" ht="31.75">
       <c r="A244" s="3" t="s">
         <v>466</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="47.25">
+    <row r="247" spans="1:2" ht="47.6">
       <c r="A247" s="3" t="s">
         <v>471</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="31.5">
+    <row r="249" spans="1:2" ht="31.75">
       <c r="A249" s="3" t="s">
         <v>476</v>
       </c>
@@ -6798,7 +6798,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="31.5">
+    <row r="250" spans="1:2" ht="31.75">
       <c r="A250" s="3" t="s">
         <v>478</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="31.5">
+    <row r="254" spans="1:2" ht="31.75">
       <c r="A254" s="3" t="s">
         <v>484</v>
       </c>
@@ -6838,7 +6838,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="31.5">
+    <row r="255" spans="1:2" ht="31.75">
       <c r="A255" s="3" t="s">
         <v>486</v>
       </c>
@@ -6846,7 +6846,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="31.5">
+    <row r="256" spans="1:2" ht="31.75">
       <c r="A256" s="3" t="s">
         <v>489</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="47.25">
+    <row r="257" spans="1:2" ht="47.6">
       <c r="A257" s="3" t="s">
         <v>491</v>
       </c>
@@ -6862,7 +6862,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="47.25">
+    <row r="258" spans="1:2" ht="47.6">
       <c r="A258" s="3" t="s">
         <v>494</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="63">
+    <row r="259" spans="1:2" ht="63.45">
       <c r="A259" s="3" t="s">
         <v>496</v>
       </c>
@@ -6878,7 +6878,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="78.75">
+    <row r="260" spans="1:2" ht="79.3">
       <c r="A260" s="3" t="s">
         <v>498</v>
       </c>
@@ -6886,7 +6886,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="78.75">
+    <row r="261" spans="1:2" ht="79.3">
       <c r="A261" s="3" t="s">
         <v>500</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="47.25">
+    <row r="262" spans="1:2" ht="47.6">
       <c r="A262" s="3" t="s">
         <v>503</v>
       </c>
@@ -6918,7 +6918,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="265" spans="1:2" ht="47.25">
+    <row r="265" spans="1:2" ht="47.6">
       <c r="A265" s="3" t="s">
         <v>507</v>
       </c>
@@ -6934,7 +6934,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="31.5">
+    <row r="267" spans="1:2" ht="31.75">
       <c r="A267" s="3" t="s">
         <v>509</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="31.5">
+    <row r="268" spans="1:2" ht="31.75">
       <c r="A268" s="3" t="s">
         <v>510</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="272" spans="1:2" ht="31.5">
+    <row r="272" spans="1:2" ht="31.75">
       <c r="A272" s="3" t="s">
         <v>514</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="273" spans="1:2" ht="31.5">
+    <row r="273" spans="1:2" ht="31.75">
       <c r="A273" s="3" t="s">
         <v>515</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="274" spans="1:2" ht="31.5">
+    <row r="274" spans="1:2" ht="31.75">
       <c r="A274" s="3" t="s">
         <v>516</v>
       </c>
@@ -6998,7 +6998,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="275" spans="1:2" ht="47.25">
+    <row r="275" spans="1:2" ht="47.6">
       <c r="A275" s="3" t="s">
         <v>517</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="276" spans="1:2" ht="47.25">
+    <row r="276" spans="1:2" ht="47.6">
       <c r="A276" s="3" t="s">
         <v>518</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="277" spans="1:2" ht="63">
+    <row r="277" spans="1:2" ht="63.45">
       <c r="A277" s="3" t="s">
         <v>519</v>
       </c>
@@ -7022,7 +7022,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="78.75">
+    <row r="278" spans="1:2" ht="79.3">
       <c r="A278" s="3" t="s">
         <v>520</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="279" spans="1:2" ht="78.75">
+    <row r="279" spans="1:2" ht="79.3">
       <c r="A279" s="3" t="s">
         <v>521</v>
       </c>
@@ -7038,7 +7038,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="280" spans="1:2" ht="47.25">
+    <row r="280" spans="1:2" ht="47.6">
       <c r="A280" s="3" t="s">
         <v>522</v>
       </c>
@@ -7062,7 +7062,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="283" spans="1:2" ht="31.5">
+    <row r="283" spans="1:2" ht="31.75">
       <c r="A283" s="3" t="s">
         <v>524</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="31.5">
+    <row r="285" spans="1:2" ht="31.75">
       <c r="A285" s="3" t="s">
         <v>528</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="47.25">
+    <row r="288" spans="1:2" ht="47.6">
       <c r="A288" s="3" t="s">
         <v>537</v>
       </c>
@@ -7126,7 +7126,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="78.75">
+    <row r="291" spans="1:2" ht="79.3">
       <c r="A291" s="3" t="s">
         <v>545</v>
       </c>
@@ -7150,7 +7150,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="47.25">
+    <row r="294" spans="1:2" ht="47.6">
       <c r="A294" s="3" t="s">
         <v>549</v>
       </c>
@@ -7166,7 +7166,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="31.5">
+    <row r="296" spans="1:2" ht="31.75">
       <c r="A296" s="3" t="s">
         <v>551</v>
       </c>
@@ -7174,7 +7174,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="31.5">
+    <row r="297" spans="1:2" ht="31.75">
       <c r="A297" s="3" t="s">
         <v>552</v>
       </c>
@@ -7206,7 +7206,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="31.5">
+    <row r="301" spans="1:2" ht="31.75">
       <c r="A301" s="3" t="s">
         <v>556</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="31.5">
+    <row r="302" spans="1:2" ht="31.75">
       <c r="A302" s="3" t="s">
         <v>557</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="31.5">
+    <row r="303" spans="1:2" ht="31.75">
       <c r="A303" s="3" t="s">
         <v>558</v>
       </c>
@@ -7230,7 +7230,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="304" spans="1:2" ht="47.25">
+    <row r="304" spans="1:2" ht="47.6">
       <c r="A304" s="3" t="s">
         <v>559</v>
       </c>
@@ -7238,7 +7238,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="305" spans="1:2" ht="47.25">
+    <row r="305" spans="1:2" ht="47.6">
       <c r="A305" s="3" t="s">
         <v>560</v>
       </c>
@@ -7246,7 +7246,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="306" spans="1:2" ht="63">
+    <row r="306" spans="1:2" ht="63.45">
       <c r="A306" s="3" t="s">
         <v>561</v>
       </c>
@@ -7254,7 +7254,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="307" spans="1:2" ht="78.75">
+    <row r="307" spans="1:2" ht="79.3">
       <c r="A307" s="3" t="s">
         <v>562</v>
       </c>
@@ -7262,7 +7262,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="308" spans="1:2" ht="78.75">
+    <row r="308" spans="1:2" ht="79.3">
       <c r="A308" s="3" t="s">
         <v>563</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="47.25">
+    <row r="309" spans="1:2" ht="47.6">
       <c r="A309" s="3" t="s">
         <v>564</v>
       </c>
@@ -7302,7 +7302,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="313" spans="1:2" ht="94.5">
+    <row r="313" spans="1:2" ht="95.15">
       <c r="A313" s="3" t="s">
         <v>566</v>
       </c>
@@ -7310,7 +7310,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="314" spans="1:2" ht="31.5">
+    <row r="314" spans="1:2" ht="31.75">
       <c r="A314" s="3" t="s">
         <v>569</v>
       </c>
@@ -7358,7 +7358,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="320" spans="1:2" ht="31.5">
+    <row r="320" spans="1:2" ht="31.75">
       <c r="A320" s="3" t="s">
         <v>584</v>
       </c>
@@ -7390,7 +7390,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="324" spans="1:2" ht="31.5">
+    <row r="324" spans="1:2" ht="31.75">
       <c r="A324" s="3" t="s">
         <v>595</v>
       </c>
@@ -7406,7 +7406,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="326" spans="1:2" ht="31.5">
+    <row r="326" spans="1:2" ht="31.75">
       <c r="A326" s="3" t="s">
         <v>601</v>
       </c>
@@ -7422,7 +7422,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="328" spans="1:2" ht="63">
+    <row r="328" spans="1:2" ht="63.45">
       <c r="A328" s="3" t="s">
         <v>607</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="329" spans="1:2" ht="47.25">
+    <row r="329" spans="1:2" ht="47.6">
       <c r="A329" s="3" t="s">
         <v>609</v>
       </c>
@@ -7446,7 +7446,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="331" spans="1:2" ht="31.5">
+    <row r="331" spans="1:2" ht="31.75">
       <c r="A331" s="3" t="s">
         <v>613</v>
       </c>
@@ -7454,7 +7454,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="332" spans="1:2" ht="31.5">
+    <row r="332" spans="1:2" ht="31.75">
       <c r="A332" s="3" t="s">
         <v>616</v>
       </c>
@@ -7510,7 +7510,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="339" spans="1:2" ht="31.5">
+    <row r="339" spans="1:2" ht="31.75">
       <c r="A339" s="3" t="s">
         <v>630</v>
       </c>
@@ -7550,7 +7550,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="344" spans="1:2" ht="94.5">
+    <row r="344" spans="1:2" ht="95.15">
       <c r="A344" s="3" t="s">
         <v>638</v>
       </c>
@@ -7558,7 +7558,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="345" spans="1:2" ht="31.5">
+    <row r="345" spans="1:2" ht="31.75">
       <c r="A345" s="3" t="s">
         <v>639</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="351" spans="1:2" ht="31.5">
+    <row r="351" spans="1:2" ht="31.75">
       <c r="A351" s="3" t="s">
         <v>652</v>
       </c>
@@ -7614,7 +7614,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="352" spans="1:2" ht="31.5">
+    <row r="352" spans="1:2" ht="31.75">
       <c r="A352" s="3" t="s">
         <v>654</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="353" spans="1:2" ht="31.5">
+    <row r="353" spans="1:2" ht="31.75">
       <c r="A353" s="3" t="s">
         <v>656</v>
       </c>
@@ -7630,7 +7630,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="354" spans="1:2" ht="31.5">
+    <row r="354" spans="1:2" ht="47.6">
       <c r="A354" s="3" t="s">
         <v>658</v>
       </c>
@@ -7686,7 +7686,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="361" spans="1:2" ht="31.5">
+    <row r="361" spans="1:2" ht="31.75">
       <c r="A361" s="3" t="s">
         <v>667</v>
       </c>
@@ -7726,7 +7726,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="366" spans="1:2" ht="78.75">
+    <row r="366" spans="1:2" ht="79.3">
       <c r="A366" s="3" t="s">
         <v>671</v>
       </c>
@@ -7734,7 +7734,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="367" spans="1:2" ht="31.5">
+    <row r="367" spans="1:2" ht="31.75">
       <c r="A367" s="3" t="s">
         <v>673</v>
       </c>
@@ -7766,7 +7766,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="371" spans="1:2" ht="31.5">
+    <row r="371" spans="1:2" ht="31.75">
       <c r="A371" s="3" t="s">
         <v>679</v>
       </c>
@@ -7774,7 +7774,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="372" spans="1:2" ht="31.5">
+    <row r="372" spans="1:2" ht="31.75">
       <c r="A372" s="3" t="s">
         <v>682</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="374" spans="1:2" ht="31.5">
+    <row r="374" spans="1:2" ht="31.75">
       <c r="A374" s="3" t="s">
         <v>687</v>
       </c>
@@ -7798,7 +7798,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="375" spans="1:2" ht="31.5">
+    <row r="375" spans="1:2" ht="31.75">
       <c r="A375" s="3" t="s">
         <v>689</v>
       </c>
@@ -7806,7 +7806,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="376" spans="1:2" ht="31.5">
+    <row r="376" spans="1:2" ht="47.6">
       <c r="A376" s="3" t="s">
         <v>691</v>
       </c>
@@ -7862,7 +7862,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="383" spans="1:2" ht="31.5">
+    <row r="383" spans="1:2" ht="31.75">
       <c r="A383" s="3" t="s">
         <v>698</v>
       </c>
@@ -7902,7 +7902,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="388" spans="1:2" ht="78.75">
+    <row r="388" spans="1:2" ht="79.3">
       <c r="A388" s="3" t="s">
         <v>702</v>
       </c>
@@ -7910,7 +7910,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="389" spans="1:2" ht="31.5">
+    <row r="389" spans="1:2" ht="31.75">
       <c r="A389" s="3" t="s">
         <v>703</v>
       </c>
@@ -7966,7 +7966,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="396" spans="1:2" ht="31.5">
+    <row r="396" spans="1:2" ht="31.75">
       <c r="A396" s="3" t="s">
         <v>714</v>
       </c>
@@ -7990,7 +7990,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="399" spans="1:2" ht="31.5">
+    <row r="399" spans="1:2" ht="31.75">
       <c r="A399" s="3" t="s">
         <v>722</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="404" spans="1:2" ht="31.5">
+    <row r="404" spans="1:2" ht="31.75">
       <c r="A404" s="3" t="s">
         <v>732</v>
       </c>
@@ -8054,7 +8054,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="407" spans="1:2" ht="31.5">
+    <row r="407" spans="1:2" ht="31.75">
       <c r="A407" s="3" t="s">
         <v>735</v>
       </c>
@@ -8070,7 +8070,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="409" spans="1:2" ht="63">
+    <row r="409" spans="1:2" ht="63.45">
       <c r="A409" s="3" t="s">
         <v>737</v>
       </c>
@@ -8078,7 +8078,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="410" spans="1:2" ht="47.25">
+    <row r="410" spans="1:2" ht="47.6">
       <c r="A410" s="3" t="s">
         <v>739</v>
       </c>
@@ -8094,7 +8094,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="412" spans="1:2" ht="31.5">
+    <row r="412" spans="1:2" ht="31.75">
       <c r="A412" s="3" t="s">
         <v>742</v>
       </c>
@@ -8150,7 +8150,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="419" spans="1:2" ht="31.5">
+    <row r="419" spans="1:2" ht="31.75">
       <c r="A419" s="3" t="s">
         <v>749</v>
       </c>
@@ -8246,7 +8246,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="431" spans="1:2" ht="78.75">
+    <row r="431" spans="1:2" ht="79.3">
       <c r="A431" s="3" t="s">
         <v>758</v>
       </c>
@@ -8254,7 +8254,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="432" spans="1:2" ht="31.5">
+    <row r="432" spans="1:2" ht="31.75">
       <c r="A432" s="3" t="s">
         <v>759</v>
       </c>
@@ -8310,7 +8310,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="439" spans="1:2" ht="31.5">
+    <row r="439" spans="1:2" ht="31.75">
       <c r="A439" s="3" t="s">
         <v>768</v>
       </c>
@@ -8318,7 +8318,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="440" spans="1:2" ht="47.25">
+    <row r="440" spans="1:2" ht="47.6">
       <c r="A440" s="3" t="s">
         <v>770</v>
       </c>
@@ -8382,7 +8382,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="448" spans="1:2" ht="31.5">
+    <row r="448" spans="1:2" ht="31.75">
       <c r="A448" s="3" t="s">
         <v>779</v>
       </c>
@@ -8421,25 +8421,25 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView topLeftCell="A327" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B337" sqref="B337:B339"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="52" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" style="52" customWidth="1"/>
     <col min="2" max="2" width="12" style="50" customWidth="1"/>
     <col min="3" max="3" width="91.5" style="50" customWidth="1"/>
-    <col min="4" max="4" width="20.375" style="50" customWidth="1"/>
-    <col min="5" max="5" width="155.375" style="50" customWidth="1"/>
-    <col min="6" max="6" width="62.75" style="50" customWidth="1"/>
-    <col min="7" max="7" width="84.625" style="50" customWidth="1"/>
+    <col min="4" max="4" width="20.35546875" style="50" customWidth="1"/>
+    <col min="5" max="5" width="155.35546875" style="50" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="62.7109375" style="50" customWidth="1"/>
+    <col min="7" max="7" width="84.640625" style="50" customWidth="1"/>
     <col min="8" max="8" width="9" style="51"/>
     <col min="9" max="1027" width="8.5" style="34" customWidth="1"/>
     <col min="1028" max="16384" width="9" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="54" customFormat="1" ht="15.75">
+    <row r="1" spans="1:8" s="54" customFormat="1" ht="15.45">
       <c r="A1" s="33" t="s">
         <v>52</v>
       </c>
@@ -8463,7 +8463,7 @@
       </c>
       <c r="H1" s="53"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:8" ht="15.45">
       <c r="A2" s="35" t="s">
         <v>58</v>
       </c>
@@ -11181,7 +11181,7 @@
       </c>
       <c r="G147" s="38"/>
     </row>
-    <row r="148" spans="1:7" ht="30">
+    <row r="148" spans="1:7">
       <c r="A148" s="38" t="s">
         <v>131</v>
       </c>
@@ -11369,7 +11369,7 @@
       <c r="F157" s="37"/>
       <c r="G157" s="41"/>
     </row>
-    <row r="158" spans="1:7" ht="15.75">
+    <row r="158" spans="1:7" ht="15.45">
       <c r="A158" s="35" t="s">
         <v>58</v>
       </c>
@@ -11499,7 +11499,7 @@
       <c r="F165" s="41"/>
       <c r="G165" s="41"/>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:7" ht="30">
       <c r="A166" s="38" t="s">
         <v>58</v>
       </c>
@@ -11654,7 +11654,7 @@
       <c r="F174" s="40"/>
       <c r="G174" s="38"/>
     </row>
-    <row r="175" spans="1:7" ht="30">
+    <row r="175" spans="1:7" ht="45">
       <c r="A175" s="38" t="s">
         <v>58</v>
       </c>
@@ -11820,7 +11820,7 @@
       <c r="F184" s="41"/>
       <c r="G184" s="41"/>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" ht="30">
       <c r="A185" s="38" t="s">
         <v>58</v>
       </c>
@@ -11975,7 +11975,7 @@
       <c r="F193" s="40"/>
       <c r="G193" s="38"/>
     </row>
-    <row r="194" spans="1:7" ht="30">
+    <row r="194" spans="1:7" ht="45">
       <c r="A194" s="38" t="s">
         <v>58</v>
       </c>
@@ -12296,7 +12296,7 @@
       <c r="F212" s="40"/>
       <c r="G212" s="38"/>
     </row>
-    <row r="213" spans="1:7" ht="30">
+    <row r="213" spans="1:7" ht="45">
       <c r="A213" s="38" t="s">
         <v>58</v>
       </c>
@@ -12517,7 +12517,7 @@
       <c r="F225" s="38"/>
       <c r="G225" s="38"/>
     </row>
-    <row r="226" spans="1:7">
+    <row r="226" spans="1:7" ht="30">
       <c r="A226" s="38" t="s">
         <v>58</v>
       </c>
@@ -12974,7 +12974,7 @@
       <c r="F252" s="38"/>
       <c r="G252" s="38"/>
     </row>
-    <row r="253" spans="1:7" ht="15.75">
+    <row r="253" spans="1:7" ht="15.45">
       <c r="A253" s="38" t="s">
         <v>58</v>
       </c>
@@ -14343,7 +14343,7 @@
       <c r="F333" s="38"/>
       <c r="G333" s="38"/>
     </row>
-    <row r="334" spans="1:7" ht="15.75">
+    <row r="334" spans="1:7" ht="15.45">
       <c r="A334" s="38" t="s">
         <v>58</v>
       </c>
@@ -14411,7 +14411,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="338" spans="1:7" ht="45">
+    <row r="338" spans="1:7">
       <c r="A338" s="38" t="s">
         <v>58</v>
       </c>
@@ -14990,7 +14990,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="369" spans="1:7" ht="60">
+    <row r="369" spans="1:7" ht="30">
       <c r="A369" s="38" t="s">
         <v>58</v>
       </c>
@@ -15402,7 +15402,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="391" spans="1:7" ht="60">
+    <row r="391" spans="1:7" ht="30">
       <c r="A391" s="38" t="s">
         <v>58</v>
       </c>
@@ -15791,7 +15791,7 @@
       <c r="F411" s="41"/>
       <c r="G411" s="41"/>
     </row>
-    <row r="412" spans="1:7" ht="78.75">
+    <row r="412" spans="1:7" ht="45">
       <c r="A412" s="38" t="s">
         <v>58</v>
       </c>
@@ -15814,7 +15814,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="413" spans="1:7" ht="60">
+    <row r="413" spans="1:7">
       <c r="A413" s="38" t="s">
         <v>58</v>
       </c>
@@ -16858,14 +16858,14 @@
       <selection activeCell="G6" sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="45.125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.625" style="4" customWidth="1"/>
-    <col min="4" max="5" width="81.375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="45.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.640625" style="4" customWidth="1"/>
+    <col min="4" max="5" width="81.35546875" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="1025" width="8.875" style="4" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="4" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
@@ -16949,7 +16949,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="126">
+    <row r="5" spans="1:7" ht="126.9">
       <c r="A5" s="3" t="s">
         <v>71</v>
       </c>
@@ -17005,20 +17005,20 @@
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="29" customWidth="1"/>
     <col min="2" max="2" width="68.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="100" style="4" customWidth="1"/>
-    <col min="5" max="5" width="6.125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="22.875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="20" style="4" customWidth="1"/>
-    <col min="8" max="1025" width="8.875" style="4" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="4" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" s="24" customFormat="1" ht="31.5">
+    <row r="1" spans="1:1025" s="24" customFormat="1" ht="31.75">
       <c r="A1" s="8" t="s">
         <v>782</v>
       </c>
@@ -18173,7 +18173,7 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:1025" ht="31.5">
+    <row r="8" spans="1:1025">
       <c r="A8" s="3" t="s">
         <v>810</v>
       </c>
@@ -18344,7 +18344,7 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" ht="47.25">
+    <row r="17" spans="1:7" ht="47.6">
       <c r="A17" s="3" t="s">
         <v>125</v>
       </c>
@@ -18726,7 +18726,7 @@
       </c>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" ht="63">
+    <row r="37" spans="1:7" ht="63.45">
       <c r="A37" s="3" t="s">
         <v>257</v>
       </c>
@@ -18747,7 +18747,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="31.5">
+    <row r="38" spans="1:7" ht="31.75">
       <c r="A38" s="3" t="s">
         <v>526</v>
       </c>
@@ -18823,7 +18823,7 @@
       </c>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7" ht="47.25">
+    <row r="42" spans="1:7" ht="47.6">
       <c r="A42" s="3" t="s">
         <v>274</v>
       </c>
@@ -19107,19 +19107,19 @@
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="29" customWidth="1"/>
-    <col min="2" max="2" width="47.375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="4" customWidth="1"/>
-    <col min="4" max="5" width="80.875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="29" customWidth="1"/>
+    <col min="2" max="2" width="47.35546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="4" customWidth="1"/>
+    <col min="4" max="5" width="80.85546875" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="19" customWidth="1"/>
+    <col min="8" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="24" customFormat="1" ht="30.95" customHeight="1">
+    <row r="1" spans="1:256" s="24" customFormat="1" ht="31" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>782</v>
       </c>
@@ -19391,7 +19391,7 @@
       <c r="IU1" s="23"/>
       <c r="IV1" s="23"/>
     </row>
-    <row r="2" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="2" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A2" s="30" t="s">
         <v>860</v>
       </c>
@@ -19410,7 +19410,7 @@
       </c>
       <c r="G2" s="30"/>
     </row>
-    <row r="3" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A3" s="30" t="s">
         <v>863</v>
       </c>
@@ -19429,7 +19429,7 @@
       </c>
       <c r="G3" s="30"/>
     </row>
-    <row r="4" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A4" s="30" t="s">
         <v>865</v>
       </c>
@@ -19467,7 +19467,7 @@
       </c>
       <c r="G5" s="30"/>
     </row>
-    <row r="6" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A6" s="30" t="s">
         <v>869</v>
       </c>
@@ -19486,7 +19486,7 @@
       </c>
       <c r="G6" s="30"/>
     </row>
-    <row r="7" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="7" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A7" s="30" t="s">
         <v>872</v>
       </c>
@@ -19505,7 +19505,7 @@
       </c>
       <c r="G7" s="30"/>
     </row>
-    <row r="8" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="8" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A8" s="30" t="s">
         <v>875</v>
       </c>
@@ -19543,7 +19543,7 @@
       </c>
       <c r="G9" s="30"/>
     </row>
-    <row r="10" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="10" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A10" s="30" t="s">
         <v>881</v>
       </c>
@@ -19562,7 +19562,7 @@
       </c>
       <c r="G10" s="30"/>
     </row>
-    <row r="11" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A11" s="30" t="s">
         <v>883</v>
       </c>
@@ -19581,7 +19581,7 @@
       </c>
       <c r="G11" s="30"/>
     </row>
-    <row r="12" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="12" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A12" s="30" t="s">
         <v>885</v>
       </c>
@@ -19619,7 +19619,7 @@
       </c>
       <c r="G13" s="30"/>
     </row>
-    <row r="14" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="14" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A14" s="30" t="s">
         <v>890</v>
       </c>
@@ -19638,7 +19638,7 @@
       </c>
       <c r="G14" s="30"/>
     </row>
-    <row r="15" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="15" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A15" s="30" t="s">
         <v>892</v>
       </c>
@@ -19695,7 +19695,7 @@
       </c>
       <c r="G17" s="30"/>
     </row>
-    <row r="18" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="18" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A18" s="30" t="s">
         <v>894</v>
       </c>
@@ -19714,7 +19714,7 @@
       </c>
       <c r="G18" s="30"/>
     </row>
-    <row r="19" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="19" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A19" s="30" t="s">
         <v>896</v>
       </c>
@@ -19733,7 +19733,7 @@
       </c>
       <c r="G19" s="30"/>
     </row>
-    <row r="20" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A20" s="30" t="s">
         <v>898</v>
       </c>
@@ -19752,7 +19752,7 @@
       </c>
       <c r="G20" s="30"/>
     </row>
-    <row r="21" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="21" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A21" s="30" t="s">
         <v>900</v>
       </c>
@@ -19771,7 +19771,7 @@
       </c>
       <c r="G21" s="30"/>
     </row>
-    <row r="22" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="22" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A22" s="30" t="s">
         <v>903</v>
       </c>
@@ -19790,7 +19790,7 @@
       </c>
       <c r="G22" s="30"/>
     </row>
-    <row r="23" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="23" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A23" s="30" t="s">
         <v>905</v>
       </c>
@@ -19809,7 +19809,7 @@
       </c>
       <c r="G23" s="30"/>
     </row>
-    <row r="24" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="24" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A24" s="30" t="s">
         <v>907</v>
       </c>
@@ -19828,7 +19828,7 @@
       </c>
       <c r="G24" s="30"/>
     </row>
-    <row r="25" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="25" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A25" s="30" t="s">
         <v>909</v>
       </c>
@@ -19847,7 +19847,7 @@
       </c>
       <c r="G25" s="30"/>
     </row>
-    <row r="26" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="26" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A26" s="30" t="s">
         <v>912</v>
       </c>
@@ -19866,7 +19866,7 @@
       </c>
       <c r="G26" s="30"/>
     </row>
-    <row r="27" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="27" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A27" s="30" t="s">
         <v>914</v>
       </c>
@@ -19885,7 +19885,7 @@
       </c>
       <c r="G27" s="30"/>
     </row>
-    <row r="28" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="28" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A28" s="30" t="s">
         <v>917</v>
       </c>
@@ -19904,7 +19904,7 @@
       </c>
       <c r="G28" s="30"/>
     </row>
-    <row r="29" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="29" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A29" s="30" t="s">
         <v>919</v>
       </c>
@@ -19923,7 +19923,7 @@
       </c>
       <c r="G29" s="30"/>
     </row>
-    <row r="30" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="30" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A30" s="30" t="s">
         <v>921</v>
       </c>
@@ -19942,7 +19942,7 @@
       </c>
       <c r="G30" s="30"/>
     </row>
-    <row r="31" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="31" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A31" s="30" t="s">
         <v>923</v>
       </c>
@@ -19961,7 +19961,7 @@
       </c>
       <c r="G31" s="30"/>
     </row>
-    <row r="32" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="32" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A32" s="30" t="s">
         <v>926</v>
       </c>
@@ -19980,7 +19980,7 @@
       </c>
       <c r="G32" s="30"/>
     </row>
-    <row r="33" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="33" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A33" s="30" t="s">
         <v>929</v>
       </c>
@@ -19999,7 +19999,7 @@
       </c>
       <c r="G33" s="30"/>
     </row>
-    <row r="34" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="34" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A34" s="30" t="s">
         <v>932</v>
       </c>
@@ -20018,7 +20018,7 @@
       </c>
       <c r="G34" s="30"/>
     </row>
-    <row r="35" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="35" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A35" s="30" t="s">
         <v>935</v>
       </c>
@@ -20037,7 +20037,7 @@
       </c>
       <c r="G35" s="30"/>
     </row>
-    <row r="36" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="36" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A36" s="30" t="s">
         <v>938</v>
       </c>
@@ -20056,7 +20056,7 @@
       </c>
       <c r="G36" s="30"/>
     </row>
-    <row r="37" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="37" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A37" s="30" t="s">
         <v>941</v>
       </c>
@@ -20075,7 +20075,7 @@
       </c>
       <c r="G37" s="30"/>
     </row>
-    <row r="38" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="38" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A38" s="30" t="s">
         <v>944</v>
       </c>
@@ -20094,7 +20094,7 @@
       </c>
       <c r="G38" s="30"/>
     </row>
-    <row r="39" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="39" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A39" s="30" t="s">
         <v>947</v>
       </c>
@@ -20113,7 +20113,7 @@
       </c>
       <c r="G39" s="30"/>
     </row>
-    <row r="40" spans="1:7" ht="30.95" customHeight="1">
+    <row r="40" spans="1:7" ht="31" customHeight="1">
       <c r="A40" s="30" t="s">
         <v>950</v>
       </c>
@@ -20149,7 +20149,7 @@
       <c r="F41" s="30"/>
       <c r="G41" s="30"/>
     </row>
-    <row r="42" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="42" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A42" s="30" t="s">
         <v>957</v>
       </c>
@@ -20166,7 +20166,7 @@
       <c r="F42" s="30"/>
       <c r="G42" s="30"/>
     </row>
-    <row r="43" spans="1:7" ht="30.95" customHeight="1">
+    <row r="43" spans="1:7" ht="31" customHeight="1">
       <c r="A43" s="30" t="s">
         <v>960</v>
       </c>
@@ -20204,7 +20204,7 @@
       <c r="F44" s="30"/>
       <c r="G44" s="30"/>
     </row>
-    <row r="45" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="45" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A45" s="30" t="s">
         <v>968</v>
       </c>
@@ -20257,7 +20257,7 @@
       <c r="F47" s="30"/>
       <c r="G47" s="30"/>
     </row>
-    <row r="48" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="48" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A48" s="30" t="s">
         <v>978</v>
       </c>
@@ -20274,7 +20274,7 @@
       <c r="F48" s="30"/>
       <c r="G48" s="30"/>
     </row>
-    <row r="49" spans="1:256" s="57" customFormat="1" ht="31.5">
+    <row r="49" spans="1:256" s="57" customFormat="1" ht="31.75">
       <c r="A49" s="31" t="s">
         <v>981</v>
       </c>
@@ -20558,21 +20558,21 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="29" customWidth="1"/>
     <col min="2" max="2" width="33.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14.625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="44.375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="41.375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="14.640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="44.35546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="41.35546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.640625" style="4" customWidth="1"/>
     <col min="7" max="7" width="29" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="19" customWidth="1"/>
+    <col min="8" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="24" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:256" s="24" customFormat="1" ht="17.149999999999999" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>782</v>
       </c>
@@ -21272,7 +21272,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" ht="31.5">
+    <row r="24" spans="1:7" ht="31.75">
       <c r="A24" s="32" t="s">
         <v>1158</v>
       </c>
@@ -21289,7 +21289,7 @@
       <c r="F24" s="32"/>
       <c r="G24" s="32"/>
     </row>
-    <row r="25" spans="1:7" ht="47.25">
+    <row r="25" spans="1:7" ht="47.6">
       <c r="A25" s="32" t="s">
         <v>1162</v>
       </c>
@@ -21306,7 +21306,7 @@
       <c r="F25" s="32"/>
       <c r="G25" s="32"/>
     </row>
-    <row r="26" spans="1:7" ht="31.5">
+    <row r="26" spans="1:7" ht="31.75">
       <c r="A26" s="32" t="s">
         <v>1164</v>
       </c>
@@ -21323,7 +21323,7 @@
       <c r="F26" s="32"/>
       <c r="G26" s="32"/>
     </row>
-    <row r="27" spans="1:7" ht="47.25">
+    <row r="27" spans="1:7" ht="47.6">
       <c r="A27" s="32" t="s">
         <v>1167</v>
       </c>
@@ -21340,7 +21340,7 @@
       <c r="F27" s="32"/>
       <c r="G27" s="32"/>
     </row>
-    <row r="28" spans="1:7" ht="47.25">
+    <row r="28" spans="1:7" ht="31.75">
       <c r="A28" s="32" t="s">
         <v>1170</v>
       </c>
@@ -21357,7 +21357,7 @@
       <c r="F28" s="32"/>
       <c r="G28" s="32"/>
     </row>
-    <row r="29" spans="1:7" ht="31.5">
+    <row r="29" spans="1:7" ht="31.75">
       <c r="A29" s="32" t="s">
         <v>1173</v>
       </c>
@@ -21374,7 +21374,7 @@
       <c r="F29" s="32"/>
       <c r="G29" s="32"/>
     </row>
-    <row r="30" spans="1:7" ht="47.25">
+    <row r="30" spans="1:7" ht="47.6">
       <c r="A30" s="32" t="s">
         <v>1176</v>
       </c>
@@ -21405,20 +21405,20 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:IV4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="54.625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="75.625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="132.375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="54.640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="75.640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="132.35546875" style="4" customWidth="1"/>
     <col min="6" max="7" width="10.5" style="4" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="4" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="19" customWidth="1"/>
+    <col min="8" max="256" width="8.85546875" style="4" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
@@ -21445,7 +21445,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="2" spans="1:256" s="61" customFormat="1" ht="63">
+    <row r="2" spans="1:256" s="61" customFormat="1" ht="63.45">
       <c r="A2" s="8" t="s">
         <v>1031</v>
       </c>
@@ -21715,7 +21715,7 @@
       <c r="IU2" s="60"/>
       <c r="IV2" s="60"/>
     </row>
-    <row r="3" spans="1:256" ht="31.5">
+    <row r="3" spans="1:256">
       <c r="A3" s="5" t="s">
         <v>1034</v>
       </c>
@@ -21736,7 +21736,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:256" ht="63">
+    <row r="4" spans="1:256" ht="63.45">
       <c r="A4" s="5" t="s">
         <v>1036</v>
       </c>
@@ -21775,21 +21775,21 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="10.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="53.375" style="20" customWidth="1"/>
+    <col min="2" max="2" width="53.35546875" style="20" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="20" customWidth="1"/>
     <col min="4" max="4" width="44.5" style="20" customWidth="1"/>
-    <col min="5" max="5" width="31.875" style="20" customWidth="1"/>
-    <col min="6" max="6" width="11.875" style="20" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="20" customWidth="1"/>
     <col min="7" max="7" width="44.5" style="20" customWidth="1"/>
-    <col min="8" max="256" width="8.875" style="20" customWidth="1"/>
-    <col min="257" max="1025" width="8.875" style="21" customWidth="1"/>
+    <col min="8" max="256" width="8.85546875" style="20" customWidth="1"/>
+    <col min="257" max="1025" width="8.85546875" style="21" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" s="27" customFormat="1" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:256" s="27" customFormat="1" ht="17.149999999999999" customHeight="1">
       <c r="A1" s="30" t="s">
         <v>782</v>
       </c>
@@ -22082,7 +22082,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="3" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A3" s="30" t="s">
         <v>648</v>
       </c>
@@ -22101,7 +22101,7 @@
       </c>
       <c r="G3" s="30"/>
     </row>
-    <row r="4" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="4" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A4" s="30" t="s">
         <v>577</v>
       </c>
@@ -22120,7 +22120,7 @@
       </c>
       <c r="G4" s="30"/>
     </row>
-    <row r="5" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="5" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A5" s="30" t="s">
         <v>580</v>
       </c>
@@ -22139,7 +22139,7 @@
       </c>
       <c r="G5" s="30"/>
     </row>
-    <row r="6" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="6" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A6" s="30" t="s">
         <v>583</v>
       </c>
@@ -22238,7 +22238,7 @@
       </c>
       <c r="G10" s="30"/>
     </row>
-    <row r="11" spans="1:256" ht="17.100000000000001" customHeight="1">
+    <row r="11" spans="1:256" ht="17.149999999999999" customHeight="1">
       <c r="A11" s="30" t="s">
         <v>600</v>
       </c>
@@ -22257,7 +22257,7 @@
       </c>
       <c r="G11" s="30"/>
     </row>
-    <row r="12" spans="1:256" ht="33.6" customHeight="1">
+    <row r="12" spans="1:256" ht="33.65" customHeight="1">
       <c r="A12" s="30" t="s">
         <v>603</v>
       </c>
@@ -22419,7 +22419,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="20" spans="1:7" ht="17.149999999999999" customHeight="1">
       <c r="A20" s="30" t="s">
         <v>721</v>
       </c>
@@ -22484,7 +22484,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="31.5">
+    <row r="23" spans="1:7" ht="31.75">
       <c r="A23" s="30" t="s">
         <v>1114</v>
       </c>
@@ -22535,7 +22535,7 @@
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>
     </row>
-    <row r="26" spans="1:7" ht="31.5">
+    <row r="26" spans="1:7" ht="31.75">
       <c r="A26" s="30" t="s">
         <v>1109</v>
       </c>
@@ -22585,16 +22585,16 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
   <cols>
     <col min="1" max="1" width="19" style="22" customWidth="1"/>
-    <col min="2" max="2" width="53.375" style="19" customWidth="1"/>
+    <col min="2" max="2" width="53.35546875" style="19" customWidth="1"/>
     <col min="3" max="3" width="21.5" style="19" customWidth="1"/>
     <col min="4" max="4" width="25" style="19" customWidth="1"/>
     <col min="5" max="5" width="46" style="19" customWidth="1"/>
-    <col min="6" max="6" width="11.875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="19" customWidth="1"/>
     <col min="7" max="7" width="44.5" style="19" customWidth="1"/>
-    <col min="8" max="1025" width="8.875" style="19" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="19" customWidth="1"/>
     <col min="1026" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
populate missing container oids
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\gsa-devel\piv-conformance-swing\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87D595A-DBDD-42C6-85EB-1D796A0520F7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB36662-B68E-4B2C-A5FB-CC99DD6BFCA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="18472" windowHeight="11623" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3724" uniqueCount="1302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="1302">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -8421,8 +8421,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A446" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F431" sqref="F431:F471"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -16181,7 +16181,9 @@
       </c>
       <c r="D432" s="41"/>
       <c r="E432" s="41"/>
-      <c r="F432" s="41"/>
+      <c r="F432" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G432" s="41"/>
     </row>
     <row r="433" spans="1:7" ht="45">
@@ -16198,7 +16200,9 @@
         <v>606</v>
       </c>
       <c r="E433" s="40"/>
-      <c r="F433" s="40"/>
+      <c r="F433" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G433" s="44" t="s">
         <v>738</v>
       </c>
@@ -16217,7 +16221,9 @@
         <v>606</v>
       </c>
       <c r="E434" s="40"/>
-      <c r="F434" s="40"/>
+      <c r="F434" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G434" s="44"/>
     </row>
     <row r="435" spans="1:7">
@@ -16234,7 +16240,9 @@
         <v>606</v>
       </c>
       <c r="E435" s="40"/>
-      <c r="F435" s="40"/>
+      <c r="F435" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G435" s="44" t="s">
         <v>606</v>
       </c>
@@ -16253,7 +16261,9 @@
         <v>618</v>
       </c>
       <c r="E436" s="40"/>
-      <c r="F436" s="40"/>
+      <c r="F436" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G436" s="44"/>
     </row>
     <row r="437" spans="1:7">
@@ -16268,7 +16278,9 @@
       </c>
       <c r="D437" s="41"/>
       <c r="E437" s="41"/>
-      <c r="F437" s="41"/>
+      <c r="F437" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G437" s="41"/>
     </row>
     <row r="438" spans="1:7">
@@ -16285,7 +16297,9 @@
         <v>597</v>
       </c>
       <c r="E438" s="40"/>
-      <c r="F438" s="40"/>
+      <c r="F438" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G438" s="44" t="s">
         <v>1107</v>
       </c>
@@ -16306,7 +16320,9 @@
       <c r="E439" s="40" t="s">
         <v>1133</v>
       </c>
-      <c r="F439" s="40"/>
+      <c r="F439" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G439" s="38"/>
     </row>
     <row r="440" spans="1:7">
@@ -16321,7 +16337,9 @@
       </c>
       <c r="D440" s="41"/>
       <c r="E440" s="41"/>
-      <c r="F440" s="41"/>
+      <c r="F440" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G440" s="41"/>
     </row>
     <row r="441" spans="1:7">
@@ -16340,7 +16358,9 @@
       <c r="E441" s="38" t="s">
         <v>636</v>
       </c>
-      <c r="F441" s="38"/>
+      <c r="F441" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G441" s="38"/>
     </row>
     <row r="442" spans="1:7">
@@ -16355,7 +16375,9 @@
       </c>
       <c r="D442" s="41"/>
       <c r="E442" s="41"/>
-      <c r="F442" s="41"/>
+      <c r="F442" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G442" s="37"/>
     </row>
     <row r="443" spans="1:7">
@@ -16372,7 +16394,9 @@
       <c r="E443" s="44" t="s">
         <v>279</v>
       </c>
-      <c r="F443" s="44"/>
+      <c r="F443" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G443" s="44"/>
     </row>
     <row r="444" spans="1:7">
@@ -16389,7 +16413,9 @@
       <c r="E444" s="44" t="s">
         <v>279</v>
       </c>
-      <c r="F444" s="44"/>
+      <c r="F444" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G444" s="44"/>
     </row>
     <row r="445" spans="1:7">
@@ -16406,7 +16432,9 @@
       <c r="E445" s="44" t="s">
         <v>279</v>
       </c>
-      <c r="F445" s="44"/>
+      <c r="F445" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G445" s="44"/>
     </row>
     <row r="446" spans="1:7">
@@ -16421,7 +16449,9 @@
       </c>
       <c r="D446" s="41"/>
       <c r="E446" s="37"/>
-      <c r="F446" s="37"/>
+      <c r="F446" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G446" s="37"/>
     </row>
     <row r="447" spans="1:7">
@@ -16438,7 +16468,9 @@
       <c r="E447" s="44" t="s">
         <v>279</v>
       </c>
-      <c r="F447" s="44"/>
+      <c r="F447" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G447" s="44"/>
     </row>
     <row r="448" spans="1:7">
@@ -16455,7 +16487,9 @@
       <c r="E448" s="44" t="s">
         <v>279</v>
       </c>
-      <c r="F448" s="44"/>
+      <c r="F448" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G448" s="44"/>
     </row>
     <row r="449" spans="1:7">
@@ -16470,7 +16504,9 @@
       </c>
       <c r="D449" s="41"/>
       <c r="E449" s="41"/>
-      <c r="F449" s="41"/>
+      <c r="F449" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G449" s="37"/>
     </row>
     <row r="450" spans="1:7">
@@ -16485,7 +16521,9 @@
       </c>
       <c r="D450" s="41"/>
       <c r="E450" s="41"/>
-      <c r="F450" s="41"/>
+      <c r="F450" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G450" s="41"/>
     </row>
     <row r="451" spans="1:7" ht="45">
@@ -16502,7 +16540,9 @@
         <v>78.3</v>
       </c>
       <c r="E451" s="38"/>
-      <c r="F451" s="38"/>
+      <c r="F451" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G451" s="44" t="s">
         <v>568</v>
       </c>
@@ -16521,7 +16561,9 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E452" s="38"/>
-      <c r="F452" s="38"/>
+      <c r="F452" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G452" s="44"/>
     </row>
     <row r="453" spans="1:7">
@@ -16538,7 +16580,9 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E453" s="38"/>
-      <c r="F453" s="38"/>
+      <c r="F453" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G453" s="44"/>
     </row>
     <row r="454" spans="1:7">
@@ -16553,7 +16597,9 @@
       </c>
       <c r="D454" s="41"/>
       <c r="E454" s="41"/>
-      <c r="F454" s="41"/>
+      <c r="F454" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G454" s="41"/>
     </row>
     <row r="455" spans="1:7">
@@ -16568,7 +16614,9 @@
       </c>
       <c r="D455" s="41"/>
       <c r="E455" s="41"/>
-      <c r="F455" s="41"/>
+      <c r="F455" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G455" s="41"/>
     </row>
     <row r="456" spans="1:7">
@@ -16585,7 +16633,9 @@
         <v>577</v>
       </c>
       <c r="E456" s="38"/>
-      <c r="F456" s="38"/>
+      <c r="F456" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G456" s="44" t="s">
         <v>1110</v>
       </c>
@@ -16604,7 +16654,9 @@
         <v>580</v>
       </c>
       <c r="E457" s="38"/>
-      <c r="F457" s="38"/>
+      <c r="F457" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G457" s="44"/>
     </row>
     <row r="458" spans="1:7">
@@ -16621,10 +16673,12 @@
         <v>1111</v>
       </c>
       <c r="E458" s="38"/>
-      <c r="F458" s="38"/>
+      <c r="F458" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G458" s="38"/>
     </row>
-    <row r="459" spans="1:7">
+    <row r="459" spans="1:7" ht="30">
       <c r="A459" s="38" t="s">
         <v>58</v>
       </c>
@@ -16638,7 +16692,9 @@
         <v>618</v>
       </c>
       <c r="E459" s="38"/>
-      <c r="F459" s="38"/>
+      <c r="F459" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G459" s="38"/>
     </row>
     <row r="460" spans="1:7">
@@ -16653,7 +16709,9 @@
       </c>
       <c r="D460" s="38"/>
       <c r="E460" s="38"/>
-      <c r="F460" s="38"/>
+      <c r="F460" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G460" s="38"/>
     </row>
     <row r="461" spans="1:7" ht="30">
@@ -16670,7 +16728,9 @@
         <v>586</v>
       </c>
       <c r="E461" s="38"/>
-      <c r="F461" s="38"/>
+      <c r="F461" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G461" s="38"/>
     </row>
     <row r="462" spans="1:7">
@@ -16687,7 +16747,9 @@
         <v>724</v>
       </c>
       <c r="E462" s="38"/>
-      <c r="F462" s="38"/>
+      <c r="F462" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G462" s="38"/>
     </row>
     <row r="463" spans="1:7">
@@ -16702,7 +16764,9 @@
       </c>
       <c r="D463" s="41"/>
       <c r="E463" s="41"/>
-      <c r="F463" s="41"/>
+      <c r="F463" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G463" s="41"/>
     </row>
     <row r="464" spans="1:7">
@@ -16719,7 +16783,9 @@
         <v>597</v>
       </c>
       <c r="E464" s="38"/>
-      <c r="F464" s="38"/>
+      <c r="F464" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G464" s="44" t="s">
         <v>1107</v>
       </c>
@@ -16738,7 +16804,9 @@
         <v>1106</v>
       </c>
       <c r="E465" s="40"/>
-      <c r="F465" s="40"/>
+      <c r="F465" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G465" s="38"/>
     </row>
     <row r="466" spans="1:7">
@@ -16753,7 +16821,9 @@
       </c>
       <c r="D466" s="41"/>
       <c r="E466" s="41"/>
-      <c r="F466" s="41"/>
+      <c r="F466" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G466" s="41"/>
     </row>
     <row r="467" spans="1:7">
@@ -16770,7 +16840,9 @@
         <v>591</v>
       </c>
       <c r="E467" s="38"/>
-      <c r="F467" s="38"/>
+      <c r="F467" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G467" s="44" t="s">
         <v>1108</v>
       </c>
@@ -16789,7 +16861,9 @@
         <v>594</v>
       </c>
       <c r="E468" s="38"/>
-      <c r="F468" s="38"/>
+      <c r="F468" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G468" s="44"/>
     </row>
     <row r="469" spans="1:7">
@@ -16806,7 +16880,9 @@
         <v>597</v>
       </c>
       <c r="E469" s="38"/>
-      <c r="F469" s="38"/>
+      <c r="F469" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G469" s="44"/>
     </row>
     <row r="470" spans="1:7">
@@ -16823,7 +16899,9 @@
         <v>1112</v>
       </c>
       <c r="E470" s="38"/>
-      <c r="F470" s="38"/>
+      <c r="F470" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G470" s="38"/>
     </row>
     <row r="471" spans="1:7">
@@ -16840,7 +16918,9 @@
         <v>1109</v>
       </c>
       <c r="E471" s="38"/>
-      <c r="F471" s="38"/>
+      <c r="F471" s="38" t="s">
+        <v>1155</v>
+      </c>
       <c r="G471" s="38"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add missing parameter for PKIX.24
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\gsa-devel\piv-conformance-swing\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB36662-B68E-4B2C-A5FB-CC99DD6BFCA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF3F608-6A9E-463F-A8C4-E4C6A2744622}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="1302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3765" uniqueCount="1303">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3939,6 +3939,9 @@
 X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID:1.2.840.113549.1.1.1+NULL|1.2.840.10045.2.1+1.2.840.10045.3.1.7,
 X509_CERTIFICATE_FOR_DIGITAL_CERTIFICATE_OID:1.2.840.113549.1.1.1+NULL|1.2.840.10045.2.1+1.2.840.10045.3.1.7|1.2.840.10045.2.1+1.3.132.0.34,
 X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID:1.2.840.113549.1.1.1+NULL|1.2.840.10045.2.1+1.2.840.10045.3.1.7|1.2.840.10045.2.1+1.3.132.0.34</t>
+  </si>
+  <si>
+    <t>2.5.29.31</t>
   </si>
 </sst>
 </file>
@@ -8421,7 +8424,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A446" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A446" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="F431" sqref="F431:F471"/>
     </sheetView>
   </sheetViews>
@@ -21851,8 +21854,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.9"/>
@@ -22611,7 +22614,9 @@
       <c r="D25" s="30" t="s">
         <v>624</v>
       </c>
-      <c r="E25" s="30"/>
+      <c r="E25" s="30" t="s">
+        <v>1302</v>
+      </c>
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>
     </row>

</xml_diff>

<commit_message>
fix container ids for content signing cert, update parameters based on changes to PKIX.6
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF29BDA9-CEAE-4605-80E1-5C5B7C1C5EEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1455D6BD-30A3-4F34-8403-A0B484D0BB20}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3183,9 +3183,6 @@
     <t>Confirm that id- fpki-common-authentication OID is asserted in certificate policies</t>
   </si>
   <si>
-    <t>2.16.840.1.101.3.2.1.48.11</t>
-  </si>
-  <si>
     <t>PKIX_Test_7</t>
   </si>
   <si>
@@ -3942,6 +3939,9 @@
   </si>
   <si>
     <t>CARDHOLDER_IRIS_IMAGES_OID</t>
+  </si>
+  <si>
+    <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID;2.16.840.1.101.3.2.1.48.11,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID;2.16.840.1.101.3.2.1.48.9:2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID;2.16.840.1.101.3.2.1.48.9:2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID;2.16.840.1.101.3.2.1.48.13,CARD_HOLDER_UNIQUE_IDENTIFIER_OID;2.16.840.1.101.3.2.1.48.86</t>
   </si>
 </sst>
 </file>
@@ -8448,8 +8448,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A319" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F333" sqref="F333"/>
+    <sheetView tabSelected="1" topLeftCell="A445" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F449" sqref="F449:F471"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8483,7 +8483,7 @@
         <v>56</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G1" s="33" t="s">
         <v>55</v>
@@ -8495,7 +8495,7 @@
         <v>58</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C2" s="36" t="s">
         <v>0</v>
@@ -8525,10 +8525,10 @@
         <v>58</v>
       </c>
       <c r="B4" s="38" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C4" s="37" t="s">
         <v>1254</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>1255</v>
       </c>
       <c r="D4" s="37"/>
       <c r="E4" s="37"/>
@@ -8550,7 +8550,7 @@
       </c>
       <c r="E5" s="38"/>
       <c r="F5" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G5" s="38" t="s">
         <v>61</v>
@@ -8571,7 +8571,7 @@
       </c>
       <c r="E6" s="38"/>
       <c r="F6" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G6" s="38"/>
     </row>
@@ -8590,7 +8590,7 @@
       </c>
       <c r="E7" s="38"/>
       <c r="F7" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G7" s="38"/>
     </row>
@@ -8609,7 +8609,7 @@
       </c>
       <c r="E8" s="38"/>
       <c r="F8" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G8" s="38"/>
     </row>
@@ -8628,7 +8628,7 @@
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G9" s="38"/>
     </row>
@@ -8647,7 +8647,7 @@
       </c>
       <c r="E10" s="38"/>
       <c r="F10" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G10" s="38"/>
     </row>
@@ -8666,7 +8666,7 @@
       </c>
       <c r="E11" s="38"/>
       <c r="F11" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G11" s="38"/>
     </row>
@@ -8685,7 +8685,7 @@
       </c>
       <c r="E12" s="38"/>
       <c r="F12" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G12" s="38"/>
     </row>
@@ -8704,7 +8704,7 @@
       </c>
       <c r="E13" s="38"/>
       <c r="F13" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G13" s="38"/>
     </row>
@@ -8723,7 +8723,7 @@
       </c>
       <c r="E14" s="38"/>
       <c r="F14" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G14" s="38"/>
     </row>
@@ -8742,7 +8742,7 @@
       </c>
       <c r="E15" s="38"/>
       <c r="F15" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G15" s="38"/>
     </row>
@@ -8766,10 +8766,10 @@
         <v>58</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D17" s="37"/>
       <c r="E17" s="37"/>
@@ -8791,7 +8791,7 @@
       </c>
       <c r="E18" s="38"/>
       <c r="F18" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G18" s="38" t="s">
         <v>95</v>
@@ -8812,7 +8812,7 @@
       </c>
       <c r="E19" s="38"/>
       <c r="F19" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G19" s="38"/>
     </row>
@@ -8831,7 +8831,7 @@
       </c>
       <c r="E20" s="38"/>
       <c r="F20" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G20" s="38"/>
     </row>
@@ -8850,7 +8850,7 @@
       </c>
       <c r="E21" s="38"/>
       <c r="F21" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G21" s="38"/>
     </row>
@@ -8869,7 +8869,7 @@
       </c>
       <c r="E22" s="38"/>
       <c r="F22" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G22" s="38"/>
     </row>
@@ -8881,14 +8881,14 @@
         <v>102</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="D23" s="38" t="s">
         <v>104</v>
       </c>
       <c r="E23" s="38"/>
       <c r="F23" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G23" s="38"/>
     </row>
@@ -8900,14 +8900,14 @@
         <v>105</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="E24" s="39"/>
       <c r="F24" s="39" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G24" s="39"/>
     </row>
@@ -8926,7 +8926,7 @@
       </c>
       <c r="E25" s="38"/>
       <c r="F25" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G25" s="38"/>
     </row>
@@ -8938,14 +8938,14 @@
         <v>111</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="D26" s="38" t="s">
         <v>110</v>
       </c>
       <c r="E26" s="38"/>
       <c r="F26" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G26" s="38"/>
     </row>
@@ -8957,14 +8957,14 @@
         <v>114</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="39" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G27" s="39"/>
     </row>
@@ -8976,14 +8976,14 @@
         <v>117</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="39" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G28" s="39"/>
     </row>
@@ -8992,34 +8992,34 @@
         <v>58</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G29" s="39"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="39"/>
       <c r="B30" s="39" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="E30" s="39"/>
       <c r="F30" s="39" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G30" s="39"/>
     </row>
@@ -9028,17 +9028,17 @@
         <v>58</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="D31" s="38" t="s">
         <v>113</v>
       </c>
       <c r="E31" s="38"/>
       <c r="F31" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G31" s="38"/>
     </row>
@@ -9047,7 +9047,7 @@
         <v>58</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C32" s="38" t="s">
         <v>115</v>
@@ -9057,7 +9057,7 @@
       </c>
       <c r="E32" s="38"/>
       <c r="F32" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G32" s="38"/>
     </row>
@@ -9066,17 +9066,17 @@
         <v>58</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="E33" s="39"/>
       <c r="F33" s="39" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G33" s="39"/>
     </row>
@@ -9085,17 +9085,17 @@
         <v>58</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="E34" s="39"/>
       <c r="F34" s="39" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G34" s="39"/>
     </row>
@@ -9104,17 +9104,17 @@
         <v>58</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="E35" s="39"/>
       <c r="F35" s="39" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G35" s="39"/>
     </row>
@@ -9123,17 +9123,17 @@
         <v>58</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="D36" s="39" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="E36" s="39"/>
       <c r="F36" s="39" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G36" s="39"/>
     </row>
@@ -9142,7 +9142,7 @@
         <v>58</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="C37" s="38" t="s">
         <v>118</v>
@@ -9152,7 +9152,7 @@
       </c>
       <c r="E37" s="38"/>
       <c r="F37" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G37" s="38"/>
     </row>
@@ -9171,7 +9171,7 @@
       </c>
       <c r="E38" s="38"/>
       <c r="F38" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G38" s="38"/>
     </row>
@@ -9190,7 +9190,7 @@
       </c>
       <c r="E39" s="38"/>
       <c r="F39" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G39" s="38"/>
     </row>
@@ -9209,7 +9209,7 @@
       </c>
       <c r="E40" s="38"/>
       <c r="F40" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G40" s="38"/>
     </row>
@@ -9228,7 +9228,7 @@
       </c>
       <c r="E41" s="38"/>
       <c r="F41" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G41" s="38"/>
     </row>
@@ -9237,7 +9237,7 @@
         <v>131</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="C42" s="38" t="s">
         <v>133</v>
@@ -9247,7 +9247,7 @@
       </c>
       <c r="E42" s="38"/>
       <c r="F42" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G42" s="38"/>
     </row>
@@ -9271,10 +9271,10 @@
         <v>58</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D44" s="37"/>
       <c r="E44" s="37"/>
@@ -9296,7 +9296,7 @@
       </c>
       <c r="E45" s="38"/>
       <c r="F45" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G45" s="38" t="s">
         <v>136</v>
@@ -9317,7 +9317,7 @@
       </c>
       <c r="E46" s="38"/>
       <c r="F46" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G46" s="38"/>
     </row>
@@ -9336,7 +9336,7 @@
       </c>
       <c r="E47" s="38"/>
       <c r="F47" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G47" s="38"/>
     </row>
@@ -9355,7 +9355,7 @@
       </c>
       <c r="E48" s="38"/>
       <c r="F48" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G48" s="38"/>
     </row>
@@ -9374,7 +9374,7 @@
       </c>
       <c r="E49" s="38"/>
       <c r="F49" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G49" s="38"/>
     </row>
@@ -9393,7 +9393,7 @@
       </c>
       <c r="E50" s="38"/>
       <c r="F50" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G50" s="38"/>
     </row>
@@ -9412,7 +9412,7 @@
       </c>
       <c r="E51" s="38"/>
       <c r="F51" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G51" s="38"/>
     </row>
@@ -9431,7 +9431,7 @@
       </c>
       <c r="E52" s="38"/>
       <c r="F52" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G52" s="38"/>
     </row>
@@ -9450,7 +9450,7 @@
       </c>
       <c r="E53" s="38"/>
       <c r="F53" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G53" s="38"/>
     </row>
@@ -9459,7 +9459,7 @@
         <v>131</v>
       </c>
       <c r="B54" s="38" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="C54" s="38" t="s">
         <v>133</v>
@@ -9469,7 +9469,7 @@
       </c>
       <c r="E54" s="38"/>
       <c r="F54" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G54" s="38"/>
     </row>
@@ -9493,10 +9493,10 @@
         <v>58</v>
       </c>
       <c r="B56" s="38" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="C56" s="37" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D56" s="37"/>
       <c r="E56" s="37"/>
@@ -9518,7 +9518,7 @@
       </c>
       <c r="E57" s="38"/>
       <c r="F57" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G57" s="38" t="s">
         <v>158</v>
@@ -9539,7 +9539,7 @@
       </c>
       <c r="E58" s="38"/>
       <c r="F58" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G58" s="38"/>
     </row>
@@ -9558,7 +9558,7 @@
       </c>
       <c r="E59" s="38"/>
       <c r="F59" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G59" s="38"/>
     </row>
@@ -9577,7 +9577,7 @@
       </c>
       <c r="E60" s="38"/>
       <c r="F60" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G60" s="38"/>
     </row>
@@ -9596,7 +9596,7 @@
       </c>
       <c r="E61" s="38"/>
       <c r="F61" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G61" s="38"/>
     </row>
@@ -9615,7 +9615,7 @@
       </c>
       <c r="E62" s="38"/>
       <c r="F62" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G62" s="38"/>
     </row>
@@ -9634,7 +9634,7 @@
       </c>
       <c r="E63" s="38"/>
       <c r="F63" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G63" s="38"/>
     </row>
@@ -9653,7 +9653,7 @@
       </c>
       <c r="E64" s="38"/>
       <c r="F64" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G64" s="38"/>
     </row>
@@ -9672,7 +9672,7 @@
       </c>
       <c r="E65" s="38"/>
       <c r="F65" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G65" s="38"/>
     </row>
@@ -9696,10 +9696,10 @@
         <v>58</v>
       </c>
       <c r="B67" s="38" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D67" s="37"/>
       <c r="E67" s="37"/>
@@ -9721,7 +9721,7 @@
       </c>
       <c r="E68" s="38"/>
       <c r="F68" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G68" s="38" t="s">
         <v>169</v>
@@ -9742,7 +9742,7 @@
       </c>
       <c r="E69" s="38"/>
       <c r="F69" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G69" s="38"/>
     </row>
@@ -9761,7 +9761,7 @@
       </c>
       <c r="E70" s="38"/>
       <c r="F70" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G70" s="38"/>
     </row>
@@ -9780,7 +9780,7 @@
       </c>
       <c r="E71" s="38"/>
       <c r="F71" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G71" s="38"/>
     </row>
@@ -9799,7 +9799,7 @@
       </c>
       <c r="E72" s="40"/>
       <c r="F72" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G72" s="38"/>
     </row>
@@ -9818,7 +9818,7 @@
       </c>
       <c r="E73" s="38"/>
       <c r="F73" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G73" s="38"/>
     </row>
@@ -9830,14 +9830,14 @@
         <v>179</v>
       </c>
       <c r="C74" s="39" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="D74" s="39" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="E74" s="39"/>
       <c r="F74" s="39" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G74" s="39"/>
     </row>
@@ -9849,14 +9849,14 @@
         <v>182</v>
       </c>
       <c r="C75" s="39" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="D75" s="39" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="E75" s="39"/>
       <c r="F75" s="39" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G75" s="39"/>
     </row>
@@ -9875,7 +9875,7 @@
       </c>
       <c r="E76" s="38"/>
       <c r="F76" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G76" s="38"/>
     </row>
@@ -9884,7 +9884,7 @@
         <v>58</v>
       </c>
       <c r="B77" s="38" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="C77" s="38" t="s">
         <v>183</v>
@@ -9894,7 +9894,7 @@
       </c>
       <c r="E77" s="38"/>
       <c r="F77" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G77" s="38"/>
     </row>
@@ -9903,7 +9903,7 @@
         <v>58</v>
       </c>
       <c r="B78" s="38" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C78" s="38" t="s">
         <v>186</v>
@@ -9913,7 +9913,7 @@
       </c>
       <c r="E78" s="38"/>
       <c r="F78" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G78" s="38"/>
     </row>
@@ -9922,7 +9922,7 @@
         <v>131</v>
       </c>
       <c r="B79" s="38" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="C79" s="38" t="s">
         <v>133</v>
@@ -9932,7 +9932,7 @@
       </c>
       <c r="E79" s="38"/>
       <c r="F79" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G79" s="38"/>
     </row>
@@ -9941,7 +9941,7 @@
         <v>58</v>
       </c>
       <c r="B80" s="38" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="C80" s="37" t="s">
         <v>6</v>
@@ -9956,10 +9956,10 @@
         <v>58</v>
       </c>
       <c r="B81" s="38" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="C81" s="37" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D81" s="37"/>
       <c r="E81" s="37"/>
@@ -9981,7 +9981,7 @@
       </c>
       <c r="E82" s="38"/>
       <c r="F82" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G82" s="38" t="s">
         <v>191</v>
@@ -10002,7 +10002,7 @@
       </c>
       <c r="E83" s="38"/>
       <c r="F83" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G83" s="38"/>
     </row>
@@ -10021,7 +10021,7 @@
       </c>
       <c r="E84" s="38"/>
       <c r="F84" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G84" s="38"/>
     </row>
@@ -10040,7 +10040,7 @@
       </c>
       <c r="E85" s="38"/>
       <c r="F85" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G85" s="38"/>
     </row>
@@ -10059,7 +10059,7 @@
       </c>
       <c r="E86" s="38"/>
       <c r="F86" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G86" s="38"/>
     </row>
@@ -10078,7 +10078,7 @@
       </c>
       <c r="E87" s="38"/>
       <c r="F87" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G87" s="38"/>
     </row>
@@ -10097,7 +10097,7 @@
       </c>
       <c r="E88" s="38"/>
       <c r="F88" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G88" s="38"/>
     </row>
@@ -10106,7 +10106,7 @@
         <v>131</v>
       </c>
       <c r="B89" s="38" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C89" s="38" t="s">
         <v>133</v>
@@ -10116,7 +10116,7 @@
       </c>
       <c r="E89" s="38"/>
       <c r="F89" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G89" s="38"/>
     </row>
@@ -10140,10 +10140,10 @@
         <v>58</v>
       </c>
       <c r="B91" s="38" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="C91" s="37" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D91" s="37"/>
       <c r="E91" s="37"/>
@@ -10165,7 +10165,7 @@
       </c>
       <c r="E92" s="38"/>
       <c r="F92" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G92" s="38" t="s">
         <v>207</v>
@@ -10186,7 +10186,7 @@
       </c>
       <c r="E93" s="38"/>
       <c r="F93" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G93" s="38"/>
     </row>
@@ -10205,7 +10205,7 @@
       </c>
       <c r="E94" s="38"/>
       <c r="F94" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G94" s="38"/>
     </row>
@@ -10224,7 +10224,7 @@
       </c>
       <c r="E95" s="38"/>
       <c r="F95" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G95" s="38"/>
     </row>
@@ -10243,7 +10243,7 @@
       </c>
       <c r="E96" s="38"/>
       <c r="F96" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G96" s="38"/>
     </row>
@@ -10262,7 +10262,7 @@
       </c>
       <c r="E97" s="38"/>
       <c r="F97" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G97" s="38"/>
     </row>
@@ -10281,7 +10281,7 @@
       </c>
       <c r="E98" s="38"/>
       <c r="F98" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G98" s="38"/>
     </row>
@@ -10300,7 +10300,7 @@
       </c>
       <c r="E99" s="38"/>
       <c r="F99" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G99" s="38"/>
     </row>
@@ -10319,7 +10319,7 @@
       </c>
       <c r="E100" s="38"/>
       <c r="F100" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G100" s="38"/>
     </row>
@@ -10328,7 +10328,7 @@
         <v>131</v>
       </c>
       <c r="B101" s="38" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="C101" s="38" t="s">
         <v>133</v>
@@ -10338,7 +10338,7 @@
       </c>
       <c r="E101" s="38"/>
       <c r="F101" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G101" s="38"/>
     </row>
@@ -10362,10 +10362,10 @@
         <v>58</v>
       </c>
       <c r="B103" s="38" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="C103" s="37" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D103" s="37"/>
       <c r="E103" s="37"/>
@@ -10387,7 +10387,7 @@
       </c>
       <c r="E104" s="38"/>
       <c r="F104" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G104" s="38" t="s">
         <v>219</v>
@@ -10408,7 +10408,7 @@
       </c>
       <c r="E105" s="38"/>
       <c r="F105" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G105" s="38"/>
     </row>
@@ -10427,7 +10427,7 @@
       </c>
       <c r="E106" s="38"/>
       <c r="F106" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G106" s="38"/>
     </row>
@@ -10446,7 +10446,7 @@
       </c>
       <c r="E107" s="38"/>
       <c r="F107" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G107" s="38"/>
     </row>
@@ -10465,7 +10465,7 @@
       </c>
       <c r="E108" s="38"/>
       <c r="F108" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G108" s="38"/>
     </row>
@@ -10484,7 +10484,7 @@
       </c>
       <c r="E109" s="38"/>
       <c r="F109" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G109" s="38"/>
     </row>
@@ -10503,7 +10503,7 @@
       </c>
       <c r="E110" s="38"/>
       <c r="F110" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G110" s="38"/>
     </row>
@@ -10522,7 +10522,7 @@
       </c>
       <c r="E111" s="38"/>
       <c r="F111" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G111" s="38"/>
     </row>
@@ -10541,7 +10541,7 @@
       </c>
       <c r="E112" s="38"/>
       <c r="F112" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G112" s="38"/>
     </row>
@@ -10550,7 +10550,7 @@
         <v>131</v>
       </c>
       <c r="B113" s="38" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="C113" s="38" t="s">
         <v>133</v>
@@ -10560,7 +10560,7 @@
       </c>
       <c r="E113" s="38"/>
       <c r="F113" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G113" s="38"/>
     </row>
@@ -10584,10 +10584,10 @@
         <v>58</v>
       </c>
       <c r="B115" s="38" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="C115" s="37" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D115" s="37"/>
       <c r="E115" s="37"/>
@@ -10609,7 +10609,7 @@
       </c>
       <c r="E116" s="38"/>
       <c r="F116" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G116" s="38" t="s">
         <v>136</v>
@@ -10630,7 +10630,7 @@
       </c>
       <c r="E117" s="38"/>
       <c r="F117" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G117" s="38"/>
     </row>
@@ -10649,7 +10649,7 @@
       </c>
       <c r="E118" s="38"/>
       <c r="F118" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G118" s="38"/>
     </row>
@@ -10668,7 +10668,7 @@
       </c>
       <c r="E119" s="38"/>
       <c r="F119" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G119" s="38"/>
     </row>
@@ -10687,7 +10687,7 @@
       </c>
       <c r="E120" s="38"/>
       <c r="F120" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G120" s="38"/>
     </row>
@@ -10706,7 +10706,7 @@
       </c>
       <c r="E121" s="38"/>
       <c r="F121" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G121" s="38"/>
     </row>
@@ -10725,7 +10725,7 @@
       </c>
       <c r="E122" s="38"/>
       <c r="F122" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G122" s="38"/>
     </row>
@@ -10744,7 +10744,7 @@
       </c>
       <c r="E123" s="38"/>
       <c r="F123" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G123" s="38"/>
     </row>
@@ -10763,7 +10763,7 @@
       </c>
       <c r="E124" s="38"/>
       <c r="F124" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G124" s="38"/>
     </row>
@@ -10772,7 +10772,7 @@
         <v>131</v>
       </c>
       <c r="B125" s="38" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="C125" s="38" t="s">
         <v>133</v>
@@ -10782,7 +10782,7 @@
       </c>
       <c r="E125" s="38"/>
       <c r="F125" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G125" s="38"/>
     </row>
@@ -10791,7 +10791,7 @@
         <v>58</v>
       </c>
       <c r="B126" s="38" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C126" s="37" t="s">
         <v>10</v>
@@ -10806,10 +10806,10 @@
         <v>58</v>
       </c>
       <c r="B127" s="38" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="C127" s="37" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D127" s="37"/>
       <c r="E127" s="37"/>
@@ -10831,7 +10831,7 @@
       </c>
       <c r="E128" s="38"/>
       <c r="F128" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G128" s="38" t="s">
         <v>242</v>
@@ -10852,7 +10852,7 @@
       </c>
       <c r="E129" s="38"/>
       <c r="F129" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G129" s="38"/>
     </row>
@@ -10871,7 +10871,7 @@
       </c>
       <c r="E130" s="38"/>
       <c r="F130" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G130" s="38"/>
     </row>
@@ -10890,7 +10890,7 @@
       </c>
       <c r="E131" s="38"/>
       <c r="F131" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G131" s="38"/>
     </row>
@@ -10909,7 +10909,7 @@
       </c>
       <c r="E132" s="38"/>
       <c r="F132" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G132" s="38"/>
     </row>
@@ -10921,14 +10921,14 @@
         <v>249</v>
       </c>
       <c r="C133" s="38" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="D133" s="38" t="s">
         <v>251</v>
       </c>
       <c r="E133" s="38"/>
       <c r="F133" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G133" s="38"/>
     </row>
@@ -10940,14 +10940,14 @@
         <v>252</v>
       </c>
       <c r="C134" s="39" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="D134" s="39" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="E134" s="39"/>
       <c r="F134" s="39" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G134" s="39"/>
     </row>
@@ -10966,7 +10966,7 @@
       </c>
       <c r="E135" s="38"/>
       <c r="F135" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G135" s="38"/>
     </row>
@@ -10975,7 +10975,7 @@
         <v>58</v>
       </c>
       <c r="B136" s="38" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="C136" s="38" t="s">
         <v>256</v>
@@ -10985,7 +10985,7 @@
       </c>
       <c r="E136" s="38"/>
       <c r="F136" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G136" s="38"/>
     </row>
@@ -11009,10 +11009,10 @@
         <v>58</v>
       </c>
       <c r="B138" s="38" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C138" s="37" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="D138" s="37"/>
       <c r="E138" s="37"/>
@@ -11036,10 +11036,10 @@
         <v>260</v>
       </c>
       <c r="F139" s="38" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G139" s="38" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -11059,7 +11059,7 @@
         <v>260</v>
       </c>
       <c r="F140" s="38" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G140" s="38"/>
     </row>
@@ -11080,7 +11080,7 @@
         <v>260</v>
       </c>
       <c r="F141" s="38" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G141" s="38"/>
     </row>
@@ -11101,7 +11101,7 @@
         <v>260</v>
       </c>
       <c r="F142" s="38" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G142" s="38"/>
     </row>
@@ -11113,7 +11113,7 @@
         <v>267</v>
       </c>
       <c r="C143" s="38" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="D143" s="38" t="s">
         <v>269</v>
@@ -11122,7 +11122,7 @@
         <v>260</v>
       </c>
       <c r="F143" s="38" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G143" s="38"/>
     </row>
@@ -11134,7 +11134,7 @@
         <v>270</v>
       </c>
       <c r="C144" s="38" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="D144" s="38" t="s">
         <v>266</v>
@@ -11143,7 +11143,7 @@
         <v>260</v>
       </c>
       <c r="F144" s="38" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G144" s="38"/>
     </row>
@@ -11155,14 +11155,14 @@
         <v>272</v>
       </c>
       <c r="C145" s="39" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D145" s="39" t="s">
         <v>1241</v>
-      </c>
-      <c r="D145" s="39" t="s">
-        <v>1242</v>
       </c>
       <c r="E145" s="39"/>
       <c r="F145" s="39" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G145" s="39"/>
     </row>
@@ -11171,19 +11171,19 @@
         <v>58</v>
       </c>
       <c r="B146" s="38" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="C146" s="38" t="s">
         <v>271</v>
       </c>
       <c r="D146" s="38" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E146" s="38" t="s">
         <v>260</v>
       </c>
       <c r="F146" s="38" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G146" s="38"/>
     </row>
@@ -11192,7 +11192,7 @@
         <v>58</v>
       </c>
       <c r="B147" s="38" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="C147" s="38" t="s">
         <v>273</v>
@@ -11204,7 +11204,7 @@
         <v>260</v>
       </c>
       <c r="F147" s="38" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G147" s="38"/>
     </row>
@@ -11213,19 +11213,19 @@
         <v>131</v>
       </c>
       <c r="B148" s="38" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="C148" s="38" t="s">
         <v>133</v>
       </c>
       <c r="D148" s="38" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E148" s="38" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="F148" s="38" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G148" s="38"/>
     </row>
@@ -11234,7 +11234,7 @@
         <v>131</v>
       </c>
       <c r="B149" s="38" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="C149" s="38" t="s">
         <v>277</v>
@@ -11244,7 +11244,7 @@
       </c>
       <c r="E149" s="38"/>
       <c r="F149" s="38" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="G149" s="38"/>
     </row>
@@ -11293,14 +11293,14 @@
         <v>14</v>
       </c>
       <c r="D152" s="38" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E152" s="38" t="s">
         <v>281</v>
       </c>
       <c r="F152" s="38"/>
       <c r="G152" s="38" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -11314,14 +11314,14 @@
         <v>15</v>
       </c>
       <c r="D153" s="38" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E153" s="38" t="s">
         <v>281</v>
       </c>
       <c r="F153" s="38"/>
       <c r="G153" s="38" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -11335,14 +11335,14 @@
         <v>283</v>
       </c>
       <c r="D154" s="38" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E154" s="38" t="s">
         <v>284</v>
       </c>
       <c r="F154" s="38"/>
       <c r="G154" s="38" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -11401,7 +11401,7 @@
         <v>58</v>
       </c>
       <c r="B158" s="35" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="C158" s="36" t="s">
         <v>19</v>
@@ -11587,7 +11587,7 @@
         <v>303</v>
       </c>
       <c r="C169" s="38" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="D169" s="40" t="s">
         <v>949</v>
@@ -11908,7 +11908,7 @@
         <v>330</v>
       </c>
       <c r="C188" s="38" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D188" s="40" t="s">
         <v>949</v>
@@ -12420,7 +12420,7 @@
       <c r="E218" s="38"/>
       <c r="F218" s="38"/>
       <c r="G218" s="38" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="219" spans="1:7">
@@ -12533,13 +12533,13 @@
         <v>382</v>
       </c>
       <c r="C225" s="40" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D225" s="40" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E225" s="38" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="F225" s="38"/>
       <c r="G225" s="38"/>
@@ -12555,10 +12555,10 @@
         <v>385</v>
       </c>
       <c r="D226" s="40" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E226" s="38" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="F226" s="38"/>
       <c r="G226" s="38"/>
@@ -12571,7 +12571,7 @@
         <v>386</v>
       </c>
       <c r="C227" s="38" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="D227" s="38">
         <v>76.16</v>
@@ -12645,7 +12645,7 @@
       <c r="E231" s="38"/>
       <c r="F231" s="38"/>
       <c r="G231" s="38" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="232" spans="1:7">
@@ -12713,7 +12713,7 @@
         <v>979</v>
       </c>
       <c r="E235" s="40" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="F235" s="40"/>
       <c r="G235" s="38"/>
@@ -13006,7 +13006,7 @@
         <v>58</v>
       </c>
       <c r="B253" s="35" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C253" s="36" t="s">
         <v>35</v>
@@ -13096,7 +13096,7 @@
         <v>441</v>
       </c>
       <c r="E258" s="59" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F258" s="38"/>
       <c r="G258" s="44"/>
@@ -13177,13 +13177,13 @@
         <v>454</v>
       </c>
       <c r="C263" s="44" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="D263" s="38" t="s">
         <v>456</v>
       </c>
       <c r="E263" s="59" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F263" s="38"/>
       <c r="G263" s="44"/>
@@ -13193,13 +13193,13 @@
         <v>58</v>
       </c>
       <c r="B264" s="38" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C264" s="44" t="s">
         <v>1288</v>
       </c>
-      <c r="C264" s="44" t="s">
-        <v>1289</v>
-      </c>
       <c r="D264" s="38" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="E264" s="38"/>
       <c r="F264" s="38"/>
@@ -13253,7 +13253,7 @@
         <v>465</v>
       </c>
       <c r="E267" s="59" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F267" s="38"/>
       <c r="G267" s="44"/>
@@ -13263,7 +13263,7 @@
         <v>58</v>
       </c>
       <c r="B268" s="38" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C268" s="44" t="s">
         <v>467</v>
@@ -13471,7 +13471,7 @@
         <v>490</v>
       </c>
       <c r="D280" s="38" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="E280" s="38"/>
       <c r="F280" s="38"/>
@@ -13577,7 +13577,7 @@
       </c>
       <c r="E286" s="38"/>
       <c r="F286" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G286" s="44"/>
     </row>
@@ -13777,7 +13777,7 @@
         <v>490</v>
       </c>
       <c r="D298" s="38" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="E298" s="38"/>
       <c r="F298" s="38"/>
@@ -13883,7 +13883,7 @@
       </c>
       <c r="E304" s="38"/>
       <c r="F304" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G304" s="44"/>
     </row>
@@ -14209,7 +14209,7 @@
         <v>58</v>
       </c>
       <c r="B324" s="38" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="C324" s="38" t="s">
         <v>483</v>
@@ -14226,7 +14226,7 @@
         <v>58</v>
       </c>
       <c r="B325" s="38" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="C325" s="38" t="s">
         <v>485</v>
@@ -14266,7 +14266,7 @@
         <v>490</v>
       </c>
       <c r="D327" s="38" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="E327" s="38"/>
       <c r="F327" s="38"/>
@@ -14345,7 +14345,7 @@
         <v>58</v>
       </c>
       <c r="B332" s="38" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="C332" s="38" t="s">
         <v>501</v>
@@ -14362,7 +14362,7 @@
         <v>58</v>
       </c>
       <c r="B333" s="38" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="C333" s="38" t="s">
         <v>504</v>
@@ -14372,7 +14372,7 @@
       </c>
       <c r="E333" s="38"/>
       <c r="F333" s="38" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="G333" s="38"/>
     </row>
@@ -14381,7 +14381,7 @@
         <v>58</v>
       </c>
       <c r="B334" s="35" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="C334" s="49" t="s">
         <v>40</v>
@@ -14435,10 +14435,10 @@
         <v>78.3</v>
       </c>
       <c r="E337" s="38" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F337" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G337" s="44" t="s">
         <v>568</v>
@@ -14458,10 +14458,10 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E338" s="38" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="F338" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G338" s="44"/>
     </row>
@@ -14473,14 +14473,14 @@
         <v>571</v>
       </c>
       <c r="C339" s="44" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="D339" s="38">
         <v>78.099999999999994</v>
       </c>
       <c r="E339" s="38"/>
       <c r="F339" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G339" s="44"/>
     </row>
@@ -14514,7 +14514,7 @@
       </c>
       <c r="E341" s="38"/>
       <c r="F341" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G341" s="44" t="s">
         <v>576</v>
@@ -14535,7 +14535,7 @@
       </c>
       <c r="E342" s="38"/>
       <c r="F342" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G342" s="44"/>
     </row>
@@ -14554,7 +14554,7 @@
       </c>
       <c r="E343" s="38"/>
       <c r="F343" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G343" s="38"/>
     </row>
@@ -14573,7 +14573,7 @@
       </c>
       <c r="E344" s="38"/>
       <c r="F344" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G344" s="44"/>
     </row>
@@ -14607,10 +14607,10 @@
       </c>
       <c r="E346" s="38"/>
       <c r="F346" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G346" s="44" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="347" spans="1:7">
@@ -14628,7 +14628,7 @@
       </c>
       <c r="E347" s="38"/>
       <c r="F347" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G347" s="44"/>
     </row>
@@ -14640,14 +14640,14 @@
         <v>595</v>
       </c>
       <c r="C348" s="44" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D348" s="38" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E348" s="38"/>
       <c r="F348" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G348" s="44"/>
     </row>
@@ -14666,7 +14666,7 @@
       </c>
       <c r="E349" s="38"/>
       <c r="F349" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G349" s="44"/>
     </row>
@@ -14685,7 +14685,7 @@
       </c>
       <c r="E350" s="38"/>
       <c r="F350" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G350" s="44"/>
     </row>
@@ -14719,10 +14719,10 @@
       </c>
       <c r="E352" s="40"/>
       <c r="F352" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G352" s="44" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="353" spans="1:7" ht="30">
@@ -14740,7 +14740,7 @@
       </c>
       <c r="E353" s="40"/>
       <c r="F353" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G353" s="44"/>
     </row>
@@ -14755,11 +14755,11 @@
         <v>612</v>
       </c>
       <c r="D354" s="40" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="E354" s="40"/>
       <c r="F354" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G354" s="38"/>
     </row>
@@ -14778,7 +14778,7 @@
       </c>
       <c r="E355" s="40"/>
       <c r="F355" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G355" s="44"/>
     </row>
@@ -14797,7 +14797,7 @@
       </c>
       <c r="E356" s="38"/>
       <c r="F356" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G356" s="44"/>
     </row>
@@ -14831,10 +14831,10 @@
       </c>
       <c r="E358" s="38"/>
       <c r="F358" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G358" s="38" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="359" spans="1:7">
@@ -14848,11 +14848,11 @@
         <v>624</v>
       </c>
       <c r="D359" s="40" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E359" s="40"/>
       <c r="F359" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G359" s="38"/>
     </row>
@@ -14886,10 +14886,10 @@
       </c>
       <c r="E361" s="38"/>
       <c r="F361" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G361" s="44" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="362" spans="1:7">
@@ -14903,11 +14903,11 @@
         <v>629</v>
       </c>
       <c r="D362" s="38" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="E362" s="46"/>
       <c r="F362" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G362" s="44"/>
     </row>
@@ -14926,7 +14926,7 @@
       </c>
       <c r="E363" s="38"/>
       <c r="F363" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G363" s="44"/>
     </row>
@@ -14941,11 +14941,11 @@
         <v>633</v>
       </c>
       <c r="D364" s="38" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E364" s="38"/>
       <c r="F364" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G364" s="44"/>
     </row>
@@ -14960,13 +14960,13 @@
         <v>635</v>
       </c>
       <c r="D365" s="38" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E365" s="38" t="s">
         <v>636</v>
       </c>
       <c r="F365" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G365" s="38"/>
     </row>
@@ -15014,10 +15014,10 @@
         <v>1033</v>
       </c>
       <c r="E368" s="40" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F368" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G368" s="44" t="s">
         <v>568</v>
@@ -15037,10 +15037,10 @@
         <v>1028</v>
       </c>
       <c r="E369" s="40" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="F369" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G369" s="44"/>
     </row>
@@ -15058,10 +15058,10 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E370" s="38" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F370" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G370" s="44"/>
     </row>
@@ -15110,7 +15110,7 @@
       </c>
       <c r="E373" s="38"/>
       <c r="F373" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G373" s="44" t="s">
         <v>647</v>
@@ -15131,7 +15131,7 @@
       </c>
       <c r="E374" s="38"/>
       <c r="F374" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G374" s="44"/>
     </row>
@@ -15150,7 +15150,7 @@
       </c>
       <c r="E375" s="38"/>
       <c r="F375" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G375" s="44"/>
     </row>
@@ -15169,7 +15169,7 @@
       </c>
       <c r="E376" s="40"/>
       <c r="F376" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G376" s="44"/>
     </row>
@@ -15188,7 +15188,7 @@
       </c>
       <c r="E377" s="38"/>
       <c r="F377" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G377" s="44"/>
     </row>
@@ -15207,7 +15207,7 @@
       </c>
       <c r="E378" s="38"/>
       <c r="F378" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G378" s="44"/>
     </row>
@@ -15241,10 +15241,10 @@
       </c>
       <c r="E380" s="38"/>
       <c r="F380" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G380" s="44" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="381" spans="1:7">
@@ -15258,13 +15258,13 @@
         <v>624</v>
       </c>
       <c r="D381" s="40" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E381" s="40" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="F381" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G381" s="38"/>
     </row>
@@ -15298,10 +15298,10 @@
       </c>
       <c r="E383" s="38"/>
       <c r="F383" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G383" s="44" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="384" spans="1:7">
@@ -15315,11 +15315,11 @@
         <v>666</v>
       </c>
       <c r="D384" s="38" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="E384" s="46"/>
       <c r="F384" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G384" s="44"/>
     </row>
@@ -15338,7 +15338,7 @@
       </c>
       <c r="E385" s="38"/>
       <c r="F385" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G385" s="44"/>
     </row>
@@ -15353,11 +15353,11 @@
         <v>633</v>
       </c>
       <c r="D386" s="38" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E386" s="38"/>
       <c r="F386" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G386" s="38"/>
     </row>
@@ -15372,13 +15372,13 @@
         <v>635</v>
       </c>
       <c r="D387" s="38" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E387" s="38" t="s">
         <v>636</v>
       </c>
       <c r="F387" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G387" s="38"/>
     </row>
@@ -15426,10 +15426,10 @@
         <v>78.3</v>
       </c>
       <c r="E390" s="38" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F390" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G390" s="44" t="s">
         <v>568</v>
@@ -15449,10 +15449,10 @@
         <v>1028</v>
       </c>
       <c r="E391" s="40" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="F391" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G391" s="38"/>
     </row>
@@ -15470,10 +15470,10 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E392" s="38" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F392" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G392" s="44"/>
     </row>
@@ -15518,11 +15518,11 @@
         <v>680</v>
       </c>
       <c r="D395" s="38" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E395" s="38"/>
       <c r="F395" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G395" s="44" t="s">
         <v>681</v>
@@ -15543,7 +15543,7 @@
       </c>
       <c r="E396" s="38"/>
       <c r="F396" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G396" s="44"/>
     </row>
@@ -15562,7 +15562,7 @@
       </c>
       <c r="E397" s="38"/>
       <c r="F397" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G397" s="44"/>
     </row>
@@ -15581,7 +15581,7 @@
       </c>
       <c r="E398" s="38"/>
       <c r="F398" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G398" s="44"/>
     </row>
@@ -15600,7 +15600,7 @@
       </c>
       <c r="E399" s="38"/>
       <c r="F399" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G399" s="44"/>
     </row>
@@ -15619,7 +15619,7 @@
       </c>
       <c r="E400" s="38"/>
       <c r="F400" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G400" s="44"/>
     </row>
@@ -15653,10 +15653,10 @@
       </c>
       <c r="E402" s="38"/>
       <c r="F402" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G402" s="44" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="403" spans="1:7">
@@ -15670,13 +15670,13 @@
         <v>624</v>
       </c>
       <c r="D403" s="40" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E403" s="40" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="F403" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G403" s="38"/>
     </row>
@@ -15710,10 +15710,10 @@
       </c>
       <c r="E405" s="38"/>
       <c r="F405" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G405" s="44" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="406" spans="1:7">
@@ -15727,11 +15727,11 @@
         <v>666</v>
       </c>
       <c r="D406" s="38" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="E406" s="46"/>
       <c r="F406" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G406" s="44"/>
     </row>
@@ -15750,7 +15750,7 @@
       </c>
       <c r="E407" s="38"/>
       <c r="F407" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G407" s="44"/>
     </row>
@@ -15765,11 +15765,11 @@
         <v>633</v>
       </c>
       <c r="D408" s="38" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E408" s="38"/>
       <c r="F408" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G408" s="38"/>
     </row>
@@ -15784,13 +15784,13 @@
         <v>635</v>
       </c>
       <c r="D409" s="38" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E409" s="38" t="s">
         <v>636</v>
       </c>
       <c r="F409" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G409" s="38"/>
     </row>
@@ -15838,10 +15838,10 @@
         <v>78.3</v>
       </c>
       <c r="E412" s="3" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="F412" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G412" s="44" t="s">
         <v>568</v>
@@ -15861,10 +15861,10 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E413" s="38" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F413" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G413" s="44"/>
     </row>
@@ -15882,10 +15882,10 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E414" s="38" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="F414" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G414" s="44"/>
     </row>
@@ -15934,7 +15934,7 @@
       </c>
       <c r="E417" s="38"/>
       <c r="F417" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G417" s="38" t="s">
         <v>709</v>
@@ -15955,7 +15955,7 @@
       </c>
       <c r="E418" s="38"/>
       <c r="F418" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G418" s="44"/>
     </row>
@@ -15974,7 +15974,7 @@
       </c>
       <c r="E419" s="38"/>
       <c r="F419" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G419" s="44"/>
     </row>
@@ -15993,7 +15993,7 @@
       </c>
       <c r="E420" s="38"/>
       <c r="F420" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G420" s="38"/>
     </row>
@@ -16020,14 +16020,14 @@
         <v>718</v>
       </c>
       <c r="C422" s="62" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="D422" s="38" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E422" s="38"/>
       <c r="F422" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G422" s="38" t="s">
         <v>720</v>
@@ -16041,14 +16041,14 @@
         <v>722</v>
       </c>
       <c r="C423" s="62" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="D423" s="40" t="s">
         <v>721</v>
       </c>
       <c r="E423" s="40"/>
       <c r="F423" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G423" s="38"/>
     </row>
@@ -16067,7 +16067,7 @@
       </c>
       <c r="E424" s="40"/>
       <c r="F424" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G424" s="38"/>
     </row>
@@ -16101,7 +16101,7 @@
       </c>
       <c r="E426" s="40"/>
       <c r="F426" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G426" s="44" t="s">
         <v>729</v>
@@ -16122,7 +16122,7 @@
       </c>
       <c r="E427" s="40"/>
       <c r="F427" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G427" s="44"/>
     </row>
@@ -16141,7 +16141,7 @@
       </c>
       <c r="E428" s="40"/>
       <c r="F428" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G428" s="44"/>
     </row>
@@ -16160,7 +16160,7 @@
       </c>
       <c r="E429" s="40"/>
       <c r="F429" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G429" s="38"/>
     </row>
@@ -16179,7 +16179,7 @@
       </c>
       <c r="E430" s="40"/>
       <c r="F430" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G430" s="44"/>
     </row>
@@ -16198,7 +16198,7 @@
       </c>
       <c r="E431" s="40"/>
       <c r="F431" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G431" s="44"/>
     </row>
@@ -16215,7 +16215,7 @@
       <c r="D432" s="41"/>
       <c r="E432" s="41"/>
       <c r="F432" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G432" s="41"/>
     </row>
@@ -16234,7 +16234,7 @@
       </c>
       <c r="E433" s="40"/>
       <c r="F433" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G433" s="44" t="s">
         <v>738</v>
@@ -16255,7 +16255,7 @@
       </c>
       <c r="E434" s="40"/>
       <c r="F434" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G434" s="44"/>
     </row>
@@ -16274,7 +16274,7 @@
       </c>
       <c r="E435" s="40"/>
       <c r="F435" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G435" s="44" t="s">
         <v>606</v>
@@ -16295,7 +16295,7 @@
       </c>
       <c r="E436" s="40"/>
       <c r="F436" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G436" s="44"/>
     </row>
@@ -16312,7 +16312,7 @@
       <c r="D437" s="41"/>
       <c r="E437" s="41"/>
       <c r="F437" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G437" s="41"/>
     </row>
@@ -16331,10 +16331,10 @@
       </c>
       <c r="E438" s="40"/>
       <c r="F438" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G438" s="44" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="439" spans="1:7">
@@ -16348,13 +16348,13 @@
         <v>624</v>
       </c>
       <c r="D439" s="40" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E439" s="40" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="F439" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G439" s="38"/>
     </row>
@@ -16366,12 +16366,12 @@
         <v>746</v>
       </c>
       <c r="C440" s="41" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D440" s="41"/>
       <c r="E440" s="41"/>
       <c r="F440" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G440" s="41"/>
     </row>
@@ -16386,13 +16386,13 @@
         <v>635</v>
       </c>
       <c r="D441" s="38" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E441" s="38" t="s">
         <v>636</v>
       </c>
       <c r="F441" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G441" s="38"/>
     </row>
@@ -16409,7 +16409,7 @@
       <c r="D442" s="41"/>
       <c r="E442" s="41"/>
       <c r="F442" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G442" s="37"/>
     </row>
@@ -16428,7 +16428,7 @@
         <v>279</v>
       </c>
       <c r="F443" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G443" s="44"/>
     </row>
@@ -16447,7 +16447,7 @@
         <v>279</v>
       </c>
       <c r="F444" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G444" s="44"/>
     </row>
@@ -16466,7 +16466,7 @@
         <v>279</v>
       </c>
       <c r="F445" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G445" s="44"/>
     </row>
@@ -16483,7 +16483,7 @@
       <c r="D446" s="41"/>
       <c r="E446" s="37"/>
       <c r="F446" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G446" s="37"/>
     </row>
@@ -16502,7 +16502,7 @@
         <v>279</v>
       </c>
       <c r="F447" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G447" s="44"/>
     </row>
@@ -16521,7 +16521,7 @@
         <v>279</v>
       </c>
       <c r="F448" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G448" s="44"/>
     </row>
@@ -16538,7 +16538,7 @@
       <c r="D449" s="41"/>
       <c r="E449" s="41"/>
       <c r="F449" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G449" s="37"/>
     </row>
@@ -16555,7 +16555,7 @@
       <c r="D450" s="41"/>
       <c r="E450" s="41"/>
       <c r="F450" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G450" s="41"/>
     </row>
@@ -16574,7 +16574,7 @@
       </c>
       <c r="E451" s="38"/>
       <c r="F451" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G451" s="44" t="s">
         <v>568</v>
@@ -16595,7 +16595,7 @@
       </c>
       <c r="E452" s="38"/>
       <c r="F452" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G452" s="44"/>
     </row>
@@ -16614,7 +16614,7 @@
       </c>
       <c r="E453" s="38"/>
       <c r="F453" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G453" s="44"/>
     </row>
@@ -16631,7 +16631,7 @@
       <c r="D454" s="41"/>
       <c r="E454" s="41"/>
       <c r="F454" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G454" s="41"/>
     </row>
@@ -16648,7 +16648,7 @@
       <c r="D455" s="41"/>
       <c r="E455" s="41"/>
       <c r="F455" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G455" s="41"/>
     </row>
@@ -16667,10 +16667,10 @@
       </c>
       <c r="E456" s="38"/>
       <c r="F456" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G456" s="44" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="457" spans="1:7">
@@ -16688,7 +16688,7 @@
       </c>
       <c r="E457" s="38"/>
       <c r="F457" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G457" s="44"/>
     </row>
@@ -16703,15 +16703,15 @@
         <v>767</v>
       </c>
       <c r="D458" s="38" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E458" s="38"/>
       <c r="F458" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G458" s="38"/>
     </row>
-    <row r="459" spans="1:7">
+    <row r="459" spans="1:7" ht="30">
       <c r="A459" s="38" t="s">
         <v>58</v>
       </c>
@@ -16726,7 +16726,7 @@
       </c>
       <c r="E459" s="38"/>
       <c r="F459" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G459" s="38"/>
     </row>
@@ -16738,12 +16738,12 @@
         <v>770</v>
       </c>
       <c r="C460" s="38" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="D460" s="38"/>
       <c r="E460" s="38"/>
       <c r="F460" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G460" s="38"/>
     </row>
@@ -16752,7 +16752,7 @@
         <v>58</v>
       </c>
       <c r="B461" s="38" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C461" s="38" t="s">
         <v>771</v>
@@ -16762,7 +16762,7 @@
       </c>
       <c r="E461" s="38"/>
       <c r="F461" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G461" s="38"/>
     </row>
@@ -16771,17 +16771,17 @@
         <v>58</v>
       </c>
       <c r="B462" s="38" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="C462" s="38" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="D462" s="38" t="s">
         <v>724</v>
       </c>
       <c r="E462" s="38"/>
       <c r="F462" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G462" s="38"/>
     </row>
@@ -16798,7 +16798,7 @@
       <c r="D463" s="41"/>
       <c r="E463" s="41"/>
       <c r="F463" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G463" s="41"/>
     </row>
@@ -16817,10 +16817,10 @@
       </c>
       <c r="E464" s="38"/>
       <c r="F464" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G464" s="44" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="465" spans="1:7">
@@ -16834,11 +16834,11 @@
         <v>624</v>
       </c>
       <c r="D465" s="40" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="E465" s="40"/>
       <c r="F465" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G465" s="38"/>
     </row>
@@ -16855,7 +16855,7 @@
       <c r="D466" s="41"/>
       <c r="E466" s="41"/>
       <c r="F466" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G466" s="41"/>
     </row>
@@ -16874,10 +16874,10 @@
       </c>
       <c r="E467" s="38"/>
       <c r="F467" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G467" s="44" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="468" spans="1:7">
@@ -16895,7 +16895,7 @@
       </c>
       <c r="E468" s="38"/>
       <c r="F468" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G468" s="44"/>
     </row>
@@ -16914,7 +16914,7 @@
       </c>
       <c r="E469" s="38"/>
       <c r="F469" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G469" s="44"/>
     </row>
@@ -16929,11 +16929,11 @@
         <v>633</v>
       </c>
       <c r="D470" s="38" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="E470" s="38"/>
       <c r="F470" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G470" s="38"/>
     </row>
@@ -16948,15 +16948,16 @@
         <v>635</v>
       </c>
       <c r="D471" s="38" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="E471" s="38"/>
       <c r="F471" s="38" t="s">
-        <v>1152</v>
+        <v>1144</v>
       </c>
       <c r="G471" s="38"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G471" xr:uid="{D331C0AB-26E8-4A68-9DCE-42FE6AA1F39D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -17008,7 +17009,7 @@
         <v>62</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>789</v>
@@ -17027,7 +17028,7 @@
         <v>65</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>791</v>
@@ -17046,7 +17047,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>792</v>
@@ -17065,7 +17066,7 @@
         <v>71</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>793</v>
@@ -17084,7 +17085,7 @@
         <v>796</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>797</v>
@@ -18469,7 +18470,7 @@
         <v>124</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>790</v>
@@ -18882,7 +18883,7 @@
         <v>278</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>854</v>
@@ -18901,13 +18902,13 @@
         <v>269</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>855</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
@@ -18920,13 +18921,13 @@
         <v>266</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>856</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3" t="s">
@@ -18939,7 +18940,7 @@
         <v>274</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>857</v>
@@ -18955,16 +18956,16 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="32" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B43" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C43" s="32" t="s">
+        <v>1175</v>
+      </c>
+      <c r="D43" s="32" t="s">
         <v>1176</v>
-      </c>
-      <c r="D43" s="32" t="s">
-        <v>1177</v>
       </c>
       <c r="E43" s="32"/>
       <c r="F43" s="32" t="s">
@@ -18974,16 +18975,16 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="32" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B44" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="E44" s="32"/>
       <c r="F44" s="32" t="s">
@@ -18993,16 +18994,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="32" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B45" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="E45" s="32"/>
       <c r="F45" s="32" t="s">
@@ -19012,16 +19013,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="32" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B46" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="E46" s="32"/>
       <c r="F46" s="32" t="s">
@@ -19031,16 +19032,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="32" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B47" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="E47" s="32"/>
       <c r="F47" s="32" t="s">
@@ -19050,16 +19051,16 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="32" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B48" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="E48" s="32"/>
       <c r="F48" s="32" t="s">
@@ -19069,16 +19070,16 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="32" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B49" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="E49" s="32"/>
       <c r="F49" s="32" t="s">
@@ -19088,16 +19089,16 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="32" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B50" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="E50" s="32"/>
       <c r="F50" s="32" t="s">
@@ -19107,16 +19108,16 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="32" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B51" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="E51" s="32"/>
       <c r="F51" s="32" t="s">
@@ -19126,16 +19127,16 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="32" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B52" s="32" t="s">
         <v>839</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="E52" s="32"/>
       <c r="F52" s="32" t="s">
@@ -19145,16 +19146,16 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="32" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="B53" s="32" t="s">
         <v>839</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="E53" s="32"/>
       <c r="F53" s="32" t="s">
@@ -19164,16 +19165,16 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="32" t="s">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B54" s="32" t="s">
         <v>847</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E54" s="32"/>
       <c r="F54" s="32" t="s">
@@ -19183,16 +19184,16 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="32" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="E55" s="32"/>
       <c r="F55" s="32" t="s">
@@ -19770,16 +19771,16 @@
     </row>
     <row r="16" spans="1:256" ht="31.5" customHeight="1">
       <c r="A16" s="31" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>860</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30" t="s">
@@ -19789,16 +19790,16 @@
     </row>
     <row r="17" spans="1:7" ht="31.5" customHeight="1">
       <c r="A17" s="31" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>860</v>
       </c>
       <c r="C17" s="31" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D17" s="31" t="s">
         <v>1097</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>1098</v>
       </c>
       <c r="E17" s="30"/>
       <c r="F17" s="30" t="s">
@@ -19817,7 +19818,7 @@
         <v>894</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E18" s="30"/>
       <c r="F18" s="30" t="s">
@@ -20310,7 +20311,7 @@
         <v>965</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="F44" s="30"/>
       <c r="G44" s="30"/>
@@ -20396,7 +20397,7 @@
         <v>980</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="E49" s="30"/>
       <c r="F49" s="30"/>
@@ -20960,7 +20961,7 @@
         <v>435</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>981</v>
@@ -20979,7 +20980,7 @@
         <v>438</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>983</v>
@@ -20998,7 +20999,7 @@
         <v>441</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>985</v>
@@ -21017,7 +21018,7 @@
         <v>456</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>987</v>
@@ -21036,7 +21037,7 @@
         <v>444</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>989</v>
@@ -21055,7 +21056,7 @@
         <v>447</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>991</v>
@@ -21074,7 +21075,7 @@
         <v>450</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>993</v>
@@ -21093,7 +21094,7 @@
         <v>453</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>995</v>
@@ -21112,7 +21113,7 @@
         <v>459</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>997</v>
@@ -21131,7 +21132,7 @@
         <v>999</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>1000</v>
@@ -21150,7 +21151,7 @@
         <v>462</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>1002</v>
@@ -21169,7 +21170,7 @@
         <v>465</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>1004</v>
@@ -21190,7 +21191,7 @@
         <v>468</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>1007</v>
@@ -21209,7 +21210,7 @@
         <v>502</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>1009</v>
@@ -21232,7 +21233,7 @@
         <v>493</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>1013</v>
@@ -21251,7 +21252,7 @@
         <v>505</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>1015</v>
@@ -21274,7 +21275,7 @@
         <v>533</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>1019</v>
@@ -21293,7 +21294,7 @@
         <v>536</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>1020</v>
@@ -21312,7 +21313,7 @@
         <v>539</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>1021</v>
@@ -21331,7 +21332,7 @@
         <v>542</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>1023</v>
@@ -21350,7 +21351,7 @@
         <v>547</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>1025</v>
@@ -21369,7 +21370,7 @@
         <v>488</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>1027</v>
@@ -21383,16 +21384,16 @@
     </row>
     <row r="24" spans="1:7" ht="31.2">
       <c r="A24" s="32" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B24" s="32" t="s">
         <v>1155</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="C24" s="32" t="s">
         <v>1156</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="D24" s="32" t="s">
         <v>1157</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>1158</v>
       </c>
       <c r="E24" s="32"/>
       <c r="F24" s="32"/>
@@ -21400,16 +21401,16 @@
     </row>
     <row r="25" spans="1:7" ht="46.8">
       <c r="A25" s="32" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C25" s="32" t="s">
         <v>1159</v>
       </c>
-      <c r="B25" s="32" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>1160</v>
-      </c>
       <c r="D25" s="32" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
@@ -21417,16 +21418,16 @@
     </row>
     <row r="26" spans="1:7" ht="31.2">
       <c r="A26" s="32" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C26" s="32" t="s">
         <v>1161</v>
       </c>
-      <c r="B26" s="32" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C26" s="32" t="s">
+      <c r="D26" s="32" t="s">
         <v>1162</v>
-      </c>
-      <c r="D26" s="32" t="s">
-        <v>1163</v>
       </c>
       <c r="E26" s="32"/>
       <c r="F26" s="32"/>
@@ -21434,16 +21435,16 @@
     </row>
     <row r="27" spans="1:7" ht="46.8">
       <c r="A27" s="32" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C27" s="32" t="s">
         <v>1164</v>
       </c>
-      <c r="B27" s="32" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C27" s="32" t="s">
+      <c r="D27" s="32" t="s">
         <v>1165</v>
-      </c>
-      <c r="D27" s="32" t="s">
-        <v>1166</v>
       </c>
       <c r="E27" s="32"/>
       <c r="F27" s="32"/>
@@ -21451,16 +21452,16 @@
     </row>
     <row r="28" spans="1:7" ht="46.8">
       <c r="A28" s="32" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C28" s="32" t="s">
         <v>1167</v>
       </c>
-      <c r="B28" s="32" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C28" s="32" t="s">
+      <c r="D28" s="32" t="s">
         <v>1168</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>1169</v>
       </c>
       <c r="E28" s="32"/>
       <c r="F28" s="32"/>
@@ -21468,16 +21469,16 @@
     </row>
     <row r="29" spans="1:7" ht="46.8">
       <c r="A29" s="32" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C29" s="32" t="s">
         <v>1170</v>
       </c>
-      <c r="B29" s="32" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C29" s="32" t="s">
+      <c r="D29" s="32" t="s">
         <v>1171</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>1172</v>
       </c>
       <c r="E29" s="32"/>
       <c r="F29" s="32"/>
@@ -21485,16 +21486,16 @@
     </row>
     <row r="30" spans="1:7" ht="46.8">
       <c r="A30" s="32" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C30" s="32" t="s">
         <v>1173</v>
       </c>
-      <c r="B30" s="32" t="s">
-        <v>1156</v>
-      </c>
-      <c r="C30" s="32" t="s">
+      <c r="D30" s="32" t="s">
         <v>1174</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>1175</v>
       </c>
       <c r="E30" s="32"/>
       <c r="F30" s="32"/>
@@ -21563,7 +21564,7 @@
         <v>1030</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="E2" s="64"/>
       <c r="F2" s="28" t="s">
@@ -21831,7 +21832,7 @@
         <v>1032</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="E3" s="65"/>
       <c r="F3" s="3" t="s">
@@ -21850,7 +21851,7 @@
         <v>1034</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="E4" s="64"/>
       <c r="F4" s="3" t="s">
@@ -21872,7 +21873,9 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <cols>
@@ -22271,13 +22274,13 @@
         <v>1049</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>1050</v>
+        <v>1302</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>790</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="8" spans="1:256" ht="31.5" customHeight="1">
@@ -22288,10 +22291,10 @@
         <v>1036</v>
       </c>
       <c r="C8" s="30" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>1051</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>1052</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="30" t="s">
@@ -22307,10 +22310,10 @@
         <v>1036</v>
       </c>
       <c r="C9" s="30" t="s">
+        <v>1052</v>
+      </c>
+      <c r="D9" s="30" t="s">
         <v>1053</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>1054</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="30" t="s">
@@ -22326,10 +22329,10 @@
         <v>1036</v>
       </c>
       <c r="C10" s="30" t="s">
+        <v>1054</v>
+      </c>
+      <c r="D10" s="30" t="s">
         <v>1055</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>1056</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30" t="s">
@@ -22345,10 +22348,10 @@
         <v>1036</v>
       </c>
       <c r="C11" s="30" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D11" s="30" t="s">
         <v>1057</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>1058</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="30" t="s">
@@ -22364,7 +22367,7 @@
         <v>1036</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>602</v>
@@ -22383,10 +22386,10 @@
         <v>1036</v>
       </c>
       <c r="C13" s="30" t="s">
+        <v>1059</v>
+      </c>
+      <c r="D13" s="30" t="s">
         <v>1060</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>1061</v>
       </c>
       <c r="E13" s="30" t="s">
         <v>1017</v>
@@ -22395,7 +22398,7 @@
         <v>790</v>
       </c>
       <c r="G13" s="30" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="14" spans="1:256" ht="31.5" customHeight="1">
@@ -22406,17 +22409,17 @@
         <v>1036</v>
       </c>
       <c r="C14" s="30" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D14" s="30" t="s">
         <v>1063</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>1064</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="30" t="s">
         <v>790</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="15" spans="1:256" ht="31.5" customHeight="1">
@@ -22427,10 +22430,10 @@
         <v>1036</v>
       </c>
       <c r="C15" s="30" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D15" s="30" t="s">
         <v>1066</v>
-      </c>
-      <c r="D15" s="30" t="s">
-        <v>1067</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="30" t="s">
@@ -22446,10 +22449,10 @@
         <v>1036</v>
       </c>
       <c r="C16" s="30" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D16" s="30" t="s">
         <v>1068</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>1069</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30" t="s">
@@ -22459,16 +22462,16 @@
     </row>
     <row r="17" spans="1:7" ht="31.5" customHeight="1">
       <c r="A17" s="30" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C17" s="30" t="s">
+        <v>1070</v>
+      </c>
+      <c r="D17" s="30" t="s">
         <v>1071</v>
-      </c>
-      <c r="D17" s="30" t="s">
-        <v>1072</v>
       </c>
       <c r="E17" s="30"/>
       <c r="F17" s="30" t="s">
@@ -22484,10 +22487,10 @@
         <v>1036</v>
       </c>
       <c r="C18" s="30" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D18" s="30" t="s">
         <v>1073</v>
-      </c>
-      <c r="D18" s="30" t="s">
-        <v>1074</v>
       </c>
       <c r="E18" s="30"/>
       <c r="F18" s="30" t="s">
@@ -22497,25 +22500,25 @@
     </row>
     <row r="19" spans="1:7" ht="31.5" customHeight="1">
       <c r="A19" s="30" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C19" s="30" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D19" s="30" t="s">
         <v>1076</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="E19" s="30" t="s">
         <v>1077</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>1078</v>
       </c>
       <c r="F19" s="30" t="s">
         <v>790</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.100000000000001" customHeight="1">
@@ -22526,10 +22529,10 @@
         <v>1036</v>
       </c>
       <c r="C20" s="30" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D20" s="30" t="s">
         <v>1079</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>1080</v>
       </c>
       <c r="E20" s="30"/>
       <c r="F20" s="30" t="s">
@@ -22545,53 +22548,53 @@
         <v>1036</v>
       </c>
       <c r="C21" s="30" t="s">
+        <v>1080</v>
+      </c>
+      <c r="D21" s="30" t="s">
         <v>1081</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="E21" s="30" t="s">
         <v>1082</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>1083</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>790</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="31.5" customHeight="1">
       <c r="A22" s="30" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C22" s="30" t="s">
+        <v>1085</v>
+      </c>
+      <c r="D22" s="30" t="s">
         <v>1086</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="E22" s="30" t="s">
         <v>1087</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>1088</v>
       </c>
       <c r="F22" s="30" t="s">
         <v>809</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="31.2">
       <c r="A23" s="30" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="D23" s="30" t="s">
         <v>629</v>
@@ -22602,13 +22605,13 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="30" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B24" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>633</v>
@@ -22619,32 +22622,32 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="30" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D25" s="30" t="s">
         <v>624</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>
     </row>
     <row r="26" spans="1:7" ht="31.2">
       <c r="A26" s="30" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>635</v>
@@ -22655,13 +22658,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="58" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D27" s="30" t="s">
         <v>767</v>
@@ -22973,40 +22976,40 @@
     </row>
     <row r="2" spans="1:256">
       <c r="A2" s="7" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
         <v>790</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="3" spans="1:256">
       <c r="A3" s="7" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>1136</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>1090</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>1137</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>809</v>
@@ -23015,19 +23018,19 @@
     </row>
     <row r="4" spans="1:256">
       <c r="A4" s="6" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>1141</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>1142</v>
-      </c>
       <c r="C4" s="6" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>1139</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>1090</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>1140</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>809</v>

</xml_diff>

<commit_message>
make spreadsheet match updates
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1455D6BD-30A3-4F34-8403-A0B484D0BB20}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF8F7BA-6B4C-4BDE-947E-668BAC046960}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="1303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="1304">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3942,6 +3942,9 @@
   </si>
   <si>
     <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID;2.16.840.1.101.3.2.1.48.11,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID;2.16.840.1.101.3.2.1.48.9:2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID;2.16.840.1.101.3.2.1.48.9:2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID;2.16.840.1.101.3.2.1.48.13,CARD_HOLDER_UNIQUE_IDENTIFIER_OID;2.16.840.1.101.3.2.1.48.86</t>
+  </si>
+  <si>
+    <t>Confirm that version of signed data structure is 3</t>
   </si>
 </sst>
 </file>
@@ -8448,7 +8451,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A445" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView topLeftCell="A445" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="F449" sqref="F449:F471"/>
     </sheetView>
   </sheetViews>
@@ -20666,8 +20669,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:IV30"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -21281,7 +21284,7 @@
         <v>1019</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>532</v>
+        <v>1303</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">

</xml_diff>

<commit_message>
testing fix for pkix.20
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF8F7BA-6B4C-4BDE-947E-668BAC046960}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CBA72E-FD6E-4640-977C-85DF09533163}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="1304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3764" uniqueCount="1303">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3277,9 +3277,6 @@
   </si>
   <si>
     <t>Confirm id-PIV-cardAuth exists in extendedKeyUsage extension and does not assert any other OIDs</t>
-  </si>
-  <si>
-    <t>2.16.840.1.101.3.6.8</t>
   </si>
   <si>
     <t>Card Auth id-PIV-cardAuth EKU keyPurposeID OID</t>
@@ -8486,7 +8483,7 @@
         <v>56</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="G1" s="33" t="s">
         <v>55</v>
@@ -8498,7 +8495,7 @@
         <v>58</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
       <c r="C2" s="36" t="s">
         <v>0</v>
@@ -8528,10 +8525,10 @@
         <v>58</v>
       </c>
       <c r="B4" s="38" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C4" s="37" t="s">
         <v>1253</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>1254</v>
       </c>
       <c r="D4" s="37"/>
       <c r="E4" s="37"/>
@@ -8553,7 +8550,7 @@
       </c>
       <c r="E5" s="38"/>
       <c r="F5" s="38" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G5" s="38" t="s">
         <v>61</v>
@@ -8574,7 +8571,7 @@
       </c>
       <c r="E6" s="38"/>
       <c r="F6" s="38" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G6" s="38"/>
     </row>
@@ -8593,7 +8590,7 @@
       </c>
       <c r="E7" s="38"/>
       <c r="F7" s="38" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G7" s="38"/>
     </row>
@@ -8612,7 +8609,7 @@
       </c>
       <c r="E8" s="38"/>
       <c r="F8" s="38" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G8" s="38"/>
     </row>
@@ -8631,7 +8628,7 @@
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="38" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G9" s="38"/>
     </row>
@@ -8650,7 +8647,7 @@
       </c>
       <c r="E10" s="38"/>
       <c r="F10" s="38" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G10" s="38"/>
     </row>
@@ -8669,7 +8666,7 @@
       </c>
       <c r="E11" s="38"/>
       <c r="F11" s="38" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G11" s="38"/>
     </row>
@@ -8688,7 +8685,7 @@
       </c>
       <c r="E12" s="38"/>
       <c r="F12" s="38" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G12" s="38"/>
     </row>
@@ -8707,7 +8704,7 @@
       </c>
       <c r="E13" s="38"/>
       <c r="F13" s="38" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G13" s="38"/>
     </row>
@@ -8726,7 +8723,7 @@
       </c>
       <c r="E14" s="38"/>
       <c r="F14" s="38" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G14" s="38"/>
     </row>
@@ -8745,7 +8742,7 @@
       </c>
       <c r="E15" s="38"/>
       <c r="F15" s="38" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="G15" s="38"/>
     </row>
@@ -8769,10 +8766,10 @@
         <v>58</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>1255</v>
+        <v>1254</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D17" s="37"/>
       <c r="E17" s="37"/>
@@ -8794,7 +8791,7 @@
       </c>
       <c r="E18" s="38"/>
       <c r="F18" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G18" s="38" t="s">
         <v>95</v>
@@ -8815,7 +8812,7 @@
       </c>
       <c r="E19" s="38"/>
       <c r="F19" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G19" s="38"/>
     </row>
@@ -8834,7 +8831,7 @@
       </c>
       <c r="E20" s="38"/>
       <c r="F20" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G20" s="38"/>
     </row>
@@ -8853,7 +8850,7 @@
       </c>
       <c r="E21" s="38"/>
       <c r="F21" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G21" s="38"/>
     </row>
@@ -8872,7 +8869,7 @@
       </c>
       <c r="E22" s="38"/>
       <c r="F22" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G22" s="38"/>
     </row>
@@ -8884,14 +8881,14 @@
         <v>102</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="D23" s="38" t="s">
         <v>104</v>
       </c>
       <c r="E23" s="38"/>
       <c r="F23" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G23" s="38"/>
     </row>
@@ -8903,14 +8900,14 @@
         <v>105</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="D24" s="39" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="E24" s="39"/>
       <c r="F24" s="39" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G24" s="39"/>
     </row>
@@ -8929,7 +8926,7 @@
       </c>
       <c r="E25" s="38"/>
       <c r="F25" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G25" s="38"/>
     </row>
@@ -8941,14 +8938,14 @@
         <v>111</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="D26" s="38" t="s">
         <v>110</v>
       </c>
       <c r="E26" s="38"/>
       <c r="F26" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G26" s="38"/>
     </row>
@@ -8960,14 +8957,14 @@
         <v>114</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="E27" s="39"/>
       <c r="F27" s="39" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G27" s="39"/>
     </row>
@@ -8979,14 +8976,14 @@
         <v>117</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="E28" s="39"/>
       <c r="F28" s="39" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G28" s="39"/>
     </row>
@@ -8995,34 +8992,34 @@
         <v>58</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="D29" s="39" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G29" s="39"/>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" s="39"/>
       <c r="B30" s="39" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="D30" s="39" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="E30" s="39"/>
       <c r="F30" s="39" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G30" s="39"/>
     </row>
@@ -9031,17 +9028,17 @@
         <v>58</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="D31" s="38" t="s">
         <v>113</v>
       </c>
       <c r="E31" s="38"/>
       <c r="F31" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G31" s="38"/>
     </row>
@@ -9050,7 +9047,7 @@
         <v>58</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="C32" s="38" t="s">
         <v>115</v>
@@ -9060,7 +9057,7 @@
       </c>
       <c r="E32" s="38"/>
       <c r="F32" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G32" s="38"/>
     </row>
@@ -9069,17 +9066,17 @@
         <v>58</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="C33" s="39" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="D33" s="39" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="E33" s="39"/>
       <c r="F33" s="39" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G33" s="39"/>
     </row>
@@ -9088,17 +9085,17 @@
         <v>58</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="C34" s="39" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="E34" s="39"/>
       <c r="F34" s="39" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G34" s="39"/>
     </row>
@@ -9107,17 +9104,17 @@
         <v>58</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="E35" s="39"/>
       <c r="F35" s="39" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G35" s="39"/>
     </row>
@@ -9126,17 +9123,17 @@
         <v>58</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="D36" s="39" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="E36" s="39"/>
       <c r="F36" s="39" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G36" s="39"/>
     </row>
@@ -9145,7 +9142,7 @@
         <v>58</v>
       </c>
       <c r="B37" s="38" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="C37" s="38" t="s">
         <v>118</v>
@@ -9155,7 +9152,7 @@
       </c>
       <c r="E37" s="38"/>
       <c r="F37" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G37" s="38"/>
     </row>
@@ -9174,7 +9171,7 @@
       </c>
       <c r="E38" s="38"/>
       <c r="F38" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G38" s="38"/>
     </row>
@@ -9193,7 +9190,7 @@
       </c>
       <c r="E39" s="38"/>
       <c r="F39" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G39" s="38"/>
     </row>
@@ -9212,7 +9209,7 @@
       </c>
       <c r="E40" s="38"/>
       <c r="F40" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G40" s="38"/>
     </row>
@@ -9231,7 +9228,7 @@
       </c>
       <c r="E41" s="38"/>
       <c r="F41" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G41" s="38"/>
     </row>
@@ -9240,7 +9237,7 @@
         <v>131</v>
       </c>
       <c r="B42" s="38" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
       <c r="C42" s="38" t="s">
         <v>133</v>
@@ -9250,7 +9247,7 @@
       </c>
       <c r="E42" s="38"/>
       <c r="F42" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G42" s="38"/>
     </row>
@@ -9274,10 +9271,10 @@
         <v>58</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D44" s="37"/>
       <c r="E44" s="37"/>
@@ -9299,7 +9296,7 @@
       </c>
       <c r="E45" s="38"/>
       <c r="F45" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G45" s="38" t="s">
         <v>136</v>
@@ -9320,7 +9317,7 @@
       </c>
       <c r="E46" s="38"/>
       <c r="F46" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G46" s="38"/>
     </row>
@@ -9339,7 +9336,7 @@
       </c>
       <c r="E47" s="38"/>
       <c r="F47" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G47" s="38"/>
     </row>
@@ -9358,7 +9355,7 @@
       </c>
       <c r="E48" s="38"/>
       <c r="F48" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G48" s="38"/>
     </row>
@@ -9377,7 +9374,7 @@
       </c>
       <c r="E49" s="38"/>
       <c r="F49" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G49" s="38"/>
     </row>
@@ -9396,7 +9393,7 @@
       </c>
       <c r="E50" s="38"/>
       <c r="F50" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G50" s="38"/>
     </row>
@@ -9415,7 +9412,7 @@
       </c>
       <c r="E51" s="38"/>
       <c r="F51" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G51" s="38"/>
     </row>
@@ -9434,7 +9431,7 @@
       </c>
       <c r="E52" s="38"/>
       <c r="F52" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G52" s="38"/>
     </row>
@@ -9453,7 +9450,7 @@
       </c>
       <c r="E53" s="38"/>
       <c r="F53" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G53" s="38"/>
     </row>
@@ -9462,7 +9459,7 @@
         <v>131</v>
       </c>
       <c r="B54" s="38" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="C54" s="38" t="s">
         <v>133</v>
@@ -9472,7 +9469,7 @@
       </c>
       <c r="E54" s="38"/>
       <c r="F54" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G54" s="38"/>
     </row>
@@ -9496,10 +9493,10 @@
         <v>58</v>
       </c>
       <c r="B56" s="38" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="C56" s="37" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D56" s="37"/>
       <c r="E56" s="37"/>
@@ -9521,7 +9518,7 @@
       </c>
       <c r="E57" s="38"/>
       <c r="F57" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G57" s="38" t="s">
         <v>158</v>
@@ -9542,7 +9539,7 @@
       </c>
       <c r="E58" s="38"/>
       <c r="F58" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G58" s="38"/>
     </row>
@@ -9561,7 +9558,7 @@
       </c>
       <c r="E59" s="38"/>
       <c r="F59" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G59" s="38"/>
     </row>
@@ -9580,7 +9577,7 @@
       </c>
       <c r="E60" s="38"/>
       <c r="F60" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G60" s="38"/>
     </row>
@@ -9599,7 +9596,7 @@
       </c>
       <c r="E61" s="38"/>
       <c r="F61" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G61" s="38"/>
     </row>
@@ -9618,7 +9615,7 @@
       </c>
       <c r="E62" s="38"/>
       <c r="F62" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G62" s="38"/>
     </row>
@@ -9637,7 +9634,7 @@
       </c>
       <c r="E63" s="38"/>
       <c r="F63" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G63" s="38"/>
     </row>
@@ -9656,7 +9653,7 @@
       </c>
       <c r="E64" s="38"/>
       <c r="F64" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G64" s="38"/>
     </row>
@@ -9675,7 +9672,7 @@
       </c>
       <c r="E65" s="38"/>
       <c r="F65" s="38" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="G65" s="38"/>
     </row>
@@ -9699,10 +9696,10 @@
         <v>58</v>
       </c>
       <c r="B67" s="38" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
       <c r="C67" s="37" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D67" s="37"/>
       <c r="E67" s="37"/>
@@ -9724,7 +9721,7 @@
       </c>
       <c r="E68" s="38"/>
       <c r="F68" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G68" s="38" t="s">
         <v>169</v>
@@ -9745,7 +9742,7 @@
       </c>
       <c r="E69" s="38"/>
       <c r="F69" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G69" s="38"/>
     </row>
@@ -9764,7 +9761,7 @@
       </c>
       <c r="E70" s="38"/>
       <c r="F70" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G70" s="38"/>
     </row>
@@ -9783,7 +9780,7 @@
       </c>
       <c r="E71" s="38"/>
       <c r="F71" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G71" s="38"/>
     </row>
@@ -9802,7 +9799,7 @@
       </c>
       <c r="E72" s="40"/>
       <c r="F72" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G72" s="38"/>
     </row>
@@ -9821,7 +9818,7 @@
       </c>
       <c r="E73" s="38"/>
       <c r="F73" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G73" s="38"/>
     </row>
@@ -9833,14 +9830,14 @@
         <v>179</v>
       </c>
       <c r="C74" s="39" t="s">
-        <v>1234</v>
+        <v>1233</v>
       </c>
       <c r="D74" s="39" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="E74" s="39"/>
       <c r="F74" s="39" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G74" s="39"/>
     </row>
@@ -9852,14 +9849,14 @@
         <v>182</v>
       </c>
       <c r="C75" s="39" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="D75" s="39" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="E75" s="39"/>
       <c r="F75" s="39" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G75" s="39"/>
     </row>
@@ -9878,7 +9875,7 @@
       </c>
       <c r="E76" s="38"/>
       <c r="F76" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G76" s="38"/>
     </row>
@@ -9887,7 +9884,7 @@
         <v>58</v>
       </c>
       <c r="B77" s="38" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="C77" s="38" t="s">
         <v>183</v>
@@ -9897,7 +9894,7 @@
       </c>
       <c r="E77" s="38"/>
       <c r="F77" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G77" s="38"/>
     </row>
@@ -9906,7 +9903,7 @@
         <v>58</v>
       </c>
       <c r="B78" s="38" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="C78" s="38" t="s">
         <v>186</v>
@@ -9916,7 +9913,7 @@
       </c>
       <c r="E78" s="38"/>
       <c r="F78" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G78" s="38"/>
     </row>
@@ -9925,7 +9922,7 @@
         <v>131</v>
       </c>
       <c r="B79" s="38" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C79" s="38" t="s">
         <v>133</v>
@@ -9935,7 +9932,7 @@
       </c>
       <c r="E79" s="38"/>
       <c r="F79" s="38" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="G79" s="38"/>
     </row>
@@ -9944,7 +9941,7 @@
         <v>58</v>
       </c>
       <c r="B80" s="38" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="C80" s="37" t="s">
         <v>6</v>
@@ -9959,10 +9956,10 @@
         <v>58</v>
       </c>
       <c r="B81" s="38" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="C81" s="37" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D81" s="37"/>
       <c r="E81" s="37"/>
@@ -9984,7 +9981,7 @@
       </c>
       <c r="E82" s="38"/>
       <c r="F82" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G82" s="38" t="s">
         <v>191</v>
@@ -10005,7 +10002,7 @@
       </c>
       <c r="E83" s="38"/>
       <c r="F83" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G83" s="38"/>
     </row>
@@ -10024,7 +10021,7 @@
       </c>
       <c r="E84" s="38"/>
       <c r="F84" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G84" s="38"/>
     </row>
@@ -10043,7 +10040,7 @@
       </c>
       <c r="E85" s="38"/>
       <c r="F85" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G85" s="38"/>
     </row>
@@ -10062,7 +10059,7 @@
       </c>
       <c r="E86" s="38"/>
       <c r="F86" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G86" s="38"/>
     </row>
@@ -10081,7 +10078,7 @@
       </c>
       <c r="E87" s="38"/>
       <c r="F87" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G87" s="38"/>
     </row>
@@ -10100,7 +10097,7 @@
       </c>
       <c r="E88" s="38"/>
       <c r="F88" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G88" s="38"/>
     </row>
@@ -10109,7 +10106,7 @@
         <v>131</v>
       </c>
       <c r="B89" s="38" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="C89" s="38" t="s">
         <v>133</v>
@@ -10119,7 +10116,7 @@
       </c>
       <c r="E89" s="38"/>
       <c r="F89" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G89" s="38"/>
     </row>
@@ -10143,10 +10140,10 @@
         <v>58</v>
       </c>
       <c r="B91" s="38" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="C91" s="37" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D91" s="37"/>
       <c r="E91" s="37"/>
@@ -10168,7 +10165,7 @@
       </c>
       <c r="E92" s="38"/>
       <c r="F92" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G92" s="38" t="s">
         <v>207</v>
@@ -10189,7 +10186,7 @@
       </c>
       <c r="E93" s="38"/>
       <c r="F93" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G93" s="38"/>
     </row>
@@ -10208,7 +10205,7 @@
       </c>
       <c r="E94" s="38"/>
       <c r="F94" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G94" s="38"/>
     </row>
@@ -10227,7 +10224,7 @@
       </c>
       <c r="E95" s="38"/>
       <c r="F95" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G95" s="38"/>
     </row>
@@ -10246,7 +10243,7 @@
       </c>
       <c r="E96" s="38"/>
       <c r="F96" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G96" s="38"/>
     </row>
@@ -10265,7 +10262,7 @@
       </c>
       <c r="E97" s="38"/>
       <c r="F97" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G97" s="38"/>
     </row>
@@ -10284,7 +10281,7 @@
       </c>
       <c r="E98" s="38"/>
       <c r="F98" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G98" s="38"/>
     </row>
@@ -10303,7 +10300,7 @@
       </c>
       <c r="E99" s="38"/>
       <c r="F99" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G99" s="38"/>
     </row>
@@ -10322,7 +10319,7 @@
       </c>
       <c r="E100" s="38"/>
       <c r="F100" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G100" s="38"/>
     </row>
@@ -10331,7 +10328,7 @@
         <v>131</v>
       </c>
       <c r="B101" s="38" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="C101" s="38" t="s">
         <v>133</v>
@@ -10341,7 +10338,7 @@
       </c>
       <c r="E101" s="38"/>
       <c r="F101" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G101" s="38"/>
     </row>
@@ -10365,10 +10362,10 @@
         <v>58</v>
       </c>
       <c r="B103" s="38" t="s">
-        <v>1263</v>
+        <v>1262</v>
       </c>
       <c r="C103" s="37" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D103" s="37"/>
       <c r="E103" s="37"/>
@@ -10390,7 +10387,7 @@
       </c>
       <c r="E104" s="38"/>
       <c r="F104" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G104" s="38" t="s">
         <v>219</v>
@@ -10411,7 +10408,7 @@
       </c>
       <c r="E105" s="38"/>
       <c r="F105" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G105" s="38"/>
     </row>
@@ -10430,7 +10427,7 @@
       </c>
       <c r="E106" s="38"/>
       <c r="F106" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G106" s="38"/>
     </row>
@@ -10449,7 +10446,7 @@
       </c>
       <c r="E107" s="38"/>
       <c r="F107" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G107" s="38"/>
     </row>
@@ -10468,7 +10465,7 @@
       </c>
       <c r="E108" s="38"/>
       <c r="F108" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G108" s="38"/>
     </row>
@@ -10487,7 +10484,7 @@
       </c>
       <c r="E109" s="38"/>
       <c r="F109" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G109" s="38"/>
     </row>
@@ -10506,7 +10503,7 @@
       </c>
       <c r="E110" s="38"/>
       <c r="F110" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G110" s="38"/>
     </row>
@@ -10525,7 +10522,7 @@
       </c>
       <c r="E111" s="38"/>
       <c r="F111" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G111" s="38"/>
     </row>
@@ -10544,7 +10541,7 @@
       </c>
       <c r="E112" s="38"/>
       <c r="F112" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G112" s="38"/>
     </row>
@@ -10553,7 +10550,7 @@
         <v>131</v>
       </c>
       <c r="B113" s="38" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="C113" s="38" t="s">
         <v>133</v>
@@ -10563,7 +10560,7 @@
       </c>
       <c r="E113" s="38"/>
       <c r="F113" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G113" s="38"/>
     </row>
@@ -10587,10 +10584,10 @@
         <v>58</v>
       </c>
       <c r="B115" s="38" t="s">
-        <v>1264</v>
+        <v>1263</v>
       </c>
       <c r="C115" s="37" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D115" s="37"/>
       <c r="E115" s="37"/>
@@ -10612,7 +10609,7 @@
       </c>
       <c r="E116" s="38"/>
       <c r="F116" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G116" s="38" t="s">
         <v>136</v>
@@ -10633,7 +10630,7 @@
       </c>
       <c r="E117" s="38"/>
       <c r="F117" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G117" s="38"/>
     </row>
@@ -10652,7 +10649,7 @@
       </c>
       <c r="E118" s="38"/>
       <c r="F118" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G118" s="38"/>
     </row>
@@ -10671,7 +10668,7 @@
       </c>
       <c r="E119" s="38"/>
       <c r="F119" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G119" s="38"/>
     </row>
@@ -10690,7 +10687,7 @@
       </c>
       <c r="E120" s="38"/>
       <c r="F120" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G120" s="38"/>
     </row>
@@ -10709,7 +10706,7 @@
       </c>
       <c r="E121" s="38"/>
       <c r="F121" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G121" s="38"/>
     </row>
@@ -10728,7 +10725,7 @@
       </c>
       <c r="E122" s="38"/>
       <c r="F122" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G122" s="38"/>
     </row>
@@ -10747,7 +10744,7 @@
       </c>
       <c r="E123" s="38"/>
       <c r="F123" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G123" s="38"/>
     </row>
@@ -10766,7 +10763,7 @@
       </c>
       <c r="E124" s="38"/>
       <c r="F124" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G124" s="38"/>
     </row>
@@ -10775,7 +10772,7 @@
         <v>131</v>
       </c>
       <c r="B125" s="38" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
       <c r="C125" s="38" t="s">
         <v>133</v>
@@ -10785,7 +10782,7 @@
       </c>
       <c r="E125" s="38"/>
       <c r="F125" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G125" s="38"/>
     </row>
@@ -10794,7 +10791,7 @@
         <v>58</v>
       </c>
       <c r="B126" s="38" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="C126" s="37" t="s">
         <v>10</v>
@@ -10809,10 +10806,10 @@
         <v>58</v>
       </c>
       <c r="B127" s="38" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
       <c r="C127" s="37" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D127" s="37"/>
       <c r="E127" s="37"/>
@@ -10834,7 +10831,7 @@
       </c>
       <c r="E128" s="38"/>
       <c r="F128" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G128" s="38" t="s">
         <v>242</v>
@@ -10855,7 +10852,7 @@
       </c>
       <c r="E129" s="38"/>
       <c r="F129" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G129" s="38"/>
     </row>
@@ -10874,7 +10871,7 @@
       </c>
       <c r="E130" s="38"/>
       <c r="F130" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G130" s="38"/>
     </row>
@@ -10893,7 +10890,7 @@
       </c>
       <c r="E131" s="38"/>
       <c r="F131" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G131" s="38"/>
     </row>
@@ -10912,7 +10909,7 @@
       </c>
       <c r="E132" s="38"/>
       <c r="F132" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G132" s="38"/>
     </row>
@@ -10924,14 +10921,14 @@
         <v>249</v>
       </c>
       <c r="C133" s="38" t="s">
-        <v>1236</v>
+        <v>1235</v>
       </c>
       <c r="D133" s="38" t="s">
         <v>251</v>
       </c>
       <c r="E133" s="38"/>
       <c r="F133" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G133" s="38"/>
     </row>
@@ -10943,14 +10940,14 @@
         <v>252</v>
       </c>
       <c r="C134" s="39" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="D134" s="39" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="E134" s="39"/>
       <c r="F134" s="39" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G134" s="39"/>
     </row>
@@ -10969,7 +10966,7 @@
       </c>
       <c r="E135" s="38"/>
       <c r="F135" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G135" s="38"/>
     </row>
@@ -10978,7 +10975,7 @@
         <v>58</v>
       </c>
       <c r="B136" s="38" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="C136" s="38" t="s">
         <v>256</v>
@@ -10988,7 +10985,7 @@
       </c>
       <c r="E136" s="38"/>
       <c r="F136" s="38" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="G136" s="38"/>
     </row>
@@ -11012,10 +11009,10 @@
         <v>58</v>
       </c>
       <c r="B138" s="38" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="C138" s="37" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
       <c r="D138" s="37"/>
       <c r="E138" s="37"/>
@@ -11039,10 +11036,10 @@
         <v>260</v>
       </c>
       <c r="F139" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G139" s="38" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="140" spans="1:7">
@@ -11062,7 +11059,7 @@
         <v>260</v>
       </c>
       <c r="F140" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G140" s="38"/>
     </row>
@@ -11083,7 +11080,7 @@
         <v>260</v>
       </c>
       <c r="F141" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G141" s="38"/>
     </row>
@@ -11104,7 +11101,7 @@
         <v>260</v>
       </c>
       <c r="F142" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G142" s="38"/>
     </row>
@@ -11116,7 +11113,7 @@
         <v>267</v>
       </c>
       <c r="C143" s="38" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="D143" s="38" t="s">
         <v>269</v>
@@ -11125,7 +11122,7 @@
         <v>260</v>
       </c>
       <c r="F143" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G143" s="38"/>
     </row>
@@ -11137,7 +11134,7 @@
         <v>270</v>
       </c>
       <c r="C144" s="38" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="D144" s="38" t="s">
         <v>266</v>
@@ -11146,7 +11143,7 @@
         <v>260</v>
       </c>
       <c r="F144" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G144" s="38"/>
     </row>
@@ -11158,14 +11155,14 @@
         <v>272</v>
       </c>
       <c r="C145" s="39" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D145" s="39" t="s">
         <v>1240</v>
-      </c>
-      <c r="D145" s="39" t="s">
-        <v>1241</v>
       </c>
       <c r="E145" s="39"/>
       <c r="F145" s="39" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G145" s="39"/>
     </row>
@@ -11174,19 +11171,19 @@
         <v>58</v>
       </c>
       <c r="B146" s="38" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="C146" s="38" t="s">
         <v>271</v>
       </c>
       <c r="D146" s="38" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E146" s="38" t="s">
         <v>260</v>
       </c>
       <c r="F146" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G146" s="38"/>
     </row>
@@ -11195,7 +11192,7 @@
         <v>58</v>
       </c>
       <c r="B147" s="38" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="C147" s="38" t="s">
         <v>273</v>
@@ -11207,7 +11204,7 @@
         <v>260</v>
       </c>
       <c r="F147" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G147" s="38"/>
     </row>
@@ -11216,19 +11213,19 @@
         <v>131</v>
       </c>
       <c r="B148" s="38" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="C148" s="38" t="s">
         <v>133</v>
       </c>
       <c r="D148" s="38" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E148" s="38" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="F148" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G148" s="38"/>
     </row>
@@ -11237,7 +11234,7 @@
         <v>131</v>
       </c>
       <c r="B149" s="38" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="C149" s="38" t="s">
         <v>277</v>
@@ -11247,7 +11244,7 @@
       </c>
       <c r="E149" s="38"/>
       <c r="F149" s="38" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="G149" s="38"/>
     </row>
@@ -11296,14 +11293,14 @@
         <v>14</v>
       </c>
       <c r="D152" s="38" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E152" s="38" t="s">
         <v>281</v>
       </c>
       <c r="F152" s="38"/>
       <c r="G152" s="38" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="153" spans="1:7">
@@ -11317,14 +11314,14 @@
         <v>15</v>
       </c>
       <c r="D153" s="38" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E153" s="38" t="s">
         <v>281</v>
       </c>
       <c r="F153" s="38"/>
       <c r="G153" s="38" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="154" spans="1:7">
@@ -11338,14 +11335,14 @@
         <v>283</v>
       </c>
       <c r="D154" s="38" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E154" s="38" t="s">
         <v>284</v>
       </c>
       <c r="F154" s="38"/>
       <c r="G154" s="38" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="155" spans="1:7">
@@ -11404,7 +11401,7 @@
         <v>58</v>
       </c>
       <c r="B158" s="35" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="C158" s="36" t="s">
         <v>19</v>
@@ -11590,7 +11587,7 @@
         <v>303</v>
       </c>
       <c r="C169" s="38" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D169" s="40" t="s">
         <v>949</v>
@@ -11911,7 +11908,7 @@
         <v>330</v>
       </c>
       <c r="C188" s="38" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D188" s="40" t="s">
         <v>949</v>
@@ -12423,7 +12420,7 @@
       <c r="E218" s="38"/>
       <c r="F218" s="38"/>
       <c r="G218" s="38" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="219" spans="1:7">
@@ -12536,13 +12533,13 @@
         <v>382</v>
       </c>
       <c r="C225" s="40" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D225" s="40" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E225" s="38" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="F225" s="38"/>
       <c r="G225" s="38"/>
@@ -12558,10 +12555,10 @@
         <v>385</v>
       </c>
       <c r="D226" s="40" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E226" s="38" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="F226" s="38"/>
       <c r="G226" s="38"/>
@@ -12574,7 +12571,7 @@
         <v>386</v>
       </c>
       <c r="C227" s="38" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D227" s="38">
         <v>76.16</v>
@@ -12648,7 +12645,7 @@
       <c r="E231" s="38"/>
       <c r="F231" s="38"/>
       <c r="G231" s="38" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="232" spans="1:7">
@@ -12716,7 +12713,7 @@
         <v>979</v>
       </c>
       <c r="E235" s="40" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="F235" s="40"/>
       <c r="G235" s="38"/>
@@ -13009,7 +13006,7 @@
         <v>58</v>
       </c>
       <c r="B253" s="35" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="C253" s="36" t="s">
         <v>35</v>
@@ -13099,7 +13096,7 @@
         <v>441</v>
       </c>
       <c r="E258" s="59" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F258" s="38"/>
       <c r="G258" s="44"/>
@@ -13180,13 +13177,13 @@
         <v>454</v>
       </c>
       <c r="C263" s="44" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="D263" s="38" t="s">
         <v>456</v>
       </c>
       <c r="E263" s="59" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F263" s="38"/>
       <c r="G263" s="44"/>
@@ -13196,13 +13193,13 @@
         <v>58</v>
       </c>
       <c r="B264" s="38" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C264" s="44" t="s">
         <v>1287</v>
       </c>
-      <c r="C264" s="44" t="s">
-        <v>1288</v>
-      </c>
       <c r="D264" s="38" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="E264" s="38"/>
       <c r="F264" s="38"/>
@@ -13256,7 +13253,7 @@
         <v>465</v>
       </c>
       <c r="E267" s="59" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F267" s="38"/>
       <c r="G267" s="44"/>
@@ -13266,7 +13263,7 @@
         <v>58</v>
       </c>
       <c r="B268" s="38" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="C268" s="44" t="s">
         <v>467</v>
@@ -13474,7 +13471,7 @@
         <v>490</v>
       </c>
       <c r="D280" s="38" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="E280" s="38"/>
       <c r="F280" s="38"/>
@@ -13580,7 +13577,7 @@
       </c>
       <c r="E286" s="38"/>
       <c r="F286" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G286" s="44"/>
     </row>
@@ -13780,7 +13777,7 @@
         <v>490</v>
       </c>
       <c r="D298" s="38" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="E298" s="38"/>
       <c r="F298" s="38"/>
@@ -13886,7 +13883,7 @@
       </c>
       <c r="E304" s="38"/>
       <c r="F304" s="38" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="G304" s="44"/>
     </row>
@@ -14212,7 +14209,7 @@
         <v>58</v>
       </c>
       <c r="B324" s="38" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="C324" s="38" t="s">
         <v>483</v>
@@ -14229,7 +14226,7 @@
         <v>58</v>
       </c>
       <c r="B325" s="38" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="C325" s="38" t="s">
         <v>485</v>
@@ -14269,7 +14266,7 @@
         <v>490</v>
       </c>
       <c r="D327" s="38" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="E327" s="38"/>
       <c r="F327" s="38"/>
@@ -14348,7 +14345,7 @@
         <v>58</v>
       </c>
       <c r="B332" s="38" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="C332" s="38" t="s">
         <v>501</v>
@@ -14365,7 +14362,7 @@
         <v>58</v>
       </c>
       <c r="B333" s="38" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
       <c r="C333" s="38" t="s">
         <v>504</v>
@@ -14375,7 +14372,7 @@
       </c>
       <c r="E333" s="38"/>
       <c r="F333" s="38" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="G333" s="38"/>
     </row>
@@ -14384,7 +14381,7 @@
         <v>58</v>
       </c>
       <c r="B334" s="35" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
       <c r="C334" s="49" t="s">
         <v>40</v>
@@ -14438,10 +14435,10 @@
         <v>78.3</v>
       </c>
       <c r="E337" s="38" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F337" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G337" s="44" t="s">
         <v>568</v>
@@ -14461,10 +14458,10 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E338" s="38" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F338" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G338" s="44"/>
     </row>
@@ -14476,14 +14473,14 @@
         <v>571</v>
       </c>
       <c r="C339" s="44" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="D339" s="38">
         <v>78.099999999999994</v>
       </c>
       <c r="E339" s="38"/>
       <c r="F339" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G339" s="44"/>
     </row>
@@ -14517,7 +14514,7 @@
       </c>
       <c r="E341" s="38"/>
       <c r="F341" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G341" s="44" t="s">
         <v>576</v>
@@ -14538,7 +14535,7 @@
       </c>
       <c r="E342" s="38"/>
       <c r="F342" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G342" s="44"/>
     </row>
@@ -14557,7 +14554,7 @@
       </c>
       <c r="E343" s="38"/>
       <c r="F343" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G343" s="38"/>
     </row>
@@ -14576,7 +14573,7 @@
       </c>
       <c r="E344" s="38"/>
       <c r="F344" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G344" s="44"/>
     </row>
@@ -14610,10 +14607,10 @@
       </c>
       <c r="E346" s="38"/>
       <c r="F346" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G346" s="44" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="347" spans="1:7">
@@ -14631,7 +14628,7 @@
       </c>
       <c r="E347" s="38"/>
       <c r="F347" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G347" s="44"/>
     </row>
@@ -14643,14 +14640,14 @@
         <v>595</v>
       </c>
       <c r="C348" s="44" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="D348" s="38" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E348" s="38"/>
       <c r="F348" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G348" s="44"/>
     </row>
@@ -14669,7 +14666,7 @@
       </c>
       <c r="E349" s="38"/>
       <c r="F349" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G349" s="44"/>
     </row>
@@ -14688,7 +14685,7 @@
       </c>
       <c r="E350" s="38"/>
       <c r="F350" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G350" s="44"/>
     </row>
@@ -14722,10 +14719,10 @@
       </c>
       <c r="E352" s="40"/>
       <c r="F352" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G352" s="44" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="353" spans="1:7" ht="30">
@@ -14743,7 +14740,7 @@
       </c>
       <c r="E353" s="40"/>
       <c r="F353" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G353" s="44"/>
     </row>
@@ -14758,11 +14755,11 @@
         <v>612</v>
       </c>
       <c r="D354" s="40" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="E354" s="40"/>
       <c r="F354" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G354" s="38"/>
     </row>
@@ -14781,7 +14778,7 @@
       </c>
       <c r="E355" s="40"/>
       <c r="F355" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G355" s="44"/>
     </row>
@@ -14800,7 +14797,7 @@
       </c>
       <c r="E356" s="38"/>
       <c r="F356" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G356" s="44"/>
     </row>
@@ -14834,10 +14831,10 @@
       </c>
       <c r="E358" s="38"/>
       <c r="F358" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G358" s="38" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="359" spans="1:7">
@@ -14851,11 +14848,11 @@
         <v>624</v>
       </c>
       <c r="D359" s="40" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E359" s="40"/>
       <c r="F359" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G359" s="38"/>
     </row>
@@ -14889,10 +14886,10 @@
       </c>
       <c r="E361" s="38"/>
       <c r="F361" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G361" s="44" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="362" spans="1:7">
@@ -14906,11 +14903,11 @@
         <v>629</v>
       </c>
       <c r="D362" s="38" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E362" s="46"/>
       <c r="F362" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G362" s="44"/>
     </row>
@@ -14929,7 +14926,7 @@
       </c>
       <c r="E363" s="38"/>
       <c r="F363" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G363" s="44"/>
     </row>
@@ -14944,11 +14941,11 @@
         <v>633</v>
       </c>
       <c r="D364" s="38" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E364" s="38"/>
       <c r="F364" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G364" s="44"/>
     </row>
@@ -14963,13 +14960,13 @@
         <v>635</v>
       </c>
       <c r="D365" s="38" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E365" s="38" t="s">
         <v>636</v>
       </c>
       <c r="F365" s="38" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="G365" s="38"/>
     </row>
@@ -15017,10 +15014,10 @@
         <v>1033</v>
       </c>
       <c r="E368" s="40" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F368" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G368" s="44" t="s">
         <v>568</v>
@@ -15040,10 +15037,10 @@
         <v>1028</v>
       </c>
       <c r="E369" s="40" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="F369" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G369" s="44"/>
     </row>
@@ -15061,10 +15058,10 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E370" s="38" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F370" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G370" s="44"/>
     </row>
@@ -15113,7 +15110,7 @@
       </c>
       <c r="E373" s="38"/>
       <c r="F373" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G373" s="44" t="s">
         <v>647</v>
@@ -15134,7 +15131,7 @@
       </c>
       <c r="E374" s="38"/>
       <c r="F374" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G374" s="44"/>
     </row>
@@ -15153,7 +15150,7 @@
       </c>
       <c r="E375" s="38"/>
       <c r="F375" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G375" s="44"/>
     </row>
@@ -15172,7 +15169,7 @@
       </c>
       <c r="E376" s="40"/>
       <c r="F376" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G376" s="44"/>
     </row>
@@ -15191,7 +15188,7 @@
       </c>
       <c r="E377" s="38"/>
       <c r="F377" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G377" s="44"/>
     </row>
@@ -15210,7 +15207,7 @@
       </c>
       <c r="E378" s="38"/>
       <c r="F378" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G378" s="44"/>
     </row>
@@ -15244,10 +15241,10 @@
       </c>
       <c r="E380" s="38"/>
       <c r="F380" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G380" s="44" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="381" spans="1:7">
@@ -15261,13 +15258,13 @@
         <v>624</v>
       </c>
       <c r="D381" s="40" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E381" s="40" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="F381" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G381" s="38"/>
     </row>
@@ -15301,10 +15298,10 @@
       </c>
       <c r="E383" s="38"/>
       <c r="F383" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G383" s="44" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="384" spans="1:7">
@@ -15318,11 +15315,11 @@
         <v>666</v>
       </c>
       <c r="D384" s="38" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E384" s="46"/>
       <c r="F384" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G384" s="44"/>
     </row>
@@ -15341,7 +15338,7 @@
       </c>
       <c r="E385" s="38"/>
       <c r="F385" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G385" s="44"/>
     </row>
@@ -15356,11 +15353,11 @@
         <v>633</v>
       </c>
       <c r="D386" s="38" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E386" s="38"/>
       <c r="F386" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G386" s="38"/>
     </row>
@@ -15375,13 +15372,13 @@
         <v>635</v>
       </c>
       <c r="D387" s="38" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E387" s="38" t="s">
         <v>636</v>
       </c>
       <c r="F387" s="38" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
       <c r="G387" s="38"/>
     </row>
@@ -15429,10 +15426,10 @@
         <v>78.3</v>
       </c>
       <c r="E390" s="38" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F390" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G390" s="44" t="s">
         <v>568</v>
@@ -15452,10 +15449,10 @@
         <v>1028</v>
       </c>
       <c r="E391" s="40" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="F391" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G391" s="38"/>
     </row>
@@ -15473,10 +15470,10 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E392" s="38" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F392" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G392" s="44"/>
     </row>
@@ -15525,7 +15522,7 @@
       </c>
       <c r="E395" s="38"/>
       <c r="F395" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G395" s="44" t="s">
         <v>681</v>
@@ -15546,7 +15543,7 @@
       </c>
       <c r="E396" s="38"/>
       <c r="F396" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G396" s="44"/>
     </row>
@@ -15565,7 +15562,7 @@
       </c>
       <c r="E397" s="38"/>
       <c r="F397" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G397" s="44"/>
     </row>
@@ -15584,7 +15581,7 @@
       </c>
       <c r="E398" s="38"/>
       <c r="F398" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G398" s="44"/>
     </row>
@@ -15603,7 +15600,7 @@
       </c>
       <c r="E399" s="38"/>
       <c r="F399" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G399" s="44"/>
     </row>
@@ -15622,7 +15619,7 @@
       </c>
       <c r="E400" s="38"/>
       <c r="F400" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G400" s="44"/>
     </row>
@@ -15656,10 +15653,10 @@
       </c>
       <c r="E402" s="38"/>
       <c r="F402" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G402" s="44" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="403" spans="1:7">
@@ -15673,13 +15670,13 @@
         <v>624</v>
       </c>
       <c r="D403" s="40" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E403" s="40" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="F403" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G403" s="38"/>
     </row>
@@ -15713,10 +15710,10 @@
       </c>
       <c r="E405" s="38"/>
       <c r="F405" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G405" s="44" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="406" spans="1:7">
@@ -15730,11 +15727,11 @@
         <v>666</v>
       </c>
       <c r="D406" s="38" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E406" s="46"/>
       <c r="F406" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G406" s="44"/>
     </row>
@@ -15753,7 +15750,7 @@
       </c>
       <c r="E407" s="38"/>
       <c r="F407" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G407" s="44"/>
     </row>
@@ -15768,11 +15765,11 @@
         <v>633</v>
       </c>
       <c r="D408" s="38" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E408" s="38"/>
       <c r="F408" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G408" s="38"/>
     </row>
@@ -15787,13 +15784,13 @@
         <v>635</v>
       </c>
       <c r="D409" s="38" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E409" s="38" t="s">
         <v>636</v>
       </c>
       <c r="F409" s="38" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="G409" s="38"/>
     </row>
@@ -15841,10 +15838,10 @@
         <v>78.3</v>
       </c>
       <c r="E412" s="3" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="F412" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G412" s="44" t="s">
         <v>568</v>
@@ -15864,10 +15861,10 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E413" s="38" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="F413" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G413" s="44"/>
     </row>
@@ -15885,10 +15882,10 @@
         <v>78.099999999999994</v>
       </c>
       <c r="E414" s="38" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="F414" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G414" s="44"/>
     </row>
@@ -15937,7 +15934,7 @@
       </c>
       <c r="E417" s="38"/>
       <c r="F417" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G417" s="38" t="s">
         <v>709</v>
@@ -15958,7 +15955,7 @@
       </c>
       <c r="E418" s="38"/>
       <c r="F418" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G418" s="44"/>
     </row>
@@ -15977,7 +15974,7 @@
       </c>
       <c r="E419" s="38"/>
       <c r="F419" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G419" s="44"/>
     </row>
@@ -15996,7 +15993,7 @@
       </c>
       <c r="E420" s="38"/>
       <c r="F420" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G420" s="38"/>
     </row>
@@ -16023,14 +16020,14 @@
         <v>718</v>
       </c>
       <c r="C422" s="62" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="D422" s="38" t="s">
         <v>1074</v>
       </c>
       <c r="E422" s="38"/>
       <c r="F422" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G422" s="38" t="s">
         <v>720</v>
@@ -16044,14 +16041,14 @@
         <v>722</v>
       </c>
       <c r="C423" s="62" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="D423" s="40" t="s">
         <v>721</v>
       </c>
       <c r="E423" s="40"/>
       <c r="F423" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G423" s="38"/>
     </row>
@@ -16070,7 +16067,7 @@
       </c>
       <c r="E424" s="40"/>
       <c r="F424" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G424" s="38"/>
     </row>
@@ -16104,7 +16101,7 @@
       </c>
       <c r="E426" s="40"/>
       <c r="F426" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G426" s="44" t="s">
         <v>729</v>
@@ -16125,7 +16122,7 @@
       </c>
       <c r="E427" s="40"/>
       <c r="F427" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G427" s="44"/>
     </row>
@@ -16144,7 +16141,7 @@
       </c>
       <c r="E428" s="40"/>
       <c r="F428" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G428" s="44"/>
     </row>
@@ -16163,7 +16160,7 @@
       </c>
       <c r="E429" s="40"/>
       <c r="F429" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G429" s="38"/>
     </row>
@@ -16182,7 +16179,7 @@
       </c>
       <c r="E430" s="40"/>
       <c r="F430" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G430" s="44"/>
     </row>
@@ -16201,7 +16198,7 @@
       </c>
       <c r="E431" s="40"/>
       <c r="F431" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G431" s="44"/>
     </row>
@@ -16218,7 +16215,7 @@
       <c r="D432" s="41"/>
       <c r="E432" s="41"/>
       <c r="F432" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G432" s="41"/>
     </row>
@@ -16237,7 +16234,7 @@
       </c>
       <c r="E433" s="40"/>
       <c r="F433" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G433" s="44" t="s">
         <v>738</v>
@@ -16258,7 +16255,7 @@
       </c>
       <c r="E434" s="40"/>
       <c r="F434" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G434" s="44"/>
     </row>
@@ -16277,7 +16274,7 @@
       </c>
       <c r="E435" s="40"/>
       <c r="F435" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G435" s="44" t="s">
         <v>606</v>
@@ -16298,7 +16295,7 @@
       </c>
       <c r="E436" s="40"/>
       <c r="F436" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G436" s="44"/>
     </row>
@@ -16315,7 +16312,7 @@
       <c r="D437" s="41"/>
       <c r="E437" s="41"/>
       <c r="F437" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G437" s="41"/>
     </row>
@@ -16334,10 +16331,10 @@
       </c>
       <c r="E438" s="40"/>
       <c r="F438" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G438" s="44" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="439" spans="1:7">
@@ -16351,13 +16348,13 @@
         <v>624</v>
       </c>
       <c r="D439" s="40" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E439" s="40" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="F439" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G439" s="38"/>
     </row>
@@ -16369,12 +16366,12 @@
         <v>746</v>
       </c>
       <c r="C440" s="41" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="D440" s="41"/>
       <c r="E440" s="41"/>
       <c r="F440" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G440" s="41"/>
     </row>
@@ -16389,13 +16386,13 @@
         <v>635</v>
       </c>
       <c r="D441" s="38" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E441" s="38" t="s">
         <v>636</v>
       </c>
       <c r="F441" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G441" s="38"/>
     </row>
@@ -16412,7 +16409,7 @@
       <c r="D442" s="41"/>
       <c r="E442" s="41"/>
       <c r="F442" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G442" s="37"/>
     </row>
@@ -16431,7 +16428,7 @@
         <v>279</v>
       </c>
       <c r="F443" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G443" s="44"/>
     </row>
@@ -16450,7 +16447,7 @@
         <v>279</v>
       </c>
       <c r="F444" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G444" s="44"/>
     </row>
@@ -16469,7 +16466,7 @@
         <v>279</v>
       </c>
       <c r="F445" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G445" s="44"/>
     </row>
@@ -16486,7 +16483,7 @@
       <c r="D446" s="41"/>
       <c r="E446" s="37"/>
       <c r="F446" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G446" s="37"/>
     </row>
@@ -16505,7 +16502,7 @@
         <v>279</v>
       </c>
       <c r="F447" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G447" s="44"/>
     </row>
@@ -16524,7 +16521,7 @@
         <v>279</v>
       </c>
       <c r="F448" s="38" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="G448" s="44"/>
     </row>
@@ -16541,7 +16538,7 @@
       <c r="D449" s="41"/>
       <c r="E449" s="41"/>
       <c r="F449" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G449" s="37"/>
     </row>
@@ -16558,7 +16555,7 @@
       <c r="D450" s="41"/>
       <c r="E450" s="41"/>
       <c r="F450" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G450" s="41"/>
     </row>
@@ -16577,7 +16574,7 @@
       </c>
       <c r="E451" s="38"/>
       <c r="F451" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G451" s="44" t="s">
         <v>568</v>
@@ -16598,7 +16595,7 @@
       </c>
       <c r="E452" s="38"/>
       <c r="F452" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G452" s="44"/>
     </row>
@@ -16617,7 +16614,7 @@
       </c>
       <c r="E453" s="38"/>
       <c r="F453" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G453" s="44"/>
     </row>
@@ -16634,7 +16631,7 @@
       <c r="D454" s="41"/>
       <c r="E454" s="41"/>
       <c r="F454" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G454" s="41"/>
     </row>
@@ -16651,7 +16648,7 @@
       <c r="D455" s="41"/>
       <c r="E455" s="41"/>
       <c r="F455" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G455" s="41"/>
     </row>
@@ -16670,10 +16667,10 @@
       </c>
       <c r="E456" s="38"/>
       <c r="F456" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G456" s="44" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="457" spans="1:7">
@@ -16691,7 +16688,7 @@
       </c>
       <c r="E457" s="38"/>
       <c r="F457" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G457" s="44"/>
     </row>
@@ -16706,11 +16703,11 @@
         <v>767</v>
       </c>
       <c r="D458" s="38" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="E458" s="38"/>
       <c r="F458" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G458" s="38"/>
     </row>
@@ -16729,7 +16726,7 @@
       </c>
       <c r="E459" s="38"/>
       <c r="F459" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G459" s="38"/>
     </row>
@@ -16741,12 +16738,12 @@
         <v>770</v>
       </c>
       <c r="C460" s="38" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="D460" s="38"/>
       <c r="E460" s="38"/>
       <c r="F460" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G460" s="38"/>
     </row>
@@ -16755,7 +16752,7 @@
         <v>58</v>
       </c>
       <c r="B461" s="38" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="C461" s="38" t="s">
         <v>771</v>
@@ -16765,7 +16762,7 @@
       </c>
       <c r="E461" s="38"/>
       <c r="F461" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G461" s="38"/>
     </row>
@@ -16774,17 +16771,17 @@
         <v>58</v>
       </c>
       <c r="B462" s="38" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="C462" s="38" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D462" s="38" t="s">
         <v>724</v>
       </c>
       <c r="E462" s="38"/>
       <c r="F462" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G462" s="38"/>
     </row>
@@ -16801,7 +16798,7 @@
       <c r="D463" s="41"/>
       <c r="E463" s="41"/>
       <c r="F463" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G463" s="41"/>
     </row>
@@ -16820,10 +16817,10 @@
       </c>
       <c r="E464" s="38"/>
       <c r="F464" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G464" s="44" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="465" spans="1:7">
@@ -16837,11 +16834,11 @@
         <v>624</v>
       </c>
       <c r="D465" s="40" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="E465" s="40"/>
       <c r="F465" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G465" s="38"/>
     </row>
@@ -16858,7 +16855,7 @@
       <c r="D466" s="41"/>
       <c r="E466" s="41"/>
       <c r="F466" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G466" s="41"/>
     </row>
@@ -16877,10 +16874,10 @@
       </c>
       <c r="E467" s="38"/>
       <c r="F467" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G467" s="44" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="468" spans="1:7">
@@ -16898,7 +16895,7 @@
       </c>
       <c r="E468" s="38"/>
       <c r="F468" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G468" s="44"/>
     </row>
@@ -16917,7 +16914,7 @@
       </c>
       <c r="E469" s="38"/>
       <c r="F469" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G469" s="44"/>
     </row>
@@ -16932,11 +16929,11 @@
         <v>633</v>
       </c>
       <c r="D470" s="38" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="E470" s="38"/>
       <c r="F470" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G470" s="38"/>
     </row>
@@ -16951,11 +16948,11 @@
         <v>635</v>
       </c>
       <c r="D471" s="38" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="E471" s="38"/>
       <c r="F471" s="38" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G471" s="38"/>
     </row>
@@ -17012,7 +17009,7 @@
         <v>62</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>789</v>
@@ -17031,7 +17028,7 @@
         <v>65</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>791</v>
@@ -17050,7 +17047,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>792</v>
@@ -17069,7 +17066,7 @@
         <v>71</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>793</v>
@@ -17088,7 +17085,7 @@
         <v>796</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>797</v>
@@ -18473,7 +18470,7 @@
         <v>124</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>790</v>
@@ -18886,7 +18883,7 @@
         <v>278</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>854</v>
@@ -18905,13 +18902,13 @@
         <v>269</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C40" s="28" t="s">
         <v>855</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>1250</v>
+        <v>1249</v>
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
@@ -18924,13 +18921,13 @@
         <v>266</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>856</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3" t="s">
@@ -18943,7 +18940,7 @@
         <v>274</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>857</v>
@@ -18959,16 +18956,16 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" s="32" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="B43" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C43" s="32" t="s">
+        <v>1174</v>
+      </c>
+      <c r="D43" s="32" t="s">
         <v>1175</v>
-      </c>
-      <c r="D43" s="32" t="s">
-        <v>1176</v>
       </c>
       <c r="E43" s="32"/>
       <c r="F43" s="32" t="s">
@@ -18978,16 +18975,16 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="32" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="B44" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="E44" s="32"/>
       <c r="F44" s="32" t="s">
@@ -18997,16 +18994,16 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="32" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="B45" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="D45" s="32" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="E45" s="32"/>
       <c r="F45" s="32" t="s">
@@ -19016,16 +19013,16 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" s="32" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="B46" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="E46" s="32"/>
       <c r="F46" s="32" t="s">
@@ -19035,16 +19032,16 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" s="32" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="B47" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="E47" s="32"/>
       <c r="F47" s="32" t="s">
@@ -19054,16 +19051,16 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="32" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="B48" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="E48" s="32"/>
       <c r="F48" s="32" t="s">
@@ -19073,16 +19070,16 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="32" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="B49" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="E49" s="32"/>
       <c r="F49" s="32" t="s">
@@ -19092,16 +19089,16 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="32" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="B50" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="E50" s="32"/>
       <c r="F50" s="32" t="s">
@@ -19111,16 +19108,16 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="32" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="B51" s="32" t="s">
         <v>813</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="E51" s="32"/>
       <c r="F51" s="32" t="s">
@@ -19130,16 +19127,16 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="32" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="B52" s="32" t="s">
         <v>839</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="E52" s="32"/>
       <c r="F52" s="32" t="s">
@@ -19149,16 +19146,16 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="32" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="B53" s="32" t="s">
         <v>839</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="E53" s="32"/>
       <c r="F53" s="32" t="s">
@@ -19168,16 +19165,16 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" s="32" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B54" s="32" t="s">
         <v>847</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="E54" s="32"/>
       <c r="F54" s="32" t="s">
@@ -19187,16 +19184,16 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="32" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="D55" s="32" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="E55" s="32"/>
       <c r="F55" s="32" t="s">
@@ -19774,16 +19771,16 @@
     </row>
     <row r="16" spans="1:256" ht="31.5" customHeight="1">
       <c r="A16" s="31" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>860</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="30" t="s">
@@ -19793,16 +19790,16 @@
     </row>
     <row r="17" spans="1:7" ht="31.5" customHeight="1">
       <c r="A17" s="31" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>860</v>
       </c>
       <c r="C17" s="31" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D17" s="31" t="s">
         <v>1096</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>1097</v>
       </c>
       <c r="E17" s="30"/>
       <c r="F17" s="30" t="s">
@@ -19821,7 +19818,7 @@
         <v>894</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="E18" s="30"/>
       <c r="F18" s="30" t="s">
@@ -20314,7 +20311,7 @@
         <v>965</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="F44" s="30"/>
       <c r="G44" s="30"/>
@@ -20400,7 +20397,7 @@
         <v>980</v>
       </c>
       <c r="D49" s="31" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="E49" s="30"/>
       <c r="F49" s="30"/>
@@ -20669,8 +20666,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:IV30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -20964,7 +20961,7 @@
         <v>435</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>981</v>
@@ -20983,7 +20980,7 @@
         <v>438</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>983</v>
@@ -21002,7 +20999,7 @@
         <v>441</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>985</v>
@@ -21021,7 +21018,7 @@
         <v>456</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>987</v>
@@ -21040,7 +21037,7 @@
         <v>444</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>989</v>
@@ -21059,7 +21056,7 @@
         <v>447</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>991</v>
@@ -21078,7 +21075,7 @@
         <v>450</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>993</v>
@@ -21097,7 +21094,7 @@
         <v>453</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>995</v>
@@ -21116,7 +21113,7 @@
         <v>459</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>997</v>
@@ -21135,7 +21132,7 @@
         <v>999</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>1000</v>
@@ -21154,7 +21151,7 @@
         <v>462</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>1002</v>
@@ -21173,7 +21170,7 @@
         <v>465</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>1004</v>
@@ -21194,7 +21191,7 @@
         <v>468</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>1007</v>
@@ -21213,7 +21210,7 @@
         <v>502</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>1009</v>
@@ -21236,7 +21233,7 @@
         <v>493</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>1013</v>
@@ -21255,7 +21252,7 @@
         <v>505</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>1015</v>
@@ -21278,13 +21275,13 @@
         <v>533</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>1019</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
@@ -21297,7 +21294,7 @@
         <v>536</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>1020</v>
@@ -21316,7 +21313,7 @@
         <v>539</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>1021</v>
@@ -21335,7 +21332,7 @@
         <v>542</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>1023</v>
@@ -21354,7 +21351,7 @@
         <v>547</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>1025</v>
@@ -21373,7 +21370,7 @@
         <v>488</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>1027</v>
@@ -21387,16 +21384,16 @@
     </row>
     <row r="24" spans="1:7" ht="31.2">
       <c r="A24" s="32" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B24" s="32" t="s">
         <v>1154</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="C24" s="32" t="s">
         <v>1155</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="D24" s="32" t="s">
         <v>1156</v>
-      </c>
-      <c r="D24" s="32" t="s">
-        <v>1157</v>
       </c>
       <c r="E24" s="32"/>
       <c r="F24" s="32"/>
@@ -21404,16 +21401,16 @@
     </row>
     <row r="25" spans="1:7" ht="46.8">
       <c r="A25" s="32" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B25" s="32" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C25" s="32" t="s">
         <v>1158</v>
       </c>
-      <c r="B25" s="32" t="s">
-        <v>1155</v>
-      </c>
-      <c r="C25" s="32" t="s">
-        <v>1159</v>
-      </c>
       <c r="D25" s="32" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
@@ -21421,16 +21418,16 @@
     </row>
     <row r="26" spans="1:7" ht="31.2">
       <c r="A26" s="32" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B26" s="32" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C26" s="32" t="s">
         <v>1160</v>
       </c>
-      <c r="B26" s="32" t="s">
-        <v>1155</v>
-      </c>
-      <c r="C26" s="32" t="s">
+      <c r="D26" s="32" t="s">
         <v>1161</v>
-      </c>
-      <c r="D26" s="32" t="s">
-        <v>1162</v>
       </c>
       <c r="E26" s="32"/>
       <c r="F26" s="32"/>
@@ -21438,16 +21435,16 @@
     </row>
     <row r="27" spans="1:7" ht="46.8">
       <c r="A27" s="32" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B27" s="32" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C27" s="32" t="s">
         <v>1163</v>
       </c>
-      <c r="B27" s="32" t="s">
-        <v>1155</v>
-      </c>
-      <c r="C27" s="32" t="s">
+      <c r="D27" s="32" t="s">
         <v>1164</v>
-      </c>
-      <c r="D27" s="32" t="s">
-        <v>1165</v>
       </c>
       <c r="E27" s="32"/>
       <c r="F27" s="32"/>
@@ -21455,16 +21452,16 @@
     </row>
     <row r="28" spans="1:7" ht="46.8">
       <c r="A28" s="32" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C28" s="32" t="s">
         <v>1166</v>
       </c>
-      <c r="B28" s="32" t="s">
-        <v>1155</v>
-      </c>
-      <c r="C28" s="32" t="s">
+      <c r="D28" s="32" t="s">
         <v>1167</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>1168</v>
       </c>
       <c r="E28" s="32"/>
       <c r="F28" s="32"/>
@@ -21472,16 +21469,16 @@
     </row>
     <row r="29" spans="1:7" ht="46.8">
       <c r="A29" s="32" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B29" s="32" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C29" s="32" t="s">
         <v>1169</v>
       </c>
-      <c r="B29" s="32" t="s">
-        <v>1155</v>
-      </c>
-      <c r="C29" s="32" t="s">
+      <c r="D29" s="32" t="s">
         <v>1170</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>1171</v>
       </c>
       <c r="E29" s="32"/>
       <c r="F29" s="32"/>
@@ -21489,16 +21486,16 @@
     </row>
     <row r="30" spans="1:7" ht="46.8">
       <c r="A30" s="32" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B30" s="32" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C30" s="32" t="s">
         <v>1172</v>
       </c>
-      <c r="B30" s="32" t="s">
-        <v>1155</v>
-      </c>
-      <c r="C30" s="32" t="s">
+      <c r="D30" s="32" t="s">
         <v>1173</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>1174</v>
       </c>
       <c r="E30" s="32"/>
       <c r="F30" s="32"/>
@@ -21567,7 +21564,7 @@
         <v>1030</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="E2" s="64"/>
       <c r="F2" s="28" t="s">
@@ -21835,7 +21832,7 @@
         <v>1032</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="E3" s="65"/>
       <c r="F3" s="3" t="s">
@@ -21854,7 +21851,7 @@
         <v>1034</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="E4" s="64"/>
       <c r="F4" s="3" t="s">
@@ -21876,8 +21873,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -22277,13 +22274,13 @@
         <v>1049</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>790</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="8" spans="1:256" ht="31.5" customHeight="1">
@@ -22521,7 +22518,7 @@
         <v>790</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17.100000000000001" customHeight="1">
@@ -22557,47 +22554,47 @@
         <v>1081</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>1082</v>
+        <v>1301</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>790</v>
       </c>
       <c r="G21" s="30" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="31.5" customHeight="1">
       <c r="A22" s="30" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C22" s="30" t="s">
+        <v>1084</v>
+      </c>
+      <c r="D22" s="30" t="s">
         <v>1085</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="E22" s="30" t="s">
         <v>1086</v>
-      </c>
-      <c r="E22" s="30" t="s">
-        <v>1087</v>
       </c>
       <c r="F22" s="30" t="s">
         <v>809</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="31.2">
       <c r="A23" s="30" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D23" s="30" t="s">
         <v>629</v>
@@ -22608,13 +22605,13 @@
     </row>
     <row r="24" spans="1:7">
       <c r="A24" s="30" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B24" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>633</v>
@@ -22625,32 +22622,32 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="30" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B25" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="D25" s="30" t="s">
         <v>624</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>
     </row>
     <row r="26" spans="1:7" ht="31.2">
       <c r="A26" s="30" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B26" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>635</v>
@@ -22661,13 +22658,13 @@
     </row>
     <row r="27" spans="1:7">
       <c r="A27" s="58" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B27" s="30" t="s">
         <v>1036</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D27" s="30" t="s">
         <v>767</v>
@@ -22979,40 +22976,40 @@
     </row>
     <row r="2" spans="1:256">
       <c r="A2" s="7" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
         <v>790</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="3" spans="1:256">
       <c r="A3" s="7" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>1135</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>1089</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>1136</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>809</v>
@@ -23021,19 +23018,19 @@
     </row>
     <row r="4" spans="1:256">
       <c r="A4" s="6" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>1140</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>1141</v>
-      </c>
       <c r="C4" s="6" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>1138</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>1089</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>1139</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>809</v>

</xml_diff>

<commit_message>
excel update for pkix.20
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE320434-456E-4E6C-9EAB-09C399F32D87}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866942E5-93E3-4F4D-89D8-D447F575A356}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -24,14 +24,14 @@
     <sheet name="Placeholders" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Steps Overview'!$A$1:$G$472</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Steps Overview'!$B$1:$B$472</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3776" uniqueCount="1309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3776" uniqueCount="1310">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3960,6 +3960,9 @@
   </si>
   <si>
     <t>The Patron Header Version field has a value of 0x03.</t>
+  </si>
+  <si>
+    <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.11,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID:2.16.840.1.101.3.2.1.48.9|2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID:2.16.840.1.101.3.2.1.48.9|2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.13,CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.2.1.48.86</t>
   </si>
 </sst>
 </file>
@@ -8509,8 +8512,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A325" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F333" sqref="F333"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -17038,7 +17041,6 @@
       <c r="G472" s="38"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G472" xr:uid="{D331C0AB-26E8-4A68-9DCE-42FE6AA1F39D}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -21971,7 +21973,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -22652,7 +22654,7 @@
         <v>1081</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>1301</v>
+        <v>1309</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>790</v>

</xml_diff>

<commit_message>
fix parameter on 11.7.2.4.2
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{866942E5-93E3-4F4D-89D8-D447F575A356}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D55BF9E-97CC-46D3-90B1-D62D40F8235E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <sheet name="Placeholders" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Steps Overview'!$B$1:$B$472</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Steps Overview'!$A$1:$G$472</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -3962,7 +3962,7 @@
     <t>The Patron Header Version field has a value of 0x03.</t>
   </si>
   <si>
-    <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.11,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID:2.16.840.1.101.3.2.1.48.9|2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID:2.16.840.1.101.3.2.1.48.9|2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.13,CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.2.1.48.86</t>
+    <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.11,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID:2.16.840.1.101.3.2.1.48.9|2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID:2.16.840.1.101.3.2.1.48.9|2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.13,CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.6.7</t>
   </si>
 </sst>
 </file>
@@ -8509,11 +8509,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:H472"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="F463" sqref="F463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8554,7 +8554,7 @@
       </c>
       <c r="H1" s="53"/>
     </row>
-    <row r="2" spans="1:8" ht="15.6">
+    <row r="2" spans="1:8" ht="15.6" hidden="1">
       <c r="A2" s="35" t="s">
         <v>58</v>
       </c>
@@ -8569,7 +8569,7 @@
       <c r="F2" s="37"/>
       <c r="G2" s="36"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" s="38" t="s">
         <v>58</v>
       </c>
@@ -8584,7 +8584,7 @@
       <c r="F3" s="37"/>
       <c r="G3" s="37"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" s="38" t="s">
         <v>58</v>
       </c>
@@ -8599,7 +8599,7 @@
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="30" hidden="1">
       <c r="A5" s="38" t="s">
         <v>58</v>
       </c>
@@ -8620,7 +8620,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" s="38" t="s">
         <v>58</v>
       </c>
@@ -8639,7 +8639,7 @@
       </c>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" hidden="1">
       <c r="A7" s="38" t="s">
         <v>58</v>
       </c>
@@ -8658,7 +8658,7 @@
       </c>
       <c r="G7" s="38"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" s="38" t="s">
         <v>58</v>
       </c>
@@ -8677,7 +8677,7 @@
       </c>
       <c r="G8" s="38"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" s="38" t="s">
         <v>58</v>
       </c>
@@ -8696,7 +8696,7 @@
       </c>
       <c r="G9" s="38"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" s="38" t="s">
         <v>58</v>
       </c>
@@ -8715,7 +8715,7 @@
       </c>
       <c r="G10" s="38"/>
     </row>
-    <row r="11" spans="1:8" ht="30">
+    <row r="11" spans="1:8" ht="30" hidden="1">
       <c r="A11" s="38" t="s">
         <v>58</v>
       </c>
@@ -8734,7 +8734,7 @@
       </c>
       <c r="G11" s="38"/>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:8" ht="30" hidden="1">
       <c r="A12" s="38" t="s">
         <v>58</v>
       </c>
@@ -8753,7 +8753,7 @@
       </c>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" s="38" t="s">
         <v>58</v>
       </c>
@@ -8772,7 +8772,7 @@
       </c>
       <c r="G13" s="38"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" hidden="1">
       <c r="A14" s="38" t="s">
         <v>58</v>
       </c>
@@ -8791,7 +8791,7 @@
       </c>
       <c r="G14" s="38"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" s="38" t="s">
         <v>58</v>
       </c>
@@ -8810,7 +8810,7 @@
       </c>
       <c r="G15" s="38"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" hidden="1">
       <c r="A16" s="38" t="s">
         <v>58</v>
       </c>
@@ -8825,7 +8825,7 @@
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" hidden="1">
       <c r="A17" s="38" t="s">
         <v>58</v>
       </c>
@@ -8840,7 +8840,7 @@
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
     </row>
-    <row r="18" spans="1:7" ht="30">
+    <row r="18" spans="1:7" ht="30" hidden="1">
       <c r="A18" s="38" t="s">
         <v>58</v>
       </c>
@@ -8861,7 +8861,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" hidden="1">
       <c r="A19" s="38" t="s">
         <v>58</v>
       </c>
@@ -8880,7 +8880,7 @@
       </c>
       <c r="G19" s="38"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" hidden="1">
       <c r="A20" s="38" t="s">
         <v>58</v>
       </c>
@@ -8899,7 +8899,7 @@
       </c>
       <c r="G20" s="38"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" hidden="1">
       <c r="A21" s="38" t="s">
         <v>58</v>
       </c>
@@ -8918,7 +8918,7 @@
       </c>
       <c r="G21" s="38"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" s="38" t="s">
         <v>58</v>
       </c>
@@ -8937,7 +8937,7 @@
       </c>
       <c r="G22" s="38"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23" s="38" t="s">
         <v>58</v>
       </c>
@@ -8956,7 +8956,7 @@
       </c>
       <c r="G23" s="38"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" hidden="1">
       <c r="A24" s="39" t="s">
         <v>58</v>
       </c>
@@ -8975,7 +8975,7 @@
       </c>
       <c r="G24" s="39"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" hidden="1">
       <c r="A25" s="38" t="s">
         <v>58</v>
       </c>
@@ -8994,7 +8994,7 @@
       </c>
       <c r="G25" s="38"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" hidden="1">
       <c r="A26" s="38" t="s">
         <v>58</v>
       </c>
@@ -9013,7 +9013,7 @@
       </c>
       <c r="G26" s="38"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="39" t="s">
         <v>58</v>
       </c>
@@ -9032,7 +9032,7 @@
       </c>
       <c r="G27" s="39"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="39" t="s">
         <v>58</v>
       </c>
@@ -9051,7 +9051,7 @@
       </c>
       <c r="G28" s="39"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="39" t="s">
         <v>58</v>
       </c>
@@ -9070,7 +9070,7 @@
       </c>
       <c r="G29" s="39"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" hidden="1">
       <c r="A30" s="39"/>
       <c r="B30" s="39" t="s">
         <v>1217</v>
@@ -9087,7 +9087,7 @@
       </c>
       <c r="G30" s="39"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" hidden="1">
       <c r="A31" s="38" t="s">
         <v>58</v>
       </c>
@@ -9106,7 +9106,7 @@
       </c>
       <c r="G31" s="38"/>
     </row>
-    <row r="32" spans="1:7" ht="30">
+    <row r="32" spans="1:7" ht="30" hidden="1">
       <c r="A32" s="38" t="s">
         <v>58</v>
       </c>
@@ -9125,7 +9125,7 @@
       </c>
       <c r="G32" s="38"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" hidden="1">
       <c r="A33" s="39" t="s">
         <v>58</v>
       </c>
@@ -9144,7 +9144,7 @@
       </c>
       <c r="G33" s="39"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" hidden="1">
       <c r="A34" s="39" t="s">
         <v>58</v>
       </c>
@@ -9163,7 +9163,7 @@
       </c>
       <c r="G34" s="39"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" hidden="1">
       <c r="A35" s="39" t="s">
         <v>58</v>
       </c>
@@ -9182,7 +9182,7 @@
       </c>
       <c r="G35" s="39"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="39" t="s">
         <v>58</v>
       </c>
@@ -9201,7 +9201,7 @@
       </c>
       <c r="G36" s="39"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" hidden="1">
       <c r="A37" s="38" t="s">
         <v>58</v>
       </c>
@@ -9220,7 +9220,7 @@
       </c>
       <c r="G37" s="38"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" hidden="1">
       <c r="A38" s="38" t="s">
         <v>58</v>
       </c>
@@ -9239,7 +9239,7 @@
       </c>
       <c r="G38" s="38"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" hidden="1">
       <c r="A39" s="38" t="s">
         <v>58</v>
       </c>
@@ -9258,7 +9258,7 @@
       </c>
       <c r="G39" s="38"/>
     </row>
-    <row r="40" spans="1:7" ht="30">
+    <row r="40" spans="1:7" ht="30" hidden="1">
       <c r="A40" s="38" t="s">
         <v>58</v>
       </c>
@@ -9277,7 +9277,7 @@
       </c>
       <c r="G40" s="38"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" hidden="1">
       <c r="A41" s="38" t="s">
         <v>58</v>
       </c>
@@ -9296,7 +9296,7 @@
       </c>
       <c r="G41" s="38"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" hidden="1">
       <c r="A42" s="38" t="s">
         <v>131</v>
       </c>
@@ -9315,7 +9315,7 @@
       </c>
       <c r="G42" s="38"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" hidden="1">
       <c r="A43" s="38" t="s">
         <v>58</v>
       </c>
@@ -9330,7 +9330,7 @@
       <c r="F43" s="37"/>
       <c r="G43" s="37"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" hidden="1">
       <c r="A44" s="38" t="s">
         <v>58</v>
       </c>
@@ -9345,7 +9345,7 @@
       <c r="F44" s="37"/>
       <c r="G44" s="37"/>
     </row>
-    <row r="45" spans="1:7" ht="30">
+    <row r="45" spans="1:7" ht="30" hidden="1">
       <c r="A45" s="38" t="s">
         <v>58</v>
       </c>
@@ -9366,7 +9366,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" hidden="1">
       <c r="A46" s="38" t="s">
         <v>58</v>
       </c>
@@ -9385,7 +9385,7 @@
       </c>
       <c r="G46" s="38"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" hidden="1">
       <c r="A47" s="38" t="s">
         <v>58</v>
       </c>
@@ -9404,7 +9404,7 @@
       </c>
       <c r="G47" s="38"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" hidden="1">
       <c r="A48" s="38" t="s">
         <v>58</v>
       </c>
@@ -9423,7 +9423,7 @@
       </c>
       <c r="G48" s="38"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" hidden="1">
       <c r="A49" s="38" t="s">
         <v>58</v>
       </c>
@@ -9442,7 +9442,7 @@
       </c>
       <c r="G49" s="38"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" hidden="1">
       <c r="A50" s="38" t="s">
         <v>58</v>
       </c>
@@ -9461,7 +9461,7 @@
       </c>
       <c r="G50" s="38"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" hidden="1">
       <c r="A51" s="38" t="s">
         <v>58</v>
       </c>
@@ -9480,7 +9480,7 @@
       </c>
       <c r="G51" s="38"/>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" hidden="1">
       <c r="A52" s="38" t="s">
         <v>58</v>
       </c>
@@ -9499,7 +9499,7 @@
       </c>
       <c r="G52" s="38"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" hidden="1">
       <c r="A53" s="38" t="s">
         <v>58</v>
       </c>
@@ -9518,7 +9518,7 @@
       </c>
       <c r="G53" s="38"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" hidden="1">
       <c r="A54" s="38" t="s">
         <v>131</v>
       </c>
@@ -9537,7 +9537,7 @@
       </c>
       <c r="G54" s="38"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" hidden="1">
       <c r="A55" s="38" t="s">
         <v>58</v>
       </c>
@@ -9552,7 +9552,7 @@
       <c r="F55" s="37"/>
       <c r="G55" s="37"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" hidden="1">
       <c r="A56" s="38" t="s">
         <v>58</v>
       </c>
@@ -9567,7 +9567,7 @@
       <c r="F56" s="37"/>
       <c r="G56" s="37"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" hidden="1">
       <c r="A57" s="38" t="s">
         <v>58</v>
       </c>
@@ -9588,7 +9588,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" hidden="1">
       <c r="A58" s="38" t="s">
         <v>58</v>
       </c>
@@ -9607,7 +9607,7 @@
       </c>
       <c r="G58" s="38"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" hidden="1">
       <c r="A59" s="38" t="s">
         <v>58</v>
       </c>
@@ -9626,7 +9626,7 @@
       </c>
       <c r="G59" s="38"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" hidden="1">
       <c r="A60" s="38" t="s">
         <v>58</v>
       </c>
@@ -9645,7 +9645,7 @@
       </c>
       <c r="G60" s="38"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" hidden="1">
       <c r="A61" s="38" t="s">
         <v>58</v>
       </c>
@@ -9664,7 +9664,7 @@
       </c>
       <c r="G61" s="38"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" hidden="1">
       <c r="A62" s="38" t="s">
         <v>58</v>
       </c>
@@ -9683,7 +9683,7 @@
       </c>
       <c r="G62" s="38"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" hidden="1">
       <c r="A63" s="38" t="s">
         <v>58</v>
       </c>
@@ -9702,7 +9702,7 @@
       </c>
       <c r="G63" s="38"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" hidden="1">
       <c r="A64" s="38" t="s">
         <v>58</v>
       </c>
@@ -9721,7 +9721,7 @@
       </c>
       <c r="G64" s="38"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" hidden="1">
       <c r="A65" s="38" t="s">
         <v>58</v>
       </c>
@@ -9740,7 +9740,7 @@
       </c>
       <c r="G65" s="38"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" hidden="1">
       <c r="A66" s="38" t="s">
         <v>58</v>
       </c>
@@ -9755,7 +9755,7 @@
       <c r="F66" s="37"/>
       <c r="G66" s="37"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" hidden="1">
       <c r="A67" s="38" t="s">
         <v>58</v>
       </c>
@@ -9770,7 +9770,7 @@
       <c r="F67" s="37"/>
       <c r="G67" s="37"/>
     </row>
-    <row r="68" spans="1:7" ht="30">
+    <row r="68" spans="1:7" ht="30" hidden="1">
       <c r="A68" s="38" t="s">
         <v>58</v>
       </c>
@@ -9791,7 +9791,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" hidden="1">
       <c r="A69" s="38" t="s">
         <v>58</v>
       </c>
@@ -9810,7 +9810,7 @@
       </c>
       <c r="G69" s="38"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" hidden="1">
       <c r="A70" s="38" t="s">
         <v>58</v>
       </c>
@@ -9829,7 +9829,7 @@
       </c>
       <c r="G70" s="38"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" hidden="1">
       <c r="A71" s="38" t="s">
         <v>58</v>
       </c>
@@ -9848,7 +9848,7 @@
       </c>
       <c r="G71" s="38"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" hidden="1">
       <c r="A72" s="38" t="s">
         <v>58</v>
       </c>
@@ -9867,7 +9867,7 @@
       </c>
       <c r="G72" s="38"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" hidden="1">
       <c r="A73" s="38" t="s">
         <v>58</v>
       </c>
@@ -9886,7 +9886,7 @@
       </c>
       <c r="G73" s="38"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" hidden="1">
       <c r="A74" s="39" t="s">
         <v>58</v>
       </c>
@@ -9905,7 +9905,7 @@
       </c>
       <c r="G74" s="39"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" hidden="1">
       <c r="A75" s="39" t="s">
         <v>58</v>
       </c>
@@ -9924,7 +9924,7 @@
       </c>
       <c r="G75" s="39"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" hidden="1">
       <c r="A76" s="38" t="s">
         <v>58</v>
       </c>
@@ -9943,7 +9943,7 @@
       </c>
       <c r="G76" s="38"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" hidden="1">
       <c r="A77" s="38" t="s">
         <v>58</v>
       </c>
@@ -9962,7 +9962,7 @@
       </c>
       <c r="G77" s="38"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" hidden="1">
       <c r="A78" s="38" t="s">
         <v>58</v>
       </c>
@@ -9981,7 +9981,7 @@
       </c>
       <c r="G78" s="38"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" hidden="1">
       <c r="A79" s="38" t="s">
         <v>131</v>
       </c>
@@ -10000,7 +10000,7 @@
       </c>
       <c r="G79" s="38"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" hidden="1">
       <c r="A80" s="38" t="s">
         <v>58</v>
       </c>
@@ -10015,7 +10015,7 @@
       <c r="F80" s="37"/>
       <c r="G80" s="37"/>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" hidden="1">
       <c r="A81" s="38" t="s">
         <v>58</v>
       </c>
@@ -10030,7 +10030,7 @@
       <c r="F81" s="37"/>
       <c r="G81" s="37"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" hidden="1">
       <c r="A82" s="38" t="s">
         <v>58</v>
       </c>
@@ -10051,7 +10051,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" hidden="1">
       <c r="A83" s="38" t="s">
         <v>58</v>
       </c>
@@ -10070,7 +10070,7 @@
       </c>
       <c r="G83" s="38"/>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" hidden="1">
       <c r="A84" s="38" t="s">
         <v>58</v>
       </c>
@@ -10089,7 +10089,7 @@
       </c>
       <c r="G84" s="38"/>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" hidden="1">
       <c r="A85" s="38" t="s">
         <v>58</v>
       </c>
@@ -10108,7 +10108,7 @@
       </c>
       <c r="G85" s="38"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" hidden="1">
       <c r="A86" s="38" t="s">
         <v>58</v>
       </c>
@@ -10127,7 +10127,7 @@
       </c>
       <c r="G86" s="38"/>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" hidden="1">
       <c r="A87" s="38" t="s">
         <v>58</v>
       </c>
@@ -10146,7 +10146,7 @@
       </c>
       <c r="G87" s="38"/>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" hidden="1">
       <c r="A88" s="38" t="s">
         <v>58</v>
       </c>
@@ -10165,7 +10165,7 @@
       </c>
       <c r="G88" s="38"/>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" hidden="1">
       <c r="A89" s="38" t="s">
         <v>131</v>
       </c>
@@ -10184,7 +10184,7 @@
       </c>
       <c r="G89" s="38"/>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" hidden="1">
       <c r="A90" s="38" t="s">
         <v>58</v>
       </c>
@@ -10199,7 +10199,7 @@
       <c r="F90" s="37"/>
       <c r="G90" s="37"/>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" hidden="1">
       <c r="A91" s="38" t="s">
         <v>58</v>
       </c>
@@ -10214,7 +10214,7 @@
       <c r="F91" s="37"/>
       <c r="G91" s="37"/>
     </row>
-    <row r="92" spans="1:7" ht="30">
+    <row r="92" spans="1:7" ht="30" hidden="1">
       <c r="A92" s="38" t="s">
         <v>58</v>
       </c>
@@ -10235,7 +10235,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" hidden="1">
       <c r="A93" s="38" t="s">
         <v>58</v>
       </c>
@@ -10254,7 +10254,7 @@
       </c>
       <c r="G93" s="38"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" hidden="1">
       <c r="A94" s="38" t="s">
         <v>58</v>
       </c>
@@ -10273,7 +10273,7 @@
       </c>
       <c r="G94" s="38"/>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" hidden="1">
       <c r="A95" s="38" t="s">
         <v>58</v>
       </c>
@@ -10292,7 +10292,7 @@
       </c>
       <c r="G95" s="38"/>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" hidden="1">
       <c r="A96" s="38" t="s">
         <v>58</v>
       </c>
@@ -10311,7 +10311,7 @@
       </c>
       <c r="G96" s="38"/>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" hidden="1">
       <c r="A97" s="38" t="s">
         <v>58</v>
       </c>
@@ -10330,7 +10330,7 @@
       </c>
       <c r="G97" s="38"/>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" hidden="1">
       <c r="A98" s="38" t="s">
         <v>58</v>
       </c>
@@ -10349,7 +10349,7 @@
       </c>
       <c r="G98" s="38"/>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" hidden="1">
       <c r="A99" s="38" t="s">
         <v>58</v>
       </c>
@@ -10368,7 +10368,7 @@
       </c>
       <c r="G99" s="38"/>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" hidden="1">
       <c r="A100" s="38" t="s">
         <v>58</v>
       </c>
@@ -10387,7 +10387,7 @@
       </c>
       <c r="G100" s="38"/>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" hidden="1">
       <c r="A101" s="38" t="s">
         <v>131</v>
       </c>
@@ -10406,7 +10406,7 @@
       </c>
       <c r="G101" s="38"/>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" hidden="1">
       <c r="A102" s="38" t="s">
         <v>58</v>
       </c>
@@ -10421,7 +10421,7 @@
       <c r="F102" s="37"/>
       <c r="G102" s="37"/>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" hidden="1">
       <c r="A103" s="38" t="s">
         <v>58</v>
       </c>
@@ -10436,7 +10436,7 @@
       <c r="F103" s="37"/>
       <c r="G103" s="37"/>
     </row>
-    <row r="104" spans="1:7" ht="30">
+    <row r="104" spans="1:7" ht="30" hidden="1">
       <c r="A104" s="38" t="s">
         <v>58</v>
       </c>
@@ -10457,7 +10457,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" hidden="1">
       <c r="A105" s="38" t="s">
         <v>58</v>
       </c>
@@ -10476,7 +10476,7 @@
       </c>
       <c r="G105" s="38"/>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" hidden="1">
       <c r="A106" s="38" t="s">
         <v>58</v>
       </c>
@@ -10495,7 +10495,7 @@
       </c>
       <c r="G106" s="38"/>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" hidden="1">
       <c r="A107" s="38" t="s">
         <v>58</v>
       </c>
@@ -10514,7 +10514,7 @@
       </c>
       <c r="G107" s="38"/>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" hidden="1">
       <c r="A108" s="38" t="s">
         <v>58</v>
       </c>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="G108" s="38"/>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" hidden="1">
       <c r="A109" s="38" t="s">
         <v>58</v>
       </c>
@@ -10552,7 +10552,7 @@
       </c>
       <c r="G109" s="38"/>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" hidden="1">
       <c r="A110" s="38" t="s">
         <v>58</v>
       </c>
@@ -10571,7 +10571,7 @@
       </c>
       <c r="G110" s="38"/>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" hidden="1">
       <c r="A111" s="38" t="s">
         <v>58</v>
       </c>
@@ -10590,7 +10590,7 @@
       </c>
       <c r="G111" s="38"/>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" hidden="1">
       <c r="A112" s="38" t="s">
         <v>58</v>
       </c>
@@ -10609,7 +10609,7 @@
       </c>
       <c r="G112" s="38"/>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" hidden="1">
       <c r="A113" s="38" t="s">
         <v>131</v>
       </c>
@@ -10628,7 +10628,7 @@
       </c>
       <c r="G113" s="38"/>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" hidden="1">
       <c r="A114" s="38" t="s">
         <v>58</v>
       </c>
@@ -10643,7 +10643,7 @@
       <c r="F114" s="37"/>
       <c r="G114" s="37"/>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" hidden="1">
       <c r="A115" s="38" t="s">
         <v>58</v>
       </c>
@@ -10658,7 +10658,7 @@
       <c r="F115" s="37"/>
       <c r="G115" s="37"/>
     </row>
-    <row r="116" spans="1:7" ht="30">
+    <row r="116" spans="1:7" ht="30" hidden="1">
       <c r="A116" s="38" t="s">
         <v>58</v>
       </c>
@@ -10679,7 +10679,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" hidden="1">
       <c r="A117" s="38" t="s">
         <v>58</v>
       </c>
@@ -10698,7 +10698,7 @@
       </c>
       <c r="G117" s="38"/>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" hidden="1">
       <c r="A118" s="38" t="s">
         <v>58</v>
       </c>
@@ -10717,7 +10717,7 @@
       </c>
       <c r="G118" s="38"/>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" hidden="1">
       <c r="A119" s="38" t="s">
         <v>58</v>
       </c>
@@ -10736,7 +10736,7 @@
       </c>
       <c r="G119" s="38"/>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" hidden="1">
       <c r="A120" s="38" t="s">
         <v>58</v>
       </c>
@@ -10755,7 +10755,7 @@
       </c>
       <c r="G120" s="38"/>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" hidden="1">
       <c r="A121" s="38" t="s">
         <v>58</v>
       </c>
@@ -10774,7 +10774,7 @@
       </c>
       <c r="G121" s="38"/>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" hidden="1">
       <c r="A122" s="38" t="s">
         <v>58</v>
       </c>
@@ -10793,7 +10793,7 @@
       </c>
       <c r="G122" s="38"/>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" hidden="1">
       <c r="A123" s="38" t="s">
         <v>58</v>
       </c>
@@ -10812,7 +10812,7 @@
       </c>
       <c r="G123" s="38"/>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" hidden="1">
       <c r="A124" s="38" t="s">
         <v>58</v>
       </c>
@@ -10831,7 +10831,7 @@
       </c>
       <c r="G124" s="38"/>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" hidden="1">
       <c r="A125" s="38" t="s">
         <v>131</v>
       </c>
@@ -10850,7 +10850,7 @@
       </c>
       <c r="G125" s="38"/>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" hidden="1">
       <c r="A126" s="38" t="s">
         <v>58</v>
       </c>
@@ -10865,7 +10865,7 @@
       <c r="F126" s="37"/>
       <c r="G126" s="37"/>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" hidden="1">
       <c r="A127" s="38" t="s">
         <v>58</v>
       </c>
@@ -10880,7 +10880,7 @@
       <c r="F127" s="37"/>
       <c r="G127" s="37"/>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" hidden="1">
       <c r="A128" s="38" t="s">
         <v>58</v>
       </c>
@@ -10901,7 +10901,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" hidden="1">
       <c r="A129" s="38" t="s">
         <v>58</v>
       </c>
@@ -10920,7 +10920,7 @@
       </c>
       <c r="G129" s="38"/>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" hidden="1">
       <c r="A130" s="38" t="s">
         <v>58</v>
       </c>
@@ -10939,7 +10939,7 @@
       </c>
       <c r="G130" s="38"/>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" hidden="1">
       <c r="A131" s="38" t="s">
         <v>58</v>
       </c>
@@ -10958,7 +10958,7 @@
       </c>
       <c r="G131" s="38"/>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" hidden="1">
       <c r="A132" s="38" t="s">
         <v>58</v>
       </c>
@@ -10977,7 +10977,7 @@
       </c>
       <c r="G132" s="38"/>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" hidden="1">
       <c r="A133" s="38" t="s">
         <v>58</v>
       </c>
@@ -10996,7 +10996,7 @@
       </c>
       <c r="G133" s="38"/>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" hidden="1">
       <c r="A134" s="39" t="s">
         <v>58</v>
       </c>
@@ -11015,7 +11015,7 @@
       </c>
       <c r="G134" s="39"/>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" hidden="1">
       <c r="A135" s="38" t="s">
         <v>58</v>
       </c>
@@ -11034,7 +11034,7 @@
       </c>
       <c r="G135" s="38"/>
     </row>
-    <row r="136" spans="1:7" ht="30">
+    <row r="136" spans="1:7" ht="30" hidden="1">
       <c r="A136" s="38" t="s">
         <v>58</v>
       </c>
@@ -11053,7 +11053,7 @@
       </c>
       <c r="G136" s="38"/>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" hidden="1">
       <c r="A137" s="38" t="s">
         <v>58</v>
       </c>
@@ -11068,7 +11068,7 @@
       <c r="F137" s="37"/>
       <c r="G137" s="37"/>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" hidden="1">
       <c r="A138" s="38" t="s">
         <v>58</v>
       </c>
@@ -11083,7 +11083,7 @@
       <c r="F138" s="37"/>
       <c r="G138" s="37"/>
     </row>
-    <row r="139" spans="1:7" ht="30">
+    <row r="139" spans="1:7" ht="30" hidden="1">
       <c r="A139" s="38" t="s">
         <v>58</v>
       </c>
@@ -11106,7 +11106,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" hidden="1">
       <c r="A140" s="38" t="s">
         <v>58</v>
       </c>
@@ -11127,7 +11127,7 @@
       </c>
       <c r="G140" s="38"/>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" hidden="1">
       <c r="A141" s="38" t="s">
         <v>58</v>
       </c>
@@ -11148,7 +11148,7 @@
       </c>
       <c r="G141" s="38"/>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" hidden="1">
       <c r="A142" s="38" t="s">
         <v>58</v>
       </c>
@@ -11169,7 +11169,7 @@
       </c>
       <c r="G142" s="38"/>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" hidden="1">
       <c r="A143" s="38" t="s">
         <v>58</v>
       </c>
@@ -11190,7 +11190,7 @@
       </c>
       <c r="G143" s="38"/>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" hidden="1">
       <c r="A144" s="38" t="s">
         <v>58</v>
       </c>
@@ -11211,7 +11211,7 @@
       </c>
       <c r="G144" s="38"/>
     </row>
-    <row r="145" spans="1:7" ht="19.5" customHeight="1">
+    <row r="145" spans="1:7" ht="19.5" hidden="1" customHeight="1">
       <c r="A145" s="39" t="s">
         <v>58</v>
       </c>
@@ -11230,7 +11230,7 @@
       </c>
       <c r="G145" s="39"/>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" hidden="1">
       <c r="A146" s="38" t="s">
         <v>58</v>
       </c>
@@ -11251,7 +11251,7 @@
       </c>
       <c r="G146" s="38"/>
     </row>
-    <row r="147" spans="1:7" ht="45">
+    <row r="147" spans="1:7" ht="45" hidden="1">
       <c r="A147" s="38" t="s">
         <v>58</v>
       </c>
@@ -11272,7 +11272,7 @@
       </c>
       <c r="G147" s="38"/>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" hidden="1">
       <c r="A148" s="38" t="s">
         <v>131</v>
       </c>
@@ -11293,7 +11293,7 @@
       </c>
       <c r="G148" s="38"/>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" hidden="1">
       <c r="A149" s="38" t="s">
         <v>131</v>
       </c>
@@ -11312,7 +11312,7 @@
       </c>
       <c r="G149" s="38"/>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" hidden="1">
       <c r="A150" s="38" t="s">
         <v>58</v>
       </c>
@@ -11329,7 +11329,7 @@
       <c r="F150" s="37"/>
       <c r="G150" s="37"/>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" hidden="1">
       <c r="A151" s="38" t="s">
         <v>58</v>
       </c>
@@ -11346,7 +11346,7 @@
       <c r="F151" s="37"/>
       <c r="G151" s="37"/>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" hidden="1">
       <c r="A152" s="38" t="s">
         <v>58</v>
       </c>
@@ -11367,7 +11367,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" hidden="1">
       <c r="A153" s="38" t="s">
         <v>58</v>
       </c>
@@ -11388,7 +11388,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" hidden="1">
       <c r="A154" s="38" t="s">
         <v>58</v>
       </c>
@@ -11409,7 +11409,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" hidden="1">
       <c r="A155" s="38" t="s">
         <v>58</v>
       </c>
@@ -11426,7 +11426,7 @@
       <c r="F155" s="37"/>
       <c r="G155" s="41"/>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" hidden="1">
       <c r="A156" s="38" t="s">
         <v>58</v>
       </c>
@@ -11443,7 +11443,7 @@
       <c r="F156" s="37"/>
       <c r="G156" s="41"/>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" hidden="1">
       <c r="A157" s="38" t="s">
         <v>58</v>
       </c>
@@ -11460,7 +11460,7 @@
       <c r="F157" s="37"/>
       <c r="G157" s="41"/>
     </row>
-    <row r="158" spans="1:7" ht="15.6">
+    <row r="158" spans="1:7" ht="15.6" hidden="1">
       <c r="A158" s="35" t="s">
         <v>58</v>
       </c>
@@ -11475,7 +11475,7 @@
       <c r="F158" s="37"/>
       <c r="G158" s="36"/>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" hidden="1">
       <c r="A159" s="38" t="s">
         <v>58</v>
       </c>
@@ -11490,7 +11490,7 @@
       <c r="F159" s="37"/>
       <c r="G159" s="37"/>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" hidden="1">
       <c r="A160" s="38" t="s">
         <v>58</v>
       </c>
@@ -11505,7 +11505,7 @@
       <c r="F160" s="37"/>
       <c r="G160" s="41"/>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" hidden="1">
       <c r="A161" s="38" t="s">
         <v>58</v>
       </c>
@@ -11524,7 +11524,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" hidden="1">
       <c r="A162" s="38" t="s">
         <v>58</v>
       </c>
@@ -11541,7 +11541,7 @@
       <c r="F162" s="38"/>
       <c r="G162" s="38"/>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" hidden="1">
       <c r="A163" s="38" t="s">
         <v>58</v>
       </c>
@@ -11558,7 +11558,7 @@
       <c r="F163" s="38"/>
       <c r="G163" s="38"/>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" hidden="1">
       <c r="A164" s="38" t="s">
         <v>58</v>
       </c>
@@ -11575,7 +11575,7 @@
       <c r="F164" s="38"/>
       <c r="G164" s="38"/>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" hidden="1">
       <c r="A165" s="38" t="s">
         <v>58</v>
       </c>
@@ -11594,7 +11594,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" hidden="1">
       <c r="A166" s="38" t="s">
         <v>58</v>
       </c>
@@ -11609,7 +11609,7 @@
       <c r="F166" s="41"/>
       <c r="G166" s="41"/>
     </row>
-    <row r="167" spans="1:8" s="70" customFormat="1">
+    <row r="167" spans="1:8" s="70" customFormat="1" hidden="1">
       <c r="A167" s="40" t="s">
         <v>58</v>
       </c>
@@ -11627,7 +11627,7 @@
       <c r="G167" s="40"/>
       <c r="H167" s="69"/>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" hidden="1">
       <c r="A168" s="38" t="s">
         <v>58</v>
       </c>
@@ -11644,7 +11644,7 @@
       <c r="F168" s="38"/>
       <c r="G168" s="38"/>
     </row>
-    <row r="169" spans="1:8" ht="30">
+    <row r="169" spans="1:8" ht="30" hidden="1">
       <c r="A169" s="38" t="s">
         <v>58</v>
       </c>
@@ -11661,7 +11661,7 @@
       <c r="F169" s="38"/>
       <c r="G169" s="38"/>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" hidden="1">
       <c r="A170" s="38" t="s">
         <v>58</v>
       </c>
@@ -11678,7 +11678,7 @@
       <c r="F170" s="40"/>
       <c r="G170" s="38"/>
     </row>
-    <row r="171" spans="1:8" ht="30">
+    <row r="171" spans="1:8" ht="30" hidden="1">
       <c r="A171" s="38" t="s">
         <v>58</v>
       </c>
@@ -11695,7 +11695,7 @@
       <c r="F171" s="40"/>
       <c r="G171" s="38"/>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" hidden="1">
       <c r="A172" s="38" t="s">
         <v>58</v>
       </c>
@@ -11712,7 +11712,7 @@
       <c r="F172" s="40"/>
       <c r="G172" s="38"/>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" hidden="1">
       <c r="A173" s="38" t="s">
         <v>58</v>
       </c>
@@ -11729,7 +11729,7 @@
       <c r="F173" s="40"/>
       <c r="G173" s="38"/>
     </row>
-    <row r="174" spans="1:8" ht="30">
+    <row r="174" spans="1:8" ht="30" hidden="1">
       <c r="A174" s="38" t="s">
         <v>58</v>
       </c>
@@ -11746,7 +11746,7 @@
       <c r="F174" s="40"/>
       <c r="G174" s="38"/>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" hidden="1">
       <c r="A175" s="38" t="s">
         <v>58</v>
       </c>
@@ -11763,7 +11763,7 @@
       <c r="F175" s="40"/>
       <c r="G175" s="38"/>
     </row>
-    <row r="176" spans="1:8" ht="45">
+    <row r="176" spans="1:8" ht="45" hidden="1">
       <c r="A176" s="38" t="s">
         <v>58</v>
       </c>
@@ -11780,7 +11780,7 @@
       <c r="F176" s="38"/>
       <c r="G176" s="38"/>
     </row>
-    <row r="177" spans="1:7" ht="30">
+    <row r="177" spans="1:7" ht="30" hidden="1">
       <c r="A177" s="38" t="s">
         <v>58</v>
       </c>
@@ -11797,7 +11797,7 @@
       <c r="F177" s="38"/>
       <c r="G177" s="38"/>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" hidden="1">
       <c r="A178" s="38" t="s">
         <v>58</v>
       </c>
@@ -11814,7 +11814,7 @@
       <c r="F178" s="38"/>
       <c r="G178" s="38"/>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" hidden="1">
       <c r="A179" s="38" t="s">
         <v>58</v>
       </c>
@@ -11829,7 +11829,7 @@
       <c r="F179" s="41"/>
       <c r="G179" s="42"/>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" hidden="1">
       <c r="A180" s="38" t="s">
         <v>58</v>
       </c>
@@ -11844,7 +11844,7 @@
       <c r="F180" s="41"/>
       <c r="G180" s="41"/>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" hidden="1">
       <c r="A181" s="38" t="s">
         <v>58</v>
       </c>
@@ -11863,7 +11863,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" hidden="1">
       <c r="A182" s="38" t="s">
         <v>58</v>
       </c>
@@ -11880,7 +11880,7 @@
       <c r="F182" s="38"/>
       <c r="G182" s="38"/>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" hidden="1">
       <c r="A183" s="38" t="s">
         <v>58</v>
       </c>
@@ -11897,7 +11897,7 @@
       <c r="F183" s="38"/>
       <c r="G183" s="38"/>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" hidden="1">
       <c r="A184" s="38" t="s">
         <v>58</v>
       </c>
@@ -11914,7 +11914,7 @@
       <c r="F184" s="38"/>
       <c r="G184" s="38"/>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" hidden="1">
       <c r="A185" s="38" t="s">
         <v>58</v>
       </c>
@@ -11929,7 +11929,7 @@
       <c r="F185" s="41"/>
       <c r="G185" s="41"/>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" hidden="1">
       <c r="A186" s="38" t="s">
         <v>58</v>
       </c>
@@ -11948,7 +11948,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" hidden="1">
       <c r="A187" s="38" t="s">
         <v>58</v>
       </c>
@@ -11965,7 +11965,7 @@
       <c r="F187" s="38"/>
       <c r="G187" s="38"/>
     </row>
-    <row r="188" spans="1:7" ht="30">
+    <row r="188" spans="1:7" ht="30" hidden="1">
       <c r="A188" s="38" t="s">
         <v>58</v>
       </c>
@@ -11982,7 +11982,7 @@
       <c r="F188" s="38"/>
       <c r="G188" s="38"/>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" hidden="1">
       <c r="A189" s="38" t="s">
         <v>58</v>
       </c>
@@ -11999,7 +11999,7 @@
       <c r="F189" s="40"/>
       <c r="G189" s="38"/>
     </row>
-    <row r="190" spans="1:7" ht="30">
+    <row r="190" spans="1:7" ht="30" hidden="1">
       <c r="A190" s="38" t="s">
         <v>58</v>
       </c>
@@ -12016,7 +12016,7 @@
       <c r="F190" s="40"/>
       <c r="G190" s="38"/>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" hidden="1">
       <c r="A191" s="38" t="s">
         <v>58</v>
       </c>
@@ -12033,7 +12033,7 @@
       <c r="F191" s="40"/>
       <c r="G191" s="38"/>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" hidden="1">
       <c r="A192" s="38" t="s">
         <v>58</v>
       </c>
@@ -12050,7 +12050,7 @@
       <c r="F192" s="40"/>
       <c r="G192" s="38"/>
     </row>
-    <row r="193" spans="1:7" ht="30">
+    <row r="193" spans="1:7" ht="30" hidden="1">
       <c r="A193" s="38" t="s">
         <v>58</v>
       </c>
@@ -12067,7 +12067,7 @@
       <c r="F193" s="40"/>
       <c r="G193" s="38"/>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" hidden="1">
       <c r="A194" s="38" t="s">
         <v>58</v>
       </c>
@@ -12084,7 +12084,7 @@
       <c r="F194" s="40"/>
       <c r="G194" s="38"/>
     </row>
-    <row r="195" spans="1:7" ht="45">
+    <row r="195" spans="1:7" ht="45" hidden="1">
       <c r="A195" s="38" t="s">
         <v>58</v>
       </c>
@@ -12101,7 +12101,7 @@
       <c r="F195" s="38"/>
       <c r="G195" s="38"/>
     </row>
-    <row r="196" spans="1:7" ht="30">
+    <row r="196" spans="1:7" ht="30" hidden="1">
       <c r="A196" s="38" t="s">
         <v>58</v>
       </c>
@@ -12118,7 +12118,7 @@
       <c r="F196" s="38"/>
       <c r="G196" s="38"/>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" hidden="1">
       <c r="A197" s="38" t="s">
         <v>58</v>
       </c>
@@ -12135,7 +12135,7 @@
       <c r="F197" s="38"/>
       <c r="G197" s="38"/>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:7" hidden="1">
       <c r="A198" s="38" t="s">
         <v>58</v>
       </c>
@@ -12150,7 +12150,7 @@
       <c r="F198" s="41"/>
       <c r="G198" s="41"/>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" hidden="1">
       <c r="A199" s="38" t="s">
         <v>58</v>
       </c>
@@ -12165,7 +12165,7 @@
       <c r="F199" s="41"/>
       <c r="G199" s="41"/>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" hidden="1">
       <c r="A200" s="38" t="s">
         <v>58</v>
       </c>
@@ -12184,7 +12184,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:7" hidden="1">
       <c r="A201" s="38" t="s">
         <v>58</v>
       </c>
@@ -12201,7 +12201,7 @@
       <c r="F201" s="38"/>
       <c r="G201" s="38"/>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:7" hidden="1">
       <c r="A202" s="38" t="s">
         <v>58</v>
       </c>
@@ -12218,7 +12218,7 @@
       <c r="F202" s="38"/>
       <c r="G202" s="38"/>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:7" hidden="1">
       <c r="A203" s="38" t="s">
         <v>58</v>
       </c>
@@ -12235,7 +12235,7 @@
       <c r="F203" s="38"/>
       <c r="G203" s="38"/>
     </row>
-    <row r="204" spans="1:7">
+    <row r="204" spans="1:7" hidden="1">
       <c r="A204" s="38" t="s">
         <v>58</v>
       </c>
@@ -12250,7 +12250,7 @@
       <c r="F204" s="41"/>
       <c r="G204" s="41"/>
     </row>
-    <row r="205" spans="1:7" ht="42" customHeight="1">
+    <row r="205" spans="1:7" ht="42" hidden="1" customHeight="1">
       <c r="A205" s="38" t="s">
         <v>58</v>
       </c>
@@ -12269,7 +12269,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="206" spans="1:7">
+    <row r="206" spans="1:7" hidden="1">
       <c r="A206" s="38" t="s">
         <v>58</v>
       </c>
@@ -12286,7 +12286,7 @@
       <c r="F206" s="38"/>
       <c r="G206" s="38"/>
     </row>
-    <row r="207" spans="1:7" ht="36.75" customHeight="1">
+    <row r="207" spans="1:7" ht="36.75" hidden="1" customHeight="1">
       <c r="A207" s="38" t="s">
         <v>58</v>
       </c>
@@ -12303,7 +12303,7 @@
       <c r="F207" s="38"/>
       <c r="G207" s="38"/>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:7" hidden="1">
       <c r="A208" s="38" t="s">
         <v>58</v>
       </c>
@@ -12320,7 +12320,7 @@
       <c r="F208" s="40"/>
       <c r="G208" s="38"/>
     </row>
-    <row r="209" spans="1:7" ht="30">
+    <row r="209" spans="1:7" ht="30" hidden="1">
       <c r="A209" s="38" t="s">
         <v>58</v>
       </c>
@@ -12337,7 +12337,7 @@
       <c r="F209" s="40"/>
       <c r="G209" s="38"/>
     </row>
-    <row r="210" spans="1:7">
+    <row r="210" spans="1:7" hidden="1">
       <c r="A210" s="38" t="s">
         <v>58</v>
       </c>
@@ -12354,7 +12354,7 @@
       <c r="F210" s="40"/>
       <c r="G210" s="38"/>
     </row>
-    <row r="211" spans="1:7">
+    <row r="211" spans="1:7" hidden="1">
       <c r="A211" s="38" t="s">
         <v>58</v>
       </c>
@@ -12371,7 +12371,7 @@
       <c r="F211" s="40"/>
       <c r="G211" s="38"/>
     </row>
-    <row r="212" spans="1:7" ht="30">
+    <row r="212" spans="1:7" ht="30" hidden="1">
       <c r="A212" s="38" t="s">
         <v>58</v>
       </c>
@@ -12388,7 +12388,7 @@
       <c r="F212" s="40"/>
       <c r="G212" s="38"/>
     </row>
-    <row r="213" spans="1:7">
+    <row r="213" spans="1:7" hidden="1">
       <c r="A213" s="38" t="s">
         <v>58</v>
       </c>
@@ -12405,7 +12405,7 @@
       <c r="F213" s="40"/>
       <c r="G213" s="38"/>
     </row>
-    <row r="214" spans="1:7" ht="45">
+    <row r="214" spans="1:7" ht="45" hidden="1">
       <c r="A214" s="38" t="s">
         <v>58</v>
       </c>
@@ -12422,7 +12422,7 @@
       <c r="F214" s="38"/>
       <c r="G214" s="38"/>
     </row>
-    <row r="215" spans="1:7" ht="30">
+    <row r="215" spans="1:7" ht="30" hidden="1">
       <c r="A215" s="38" t="s">
         <v>58</v>
       </c>
@@ -12439,7 +12439,7 @@
       <c r="F215" s="38"/>
       <c r="G215" s="38"/>
     </row>
-    <row r="216" spans="1:7">
+    <row r="216" spans="1:7" hidden="1">
       <c r="A216" s="38" t="s">
         <v>58</v>
       </c>
@@ -12456,7 +12456,7 @@
       <c r="F216" s="38"/>
       <c r="G216" s="38"/>
     </row>
-    <row r="217" spans="1:7">
+    <row r="217" spans="1:7" hidden="1">
       <c r="A217" s="38" t="s">
         <v>58</v>
       </c>
@@ -12471,7 +12471,7 @@
       <c r="F217" s="41"/>
       <c r="G217" s="43"/>
     </row>
-    <row r="218" spans="1:7">
+    <row r="218" spans="1:7" hidden="1">
       <c r="A218" s="38" t="s">
         <v>58</v>
       </c>
@@ -12486,7 +12486,7 @@
       <c r="F218" s="41"/>
       <c r="G218" s="41"/>
     </row>
-    <row r="219" spans="1:7" ht="30">
+    <row r="219" spans="1:7" ht="30" hidden="1">
       <c r="A219" s="38" t="s">
         <v>58</v>
       </c>
@@ -12505,7 +12505,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="220" spans="1:7">
+    <row r="220" spans="1:7" hidden="1">
       <c r="A220" s="38" t="s">
         <v>58</v>
       </c>
@@ -12522,7 +12522,7 @@
       <c r="F220" s="38"/>
       <c r="G220" s="38"/>
     </row>
-    <row r="221" spans="1:7">
+    <row r="221" spans="1:7" hidden="1">
       <c r="A221" s="38" t="s">
         <v>58</v>
       </c>
@@ -12539,7 +12539,7 @@
       <c r="F221" s="38"/>
       <c r="G221" s="38"/>
     </row>
-    <row r="222" spans="1:7" ht="30">
+    <row r="222" spans="1:7" ht="30" hidden="1">
       <c r="A222" s="38" t="s">
         <v>58</v>
       </c>
@@ -12556,7 +12556,7 @@
       <c r="F222" s="38"/>
       <c r="G222" s="38"/>
     </row>
-    <row r="223" spans="1:7" ht="30">
+    <row r="223" spans="1:7" ht="30" hidden="1">
       <c r="A223" s="38" t="s">
         <v>58</v>
       </c>
@@ -12573,7 +12573,7 @@
       <c r="F223" s="38"/>
       <c r="G223" s="38"/>
     </row>
-    <row r="224" spans="1:7">
+    <row r="224" spans="1:7" hidden="1">
       <c r="A224" s="38" t="s">
         <v>58</v>
       </c>
@@ -12590,7 +12590,7 @@
       <c r="F224" s="40"/>
       <c r="G224" s="38"/>
     </row>
-    <row r="225" spans="1:7">
+    <row r="225" spans="1:7" hidden="1">
       <c r="A225" s="38" t="s">
         <v>58</v>
       </c>
@@ -12607,7 +12607,7 @@
       <c r="F225" s="38"/>
       <c r="G225" s="38"/>
     </row>
-    <row r="226" spans="1:7">
+    <row r="226" spans="1:7" hidden="1">
       <c r="A226" s="38" t="s">
         <v>58</v>
       </c>
@@ -12626,7 +12626,7 @@
       <c r="F226" s="38"/>
       <c r="G226" s="38"/>
     </row>
-    <row r="227" spans="1:7" ht="30">
+    <row r="227" spans="1:7" ht="30" hidden="1">
       <c r="A227" s="38" t="s">
         <v>58</v>
       </c>
@@ -12645,7 +12645,7 @@
       <c r="F227" s="38"/>
       <c r="G227" s="38"/>
     </row>
-    <row r="228" spans="1:7">
+    <row r="228" spans="1:7" hidden="1">
       <c r="A228" s="38" t="s">
         <v>58</v>
       </c>
@@ -12662,7 +12662,7 @@
       <c r="F228" s="38"/>
       <c r="G228" s="38"/>
     </row>
-    <row r="229" spans="1:7">
+    <row r="229" spans="1:7" hidden="1">
       <c r="A229" s="38" t="s">
         <v>58</v>
       </c>
@@ -12679,7 +12679,7 @@
       <c r="F229" s="38"/>
       <c r="G229" s="38"/>
     </row>
-    <row r="230" spans="1:7">
+    <row r="230" spans="1:7" hidden="1">
       <c r="A230" s="38" t="s">
         <v>58</v>
       </c>
@@ -12696,7 +12696,7 @@
       <c r="F230" s="38"/>
       <c r="G230" s="38"/>
     </row>
-    <row r="231" spans="1:7">
+    <row r="231" spans="1:7" hidden="1">
       <c r="A231" s="38" t="s">
         <v>58</v>
       </c>
@@ -12711,7 +12711,7 @@
       <c r="F231" s="41"/>
       <c r="G231" s="41"/>
     </row>
-    <row r="232" spans="1:7">
+    <row r="232" spans="1:7" hidden="1">
       <c r="A232" s="38" t="s">
         <v>58</v>
       </c>
@@ -12730,7 +12730,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="233" spans="1:7">
+    <row r="233" spans="1:7" hidden="1">
       <c r="A233" s="38" t="s">
         <v>58</v>
       </c>
@@ -12747,7 +12747,7 @@
       <c r="F233" s="38"/>
       <c r="G233" s="38"/>
     </row>
-    <row r="234" spans="1:7">
+    <row r="234" spans="1:7" hidden="1">
       <c r="A234" s="38" t="s">
         <v>58</v>
       </c>
@@ -12764,7 +12764,7 @@
       <c r="F234" s="38"/>
       <c r="G234" s="38"/>
     </row>
-    <row r="235" spans="1:7">
+    <row r="235" spans="1:7" hidden="1">
       <c r="A235" s="38" t="s">
         <v>58</v>
       </c>
@@ -12781,7 +12781,7 @@
       <c r="F235" s="38"/>
       <c r="G235" s="38"/>
     </row>
-    <row r="236" spans="1:7">
+    <row r="236" spans="1:7" hidden="1">
       <c r="A236" s="38" t="s">
         <v>58</v>
       </c>
@@ -12800,7 +12800,7 @@
       <c r="F236" s="40"/>
       <c r="G236" s="38"/>
     </row>
-    <row r="237" spans="1:7">
+    <row r="237" spans="1:7" hidden="1">
       <c r="A237" s="38" t="s">
         <v>58</v>
       </c>
@@ -12817,7 +12817,7 @@
       <c r="F237" s="38"/>
       <c r="G237" s="38"/>
     </row>
-    <row r="238" spans="1:7">
+    <row r="238" spans="1:7" hidden="1">
       <c r="A238" s="38" t="s">
         <v>58</v>
       </c>
@@ -12834,7 +12834,7 @@
       <c r="F238" s="38"/>
       <c r="G238" s="38"/>
     </row>
-    <row r="239" spans="1:7">
+    <row r="239" spans="1:7" hidden="1">
       <c r="A239" s="38" t="s">
         <v>58</v>
       </c>
@@ -12851,7 +12851,7 @@
       <c r="F239" s="38"/>
       <c r="G239" s="38"/>
     </row>
-    <row r="240" spans="1:7">
+    <row r="240" spans="1:7" hidden="1">
       <c r="A240" s="38" t="s">
         <v>58</v>
       </c>
@@ -12868,7 +12868,7 @@
       <c r="F240" s="38"/>
       <c r="G240" s="38"/>
     </row>
-    <row r="241" spans="1:7">
+    <row r="241" spans="1:7" hidden="1">
       <c r="A241" s="38" t="s">
         <v>58</v>
       </c>
@@ -12885,7 +12885,7 @@
       <c r="F241" s="38"/>
       <c r="G241" s="38"/>
     </row>
-    <row r="242" spans="1:7">
+    <row r="242" spans="1:7" hidden="1">
       <c r="A242" s="38" t="s">
         <v>58</v>
       </c>
@@ -12902,7 +12902,7 @@
       <c r="F242" s="38"/>
       <c r="G242" s="38"/>
     </row>
-    <row r="243" spans="1:7">
+    <row r="243" spans="1:7" hidden="1">
       <c r="A243" s="38" t="s">
         <v>58</v>
       </c>
@@ -12917,7 +12917,7 @@
       <c r="F243" s="41"/>
       <c r="G243" s="41"/>
     </row>
-    <row r="244" spans="1:7">
+    <row r="244" spans="1:7" hidden="1">
       <c r="A244" s="38" t="s">
         <v>58</v>
       </c>
@@ -12936,7 +12936,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="245" spans="1:7">
+    <row r="245" spans="1:7" hidden="1">
       <c r="A245" s="38" t="s">
         <v>58</v>
       </c>
@@ -12953,7 +12953,7 @@
       <c r="F245" s="38"/>
       <c r="G245" s="38"/>
     </row>
-    <row r="246" spans="1:7">
+    <row r="246" spans="1:7" hidden="1">
       <c r="A246" s="38" t="s">
         <v>58</v>
       </c>
@@ -12968,7 +12968,7 @@
       <c r="F246" s="41"/>
       <c r="G246" s="41"/>
     </row>
-    <row r="247" spans="1:7">
+    <row r="247" spans="1:7" hidden="1">
       <c r="A247" s="38" t="s">
         <v>58</v>
       </c>
@@ -12985,7 +12985,7 @@
       <c r="F247" s="38"/>
       <c r="G247" s="38"/>
     </row>
-    <row r="248" spans="1:7">
+    <row r="248" spans="1:7" hidden="1">
       <c r="A248" s="38" t="s">
         <v>58</v>
       </c>
@@ -13000,7 +13000,7 @@
       <c r="F248" s="38"/>
       <c r="G248" s="43"/>
     </row>
-    <row r="249" spans="1:7">
+    <row r="249" spans="1:7" hidden="1">
       <c r="A249" s="38" t="s">
         <v>58</v>
       </c>
@@ -13017,7 +13017,7 @@
       <c r="F249" s="38"/>
       <c r="G249" s="38"/>
     </row>
-    <row r="250" spans="1:7">
+    <row r="250" spans="1:7" hidden="1">
       <c r="A250" s="38" t="s">
         <v>58</v>
       </c>
@@ -13034,7 +13034,7 @@
       <c r="F250" s="38"/>
       <c r="G250" s="38"/>
     </row>
-    <row r="251" spans="1:7">
+    <row r="251" spans="1:7" hidden="1">
       <c r="A251" s="38" t="s">
         <v>58</v>
       </c>
@@ -13049,7 +13049,7 @@
       <c r="F251" s="41"/>
       <c r="G251" s="41"/>
     </row>
-    <row r="252" spans="1:7">
+    <row r="252" spans="1:7" hidden="1">
       <c r="A252" s="38" t="s">
         <v>58</v>
       </c>
@@ -13066,7 +13066,7 @@
       <c r="F252" s="38"/>
       <c r="G252" s="38"/>
     </row>
-    <row r="253" spans="1:7">
+    <row r="253" spans="1:7" hidden="1">
       <c r="A253" s="38" t="s">
         <v>58</v>
       </c>
@@ -13083,7 +13083,7 @@
       <c r="F253" s="38"/>
       <c r="G253" s="38"/>
     </row>
-    <row r="254" spans="1:7" ht="15.6">
+    <row r="254" spans="1:7" ht="15.6" hidden="1">
       <c r="A254" s="38" t="s">
         <v>58</v>
       </c>
@@ -13098,7 +13098,7 @@
       <c r="F254" s="41"/>
       <c r="G254" s="45"/>
     </row>
-    <row r="255" spans="1:7">
+    <row r="255" spans="1:7" hidden="1">
       <c r="A255" s="38" t="s">
         <v>58</v>
       </c>
@@ -13113,7 +13113,7 @@
       <c r="F255" s="41"/>
       <c r="G255" s="41"/>
     </row>
-    <row r="256" spans="1:7">
+    <row r="256" spans="1:7" hidden="1">
       <c r="A256" s="38" t="s">
         <v>58</v>
       </c>
@@ -13128,7 +13128,7 @@
       <c r="F256" s="41"/>
       <c r="G256" s="41"/>
     </row>
-    <row r="257" spans="1:7" ht="30">
+    <row r="257" spans="1:7" ht="30" hidden="1">
       <c r="A257" s="38" t="s">
         <v>58</v>
       </c>
@@ -13147,7 +13147,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="258" spans="1:7">
+    <row r="258" spans="1:7" hidden="1">
       <c r="A258" s="38" t="s">
         <v>58</v>
       </c>
@@ -13164,7 +13164,7 @@
       <c r="F258" s="38"/>
       <c r="G258" s="44"/>
     </row>
-    <row r="259" spans="1:7">
+    <row r="259" spans="1:7" hidden="1">
       <c r="A259" s="38" t="s">
         <v>58</v>
       </c>
@@ -13183,7 +13183,7 @@
       <c r="F259" s="38"/>
       <c r="G259" s="44"/>
     </row>
-    <row r="260" spans="1:7" ht="30">
+    <row r="260" spans="1:7" ht="30" hidden="1">
       <c r="A260" s="38" t="s">
         <v>58</v>
       </c>
@@ -13200,7 +13200,7 @@
       <c r="F260" s="38"/>
       <c r="G260" s="44"/>
     </row>
-    <row r="261" spans="1:7">
+    <row r="261" spans="1:7" hidden="1">
       <c r="A261" s="38" t="s">
         <v>58</v>
       </c>
@@ -13217,7 +13217,7 @@
       <c r="F261" s="38"/>
       <c r="G261" s="44"/>
     </row>
-    <row r="262" spans="1:7">
+    <row r="262" spans="1:7" hidden="1">
       <c r="A262" s="38" t="s">
         <v>58</v>
       </c>
@@ -13234,7 +13234,7 @@
       <c r="F262" s="38"/>
       <c r="G262" s="44"/>
     </row>
-    <row r="263" spans="1:7" ht="30">
+    <row r="263" spans="1:7" ht="30" hidden="1">
       <c r="A263" s="38" t="s">
         <v>58</v>
       </c>
@@ -13251,7 +13251,7 @@
       <c r="F263" s="38"/>
       <c r="G263" s="44"/>
     </row>
-    <row r="264" spans="1:7">
+    <row r="264" spans="1:7" hidden="1">
       <c r="A264" s="38" t="s">
         <v>58</v>
       </c>
@@ -13270,7 +13270,7 @@
       <c r="F264" s="38"/>
       <c r="G264" s="44"/>
     </row>
-    <row r="265" spans="1:7" ht="30">
+    <row r="265" spans="1:7" ht="30" hidden="1">
       <c r="A265" s="38" t="s">
         <v>58</v>
       </c>
@@ -13287,7 +13287,7 @@
       <c r="F265" s="38"/>
       <c r="G265" s="44"/>
     </row>
-    <row r="266" spans="1:7" ht="45">
+    <row r="266" spans="1:7" ht="45" hidden="1">
       <c r="A266" s="38" t="s">
         <v>58</v>
       </c>
@@ -13304,7 +13304,7 @@
       <c r="F266" s="38"/>
       <c r="G266" s="44"/>
     </row>
-    <row r="267" spans="1:7" ht="30">
+    <row r="267" spans="1:7" ht="30" hidden="1">
       <c r="A267" s="38" t="s">
         <v>58</v>
       </c>
@@ -13321,7 +13321,7 @@
       <c r="F267" s="38"/>
       <c r="G267" s="44"/>
     </row>
-    <row r="268" spans="1:7" ht="45">
+    <row r="268" spans="1:7" ht="45" hidden="1">
       <c r="A268" s="38" t="s">
         <v>58</v>
       </c>
@@ -13340,7 +13340,7 @@
       <c r="F268" s="38"/>
       <c r="G268" s="44"/>
     </row>
-    <row r="269" spans="1:7">
+    <row r="269" spans="1:7" hidden="1">
       <c r="A269" s="38" t="s">
         <v>58</v>
       </c>
@@ -13357,7 +13357,7 @@
       <c r="F269" s="38"/>
       <c r="G269" s="44"/>
     </row>
-    <row r="270" spans="1:7">
+    <row r="270" spans="1:7" hidden="1">
       <c r="A270" s="38" t="s">
         <v>58</v>
       </c>
@@ -13372,7 +13372,7 @@
       <c r="F270" s="41"/>
       <c r="G270" s="41"/>
     </row>
-    <row r="271" spans="1:7">
+    <row r="271" spans="1:7" hidden="1">
       <c r="A271" s="38" t="s">
         <v>58</v>
       </c>
@@ -13387,7 +13387,7 @@
       <c r="F271" s="41"/>
       <c r="G271" s="41"/>
     </row>
-    <row r="272" spans="1:7" ht="30">
+    <row r="272" spans="1:7" ht="30" hidden="1">
       <c r="A272" s="38" t="s">
         <v>58</v>
       </c>
@@ -13406,7 +13406,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="273" spans="1:7">
+    <row r="273" spans="1:7" hidden="1">
       <c r="A273" s="38" t="s">
         <v>58</v>
       </c>
@@ -13423,7 +13423,7 @@
       <c r="F273" s="38"/>
       <c r="G273" s="44"/>
     </row>
-    <row r="274" spans="1:7">
+    <row r="274" spans="1:7" hidden="1">
       <c r="A274" s="38" t="s">
         <v>58</v>
       </c>
@@ -13440,7 +13440,7 @@
       <c r="F274" s="38"/>
       <c r="G274" s="44"/>
     </row>
-    <row r="275" spans="1:7" ht="30">
+    <row r="275" spans="1:7" ht="30" hidden="1">
       <c r="A275" s="38" t="s">
         <v>58</v>
       </c>
@@ -13457,7 +13457,7 @@
       <c r="F275" s="38"/>
       <c r="G275" s="44"/>
     </row>
-    <row r="276" spans="1:7">
+    <row r="276" spans="1:7" hidden="1">
       <c r="A276" s="38" t="s">
         <v>58</v>
       </c>
@@ -13474,7 +13474,7 @@
       <c r="F276" s="38"/>
       <c r="G276" s="44"/>
     </row>
-    <row r="277" spans="1:7">
+    <row r="277" spans="1:7" hidden="1">
       <c r="A277" s="38" t="s">
         <v>58</v>
       </c>
@@ -13491,7 +13491,7 @@
       <c r="F277" s="38"/>
       <c r="G277" s="44"/>
     </row>
-    <row r="278" spans="1:7">
+    <row r="278" spans="1:7" hidden="1">
       <c r="A278" s="38" t="s">
         <v>58</v>
       </c>
@@ -13508,7 +13508,7 @@
       <c r="F278" s="38"/>
       <c r="G278" s="44"/>
     </row>
-    <row r="279" spans="1:7" ht="30">
+    <row r="279" spans="1:7" ht="30" hidden="1">
       <c r="A279" s="38" t="s">
         <v>58</v>
       </c>
@@ -13525,7 +13525,7 @@
       <c r="F279" s="38"/>
       <c r="G279" s="44"/>
     </row>
-    <row r="280" spans="1:7">
+    <row r="280" spans="1:7" hidden="1">
       <c r="A280" s="38" t="s">
         <v>58</v>
       </c>
@@ -13542,7 +13542,7 @@
       <c r="F280" s="38"/>
       <c r="G280" s="44"/>
     </row>
-    <row r="281" spans="1:7" ht="30">
+    <row r="281" spans="1:7" ht="30" hidden="1">
       <c r="A281" s="38" t="s">
         <v>58</v>
       </c>
@@ -13559,7 +13559,7 @@
       <c r="F281" s="38"/>
       <c r="G281" s="44"/>
     </row>
-    <row r="282" spans="1:7" ht="30">
+    <row r="282" spans="1:7" ht="30" hidden="1">
       <c r="A282" s="38" t="s">
         <v>58</v>
       </c>
@@ -13576,7 +13576,7 @@
       <c r="F282" s="38"/>
       <c r="G282" s="44"/>
     </row>
-    <row r="283" spans="1:7" ht="30">
+    <row r="283" spans="1:7" ht="30" hidden="1">
       <c r="A283" s="38" t="s">
         <v>58</v>
       </c>
@@ -13593,7 +13593,7 @@
       <c r="F283" s="38"/>
       <c r="G283" s="38"/>
     </row>
-    <row r="284" spans="1:7" ht="45">
+    <row r="284" spans="1:7" ht="45" hidden="1">
       <c r="A284" s="38" t="s">
         <v>58</v>
       </c>
@@ -13610,7 +13610,7 @@
       <c r="F284" s="38"/>
       <c r="G284" s="44"/>
     </row>
-    <row r="285" spans="1:7" ht="45">
+    <row r="285" spans="1:7" ht="45" hidden="1">
       <c r="A285" s="38" t="s">
         <v>58</v>
       </c>
@@ -13627,7 +13627,7 @@
       <c r="F285" s="38"/>
       <c r="G285" s="38"/>
     </row>
-    <row r="286" spans="1:7" ht="45">
+    <row r="286" spans="1:7" ht="45" hidden="1">
       <c r="A286" s="38" t="s">
         <v>58</v>
       </c>
@@ -13644,7 +13644,7 @@
       <c r="F286" s="38"/>
       <c r="G286" s="44"/>
     </row>
-    <row r="287" spans="1:7" ht="30">
+    <row r="287" spans="1:7" ht="30" hidden="1">
       <c r="A287" s="38" t="s">
         <v>58</v>
       </c>
@@ -13663,7 +13663,7 @@
       </c>
       <c r="G287" s="44"/>
     </row>
-    <row r="288" spans="1:7">
+    <row r="288" spans="1:7" hidden="1">
       <c r="A288" s="38" t="s">
         <v>58</v>
       </c>
@@ -13678,7 +13678,7 @@
       <c r="F288" s="41"/>
       <c r="G288" s="41"/>
     </row>
-    <row r="289" spans="1:7">
+    <row r="289" spans="1:7" hidden="1">
       <c r="A289" s="38" t="s">
         <v>58</v>
       </c>
@@ -13693,7 +13693,7 @@
       <c r="F289" s="41"/>
       <c r="G289" s="41"/>
     </row>
-    <row r="290" spans="1:7" ht="30">
+    <row r="290" spans="1:7" ht="30" hidden="1">
       <c r="A290" s="38" t="s">
         <v>58</v>
       </c>
@@ -13712,7 +13712,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="291" spans="1:7">
+    <row r="291" spans="1:7" hidden="1">
       <c r="A291" s="38" t="s">
         <v>58</v>
       </c>
@@ -13729,7 +13729,7 @@
       <c r="F291" s="38"/>
       <c r="G291" s="44"/>
     </row>
-    <row r="292" spans="1:7">
+    <row r="292" spans="1:7" hidden="1">
       <c r="A292" s="38" t="s">
         <v>58</v>
       </c>
@@ -13746,7 +13746,7 @@
       <c r="F292" s="38"/>
       <c r="G292" s="44"/>
     </row>
-    <row r="293" spans="1:7" ht="30">
+    <row r="293" spans="1:7" ht="30" hidden="1">
       <c r="A293" s="38" t="s">
         <v>58</v>
       </c>
@@ -13763,7 +13763,7 @@
       <c r="F293" s="38"/>
       <c r="G293" s="44"/>
     </row>
-    <row r="294" spans="1:7">
+    <row r="294" spans="1:7" hidden="1">
       <c r="A294" s="38" t="s">
         <v>58</v>
       </c>
@@ -13780,7 +13780,7 @@
       <c r="F294" s="38"/>
       <c r="G294" s="44"/>
     </row>
-    <row r="295" spans="1:7">
+    <row r="295" spans="1:7" hidden="1">
       <c r="A295" s="38" t="s">
         <v>58</v>
       </c>
@@ -13797,7 +13797,7 @@
       <c r="F295" s="38"/>
       <c r="G295" s="44"/>
     </row>
-    <row r="296" spans="1:7">
+    <row r="296" spans="1:7" hidden="1">
       <c r="A296" s="38" t="s">
         <v>58</v>
       </c>
@@ -13814,7 +13814,7 @@
       <c r="F296" s="38"/>
       <c r="G296" s="44"/>
     </row>
-    <row r="297" spans="1:7" ht="30">
+    <row r="297" spans="1:7" ht="30" hidden="1">
       <c r="A297" s="38" t="s">
         <v>58</v>
       </c>
@@ -13831,7 +13831,7 @@
       <c r="F297" s="38"/>
       <c r="G297" s="44"/>
     </row>
-    <row r="298" spans="1:7">
+    <row r="298" spans="1:7" hidden="1">
       <c r="A298" s="38" t="s">
         <v>58</v>
       </c>
@@ -13848,7 +13848,7 @@
       <c r="F298" s="38"/>
       <c r="G298" s="44"/>
     </row>
-    <row r="299" spans="1:7" ht="30">
+    <row r="299" spans="1:7" ht="30" hidden="1">
       <c r="A299" s="38" t="s">
         <v>58</v>
       </c>
@@ -13865,7 +13865,7 @@
       <c r="F299" s="38"/>
       <c r="G299" s="44"/>
     </row>
-    <row r="300" spans="1:7" ht="30">
+    <row r="300" spans="1:7" ht="30" hidden="1">
       <c r="A300" s="38" t="s">
         <v>58</v>
       </c>
@@ -13882,7 +13882,7 @@
       <c r="F300" s="38"/>
       <c r="G300" s="44"/>
     </row>
-    <row r="301" spans="1:7" ht="30">
+    <row r="301" spans="1:7" ht="30" hidden="1">
       <c r="A301" s="38" t="s">
         <v>58</v>
       </c>
@@ -13899,7 +13899,7 @@
       <c r="F301" s="38"/>
       <c r="G301" s="38"/>
     </row>
-    <row r="302" spans="1:7" ht="45">
+    <row r="302" spans="1:7" ht="45" hidden="1">
       <c r="A302" s="38" t="s">
         <v>58</v>
       </c>
@@ -13916,7 +13916,7 @@
       <c r="F302" s="38"/>
       <c r="G302" s="44"/>
     </row>
-    <row r="303" spans="1:7" ht="45">
+    <row r="303" spans="1:7" ht="45" hidden="1">
       <c r="A303" s="38" t="s">
         <v>58</v>
       </c>
@@ -13933,7 +13933,7 @@
       <c r="F303" s="38"/>
       <c r="G303" s="38"/>
     </row>
-    <row r="304" spans="1:7" ht="45">
+    <row r="304" spans="1:7" ht="45" hidden="1">
       <c r="A304" s="38" t="s">
         <v>58</v>
       </c>
@@ -13950,7 +13950,7 @@
       <c r="F304" s="38"/>
       <c r="G304" s="44"/>
     </row>
-    <row r="305" spans="1:7" ht="30">
+    <row r="305" spans="1:7" ht="30" hidden="1">
       <c r="A305" s="38" t="s">
         <v>58</v>
       </c>
@@ -13969,7 +13969,7 @@
       </c>
       <c r="G305" s="44"/>
     </row>
-    <row r="306" spans="1:7">
+    <row r="306" spans="1:7" hidden="1">
       <c r="A306" s="38" t="s">
         <v>58</v>
       </c>
@@ -13984,7 +13984,7 @@
       <c r="F306" s="41"/>
       <c r="G306" s="41"/>
     </row>
-    <row r="307" spans="1:7">
+    <row r="307" spans="1:7" hidden="1">
       <c r="A307" s="38" t="s">
         <v>58</v>
       </c>
@@ -13999,7 +13999,7 @@
       <c r="F307" s="41"/>
       <c r="G307" s="41"/>
     </row>
-    <row r="308" spans="1:7" ht="30">
+    <row r="308" spans="1:7" ht="30" hidden="1">
       <c r="A308" s="38" t="s">
         <v>58</v>
       </c>
@@ -14016,7 +14016,7 @@
       <c r="F308" s="38"/>
       <c r="G308" s="44"/>
     </row>
-    <row r="309" spans="1:7">
+    <row r="309" spans="1:7" hidden="1">
       <c r="A309" s="38" t="s">
         <v>58</v>
       </c>
@@ -14031,7 +14031,7 @@
       <c r="F309" s="41"/>
       <c r="G309" s="41"/>
     </row>
-    <row r="310" spans="1:7" ht="30">
+    <row r="310" spans="1:7" ht="30" hidden="1">
       <c r="A310" s="38" t="s">
         <v>58</v>
       </c>
@@ -14050,7 +14050,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="311" spans="1:7">
+    <row r="311" spans="1:7" hidden="1">
       <c r="A311" s="38" t="s">
         <v>58</v>
       </c>
@@ -14067,7 +14067,7 @@
       <c r="F311" s="38"/>
       <c r="G311" s="44"/>
     </row>
-    <row r="312" spans="1:7">
+    <row r="312" spans="1:7" hidden="1">
       <c r="A312" s="38" t="s">
         <v>58</v>
       </c>
@@ -14084,7 +14084,7 @@
       <c r="F312" s="38"/>
       <c r="G312" s="44"/>
     </row>
-    <row r="313" spans="1:7" ht="30">
+    <row r="313" spans="1:7" ht="30" hidden="1">
       <c r="A313" s="38" t="s">
         <v>58</v>
       </c>
@@ -14101,7 +14101,7 @@
       <c r="F313" s="38"/>
       <c r="G313" s="44"/>
     </row>
-    <row r="314" spans="1:7">
+    <row r="314" spans="1:7" hidden="1">
       <c r="A314" s="38" t="s">
         <v>58</v>
       </c>
@@ -14118,7 +14118,7 @@
       <c r="F314" s="38"/>
       <c r="G314" s="44"/>
     </row>
-    <row r="315" spans="1:7">
+    <row r="315" spans="1:7" hidden="1">
       <c r="A315" s="38" t="s">
         <v>58</v>
       </c>
@@ -14135,7 +14135,7 @@
       <c r="F315" s="38"/>
       <c r="G315" s="44"/>
     </row>
-    <row r="316" spans="1:7" ht="45">
+    <row r="316" spans="1:7" ht="45" hidden="1">
       <c r="A316" s="38" t="s">
         <v>58</v>
       </c>
@@ -14152,7 +14152,7 @@
       <c r="F316" s="38"/>
       <c r="G316" s="44"/>
     </row>
-    <row r="317" spans="1:7">
+    <row r="317" spans="1:7" hidden="1">
       <c r="A317" s="38" t="s">
         <v>58</v>
       </c>
@@ -14167,7 +14167,7 @@
       <c r="F317" s="41"/>
       <c r="G317" s="48"/>
     </row>
-    <row r="318" spans="1:7">
+    <row r="318" spans="1:7" hidden="1">
       <c r="A318" s="38" t="s">
         <v>58</v>
       </c>
@@ -14182,7 +14182,7 @@
       <c r="F318" s="41"/>
       <c r="G318" s="48"/>
     </row>
-    <row r="319" spans="1:7" ht="30">
+    <row r="319" spans="1:7" ht="30" hidden="1">
       <c r="A319" s="38" t="s">
         <v>58</v>
       </c>
@@ -14201,7 +14201,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="320" spans="1:7">
+    <row r="320" spans="1:7" hidden="1">
       <c r="A320" s="38" t="s">
         <v>58</v>
       </c>
@@ -14218,7 +14218,7 @@
       <c r="F320" s="38"/>
       <c r="G320" s="38"/>
     </row>
-    <row r="321" spans="1:7">
+    <row r="321" spans="1:7" hidden="1">
       <c r="A321" s="38" t="s">
         <v>58</v>
       </c>
@@ -14235,7 +14235,7 @@
       <c r="F321" s="38"/>
       <c r="G321" s="38"/>
     </row>
-    <row r="322" spans="1:7" ht="30">
+    <row r="322" spans="1:7" ht="30" hidden="1">
       <c r="A322" s="38" t="s">
         <v>58</v>
       </c>
@@ -14252,7 +14252,7 @@
       <c r="F322" s="38"/>
       <c r="G322" s="38"/>
     </row>
-    <row r="323" spans="1:7">
+    <row r="323" spans="1:7" hidden="1">
       <c r="A323" s="38" t="s">
         <v>58</v>
       </c>
@@ -14269,7 +14269,7 @@
       <c r="F323" s="38"/>
       <c r="G323" s="38"/>
     </row>
-    <row r="324" spans="1:7">
+    <row r="324" spans="1:7" hidden="1">
       <c r="A324" s="38" t="s">
         <v>58</v>
       </c>
@@ -14286,7 +14286,7 @@
       <c r="F324" s="38"/>
       <c r="G324" s="38"/>
     </row>
-    <row r="325" spans="1:7">
+    <row r="325" spans="1:7" hidden="1">
       <c r="A325" s="38" t="s">
         <v>58</v>
       </c>
@@ -14303,7 +14303,7 @@
       <c r="F325" s="38"/>
       <c r="G325" s="38"/>
     </row>
-    <row r="326" spans="1:7" ht="30">
+    <row r="326" spans="1:7" ht="30" hidden="1">
       <c r="A326" s="38" t="s">
         <v>58</v>
       </c>
@@ -14320,7 +14320,7 @@
       <c r="F326" s="38"/>
       <c r="G326" s="38"/>
     </row>
-    <row r="327" spans="1:7">
+    <row r="327" spans="1:7" hidden="1">
       <c r="A327" s="38" t="s">
         <v>58</v>
       </c>
@@ -14337,7 +14337,7 @@
       <c r="F327" s="38"/>
       <c r="G327" s="38"/>
     </row>
-    <row r="328" spans="1:7" ht="30">
+    <row r="328" spans="1:7" ht="30" hidden="1">
       <c r="A328" s="38" t="s">
         <v>58</v>
       </c>
@@ -14354,7 +14354,7 @@
       <c r="F328" s="38"/>
       <c r="G328" s="38"/>
     </row>
-    <row r="329" spans="1:7" ht="30">
+    <row r="329" spans="1:7" ht="30" hidden="1">
       <c r="A329" s="38" t="s">
         <v>58</v>
       </c>
@@ -14371,7 +14371,7 @@
       <c r="F329" s="38"/>
       <c r="G329" s="38"/>
     </row>
-    <row r="330" spans="1:7" ht="30">
+    <row r="330" spans="1:7" ht="30" hidden="1">
       <c r="A330" s="38" t="s">
         <v>58</v>
       </c>
@@ -14388,7 +14388,7 @@
       <c r="F330" s="38"/>
       <c r="G330" s="38"/>
     </row>
-    <row r="331" spans="1:7" ht="45">
+    <row r="331" spans="1:7" ht="45" hidden="1">
       <c r="A331" s="38" t="s">
         <v>58</v>
       </c>
@@ -14405,7 +14405,7 @@
       <c r="F331" s="38"/>
       <c r="G331" s="38"/>
     </row>
-    <row r="332" spans="1:7" ht="45">
+    <row r="332" spans="1:7" ht="45" hidden="1">
       <c r="A332" s="38" t="s">
         <v>58</v>
       </c>
@@ -14422,7 +14422,7 @@
       <c r="F332" s="38"/>
       <c r="G332" s="38"/>
     </row>
-    <row r="333" spans="1:7" ht="45">
+    <row r="333" spans="1:7" ht="45" hidden="1">
       <c r="A333" s="38" t="s">
         <v>58</v>
       </c>
@@ -14441,7 +14441,7 @@
       </c>
       <c r="G333" s="38"/>
     </row>
-    <row r="334" spans="1:7" ht="30">
+    <row r="334" spans="1:7" ht="30" hidden="1">
       <c r="A334" s="38" t="s">
         <v>58</v>
       </c>
@@ -14460,7 +14460,7 @@
       </c>
       <c r="G334" s="38"/>
     </row>
-    <row r="335" spans="1:7" ht="15.6">
+    <row r="335" spans="1:7" ht="15.6" hidden="1">
       <c r="A335" s="38" t="s">
         <v>58</v>
       </c>
@@ -14475,7 +14475,7 @@
       <c r="F335" s="41"/>
       <c r="G335" s="49"/>
     </row>
-    <row r="336" spans="1:7">
+    <row r="336" spans="1:7" hidden="1">
       <c r="A336" s="38" t="s">
         <v>58</v>
       </c>
@@ -14490,7 +14490,7 @@
       <c r="F336" s="41"/>
       <c r="G336" s="48"/>
     </row>
-    <row r="337" spans="1:7">
+    <row r="337" spans="1:7" hidden="1">
       <c r="A337" s="38" t="s">
         <v>58</v>
       </c>
@@ -14505,7 +14505,7 @@
       <c r="F337" s="41"/>
       <c r="G337" s="48"/>
     </row>
-    <row r="338" spans="1:7" ht="60">
+    <row r="338" spans="1:7" ht="60" hidden="1">
       <c r="A338" s="38" t="s">
         <v>58</v>
       </c>
@@ -14528,7 +14528,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="339" spans="1:7">
+    <row r="339" spans="1:7" hidden="1">
       <c r="A339" s="38" t="s">
         <v>58</v>
       </c>
@@ -14549,7 +14549,7 @@
       </c>
       <c r="G339" s="44"/>
     </row>
-    <row r="340" spans="1:7">
+    <row r="340" spans="1:7" hidden="1">
       <c r="A340" s="38" t="s">
         <v>58</v>
       </c>
@@ -14568,7 +14568,7 @@
       </c>
       <c r="G340" s="44"/>
     </row>
-    <row r="341" spans="1:7">
+    <row r="341" spans="1:7" hidden="1">
       <c r="A341" s="38" t="s">
         <v>58</v>
       </c>
@@ -14583,7 +14583,7 @@
       <c r="F341" s="41"/>
       <c r="G341" s="41"/>
     </row>
-    <row r="342" spans="1:7">
+    <row r="342" spans="1:7" hidden="1">
       <c r="A342" s="38" t="s">
         <v>58</v>
       </c>
@@ -14604,7 +14604,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="343" spans="1:7">
+    <row r="343" spans="1:7" hidden="1">
       <c r="A343" s="38" t="s">
         <v>58</v>
       </c>
@@ -14623,7 +14623,7 @@
       </c>
       <c r="G343" s="44"/>
     </row>
-    <row r="344" spans="1:7">
+    <row r="344" spans="1:7" hidden="1">
       <c r="A344" s="38" t="s">
         <v>58</v>
       </c>
@@ -14642,7 +14642,7 @@
       </c>
       <c r="G344" s="38"/>
     </row>
-    <row r="345" spans="1:7">
+    <row r="345" spans="1:7" hidden="1">
       <c r="A345" s="38" t="s">
         <v>58</v>
       </c>
@@ -14661,7 +14661,7 @@
       </c>
       <c r="G345" s="44"/>
     </row>
-    <row r="346" spans="1:7">
+    <row r="346" spans="1:7" hidden="1">
       <c r="A346" s="38" t="s">
         <v>58</v>
       </c>
@@ -14676,7 +14676,7 @@
       <c r="F346" s="41"/>
       <c r="G346" s="41"/>
     </row>
-    <row r="347" spans="1:7">
+    <row r="347" spans="1:7" hidden="1">
       <c r="A347" s="38" t="s">
         <v>58</v>
       </c>
@@ -14697,7 +14697,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="348" spans="1:7">
+    <row r="348" spans="1:7" hidden="1">
       <c r="A348" s="38" t="s">
         <v>58</v>
       </c>
@@ -14716,7 +14716,7 @@
       </c>
       <c r="G348" s="44"/>
     </row>
-    <row r="349" spans="1:7">
+    <row r="349" spans="1:7" hidden="1">
       <c r="A349" s="38" t="s">
         <v>58</v>
       </c>
@@ -14735,7 +14735,7 @@
       </c>
       <c r="G349" s="44"/>
     </row>
-    <row r="350" spans="1:7">
+    <row r="350" spans="1:7" hidden="1">
       <c r="A350" s="38" t="s">
         <v>58</v>
       </c>
@@ -14754,7 +14754,7 @@
       </c>
       <c r="G350" s="44"/>
     </row>
-    <row r="351" spans="1:7">
+    <row r="351" spans="1:7" hidden="1">
       <c r="A351" s="38" t="s">
         <v>58</v>
       </c>
@@ -14773,7 +14773,7 @@
       </c>
       <c r="G351" s="44"/>
     </row>
-    <row r="352" spans="1:7">
+    <row r="352" spans="1:7" hidden="1">
       <c r="A352" s="38" t="s">
         <v>58</v>
       </c>
@@ -14788,7 +14788,7 @@
       <c r="F352" s="41"/>
       <c r="G352" s="41"/>
     </row>
-    <row r="353" spans="1:7" ht="45">
+    <row r="353" spans="1:7" ht="45" hidden="1">
       <c r="A353" s="38" t="s">
         <v>58</v>
       </c>
@@ -14809,7 +14809,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="354" spans="1:7" ht="30">
+    <row r="354" spans="1:7" ht="30" hidden="1">
       <c r="A354" s="38" t="s">
         <v>58</v>
       </c>
@@ -14828,7 +14828,7 @@
       </c>
       <c r="G354" s="44"/>
     </row>
-    <row r="355" spans="1:7" ht="37.5" customHeight="1">
+    <row r="355" spans="1:7" ht="37.5" hidden="1" customHeight="1">
       <c r="A355" s="38" t="s">
         <v>58</v>
       </c>
@@ -14847,7 +14847,7 @@
       </c>
       <c r="G355" s="38"/>
     </row>
-    <row r="356" spans="1:7" ht="30">
+    <row r="356" spans="1:7" ht="30" hidden="1">
       <c r="A356" s="38" t="s">
         <v>58</v>
       </c>
@@ -14866,7 +14866,7 @@
       </c>
       <c r="G356" s="44"/>
     </row>
-    <row r="357" spans="1:7">
+    <row r="357" spans="1:7" hidden="1">
       <c r="A357" s="38" t="s">
         <v>58</v>
       </c>
@@ -14885,7 +14885,7 @@
       </c>
       <c r="G357" s="44"/>
     </row>
-    <row r="358" spans="1:7">
+    <row r="358" spans="1:7" hidden="1">
       <c r="A358" s="38" t="s">
         <v>58</v>
       </c>
@@ -14900,7 +14900,7 @@
       <c r="F358" s="41"/>
       <c r="G358" s="41"/>
     </row>
-    <row r="359" spans="1:7">
+    <row r="359" spans="1:7" hidden="1">
       <c r="A359" s="38" t="s">
         <v>58</v>
       </c>
@@ -14921,7 +14921,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="360" spans="1:7">
+    <row r="360" spans="1:7" hidden="1">
       <c r="A360" s="38" t="s">
         <v>58</v>
       </c>
@@ -14940,7 +14940,7 @@
       </c>
       <c r="G360" s="38"/>
     </row>
-    <row r="361" spans="1:7">
+    <row r="361" spans="1:7" hidden="1">
       <c r="A361" s="38" t="s">
         <v>58</v>
       </c>
@@ -14955,7 +14955,7 @@
       <c r="F361" s="41"/>
       <c r="G361" s="41"/>
     </row>
-    <row r="362" spans="1:7">
+    <row r="362" spans="1:7" hidden="1">
       <c r="A362" s="38" t="s">
         <v>58</v>
       </c>
@@ -14976,7 +14976,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="363" spans="1:7">
+    <row r="363" spans="1:7" hidden="1">
       <c r="A363" s="38" t="s">
         <v>58</v>
       </c>
@@ -14995,7 +14995,7 @@
       </c>
       <c r="G363" s="44"/>
     </row>
-    <row r="364" spans="1:7">
+    <row r="364" spans="1:7" hidden="1">
       <c r="A364" s="38" t="s">
         <v>58</v>
       </c>
@@ -15014,7 +15014,7 @@
       </c>
       <c r="G364" s="44"/>
     </row>
-    <row r="365" spans="1:7">
+    <row r="365" spans="1:7" hidden="1">
       <c r="A365" s="38" t="s">
         <v>58</v>
       </c>
@@ -15033,7 +15033,7 @@
       </c>
       <c r="G365" s="44"/>
     </row>
-    <row r="366" spans="1:7">
+    <row r="366" spans="1:7" hidden="1">
       <c r="A366" s="38" t="s">
         <v>58</v>
       </c>
@@ -15054,7 +15054,7 @@
       </c>
       <c r="G366" s="38"/>
     </row>
-    <row r="367" spans="1:7">
+    <row r="367" spans="1:7" hidden="1">
       <c r="A367" s="38" t="s">
         <v>58</v>
       </c>
@@ -15069,7 +15069,7 @@
       <c r="F367" s="41"/>
       <c r="G367" s="41"/>
     </row>
-    <row r="368" spans="1:7">
+    <row r="368" spans="1:7" hidden="1">
       <c r="A368" s="38" t="s">
         <v>58</v>
       </c>
@@ -15084,7 +15084,7 @@
       <c r="F368" s="41"/>
       <c r="G368" s="41"/>
     </row>
-    <row r="369" spans="1:7" ht="60">
+    <row r="369" spans="1:7" ht="60" hidden="1">
       <c r="A369" s="38" t="s">
         <v>58</v>
       </c>
@@ -15107,7 +15107,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="370" spans="1:7" ht="30">
+    <row r="370" spans="1:7" ht="30" hidden="1">
       <c r="A370" s="38" t="s">
         <v>58</v>
       </c>
@@ -15128,7 +15128,7 @@
       </c>
       <c r="G370" s="44"/>
     </row>
-    <row r="371" spans="1:7">
+    <row r="371" spans="1:7" hidden="1">
       <c r="A371" s="38" t="s">
         <v>58</v>
       </c>
@@ -15149,7 +15149,7 @@
       </c>
       <c r="G371" s="44"/>
     </row>
-    <row r="372" spans="1:7">
+    <row r="372" spans="1:7" hidden="1">
       <c r="A372" s="38" t="s">
         <v>58</v>
       </c>
@@ -15164,7 +15164,7 @@
       <c r="F372" s="41"/>
       <c r="G372" s="41"/>
     </row>
-    <row r="373" spans="1:7">
+    <row r="373" spans="1:7" hidden="1">
       <c r="A373" s="38" t="s">
         <v>58</v>
       </c>
@@ -15179,7 +15179,7 @@
       <c r="F373" s="41"/>
       <c r="G373" s="41"/>
     </row>
-    <row r="374" spans="1:7">
+    <row r="374" spans="1:7" hidden="1">
       <c r="A374" s="38" t="s">
         <v>58</v>
       </c>
@@ -15200,7 +15200,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="375" spans="1:7">
+    <row r="375" spans="1:7" hidden="1">
       <c r="A375" s="38" t="s">
         <v>58</v>
       </c>
@@ -15219,7 +15219,7 @@
       </c>
       <c r="G375" s="44"/>
     </row>
-    <row r="376" spans="1:7" ht="30">
+    <row r="376" spans="1:7" ht="30" hidden="1">
       <c r="A376" s="38" t="s">
         <v>58</v>
       </c>
@@ -15238,7 +15238,7 @@
       </c>
       <c r="G376" s="44"/>
     </row>
-    <row r="377" spans="1:7" ht="30">
+    <row r="377" spans="1:7" ht="30" hidden="1">
       <c r="A377" s="38" t="s">
         <v>58</v>
       </c>
@@ -15257,7 +15257,7 @@
       </c>
       <c r="G377" s="44"/>
     </row>
-    <row r="378" spans="1:7">
+    <row r="378" spans="1:7" hidden="1">
       <c r="A378" s="38" t="s">
         <v>58</v>
       </c>
@@ -15276,7 +15276,7 @@
       </c>
       <c r="G378" s="44"/>
     </row>
-    <row r="379" spans="1:7" ht="30">
+    <row r="379" spans="1:7" ht="30" hidden="1">
       <c r="A379" s="38" t="s">
         <v>58</v>
       </c>
@@ -15295,7 +15295,7 @@
       </c>
       <c r="G379" s="44"/>
     </row>
-    <row r="380" spans="1:7">
+    <row r="380" spans="1:7" hidden="1">
       <c r="A380" s="38" t="s">
         <v>58</v>
       </c>
@@ -15310,7 +15310,7 @@
       <c r="F380" s="41"/>
       <c r="G380" s="41"/>
     </row>
-    <row r="381" spans="1:7">
+    <row r="381" spans="1:7" hidden="1">
       <c r="A381" s="38" t="s">
         <v>58</v>
       </c>
@@ -15331,7 +15331,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="382" spans="1:7">
+    <row r="382" spans="1:7" hidden="1">
       <c r="A382" s="38" t="s">
         <v>58</v>
       </c>
@@ -15352,7 +15352,7 @@
       </c>
       <c r="G382" s="38"/>
     </row>
-    <row r="383" spans="1:7">
+    <row r="383" spans="1:7" hidden="1">
       <c r="A383" s="38" t="s">
         <v>58</v>
       </c>
@@ -15367,7 +15367,7 @@
       <c r="F383" s="41"/>
       <c r="G383" s="41"/>
     </row>
-    <row r="384" spans="1:7">
+    <row r="384" spans="1:7" hidden="1">
       <c r="A384" s="38" t="s">
         <v>58</v>
       </c>
@@ -15388,7 +15388,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="385" spans="1:7">
+    <row r="385" spans="1:7" hidden="1">
       <c r="A385" s="38" t="s">
         <v>58</v>
       </c>
@@ -15407,7 +15407,7 @@
       </c>
       <c r="G385" s="44"/>
     </row>
-    <row r="386" spans="1:7">
+    <row r="386" spans="1:7" hidden="1">
       <c r="A386" s="38" t="s">
         <v>58</v>
       </c>
@@ -15426,7 +15426,7 @@
       </c>
       <c r="G386" s="44"/>
     </row>
-    <row r="387" spans="1:7">
+    <row r="387" spans="1:7" hidden="1">
       <c r="A387" s="38" t="s">
         <v>58</v>
       </c>
@@ -15445,7 +15445,7 @@
       </c>
       <c r="G387" s="38"/>
     </row>
-    <row r="388" spans="1:7">
+    <row r="388" spans="1:7" hidden="1">
       <c r="A388" s="38" t="s">
         <v>58</v>
       </c>
@@ -15466,7 +15466,7 @@
       </c>
       <c r="G388" s="38"/>
     </row>
-    <row r="389" spans="1:7">
+    <row r="389" spans="1:7" hidden="1">
       <c r="A389" s="38" t="s">
         <v>58</v>
       </c>
@@ -15481,7 +15481,7 @@
       <c r="F389" s="41"/>
       <c r="G389" s="41"/>
     </row>
-    <row r="390" spans="1:7">
+    <row r="390" spans="1:7" hidden="1">
       <c r="A390" s="38" t="s">
         <v>58</v>
       </c>
@@ -15496,7 +15496,7 @@
       <c r="F390" s="41"/>
       <c r="G390" s="41"/>
     </row>
-    <row r="391" spans="1:7" ht="45">
+    <row r="391" spans="1:7" ht="45" hidden="1">
       <c r="A391" s="38" t="s">
         <v>58</v>
       </c>
@@ -15519,7 +15519,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="392" spans="1:7" ht="30">
+    <row r="392" spans="1:7" ht="30" hidden="1">
       <c r="A392" s="38" t="s">
         <v>58</v>
       </c>
@@ -15540,7 +15540,7 @@
       </c>
       <c r="G392" s="38"/>
     </row>
-    <row r="393" spans="1:7">
+    <row r="393" spans="1:7" hidden="1">
       <c r="A393" s="38" t="s">
         <v>58</v>
       </c>
@@ -15561,7 +15561,7 @@
       </c>
       <c r="G393" s="44"/>
     </row>
-    <row r="394" spans="1:7">
+    <row r="394" spans="1:7" hidden="1">
       <c r="A394" s="38" t="s">
         <v>58</v>
       </c>
@@ -15576,7 +15576,7 @@
       <c r="F394" s="41"/>
       <c r="G394" s="41"/>
     </row>
-    <row r="395" spans="1:7">
+    <row r="395" spans="1:7" hidden="1">
       <c r="A395" s="38" t="s">
         <v>58</v>
       </c>
@@ -15591,7 +15591,7 @@
       <c r="F395" s="41"/>
       <c r="G395" s="41"/>
     </row>
-    <row r="396" spans="1:7">
+    <row r="396" spans="1:7" hidden="1">
       <c r="A396" s="38" t="s">
         <v>58</v>
       </c>
@@ -15612,7 +15612,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="397" spans="1:7">
+    <row r="397" spans="1:7" hidden="1">
       <c r="A397" s="38" t="s">
         <v>58</v>
       </c>
@@ -15631,7 +15631,7 @@
       </c>
       <c r="G397" s="44"/>
     </row>
-    <row r="398" spans="1:7">
+    <row r="398" spans="1:7" hidden="1">
       <c r="A398" s="38" t="s">
         <v>58</v>
       </c>
@@ -15650,7 +15650,7 @@
       </c>
       <c r="G398" s="44"/>
     </row>
-    <row r="399" spans="1:7" ht="30">
+    <row r="399" spans="1:7" ht="30" hidden="1">
       <c r="A399" s="38" t="s">
         <v>58</v>
       </c>
@@ -15669,7 +15669,7 @@
       </c>
       <c r="G399" s="44"/>
     </row>
-    <row r="400" spans="1:7">
+    <row r="400" spans="1:7" hidden="1">
       <c r="A400" s="38" t="s">
         <v>58</v>
       </c>
@@ -15688,7 +15688,7 @@
       </c>
       <c r="G400" s="44"/>
     </row>
-    <row r="401" spans="1:7" ht="30">
+    <row r="401" spans="1:7" ht="30" hidden="1">
       <c r="A401" s="38" t="s">
         <v>58</v>
       </c>
@@ -15707,7 +15707,7 @@
       </c>
       <c r="G401" s="44"/>
     </row>
-    <row r="402" spans="1:7">
+    <row r="402" spans="1:7" hidden="1">
       <c r="A402" s="38" t="s">
         <v>58</v>
       </c>
@@ -15722,7 +15722,7 @@
       <c r="F402" s="41"/>
       <c r="G402" s="41"/>
     </row>
-    <row r="403" spans="1:7">
+    <row r="403" spans="1:7" hidden="1">
       <c r="A403" s="38" t="s">
         <v>58</v>
       </c>
@@ -15743,7 +15743,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="404" spans="1:7">
+    <row r="404" spans="1:7" hidden="1">
       <c r="A404" s="38" t="s">
         <v>58</v>
       </c>
@@ -15764,7 +15764,7 @@
       </c>
       <c r="G404" s="38"/>
     </row>
-    <row r="405" spans="1:7">
+    <row r="405" spans="1:7" hidden="1">
       <c r="A405" s="38" t="s">
         <v>58</v>
       </c>
@@ -15779,7 +15779,7 @@
       <c r="F405" s="41"/>
       <c r="G405" s="41"/>
     </row>
-    <row r="406" spans="1:7">
+    <row r="406" spans="1:7" hidden="1">
       <c r="A406" s="38" t="s">
         <v>58</v>
       </c>
@@ -15800,7 +15800,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="407" spans="1:7">
+    <row r="407" spans="1:7" hidden="1">
       <c r="A407" s="38" t="s">
         <v>58</v>
       </c>
@@ -15819,7 +15819,7 @@
       </c>
       <c r="G407" s="44"/>
     </row>
-    <row r="408" spans="1:7">
+    <row r="408" spans="1:7" hidden="1">
       <c r="A408" s="38" t="s">
         <v>58</v>
       </c>
@@ -15838,7 +15838,7 @@
       </c>
       <c r="G408" s="44"/>
     </row>
-    <row r="409" spans="1:7">
+    <row r="409" spans="1:7" hidden="1">
       <c r="A409" s="38" t="s">
         <v>58</v>
       </c>
@@ -15857,7 +15857,7 @@
       </c>
       <c r="G409" s="38"/>
     </row>
-    <row r="410" spans="1:7">
+    <row r="410" spans="1:7" hidden="1">
       <c r="A410" s="38" t="s">
         <v>58</v>
       </c>
@@ -15878,7 +15878,7 @@
       </c>
       <c r="G410" s="38"/>
     </row>
-    <row r="411" spans="1:7">
+    <row r="411" spans="1:7" hidden="1">
       <c r="A411" s="38" t="s">
         <v>58</v>
       </c>
@@ -15893,7 +15893,7 @@
       <c r="F411" s="41"/>
       <c r="G411" s="41"/>
     </row>
-    <row r="412" spans="1:7">
+    <row r="412" spans="1:7" hidden="1">
       <c r="A412" s="38" t="s">
         <v>58</v>
       </c>
@@ -15908,7 +15908,7 @@
       <c r="F412" s="41"/>
       <c r="G412" s="41"/>
     </row>
-    <row r="413" spans="1:7" ht="45">
+    <row r="413" spans="1:7" ht="45" hidden="1">
       <c r="A413" s="38" t="s">
         <v>58</v>
       </c>
@@ -15931,7 +15931,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="414" spans="1:7">
+    <row r="414" spans="1:7" hidden="1">
       <c r="A414" s="38" t="s">
         <v>58</v>
       </c>
@@ -15952,7 +15952,7 @@
       </c>
       <c r="G414" s="44"/>
     </row>
-    <row r="415" spans="1:7">
+    <row r="415" spans="1:7" hidden="1">
       <c r="A415" s="38" t="s">
         <v>58</v>
       </c>
@@ -15973,7 +15973,7 @@
       </c>
       <c r="G415" s="44"/>
     </row>
-    <row r="416" spans="1:7">
+    <row r="416" spans="1:7" hidden="1">
       <c r="A416" s="38" t="s">
         <v>58</v>
       </c>
@@ -15988,7 +15988,7 @@
       <c r="F416" s="41"/>
       <c r="G416" s="41"/>
     </row>
-    <row r="417" spans="1:7">
+    <row r="417" spans="1:7" hidden="1">
       <c r="A417" s="38" t="s">
         <v>58</v>
       </c>
@@ -16003,7 +16003,7 @@
       <c r="F417" s="41"/>
       <c r="G417" s="41"/>
     </row>
-    <row r="418" spans="1:7">
+    <row r="418" spans="1:7" hidden="1">
       <c r="A418" s="38" t="s">
         <v>58</v>
       </c>
@@ -16024,7 +16024,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="419" spans="1:7">
+    <row r="419" spans="1:7" hidden="1">
       <c r="A419" s="38" t="s">
         <v>58</v>
       </c>
@@ -16043,7 +16043,7 @@
       </c>
       <c r="G419" s="44"/>
     </row>
-    <row r="420" spans="1:7">
+    <row r="420" spans="1:7" hidden="1">
       <c r="A420" s="38" t="s">
         <v>58</v>
       </c>
@@ -16062,7 +16062,7 @@
       </c>
       <c r="G420" s="44"/>
     </row>
-    <row r="421" spans="1:7">
+    <row r="421" spans="1:7" hidden="1">
       <c r="A421" s="38" t="s">
         <v>58</v>
       </c>
@@ -16081,7 +16081,7 @@
       </c>
       <c r="G421" s="38"/>
     </row>
-    <row r="422" spans="1:7">
+    <row r="422" spans="1:7" hidden="1">
       <c r="A422" s="38" t="s">
         <v>58</v>
       </c>
@@ -16096,7 +16096,7 @@
       <c r="F422" s="41"/>
       <c r="G422" s="41"/>
     </row>
-    <row r="423" spans="1:7">
+    <row r="423" spans="1:7" hidden="1">
       <c r="A423" s="38" t="s">
         <v>58</v>
       </c>
@@ -16117,7 +16117,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="424" spans="1:7">
+    <row r="424" spans="1:7" hidden="1">
       <c r="A424" s="38" t="s">
         <v>58</v>
       </c>
@@ -16136,7 +16136,7 @@
       </c>
       <c r="G424" s="38"/>
     </row>
-    <row r="425" spans="1:7">
+    <row r="425" spans="1:7" hidden="1">
       <c r="A425" s="38" t="s">
         <v>58</v>
       </c>
@@ -16155,7 +16155,7 @@
       </c>
       <c r="G425" s="38"/>
     </row>
-    <row r="426" spans="1:7">
+    <row r="426" spans="1:7" hidden="1">
       <c r="A426" s="38" t="s">
         <v>58</v>
       </c>
@@ -16170,7 +16170,7 @@
       <c r="F426" s="41"/>
       <c r="G426" s="41"/>
     </row>
-    <row r="427" spans="1:7">
+    <row r="427" spans="1:7" hidden="1">
       <c r="A427" s="38" t="s">
         <v>58</v>
       </c>
@@ -16191,7 +16191,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="428" spans="1:7">
+    <row r="428" spans="1:7" hidden="1">
       <c r="A428" s="38" t="s">
         <v>58</v>
       </c>
@@ -16210,7 +16210,7 @@
       </c>
       <c r="G428" s="44"/>
     </row>
-    <row r="429" spans="1:7">
+    <row r="429" spans="1:7" hidden="1">
       <c r="A429" s="38" t="s">
         <v>58</v>
       </c>
@@ -16229,7 +16229,7 @@
       </c>
       <c r="G429" s="44"/>
     </row>
-    <row r="430" spans="1:7">
+    <row r="430" spans="1:7" hidden="1">
       <c r="A430" s="38" t="s">
         <v>58</v>
       </c>
@@ -16248,7 +16248,7 @@
       </c>
       <c r="G430" s="38"/>
     </row>
-    <row r="431" spans="1:7">
+    <row r="431" spans="1:7" hidden="1">
       <c r="A431" s="38" t="s">
         <v>58</v>
       </c>
@@ -16267,7 +16267,7 @@
       </c>
       <c r="G431" s="44"/>
     </row>
-    <row r="432" spans="1:7" ht="30">
+    <row r="432" spans="1:7" ht="30" hidden="1">
       <c r="A432" s="38" t="s">
         <v>58</v>
       </c>
@@ -16286,7 +16286,7 @@
       </c>
       <c r="G432" s="44"/>
     </row>
-    <row r="433" spans="1:7">
+    <row r="433" spans="1:7" hidden="1">
       <c r="A433" s="38" t="s">
         <v>58</v>
       </c>
@@ -16303,7 +16303,7 @@
       </c>
       <c r="G433" s="41"/>
     </row>
-    <row r="434" spans="1:7" ht="45">
+    <row r="434" spans="1:7" ht="45" hidden="1">
       <c r="A434" s="38" t="s">
         <v>58</v>
       </c>
@@ -16324,7 +16324,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="435" spans="1:7" ht="30">
+    <row r="435" spans="1:7" ht="30" hidden="1">
       <c r="A435" s="38" t="s">
         <v>58</v>
       </c>
@@ -16343,7 +16343,7 @@
       </c>
       <c r="G435" s="44"/>
     </row>
-    <row r="436" spans="1:7">
+    <row r="436" spans="1:7" hidden="1">
       <c r="A436" s="38" t="s">
         <v>58</v>
       </c>
@@ -16364,7 +16364,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="437" spans="1:7">
+    <row r="437" spans="1:7" hidden="1">
       <c r="A437" s="38" t="s">
         <v>58</v>
       </c>
@@ -16383,7 +16383,7 @@
       </c>
       <c r="G437" s="44"/>
     </row>
-    <row r="438" spans="1:7">
+    <row r="438" spans="1:7" hidden="1">
       <c r="A438" s="38" t="s">
         <v>58</v>
       </c>
@@ -16400,7 +16400,7 @@
       </c>
       <c r="G438" s="41"/>
     </row>
-    <row r="439" spans="1:7">
+    <row r="439" spans="1:7" hidden="1">
       <c r="A439" s="38" t="s">
         <v>58</v>
       </c>
@@ -16421,7 +16421,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="440" spans="1:7">
+    <row r="440" spans="1:7" hidden="1">
       <c r="A440" s="38" t="s">
         <v>58</v>
       </c>
@@ -16442,7 +16442,7 @@
       </c>
       <c r="G440" s="38"/>
     </row>
-    <row r="441" spans="1:7">
+    <row r="441" spans="1:7" hidden="1">
       <c r="A441" s="38" t="s">
         <v>58</v>
       </c>
@@ -16459,7 +16459,7 @@
       </c>
       <c r="G441" s="41"/>
     </row>
-    <row r="442" spans="1:7">
+    <row r="442" spans="1:7" hidden="1">
       <c r="A442" s="38" t="s">
         <v>58</v>
       </c>
@@ -16480,7 +16480,7 @@
       </c>
       <c r="G442" s="38"/>
     </row>
-    <row r="443" spans="1:7">
+    <row r="443" spans="1:7" hidden="1">
       <c r="A443" s="38" t="s">
         <v>58</v>
       </c>
@@ -16497,7 +16497,7 @@
       </c>
       <c r="G443" s="37"/>
     </row>
-    <row r="444" spans="1:7">
+    <row r="444" spans="1:7" hidden="1">
       <c r="A444" s="38" t="s">
         <v>58</v>
       </c>
@@ -16516,7 +16516,7 @@
       </c>
       <c r="G444" s="44"/>
     </row>
-    <row r="445" spans="1:7">
+    <row r="445" spans="1:7" hidden="1">
       <c r="A445" s="38" t="s">
         <v>58</v>
       </c>
@@ -16535,7 +16535,7 @@
       </c>
       <c r="G445" s="44"/>
     </row>
-    <row r="446" spans="1:7">
+    <row r="446" spans="1:7" hidden="1">
       <c r="A446" s="38" t="s">
         <v>58</v>
       </c>
@@ -16554,7 +16554,7 @@
       </c>
       <c r="G446" s="44"/>
     </row>
-    <row r="447" spans="1:7">
+    <row r="447" spans="1:7" hidden="1">
       <c r="A447" s="38" t="s">
         <v>58</v>
       </c>
@@ -16571,7 +16571,7 @@
       </c>
       <c r="G447" s="37"/>
     </row>
-    <row r="448" spans="1:7">
+    <row r="448" spans="1:7" hidden="1">
       <c r="A448" s="38" t="s">
         <v>58</v>
       </c>
@@ -16590,7 +16590,7 @@
       </c>
       <c r="G448" s="44"/>
     </row>
-    <row r="449" spans="1:7">
+    <row r="449" spans="1:7" hidden="1">
       <c r="A449" s="38" t="s">
         <v>58</v>
       </c>
@@ -16609,7 +16609,7 @@
       </c>
       <c r="G449" s="44"/>
     </row>
-    <row r="450" spans="1:7">
+    <row r="450" spans="1:7" hidden="1">
       <c r="A450" s="38" t="s">
         <v>58</v>
       </c>
@@ -16626,7 +16626,7 @@
       </c>
       <c r="G450" s="37"/>
     </row>
-    <row r="451" spans="1:7">
+    <row r="451" spans="1:7" hidden="1">
       <c r="A451" s="38" t="s">
         <v>58</v>
       </c>
@@ -16643,7 +16643,7 @@
       </c>
       <c r="G451" s="41"/>
     </row>
-    <row r="452" spans="1:7" ht="45">
+    <row r="452" spans="1:7" ht="45" hidden="1">
       <c r="A452" s="38" t="s">
         <v>58</v>
       </c>
@@ -16664,7 +16664,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="453" spans="1:7">
+    <row r="453" spans="1:7" hidden="1">
       <c r="A453" s="38" t="s">
         <v>58</v>
       </c>
@@ -16683,7 +16683,7 @@
       </c>
       <c r="G453" s="44"/>
     </row>
-    <row r="454" spans="1:7">
+    <row r="454" spans="1:7" hidden="1">
       <c r="A454" s="38" t="s">
         <v>58</v>
       </c>
@@ -16702,7 +16702,7 @@
       </c>
       <c r="G454" s="44"/>
     </row>
-    <row r="455" spans="1:7">
+    <row r="455" spans="1:7" hidden="1">
       <c r="A455" s="38" t="s">
         <v>58</v>
       </c>
@@ -16719,7 +16719,7 @@
       </c>
       <c r="G455" s="41"/>
     </row>
-    <row r="456" spans="1:7">
+    <row r="456" spans="1:7" hidden="1">
       <c r="A456" s="38" t="s">
         <v>58</v>
       </c>
@@ -16736,7 +16736,7 @@
       </c>
       <c r="G456" s="41"/>
     </row>
-    <row r="457" spans="1:7">
+    <row r="457" spans="1:7" hidden="1">
       <c r="A457" s="38" t="s">
         <v>58</v>
       </c>
@@ -16757,7 +16757,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="458" spans="1:7">
+    <row r="458" spans="1:7" hidden="1">
       <c r="A458" s="38" t="s">
         <v>58</v>
       </c>
@@ -16776,7 +16776,7 @@
       </c>
       <c r="G458" s="44"/>
     </row>
-    <row r="459" spans="1:7">
+    <row r="459" spans="1:7" hidden="1">
       <c r="A459" s="38" t="s">
         <v>58</v>
       </c>
@@ -16795,7 +16795,7 @@
       </c>
       <c r="G459" s="38"/>
     </row>
-    <row r="460" spans="1:7">
+    <row r="460" spans="1:7" hidden="1">
       <c r="A460" s="38" t="s">
         <v>58</v>
       </c>
@@ -16869,7 +16869,7 @@
       </c>
       <c r="G463" s="38"/>
     </row>
-    <row r="464" spans="1:7">
+    <row r="464" spans="1:7" hidden="1">
       <c r="A464" s="38" t="s">
         <v>58</v>
       </c>
@@ -16886,7 +16886,7 @@
       </c>
       <c r="G464" s="41"/>
     </row>
-    <row r="465" spans="1:7">
+    <row r="465" spans="1:7" hidden="1">
       <c r="A465" s="38" t="s">
         <v>58</v>
       </c>
@@ -16907,7 +16907,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="466" spans="1:7">
+    <row r="466" spans="1:7" hidden="1">
       <c r="A466" s="38" t="s">
         <v>58</v>
       </c>
@@ -16926,7 +16926,7 @@
       </c>
       <c r="G466" s="38"/>
     </row>
-    <row r="467" spans="1:7">
+    <row r="467" spans="1:7" hidden="1">
       <c r="A467" s="38" t="s">
         <v>58</v>
       </c>
@@ -16943,7 +16943,7 @@
       </c>
       <c r="G467" s="41"/>
     </row>
-    <row r="468" spans="1:7">
+    <row r="468" spans="1:7" hidden="1">
       <c r="A468" s="38" t="s">
         <v>58</v>
       </c>
@@ -16964,7 +16964,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="469" spans="1:7">
+    <row r="469" spans="1:7" hidden="1">
       <c r="A469" s="38" t="s">
         <v>58</v>
       </c>
@@ -16983,7 +16983,7 @@
       </c>
       <c r="G469" s="44"/>
     </row>
-    <row r="470" spans="1:7">
+    <row r="470" spans="1:7" hidden="1">
       <c r="A470" s="38" t="s">
         <v>58</v>
       </c>
@@ -17002,7 +17002,7 @@
       </c>
       <c r="G470" s="44"/>
     </row>
-    <row r="471" spans="1:7">
+    <row r="471" spans="1:7" hidden="1">
       <c r="A471" s="38" t="s">
         <v>58</v>
       </c>
@@ -17021,7 +17021,7 @@
       </c>
       <c r="G471" s="38"/>
     </row>
-    <row r="472" spans="1:7">
+    <row r="472" spans="1:7" hidden="1">
       <c r="A472" s="38" t="s">
         <v>58</v>
       </c>
@@ -17041,6 +17041,15 @@
       <c r="G472" s="38"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G472" xr:uid="{706EF14C-F378-4EAC-AF6D-3FBCD2E21926}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="11.7.2.4"/>
+        <filter val="11.7.2.4.1"/>
+        <filter val="11.7.2.4.2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
testing a fix to PKIX.19
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D55BF9E-97CC-46D3-90B1-D62D40F8235E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A7924A-881F-4511-AA53-FCD78BDEB849}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -8512,8 +8512,8 @@
   <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:H472"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F463" sqref="F463"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D423" sqref="D423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -16096,7 +16096,7 @@
       <c r="F422" s="41"/>
       <c r="G422" s="41"/>
     </row>
-    <row r="423" spans="1:7" hidden="1">
+    <row r="423" spans="1:7">
       <c r="A423" s="38" t="s">
         <v>58</v>
       </c>
@@ -16107,7 +16107,7 @@
         <v>1296</v>
       </c>
       <c r="D423" s="38" t="s">
-        <v>1074</v>
+        <v>721</v>
       </c>
       <c r="E423" s="38"/>
       <c r="F423" s="38" t="s">
@@ -16814,7 +16814,7 @@
       </c>
       <c r="G460" s="38"/>
     </row>
-    <row r="461" spans="1:7">
+    <row r="461" spans="1:7" hidden="1">
       <c r="A461" s="38" t="s">
         <v>58</v>
       </c>
@@ -16831,7 +16831,7 @@
       </c>
       <c r="G461" s="38"/>
     </row>
-    <row r="462" spans="1:7" ht="30">
+    <row r="462" spans="1:7" ht="30" hidden="1">
       <c r="A462" s="38" t="s">
         <v>58</v>
       </c>
@@ -16850,7 +16850,7 @@
       </c>
       <c r="G462" s="38"/>
     </row>
-    <row r="463" spans="1:7">
+    <row r="463" spans="1:7" hidden="1">
       <c r="A463" s="38" t="s">
         <v>58</v>
       </c>
@@ -17044,9 +17044,7 @@
   <autoFilter ref="A1:G472" xr:uid="{706EF14C-F378-4EAC-AF6D-3FBCD2E21926}">
     <filterColumn colId="1">
       <filters>
-        <filter val="11.7.2.4"/>
-        <filter val="11.7.2.4.1"/>
-        <filter val="11.7.2.4.2"/>
+        <filter val="11.4.2.3.1"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -21982,8 +21980,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>

</xml_diff>

<commit_message>
eliminate CMS.17 atom from 10.2.1 per email from Bob after verifying it is not in 800-85b. Issue #186.
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A7924A-881F-4511-AA53-FCD78BDEB849}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0D9361-C13E-4C31-985F-93F14E84FCB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3776" uniqueCount="1310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3776" uniqueCount="1311">
   <si>
     <t>BER_TLV_Test_Assertions</t>
   </si>
@@ -3963,6 +3963,9 @@
   </si>
   <si>
     <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.11,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID:2.16.840.1.101.3.2.1.48.9|2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID:2.16.840.1.101.3.2.1.48.9|2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID:2.16.840.1.101.3.2.1.48.13,CARD_HOLDER_UNIQUE_IDENTIFIER_OID:2.16.840.1.101.3.6.7</t>
+  </si>
+  <si>
+    <t>Per Bob, CHUID doesn't need this test. Confirmedn in SP800-85</t>
   </si>
 </sst>
 </file>
@@ -8513,7 +8516,7 @@
   <dimension ref="A1:H472"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D423" sqref="D423"/>
+      <selection activeCell="G473" sqref="G473"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -13644,7 +13647,7 @@
       <c r="F286" s="38"/>
       <c r="G286" s="44"/>
     </row>
-    <row r="287" spans="1:7" ht="30" hidden="1">
+    <row r="287" spans="1:7" ht="30">
       <c r="A287" s="38" t="s">
         <v>58</v>
       </c>
@@ -13654,14 +13657,14 @@
       <c r="C287" s="44" t="s">
         <v>504</v>
       </c>
-      <c r="D287" s="38" t="s">
-        <v>505</v>
-      </c>
+      <c r="D287" s="38"/>
       <c r="E287" s="38"/>
       <c r="F287" s="38" t="s">
         <v>1143</v>
       </c>
-      <c r="G287" s="44"/>
+      <c r="G287" s="44" t="s">
+        <v>1310</v>
+      </c>
     </row>
     <row r="288" spans="1:7" hidden="1">
       <c r="A288" s="38" t="s">
@@ -16096,7 +16099,7 @@
       <c r="F422" s="41"/>
       <c r="G422" s="41"/>
     </row>
-    <row r="423" spans="1:7">
+    <row r="423" spans="1:7" hidden="1">
       <c r="A423" s="38" t="s">
         <v>58</v>
       </c>
@@ -16795,7 +16798,7 @@
       </c>
       <c r="G459" s="38"/>
     </row>
-    <row r="460" spans="1:7" hidden="1">
+    <row r="460" spans="1:7" ht="30" hidden="1">
       <c r="A460" s="38" t="s">
         <v>58</v>
       </c>
@@ -17044,7 +17047,7 @@
   <autoFilter ref="A1:G472" xr:uid="{706EF14C-F378-4EAC-AF6D-3FBCD2E21926}">
     <filterColumn colId="1">
       <filters>
-        <filter val="11.4.2.3.1"/>
+        <filter val="10.2.1.14"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
add id-fpki-common-policy to list of IDs permitted in signature and encryption certificates.
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0D9361-C13E-4C31-985F-93F14E84FCB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C783D1-FFFB-4267-8707-6DFEB938584E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -3938,9 +3938,6 @@
     <t>CARDHOLDER_IRIS_IMAGES_OID</t>
   </si>
   <si>
-    <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID;2.16.840.1.101.3.2.1.48.11,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID;2.16.840.1.101.3.2.1.48.9:2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID;2.16.840.1.101.3.2.1.48.9:2.16.840.1.101.3.2.1.48.12,X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID;2.16.840.1.101.3.2.1.48.13,CARD_HOLDER_UNIQUE_IDENTIFIER_OID;2.16.840.1.101.3.2.1.48.86</t>
-  </si>
-  <si>
     <t>Confirm that version of signed data structure is 3</t>
   </si>
   <si>
@@ -3966,6 +3963,9 @@
   </si>
   <si>
     <t>Per Bob, CHUID doesn't need this test. Confirmedn in SP800-85</t>
+  </si>
+  <si>
+    <t>X509_CERTIFICATE_FOR_PIV_AUTHENTICATION_OID;2.16.840.1.101.3.2.1.48.11,X509_CERTIFICATE_FOR_DIGITAL_SIGNATURE_OID;2.16.840.1.101.3.2.1.48.9:2.16.840.1.101.3.2.1.48.12:2.16.840.1.101.3.2.1.48.8,X509_CERTIFICATE_FOR_KEY_MANAGEMENT_OID;2.16.840.1.101.3.2.1.48.9:2.16.840.1.101.3.2.1.48.12:2.16.840.1.101.3.2.1.48.8,X509_CERTIFICATE_FOR_CARD_AUTHENTICATION_OID;2.16.840.1.101.3.2.1.48.13,CARD_HOLDER_UNIQUE_IDENTIFIER_OID;2.16.840.1.101.3.2.1.48.86</t>
   </si>
 </sst>
 </file>
@@ -8515,8 +8515,8 @@
   <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:H472"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G473" sqref="G473"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F308" sqref="F308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -11535,7 +11535,7 @@
         <v>289</v>
       </c>
       <c r="C162" s="38" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="D162" s="38">
         <v>76.2</v>
@@ -11569,10 +11569,10 @@
         <v>293</v>
       </c>
       <c r="C164" s="38" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="D164" s="38" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="E164" s="38"/>
       <c r="F164" s="38"/>
@@ -11583,7 +11583,7 @@
         <v>58</v>
       </c>
       <c r="B165" s="38" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="C165" s="38" t="s">
         <v>297</v>
@@ -11620,7 +11620,7 @@
         <v>296</v>
       </c>
       <c r="C167" s="40" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="D167" s="40" t="s">
         <v>868</v>
@@ -13647,7 +13647,7 @@
       <c r="F286" s="38"/>
       <c r="G286" s="44"/>
     </row>
-    <row r="287" spans="1:7" ht="30">
+    <row r="287" spans="1:7" ht="30" hidden="1">
       <c r="A287" s="38" t="s">
         <v>58</v>
       </c>
@@ -13663,7 +13663,7 @@
         <v>1143</v>
       </c>
       <c r="G287" s="44" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="288" spans="1:7" hidden="1">
@@ -14002,7 +14002,7 @@
       <c r="F307" s="41"/>
       <c r="G307" s="41"/>
     </row>
-    <row r="308" spans="1:7" ht="30" hidden="1">
+    <row r="308" spans="1:7" ht="30">
       <c r="A308" s="38" t="s">
         <v>58</v>
       </c>
@@ -16798,7 +16798,7 @@
       </c>
       <c r="G459" s="38"/>
     </row>
-    <row r="460" spans="1:7" ht="30" hidden="1">
+    <row r="460" spans="1:7" hidden="1">
       <c r="A460" s="38" t="s">
         <v>58</v>
       </c>
@@ -17047,7 +17047,7 @@
   <autoFilter ref="A1:G472" xr:uid="{706EF14C-F378-4EAC-AF6D-3FBCD2E21926}">
     <filterColumn colId="1">
       <filters>
-        <filter val="10.2.1.14"/>
+        <filter val="10.4.1.1"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -17206,8 +17206,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AMK55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -19626,7 +19626,7 @@
         <v>863</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="E3" s="30"/>
       <c r="F3" s="30" t="s">
@@ -20747,16 +20747,16 @@
     </row>
     <row r="50" spans="1:256">
       <c r="A50" s="31" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="B50" s="30" t="s">
         <v>860</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
@@ -21391,7 +21391,7 @@
         <v>1019</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
@@ -21983,8 +21983,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -22384,7 +22384,7 @@
         <v>1049</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>1301</v>
+        <v>1310</v>
       </c>
       <c r="F7" s="30" t="s">
         <v>790</v>
@@ -22664,7 +22664,7 @@
         <v>1081</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="F21" s="30" t="s">
         <v>790</v>

</xml_diff>

<commit_message>
add container ids to prod sheet
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C783D1-FFFB-4267-8707-6DFEB938584E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE441D2-6758-4A99-90FD-03E761483465}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Placeholders" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Steps Overview'!$A$1:$G$472</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Steps Overview'!$B$1:$B$472</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -8515,8 +8515,8 @@
   <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:H472"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F308" sqref="F308"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="F334" sqref="F334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -14002,7 +14002,7 @@
       <c r="F307" s="41"/>
       <c r="G307" s="41"/>
     </row>
-    <row r="308" spans="1:7" ht="30">
+    <row r="308" spans="1:7" ht="30" hidden="1">
       <c r="A308" s="38" t="s">
         <v>58</v>
       </c>
@@ -14444,7 +14444,7 @@
       </c>
       <c r="G333" s="38"/>
     </row>
-    <row r="334" spans="1:7" ht="30" hidden="1">
+    <row r="334" spans="1:7" ht="30">
       <c r="A334" s="38" t="s">
         <v>58</v>
       </c>
@@ -17044,10 +17044,10 @@
       <c r="G472" s="38"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G472" xr:uid="{706EF14C-F378-4EAC-AF6D-3FBCD2E21926}">
-    <filterColumn colId="1">
+  <autoFilter ref="B1:B472" xr:uid="{7D022713-DD5E-432D-B8E4-1D5C596D7380}">
+    <filterColumn colId="0">
       <filters>
-        <filter val="10.4.1.1"/>
+        <filter val="10.5.1.16"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -21983,7 +21983,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix parameters for PKIX.19 in prod sheet, fix ordering in test sheet
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262C7348-DBDA-45A6-9D95-7C8B17B9E3FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68B8CDA-7D5A-49B3-85E9-6759BAC13686}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8515,11 +8515,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:H472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B210" sqref="B210"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D424" sqref="D424"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8560,7 +8560,7 @@
       </c>
       <c r="H1" s="53"/>
     </row>
-    <row r="2" spans="1:8" ht="15.6">
+    <row r="2" spans="1:8" ht="15.6" hidden="1">
       <c r="A2" s="35" t="s">
         <v>58</v>
       </c>
@@ -8575,7 +8575,7 @@
       <c r="F2" s="37"/>
       <c r="G2" s="36"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" s="38" t="s">
         <v>58</v>
       </c>
@@ -8590,7 +8590,7 @@
       <c r="F3" s="37"/>
       <c r="G3" s="37"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" s="38" t="s">
         <v>58</v>
       </c>
@@ -8605,7 +8605,7 @@
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="30" hidden="1">
       <c r="A5" s="38" t="s">
         <v>58</v>
       </c>
@@ -8626,7 +8626,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" s="38" t="s">
         <v>58</v>
       </c>
@@ -8645,7 +8645,7 @@
       </c>
       <c r="G6" s="38"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" hidden="1">
       <c r="A7" s="38" t="s">
         <v>58</v>
       </c>
@@ -8664,7 +8664,7 @@
       </c>
       <c r="G7" s="38"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" s="38" t="s">
         <v>58</v>
       </c>
@@ -8683,7 +8683,7 @@
       </c>
       <c r="G8" s="38"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" s="38" t="s">
         <v>58</v>
       </c>
@@ -8702,7 +8702,7 @@
       </c>
       <c r="G9" s="38"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" s="38" t="s">
         <v>58</v>
       </c>
@@ -8721,7 +8721,7 @@
       </c>
       <c r="G10" s="38"/>
     </row>
-    <row r="11" spans="1:8" ht="30">
+    <row r="11" spans="1:8" ht="30" hidden="1">
       <c r="A11" s="38" t="s">
         <v>58</v>
       </c>
@@ -8740,7 +8740,7 @@
       </c>
       <c r="G11" s="38"/>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:8" ht="30" hidden="1">
       <c r="A12" s="38" t="s">
         <v>58</v>
       </c>
@@ -8759,7 +8759,7 @@
       </c>
       <c r="G12" s="38"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" s="38" t="s">
         <v>58</v>
       </c>
@@ -8778,7 +8778,7 @@
       </c>
       <c r="G13" s="38"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" hidden="1">
       <c r="A14" s="38" t="s">
         <v>58</v>
       </c>
@@ -8797,7 +8797,7 @@
       </c>
       <c r="G14" s="38"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" s="38" t="s">
         <v>58</v>
       </c>
@@ -8816,7 +8816,7 @@
       </c>
       <c r="G15" s="38"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" hidden="1">
       <c r="A16" s="38" t="s">
         <v>58</v>
       </c>
@@ -8831,7 +8831,7 @@
       <c r="F16" s="37"/>
       <c r="G16" s="37"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" hidden="1">
       <c r="A17" s="38" t="s">
         <v>58</v>
       </c>
@@ -8846,7 +8846,7 @@
       <c r="F17" s="37"/>
       <c r="G17" s="37"/>
     </row>
-    <row r="18" spans="1:7" ht="30">
+    <row r="18" spans="1:7" ht="30" hidden="1">
       <c r="A18" s="38" t="s">
         <v>58</v>
       </c>
@@ -8867,7 +8867,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" hidden="1">
       <c r="A19" s="38" t="s">
         <v>58</v>
       </c>
@@ -8886,7 +8886,7 @@
       </c>
       <c r="G19" s="38"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" hidden="1">
       <c r="A20" s="38" t="s">
         <v>58</v>
       </c>
@@ -8905,7 +8905,7 @@
       </c>
       <c r="G20" s="38"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" hidden="1">
       <c r="A21" s="38" t="s">
         <v>58</v>
       </c>
@@ -8924,7 +8924,7 @@
       </c>
       <c r="G21" s="38"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" s="38" t="s">
         <v>58</v>
       </c>
@@ -8943,7 +8943,7 @@
       </c>
       <c r="G22" s="38"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23" s="38" t="s">
         <v>58</v>
       </c>
@@ -8962,7 +8962,7 @@
       </c>
       <c r="G23" s="38"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" hidden="1">
       <c r="A24" s="39" t="s">
         <v>58</v>
       </c>
@@ -8981,7 +8981,7 @@
       </c>
       <c r="G24" s="39"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" hidden="1">
       <c r="A25" s="38" t="s">
         <v>58</v>
       </c>
@@ -9000,7 +9000,7 @@
       </c>
       <c r="G25" s="38"/>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" hidden="1">
       <c r="A26" s="38" t="s">
         <v>58</v>
       </c>
@@ -9019,7 +9019,7 @@
       </c>
       <c r="G26" s="38"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="39" t="s">
         <v>58</v>
       </c>
@@ -9038,7 +9038,7 @@
       </c>
       <c r="G27" s="39"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="39" t="s">
         <v>58</v>
       </c>
@@ -9057,7 +9057,7 @@
       </c>
       <c r="G28" s="39"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="39" t="s">
         <v>58</v>
       </c>
@@ -9076,7 +9076,7 @@
       </c>
       <c r="G29" s="39"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" hidden="1">
       <c r="A30" s="39"/>
       <c r="B30" s="39" t="s">
         <v>1217</v>
@@ -9093,7 +9093,7 @@
       </c>
       <c r="G30" s="39"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" hidden="1">
       <c r="A31" s="38" t="s">
         <v>58</v>
       </c>
@@ -9112,7 +9112,7 @@
       </c>
       <c r="G31" s="38"/>
     </row>
-    <row r="32" spans="1:7" ht="30">
+    <row r="32" spans="1:7" ht="30" hidden="1">
       <c r="A32" s="38" t="s">
         <v>58</v>
       </c>
@@ -9131,7 +9131,7 @@
       </c>
       <c r="G32" s="38"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" hidden="1">
       <c r="A33" s="39" t="s">
         <v>58</v>
       </c>
@@ -9150,7 +9150,7 @@
       </c>
       <c r="G33" s="39"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" hidden="1">
       <c r="A34" s="39" t="s">
         <v>58</v>
       </c>
@@ -9169,7 +9169,7 @@
       </c>
       <c r="G34" s="39"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" hidden="1">
       <c r="A35" s="39" t="s">
         <v>58</v>
       </c>
@@ -9188,7 +9188,7 @@
       </c>
       <c r="G35" s="39"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="39" t="s">
         <v>58</v>
       </c>
@@ -9207,7 +9207,7 @@
       </c>
       <c r="G36" s="39"/>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" hidden="1">
       <c r="A37" s="38" t="s">
         <v>58</v>
       </c>
@@ -9226,7 +9226,7 @@
       </c>
       <c r="G37" s="38"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" hidden="1">
       <c r="A38" s="38" t="s">
         <v>58</v>
       </c>
@@ -9245,7 +9245,7 @@
       </c>
       <c r="G38" s="38"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" hidden="1">
       <c r="A39" s="38" t="s">
         <v>58</v>
       </c>
@@ -9264,7 +9264,7 @@
       </c>
       <c r="G39" s="38"/>
     </row>
-    <row r="40" spans="1:7" ht="30">
+    <row r="40" spans="1:7" ht="30" hidden="1">
       <c r="A40" s="38" t="s">
         <v>58</v>
       </c>
@@ -9283,7 +9283,7 @@
       </c>
       <c r="G40" s="38"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" hidden="1">
       <c r="A41" s="38" t="s">
         <v>58</v>
       </c>
@@ -9302,7 +9302,7 @@
       </c>
       <c r="G41" s="38"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" hidden="1">
       <c r="A42" s="38" t="s">
         <v>131</v>
       </c>
@@ -9321,7 +9321,7 @@
       </c>
       <c r="G42" s="38"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" hidden="1">
       <c r="A43" s="38" t="s">
         <v>58</v>
       </c>
@@ -9336,7 +9336,7 @@
       <c r="F43" s="37"/>
       <c r="G43" s="37"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" hidden="1">
       <c r="A44" s="38" t="s">
         <v>58</v>
       </c>
@@ -9351,7 +9351,7 @@
       <c r="F44" s="37"/>
       <c r="G44" s="37"/>
     </row>
-    <row r="45" spans="1:7" ht="30">
+    <row r="45" spans="1:7" ht="30" hidden="1">
       <c r="A45" s="38" t="s">
         <v>58</v>
       </c>
@@ -9372,7 +9372,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" hidden="1">
       <c r="A46" s="38" t="s">
         <v>58</v>
       </c>
@@ -9391,7 +9391,7 @@
       </c>
       <c r="G46" s="38"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" hidden="1">
       <c r="A47" s="38" t="s">
         <v>58</v>
       </c>
@@ -9410,7 +9410,7 @@
       </c>
       <c r="G47" s="38"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" hidden="1">
       <c r="A48" s="38" t="s">
         <v>58</v>
       </c>
@@ -9429,7 +9429,7 @@
       </c>
       <c r="G48" s="38"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" hidden="1">
       <c r="A49" s="38" t="s">
         <v>58</v>
       </c>
@@ -9448,7 +9448,7 @@
       </c>
       <c r="G49" s="38"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" hidden="1">
       <c r="A50" s="38" t="s">
         <v>58</v>
       </c>
@@ -9467,7 +9467,7 @@
       </c>
       <c r="G50" s="38"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" hidden="1">
       <c r="A51" s="38" t="s">
         <v>58</v>
       </c>
@@ -9486,7 +9486,7 @@
       </c>
       <c r="G51" s="38"/>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" hidden="1">
       <c r="A52" s="38" t="s">
         <v>58</v>
       </c>
@@ -9505,7 +9505,7 @@
       </c>
       <c r="G52" s="38"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" hidden="1">
       <c r="A53" s="38" t="s">
         <v>58</v>
       </c>
@@ -9524,7 +9524,7 @@
       </c>
       <c r="G53" s="38"/>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" hidden="1">
       <c r="A54" s="38" t="s">
         <v>131</v>
       </c>
@@ -9543,7 +9543,7 @@
       </c>
       <c r="G54" s="38"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" hidden="1">
       <c r="A55" s="38" t="s">
         <v>58</v>
       </c>
@@ -9558,7 +9558,7 @@
       <c r="F55" s="37"/>
       <c r="G55" s="37"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" hidden="1">
       <c r="A56" s="38" t="s">
         <v>58</v>
       </c>
@@ -9573,7 +9573,7 @@
       <c r="F56" s="37"/>
       <c r="G56" s="37"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" hidden="1">
       <c r="A57" s="38" t="s">
         <v>58</v>
       </c>
@@ -9594,7 +9594,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" hidden="1">
       <c r="A58" s="38" t="s">
         <v>58</v>
       </c>
@@ -9613,7 +9613,7 @@
       </c>
       <c r="G58" s="38"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" hidden="1">
       <c r="A59" s="38" t="s">
         <v>58</v>
       </c>
@@ -9632,7 +9632,7 @@
       </c>
       <c r="G59" s="38"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" hidden="1">
       <c r="A60" s="38" t="s">
         <v>58</v>
       </c>
@@ -9651,7 +9651,7 @@
       </c>
       <c r="G60" s="38"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" hidden="1">
       <c r="A61" s="38" t="s">
         <v>58</v>
       </c>
@@ -9670,7 +9670,7 @@
       </c>
       <c r="G61" s="38"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" hidden="1">
       <c r="A62" s="38" t="s">
         <v>58</v>
       </c>
@@ -9689,7 +9689,7 @@
       </c>
       <c r="G62" s="38"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" hidden="1">
       <c r="A63" s="38" t="s">
         <v>58</v>
       </c>
@@ -9708,7 +9708,7 @@
       </c>
       <c r="G63" s="38"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" hidden="1">
       <c r="A64" s="38" t="s">
         <v>58</v>
       </c>
@@ -9727,7 +9727,7 @@
       </c>
       <c r="G64" s="38"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" hidden="1">
       <c r="A65" s="38" t="s">
         <v>58</v>
       </c>
@@ -9746,7 +9746,7 @@
       </c>
       <c r="G65" s="38"/>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" hidden="1">
       <c r="A66" s="38" t="s">
         <v>58</v>
       </c>
@@ -9761,7 +9761,7 @@
       <c r="F66" s="37"/>
       <c r="G66" s="37"/>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" hidden="1">
       <c r="A67" s="38" t="s">
         <v>58</v>
       </c>
@@ -9776,7 +9776,7 @@
       <c r="F67" s="37"/>
       <c r="G67" s="37"/>
     </row>
-    <row r="68" spans="1:7" ht="30">
+    <row r="68" spans="1:7" ht="30" hidden="1">
       <c r="A68" s="38" t="s">
         <v>58</v>
       </c>
@@ -9797,7 +9797,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" hidden="1">
       <c r="A69" s="38" t="s">
         <v>58</v>
       </c>
@@ -9816,7 +9816,7 @@
       </c>
       <c r="G69" s="38"/>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" hidden="1">
       <c r="A70" s="38" t="s">
         <v>58</v>
       </c>
@@ -9835,7 +9835,7 @@
       </c>
       <c r="G70" s="38"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" hidden="1">
       <c r="A71" s="38" t="s">
         <v>58</v>
       </c>
@@ -9854,7 +9854,7 @@
       </c>
       <c r="G71" s="38"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" hidden="1">
       <c r="A72" s="38" t="s">
         <v>58</v>
       </c>
@@ -9873,7 +9873,7 @@
       </c>
       <c r="G72" s="38"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" hidden="1">
       <c r="A73" s="38" t="s">
         <v>58</v>
       </c>
@@ -9892,7 +9892,7 @@
       </c>
       <c r="G73" s="38"/>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" hidden="1">
       <c r="A74" s="39" t="s">
         <v>58</v>
       </c>
@@ -9911,7 +9911,7 @@
       </c>
       <c r="G74" s="39"/>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" hidden="1">
       <c r="A75" s="39" t="s">
         <v>58</v>
       </c>
@@ -9930,7 +9930,7 @@
       </c>
       <c r="G75" s="39"/>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" hidden="1">
       <c r="A76" s="38" t="s">
         <v>58</v>
       </c>
@@ -9949,7 +9949,7 @@
       </c>
       <c r="G76" s="38"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" hidden="1">
       <c r="A77" s="38" t="s">
         <v>58</v>
       </c>
@@ -9968,7 +9968,7 @@
       </c>
       <c r="G77" s="38"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" hidden="1">
       <c r="A78" s="38" t="s">
         <v>58</v>
       </c>
@@ -9987,7 +9987,7 @@
       </c>
       <c r="G78" s="38"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" hidden="1">
       <c r="A79" s="38" t="s">
         <v>131</v>
       </c>
@@ -10006,7 +10006,7 @@
       </c>
       <c r="G79" s="38"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" hidden="1">
       <c r="A80" s="38" t="s">
         <v>58</v>
       </c>
@@ -10021,7 +10021,7 @@
       <c r="F80" s="37"/>
       <c r="G80" s="37"/>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" hidden="1">
       <c r="A81" s="38" t="s">
         <v>58</v>
       </c>
@@ -10036,7 +10036,7 @@
       <c r="F81" s="37"/>
       <c r="G81" s="37"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" hidden="1">
       <c r="A82" s="38" t="s">
         <v>58</v>
       </c>
@@ -10057,7 +10057,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" hidden="1">
       <c r="A83" s="38" t="s">
         <v>58</v>
       </c>
@@ -10076,7 +10076,7 @@
       </c>
       <c r="G83" s="38"/>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" hidden="1">
       <c r="A84" s="38" t="s">
         <v>58</v>
       </c>
@@ -10095,7 +10095,7 @@
       </c>
       <c r="G84" s="38"/>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" hidden="1">
       <c r="A85" s="38" t="s">
         <v>58</v>
       </c>
@@ -10114,7 +10114,7 @@
       </c>
       <c r="G85" s="38"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" hidden="1">
       <c r="A86" s="38" t="s">
         <v>58</v>
       </c>
@@ -10133,7 +10133,7 @@
       </c>
       <c r="G86" s="38"/>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" hidden="1">
       <c r="A87" s="38" t="s">
         <v>58</v>
       </c>
@@ -10152,7 +10152,7 @@
       </c>
       <c r="G87" s="38"/>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" hidden="1">
       <c r="A88" s="38" t="s">
         <v>58</v>
       </c>
@@ -10171,7 +10171,7 @@
       </c>
       <c r="G88" s="38"/>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" hidden="1">
       <c r="A89" s="38" t="s">
         <v>131</v>
       </c>
@@ -10190,7 +10190,7 @@
       </c>
       <c r="G89" s="38"/>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" hidden="1">
       <c r="A90" s="38" t="s">
         <v>58</v>
       </c>
@@ -10205,7 +10205,7 @@
       <c r="F90" s="37"/>
       <c r="G90" s="37"/>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" hidden="1">
       <c r="A91" s="38" t="s">
         <v>58</v>
       </c>
@@ -10220,7 +10220,7 @@
       <c r="F91" s="37"/>
       <c r="G91" s="37"/>
     </row>
-    <row r="92" spans="1:7" ht="30">
+    <row r="92" spans="1:7" ht="30" hidden="1">
       <c r="A92" s="38" t="s">
         <v>58</v>
       </c>
@@ -10241,7 +10241,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" hidden="1">
       <c r="A93" s="38" t="s">
         <v>58</v>
       </c>
@@ -10260,7 +10260,7 @@
       </c>
       <c r="G93" s="38"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" hidden="1">
       <c r="A94" s="38" t="s">
         <v>58</v>
       </c>
@@ -10279,7 +10279,7 @@
       </c>
       <c r="G94" s="38"/>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" hidden="1">
       <c r="A95" s="38" t="s">
         <v>58</v>
       </c>
@@ -10298,7 +10298,7 @@
       </c>
       <c r="G95" s="38"/>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" hidden="1">
       <c r="A96" s="38" t="s">
         <v>58</v>
       </c>
@@ -10317,7 +10317,7 @@
       </c>
       <c r="G96" s="38"/>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" hidden="1">
       <c r="A97" s="38" t="s">
         <v>58</v>
       </c>
@@ -10336,7 +10336,7 @@
       </c>
       <c r="G97" s="38"/>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" hidden="1">
       <c r="A98" s="38" t="s">
         <v>58</v>
       </c>
@@ -10355,7 +10355,7 @@
       </c>
       <c r="G98" s="38"/>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" hidden="1">
       <c r="A99" s="38" t="s">
         <v>58</v>
       </c>
@@ -10374,7 +10374,7 @@
       </c>
       <c r="G99" s="38"/>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" hidden="1">
       <c r="A100" s="38" t="s">
         <v>58</v>
       </c>
@@ -10393,7 +10393,7 @@
       </c>
       <c r="G100" s="38"/>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" hidden="1">
       <c r="A101" s="38" t="s">
         <v>131</v>
       </c>
@@ -10412,7 +10412,7 @@
       </c>
       <c r="G101" s="38"/>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" hidden="1">
       <c r="A102" s="38" t="s">
         <v>58</v>
       </c>
@@ -10427,7 +10427,7 @@
       <c r="F102" s="37"/>
       <c r="G102" s="37"/>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" hidden="1">
       <c r="A103" s="38" t="s">
         <v>58</v>
       </c>
@@ -10442,7 +10442,7 @@
       <c r="F103" s="37"/>
       <c r="G103" s="37"/>
     </row>
-    <row r="104" spans="1:7" ht="30">
+    <row r="104" spans="1:7" ht="30" hidden="1">
       <c r="A104" s="38" t="s">
         <v>58</v>
       </c>
@@ -10463,7 +10463,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" hidden="1">
       <c r="A105" s="38" t="s">
         <v>58</v>
       </c>
@@ -10482,7 +10482,7 @@
       </c>
       <c r="G105" s="38"/>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" hidden="1">
       <c r="A106" s="38" t="s">
         <v>58</v>
       </c>
@@ -10501,7 +10501,7 @@
       </c>
       <c r="G106" s="38"/>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" hidden="1">
       <c r="A107" s="38" t="s">
         <v>58</v>
       </c>
@@ -10520,7 +10520,7 @@
       </c>
       <c r="G107" s="38"/>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" hidden="1">
       <c r="A108" s="38" t="s">
         <v>58</v>
       </c>
@@ -10539,7 +10539,7 @@
       </c>
       <c r="G108" s="38"/>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" hidden="1">
       <c r="A109" s="38" t="s">
         <v>58</v>
       </c>
@@ -10558,7 +10558,7 @@
       </c>
       <c r="G109" s="38"/>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" hidden="1">
       <c r="A110" s="38" t="s">
         <v>58</v>
       </c>
@@ -10577,7 +10577,7 @@
       </c>
       <c r="G110" s="38"/>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" hidden="1">
       <c r="A111" s="38" t="s">
         <v>58</v>
       </c>
@@ -10596,7 +10596,7 @@
       </c>
       <c r="G111" s="38"/>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" hidden="1">
       <c r="A112" s="38" t="s">
         <v>58</v>
       </c>
@@ -10615,7 +10615,7 @@
       </c>
       <c r="G112" s="38"/>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" hidden="1">
       <c r="A113" s="38" t="s">
         <v>131</v>
       </c>
@@ -10634,7 +10634,7 @@
       </c>
       <c r="G113" s="38"/>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" hidden="1">
       <c r="A114" s="38" t="s">
         <v>58</v>
       </c>
@@ -10649,7 +10649,7 @@
       <c r="F114" s="37"/>
       <c r="G114" s="37"/>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" hidden="1">
       <c r="A115" s="38" t="s">
         <v>58</v>
       </c>
@@ -10664,7 +10664,7 @@
       <c r="F115" s="37"/>
       <c r="G115" s="37"/>
     </row>
-    <row r="116" spans="1:7" ht="30">
+    <row r="116" spans="1:7" ht="30" hidden="1">
       <c r="A116" s="38" t="s">
         <v>58</v>
       </c>
@@ -10685,7 +10685,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" hidden="1">
       <c r="A117" s="38" t="s">
         <v>58</v>
       </c>
@@ -10704,7 +10704,7 @@
       </c>
       <c r="G117" s="38"/>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" hidden="1">
       <c r="A118" s="38" t="s">
         <v>58</v>
       </c>
@@ -10723,7 +10723,7 @@
       </c>
       <c r="G118" s="38"/>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" hidden="1">
       <c r="A119" s="38" t="s">
         <v>58</v>
       </c>
@@ -10742,7 +10742,7 @@
       </c>
       <c r="G119" s="38"/>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" hidden="1">
       <c r="A120" s="38" t="s">
         <v>58</v>
       </c>
@@ -10761,7 +10761,7 @@
       </c>
       <c r="G120" s="38"/>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" hidden="1">
       <c r="A121" s="38" t="s">
         <v>58</v>
       </c>
@@ -10780,7 +10780,7 @@
       </c>
       <c r="G121" s="38"/>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" hidden="1">
       <c r="A122" s="38" t="s">
         <v>58</v>
       </c>
@@ -10799,7 +10799,7 @@
       </c>
       <c r="G122" s="38"/>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" hidden="1">
       <c r="A123" s="38" t="s">
         <v>58</v>
       </c>
@@ -10818,7 +10818,7 @@
       </c>
       <c r="G123" s="38"/>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" hidden="1">
       <c r="A124" s="38" t="s">
         <v>58</v>
       </c>
@@ -10837,7 +10837,7 @@
       </c>
       <c r="G124" s="38"/>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" hidden="1">
       <c r="A125" s="38" t="s">
         <v>131</v>
       </c>
@@ -10856,7 +10856,7 @@
       </c>
       <c r="G125" s="38"/>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" hidden="1">
       <c r="A126" s="38" t="s">
         <v>58</v>
       </c>
@@ -10871,7 +10871,7 @@
       <c r="F126" s="37"/>
       <c r="G126" s="37"/>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" hidden="1">
       <c r="A127" s="38" t="s">
         <v>58</v>
       </c>
@@ -10886,7 +10886,7 @@
       <c r="F127" s="37"/>
       <c r="G127" s="37"/>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" hidden="1">
       <c r="A128" s="38" t="s">
         <v>58</v>
       </c>
@@ -10907,7 +10907,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" hidden="1">
       <c r="A129" s="38" t="s">
         <v>58</v>
       </c>
@@ -10926,7 +10926,7 @@
       </c>
       <c r="G129" s="38"/>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" hidden="1">
       <c r="A130" s="38" t="s">
         <v>58</v>
       </c>
@@ -10945,7 +10945,7 @@
       </c>
       <c r="G130" s="38"/>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" hidden="1">
       <c r="A131" s="38" t="s">
         <v>58</v>
       </c>
@@ -10964,7 +10964,7 @@
       </c>
       <c r="G131" s="38"/>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" hidden="1">
       <c r="A132" s="38" t="s">
         <v>58</v>
       </c>
@@ -10983,7 +10983,7 @@
       </c>
       <c r="G132" s="38"/>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" hidden="1">
       <c r="A133" s="38" t="s">
         <v>58</v>
       </c>
@@ -11002,7 +11002,7 @@
       </c>
       <c r="G133" s="38"/>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" hidden="1">
       <c r="A134" s="39" t="s">
         <v>58</v>
       </c>
@@ -11021,7 +11021,7 @@
       </c>
       <c r="G134" s="39"/>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" hidden="1">
       <c r="A135" s="38" t="s">
         <v>58</v>
       </c>
@@ -11040,7 +11040,7 @@
       </c>
       <c r="G135" s="38"/>
     </row>
-    <row r="136" spans="1:7" ht="30">
+    <row r="136" spans="1:7" ht="30" hidden="1">
       <c r="A136" s="38" t="s">
         <v>58</v>
       </c>
@@ -11059,7 +11059,7 @@
       </c>
       <c r="G136" s="38"/>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" hidden="1">
       <c r="A137" s="38" t="s">
         <v>58</v>
       </c>
@@ -11074,7 +11074,7 @@
       <c r="F137" s="37"/>
       <c r="G137" s="37"/>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" hidden="1">
       <c r="A138" s="38" t="s">
         <v>58</v>
       </c>
@@ -11089,7 +11089,7 @@
       <c r="F138" s="37"/>
       <c r="G138" s="37"/>
     </row>
-    <row r="139" spans="1:7" ht="30">
+    <row r="139" spans="1:7" ht="30" hidden="1">
       <c r="A139" s="38" t="s">
         <v>58</v>
       </c>
@@ -11112,7 +11112,7 @@
         <v>1248</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" hidden="1">
       <c r="A140" s="38" t="s">
         <v>58</v>
       </c>
@@ -11133,7 +11133,7 @@
       </c>
       <c r="G140" s="38"/>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" hidden="1">
       <c r="A141" s="38" t="s">
         <v>58</v>
       </c>
@@ -11154,7 +11154,7 @@
       </c>
       <c r="G141" s="38"/>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" hidden="1">
       <c r="A142" s="38" t="s">
         <v>58</v>
       </c>
@@ -11175,7 +11175,7 @@
       </c>
       <c r="G142" s="38"/>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" hidden="1">
       <c r="A143" s="38" t="s">
         <v>58</v>
       </c>
@@ -11196,7 +11196,7 @@
       </c>
       <c r="G143" s="38"/>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" hidden="1">
       <c r="A144" s="38" t="s">
         <v>58</v>
       </c>
@@ -11217,7 +11217,7 @@
       </c>
       <c r="G144" s="38"/>
     </row>
-    <row r="145" spans="1:7" ht="19.5" customHeight="1">
+    <row r="145" spans="1:7" ht="19.5" hidden="1" customHeight="1">
       <c r="A145" s="39" t="s">
         <v>58</v>
       </c>
@@ -11236,7 +11236,7 @@
       </c>
       <c r="G145" s="39"/>
     </row>
-    <row r="146" spans="1:7">
+    <row r="146" spans="1:7" hidden="1">
       <c r="A146" s="38" t="s">
         <v>58</v>
       </c>
@@ -11257,7 +11257,7 @@
       </c>
       <c r="G146" s="38"/>
     </row>
-    <row r="147" spans="1:7" ht="45">
+    <row r="147" spans="1:7" ht="45" hidden="1">
       <c r="A147" s="38" t="s">
         <v>58</v>
       </c>
@@ -11278,7 +11278,7 @@
       </c>
       <c r="G147" s="38"/>
     </row>
-    <row r="148" spans="1:7">
+    <row r="148" spans="1:7" hidden="1">
       <c r="A148" s="38" t="s">
         <v>131</v>
       </c>
@@ -11299,7 +11299,7 @@
       </c>
       <c r="G148" s="38"/>
     </row>
-    <row r="149" spans="1:7">
+    <row r="149" spans="1:7" hidden="1">
       <c r="A149" s="38" t="s">
         <v>131</v>
       </c>
@@ -11318,7 +11318,7 @@
       </c>
       <c r="G149" s="38"/>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" hidden="1">
       <c r="A150" s="38" t="s">
         <v>58</v>
       </c>
@@ -11335,7 +11335,7 @@
       <c r="F150" s="37"/>
       <c r="G150" s="37"/>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" hidden="1">
       <c r="A151" s="38" t="s">
         <v>58</v>
       </c>
@@ -11352,7 +11352,7 @@
       <c r="F151" s="37"/>
       <c r="G151" s="37"/>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" hidden="1">
       <c r="A152" s="38" t="s">
         <v>58</v>
       </c>
@@ -11373,7 +11373,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" hidden="1">
       <c r="A153" s="38" t="s">
         <v>58</v>
       </c>
@@ -11394,7 +11394,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="154" spans="1:7">
+    <row r="154" spans="1:7" hidden="1">
       <c r="A154" s="38" t="s">
         <v>58</v>
       </c>
@@ -11415,7 +11415,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" hidden="1">
       <c r="A155" s="38" t="s">
         <v>58</v>
       </c>
@@ -11432,7 +11432,7 @@
       <c r="F155" s="37"/>
       <c r="G155" s="41"/>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" hidden="1">
       <c r="A156" s="38" t="s">
         <v>58</v>
       </c>
@@ -11449,7 +11449,7 @@
       <c r="F156" s="37"/>
       <c r="G156" s="41"/>
     </row>
-    <row r="157" spans="1:7">
+    <row r="157" spans="1:7" hidden="1">
       <c r="A157" s="38" t="s">
         <v>58</v>
       </c>
@@ -11466,7 +11466,7 @@
       <c r="F157" s="37"/>
       <c r="G157" s="41"/>
     </row>
-    <row r="158" spans="1:7" ht="15.6">
+    <row r="158" spans="1:7" ht="15.6" hidden="1">
       <c r="A158" s="35" t="s">
         <v>58</v>
       </c>
@@ -11481,7 +11481,7 @@
       <c r="F158" s="37"/>
       <c r="G158" s="36"/>
     </row>
-    <row r="159" spans="1:7">
+    <row r="159" spans="1:7" hidden="1">
       <c r="A159" s="38" t="s">
         <v>58</v>
       </c>
@@ -11496,7 +11496,7 @@
       <c r="F159" s="37"/>
       <c r="G159" s="37"/>
     </row>
-    <row r="160" spans="1:7">
+    <row r="160" spans="1:7" hidden="1">
       <c r="A160" s="38" t="s">
         <v>58</v>
       </c>
@@ -11511,7 +11511,7 @@
       <c r="F160" s="37"/>
       <c r="G160" s="41"/>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" hidden="1">
       <c r="A161" s="38" t="s">
         <v>58</v>
       </c>
@@ -11530,7 +11530,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" hidden="1">
       <c r="A162" s="38" t="s">
         <v>58</v>
       </c>
@@ -11547,7 +11547,7 @@
       <c r="F162" s="38"/>
       <c r="G162" s="38"/>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" hidden="1">
       <c r="A163" s="38" t="s">
         <v>58</v>
       </c>
@@ -11564,7 +11564,7 @@
       <c r="F163" s="38"/>
       <c r="G163" s="38"/>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" hidden="1">
       <c r="A164" s="38" t="s">
         <v>58</v>
       </c>
@@ -11581,7 +11581,7 @@
       <c r="F164" s="38"/>
       <c r="G164" s="38"/>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" hidden="1">
       <c r="A165" s="38" t="s">
         <v>58</v>
       </c>
@@ -11600,7 +11600,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" hidden="1">
       <c r="A166" s="38" t="s">
         <v>58</v>
       </c>
@@ -11615,7 +11615,7 @@
       <c r="F166" s="41"/>
       <c r="G166" s="41"/>
     </row>
-    <row r="167" spans="1:8" s="70" customFormat="1">
+    <row r="167" spans="1:8" s="70" customFormat="1" hidden="1">
       <c r="A167" s="40" t="s">
         <v>58</v>
       </c>
@@ -11633,7 +11633,7 @@
       <c r="G167" s="40"/>
       <c r="H167" s="69"/>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" hidden="1">
       <c r="A168" s="38" t="s">
         <v>58</v>
       </c>
@@ -11650,7 +11650,7 @@
       <c r="F168" s="38"/>
       <c r="G168" s="38"/>
     </row>
-    <row r="169" spans="1:8" ht="30">
+    <row r="169" spans="1:8" ht="30" hidden="1">
       <c r="A169" s="38" t="s">
         <v>58</v>
       </c>
@@ -11667,7 +11667,7 @@
       <c r="F169" s="38"/>
       <c r="G169" s="38"/>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" hidden="1">
       <c r="A170" s="38" t="s">
         <v>58</v>
       </c>
@@ -11684,7 +11684,7 @@
       <c r="F170" s="40"/>
       <c r="G170" s="38"/>
     </row>
-    <row r="171" spans="1:8" ht="30">
+    <row r="171" spans="1:8" ht="30" hidden="1">
       <c r="A171" s="38" t="s">
         <v>58</v>
       </c>
@@ -11701,7 +11701,7 @@
       <c r="F171" s="40"/>
       <c r="G171" s="38"/>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" hidden="1">
       <c r="A172" s="38" t="s">
         <v>58</v>
       </c>
@@ -11718,7 +11718,7 @@
       <c r="F172" s="40"/>
       <c r="G172" s="38"/>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" hidden="1">
       <c r="A173" s="38" t="s">
         <v>58</v>
       </c>
@@ -11735,7 +11735,7 @@
       <c r="F173" s="40"/>
       <c r="G173" s="38"/>
     </row>
-    <row r="174" spans="1:8" ht="30">
+    <row r="174" spans="1:8" ht="30" hidden="1">
       <c r="A174" s="38" t="s">
         <v>58</v>
       </c>
@@ -11752,7 +11752,7 @@
       <c r="F174" s="40"/>
       <c r="G174" s="38"/>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" hidden="1">
       <c r="A175" s="38" t="s">
         <v>58</v>
       </c>
@@ -11769,7 +11769,7 @@
       <c r="F175" s="40"/>
       <c r="G175" s="38"/>
     </row>
-    <row r="176" spans="1:8" ht="45">
+    <row r="176" spans="1:8" ht="45" hidden="1">
       <c r="A176" s="38" t="s">
         <v>58</v>
       </c>
@@ -11786,7 +11786,7 @@
       <c r="F176" s="38"/>
       <c r="G176" s="38"/>
     </row>
-    <row r="177" spans="1:7" ht="30">
+    <row r="177" spans="1:7" ht="30" hidden="1">
       <c r="A177" s="38" t="s">
         <v>58</v>
       </c>
@@ -11803,7 +11803,7 @@
       <c r="F177" s="38"/>
       <c r="G177" s="38"/>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" hidden="1">
       <c r="A178" s="38" t="s">
         <v>58</v>
       </c>
@@ -11820,7 +11820,7 @@
       <c r="F178" s="38"/>
       <c r="G178" s="38"/>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" hidden="1">
       <c r="A179" s="38" t="s">
         <v>58</v>
       </c>
@@ -11835,7 +11835,7 @@
       <c r="F179" s="41"/>
       <c r="G179" s="42"/>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" hidden="1">
       <c r="A180" s="38" t="s">
         <v>58</v>
       </c>
@@ -11850,7 +11850,7 @@
       <c r="F180" s="41"/>
       <c r="G180" s="41"/>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" hidden="1">
       <c r="A181" s="38" t="s">
         <v>58</v>
       </c>
@@ -11869,7 +11869,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" hidden="1">
       <c r="A182" s="38" t="s">
         <v>58</v>
       </c>
@@ -11886,7 +11886,7 @@
       <c r="F182" s="38"/>
       <c r="G182" s="38"/>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" hidden="1">
       <c r="A183" s="38" t="s">
         <v>58</v>
       </c>
@@ -11903,7 +11903,7 @@
       <c r="F183" s="38"/>
       <c r="G183" s="38"/>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" hidden="1">
       <c r="A184" s="38" t="s">
         <v>58</v>
       </c>
@@ -11920,7 +11920,7 @@
       <c r="F184" s="38"/>
       <c r="G184" s="38"/>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" hidden="1">
       <c r="A185" s="38" t="s">
         <v>58</v>
       </c>
@@ -11935,7 +11935,7 @@
       <c r="F185" s="41"/>
       <c r="G185" s="41"/>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" hidden="1">
       <c r="A186" s="38" t="s">
         <v>58</v>
       </c>
@@ -11954,7 +11954,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" hidden="1">
       <c r="A187" s="38" t="s">
         <v>58</v>
       </c>
@@ -11971,7 +11971,7 @@
       <c r="F187" s="38"/>
       <c r="G187" s="38"/>
     </row>
-    <row r="188" spans="1:7" ht="30">
+    <row r="188" spans="1:7" ht="30" hidden="1">
       <c r="A188" s="38" t="s">
         <v>58</v>
       </c>
@@ -11988,7 +11988,7 @@
       <c r="F188" s="38"/>
       <c r="G188" s="38"/>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" hidden="1">
       <c r="A189" s="38" t="s">
         <v>58</v>
       </c>
@@ -12005,7 +12005,7 @@
       <c r="F189" s="40"/>
       <c r="G189" s="38"/>
     </row>
-    <row r="190" spans="1:7" ht="30">
+    <row r="190" spans="1:7" ht="30" hidden="1">
       <c r="A190" s="38" t="s">
         <v>58</v>
       </c>
@@ -12022,7 +12022,7 @@
       <c r="F190" s="40"/>
       <c r="G190" s="38"/>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" hidden="1">
       <c r="A191" s="38" t="s">
         <v>58</v>
       </c>
@@ -12039,7 +12039,7 @@
       <c r="F191" s="40"/>
       <c r="G191" s="38"/>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" hidden="1">
       <c r="A192" s="38" t="s">
         <v>58</v>
       </c>
@@ -12056,7 +12056,7 @@
       <c r="F192" s="40"/>
       <c r="G192" s="38"/>
     </row>
-    <row r="193" spans="1:7" ht="30">
+    <row r="193" spans="1:7" ht="30" hidden="1">
       <c r="A193" s="38" t="s">
         <v>58</v>
       </c>
@@ -12073,7 +12073,7 @@
       <c r="F193" s="40"/>
       <c r="G193" s="38"/>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" hidden="1">
       <c r="A194" s="38" t="s">
         <v>58</v>
       </c>
@@ -12090,7 +12090,7 @@
       <c r="F194" s="40"/>
       <c r="G194" s="38"/>
     </row>
-    <row r="195" spans="1:7" ht="45">
+    <row r="195" spans="1:7" ht="45" hidden="1">
       <c r="A195" s="38" t="s">
         <v>58</v>
       </c>
@@ -12107,7 +12107,7 @@
       <c r="F195" s="38"/>
       <c r="G195" s="38"/>
     </row>
-    <row r="196" spans="1:7" ht="30">
+    <row r="196" spans="1:7" ht="30" hidden="1">
       <c r="A196" s="38" t="s">
         <v>58</v>
       </c>
@@ -12124,7 +12124,7 @@
       <c r="F196" s="38"/>
       <c r="G196" s="38"/>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" hidden="1">
       <c r="A197" s="38" t="s">
         <v>58</v>
       </c>
@@ -12141,7 +12141,7 @@
       <c r="F197" s="38"/>
       <c r="G197" s="38"/>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:7" hidden="1">
       <c r="A198" s="38" t="s">
         <v>58</v>
       </c>
@@ -12156,7 +12156,7 @@
       <c r="F198" s="41"/>
       <c r="G198" s="41"/>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" hidden="1">
       <c r="A199" s="38" t="s">
         <v>58</v>
       </c>
@@ -12171,7 +12171,7 @@
       <c r="F199" s="41"/>
       <c r="G199" s="41"/>
     </row>
-    <row r="200" spans="1:7">
+    <row r="200" spans="1:7" hidden="1">
       <c r="A200" s="38" t="s">
         <v>58</v>
       </c>
@@ -12190,7 +12190,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="201" spans="1:7">
+    <row r="201" spans="1:7" hidden="1">
       <c r="A201" s="38" t="s">
         <v>58</v>
       </c>
@@ -12207,7 +12207,7 @@
       <c r="F201" s="38"/>
       <c r="G201" s="38"/>
     </row>
-    <row r="202" spans="1:7">
+    <row r="202" spans="1:7" hidden="1">
       <c r="A202" s="38" t="s">
         <v>58</v>
       </c>
@@ -12224,7 +12224,7 @@
       <c r="F202" s="38"/>
       <c r="G202" s="38"/>
     </row>
-    <row r="203" spans="1:7">
+    <row r="203" spans="1:7" hidden="1">
       <c r="A203" s="38" t="s">
         <v>58</v>
       </c>
@@ -12241,7 +12241,7 @@
       <c r="F203" s="38"/>
       <c r="G203" s="38"/>
     </row>
-    <row r="204" spans="1:7">
+    <row r="204" spans="1:7" hidden="1">
       <c r="A204" s="38" t="s">
         <v>58</v>
       </c>
@@ -12256,7 +12256,7 @@
       <c r="F204" s="41"/>
       <c r="G204" s="41"/>
     </row>
-    <row r="205" spans="1:7" ht="42" customHeight="1">
+    <row r="205" spans="1:7" ht="42" hidden="1" customHeight="1">
       <c r="A205" s="38" t="s">
         <v>58</v>
       </c>
@@ -12275,7 +12275,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="206" spans="1:7">
+    <row r="206" spans="1:7" hidden="1">
       <c r="A206" s="38" t="s">
         <v>58</v>
       </c>
@@ -12292,7 +12292,7 @@
       <c r="F206" s="38"/>
       <c r="G206" s="38"/>
     </row>
-    <row r="207" spans="1:7" ht="36.75" customHeight="1">
+    <row r="207" spans="1:7" ht="36.75" hidden="1" customHeight="1">
       <c r="A207" s="38" t="s">
         <v>58</v>
       </c>
@@ -12309,7 +12309,7 @@
       <c r="F207" s="38"/>
       <c r="G207" s="38"/>
     </row>
-    <row r="208" spans="1:7">
+    <row r="208" spans="1:7" hidden="1">
       <c r="A208" s="38" t="s">
         <v>58</v>
       </c>
@@ -12326,7 +12326,7 @@
       <c r="F208" s="40"/>
       <c r="G208" s="38"/>
     </row>
-    <row r="209" spans="1:7" ht="30">
+    <row r="209" spans="1:7" ht="30" hidden="1">
       <c r="A209" s="38" t="s">
         <v>58</v>
       </c>
@@ -12343,7 +12343,7 @@
       <c r="F209" s="40"/>
       <c r="G209" s="38"/>
     </row>
-    <row r="210" spans="1:7">
+    <row r="210" spans="1:7" hidden="1">
       <c r="A210" s="38" t="s">
         <v>58</v>
       </c>
@@ -12360,7 +12360,7 @@
       <c r="F210" s="40"/>
       <c r="G210" s="38"/>
     </row>
-    <row r="211" spans="1:7">
+    <row r="211" spans="1:7" hidden="1">
       <c r="A211" s="38" t="s">
         <v>58</v>
       </c>
@@ -12377,7 +12377,7 @@
       <c r="F211" s="40"/>
       <c r="G211" s="38"/>
     </row>
-    <row r="212" spans="1:7" ht="30">
+    <row r="212" spans="1:7" ht="30" hidden="1">
       <c r="A212" s="38" t="s">
         <v>58</v>
       </c>
@@ -12394,7 +12394,7 @@
       <c r="F212" s="40"/>
       <c r="G212" s="38"/>
     </row>
-    <row r="213" spans="1:7">
+    <row r="213" spans="1:7" hidden="1">
       <c r="A213" s="38" t="s">
         <v>58</v>
       </c>
@@ -12411,7 +12411,7 @@
       <c r="F213" s="40"/>
       <c r="G213" s="38"/>
     </row>
-    <row r="214" spans="1:7" ht="45">
+    <row r="214" spans="1:7" ht="45" hidden="1">
       <c r="A214" s="38" t="s">
         <v>58</v>
       </c>
@@ -12428,7 +12428,7 @@
       <c r="F214" s="38"/>
       <c r="G214" s="38"/>
     </row>
-    <row r="215" spans="1:7" ht="30">
+    <row r="215" spans="1:7" ht="30" hidden="1">
       <c r="A215" s="38" t="s">
         <v>58</v>
       </c>
@@ -12445,7 +12445,7 @@
       <c r="F215" s="38"/>
       <c r="G215" s="38"/>
     </row>
-    <row r="216" spans="1:7">
+    <row r="216" spans="1:7" hidden="1">
       <c r="A216" s="38" t="s">
         <v>58</v>
       </c>
@@ -12462,7 +12462,7 @@
       <c r="F216" s="38"/>
       <c r="G216" s="38"/>
     </row>
-    <row r="217" spans="1:7">
+    <row r="217" spans="1:7" hidden="1">
       <c r="A217" s="38" t="s">
         <v>58</v>
       </c>
@@ -12477,7 +12477,7 @@
       <c r="F217" s="41"/>
       <c r="G217" s="43"/>
     </row>
-    <row r="218" spans="1:7">
+    <row r="218" spans="1:7" hidden="1">
       <c r="A218" s="38" t="s">
         <v>58</v>
       </c>
@@ -12492,7 +12492,7 @@
       <c r="F218" s="41"/>
       <c r="G218" s="41"/>
     </row>
-    <row r="219" spans="1:7" ht="30">
+    <row r="219" spans="1:7" ht="30" hidden="1">
       <c r="A219" s="38" t="s">
         <v>58</v>
       </c>
@@ -12511,7 +12511,7 @@
         <v>1131</v>
       </c>
     </row>
-    <row r="220" spans="1:7">
+    <row r="220" spans="1:7" hidden="1">
       <c r="A220" s="38" t="s">
         <v>58</v>
       </c>
@@ -12528,7 +12528,7 @@
       <c r="F220" s="38"/>
       <c r="G220" s="38"/>
     </row>
-    <row r="221" spans="1:7">
+    <row r="221" spans="1:7" hidden="1">
       <c r="A221" s="38" t="s">
         <v>58</v>
       </c>
@@ -12545,7 +12545,7 @@
       <c r="F221" s="38"/>
       <c r="G221" s="38"/>
     </row>
-    <row r="222" spans="1:7" ht="30">
+    <row r="222" spans="1:7" ht="30" hidden="1">
       <c r="A222" s="38" t="s">
         <v>58</v>
       </c>
@@ -12562,7 +12562,7 @@
       <c r="F222" s="38"/>
       <c r="G222" s="38"/>
     </row>
-    <row r="223" spans="1:7" ht="30">
+    <row r="223" spans="1:7" ht="30" hidden="1">
       <c r="A223" s="38" t="s">
         <v>58</v>
       </c>
@@ -12579,7 +12579,7 @@
       <c r="F223" s="38"/>
       <c r="G223" s="38"/>
     </row>
-    <row r="224" spans="1:7">
+    <row r="224" spans="1:7" hidden="1">
       <c r="A224" s="38" t="s">
         <v>58</v>
       </c>
@@ -12596,7 +12596,7 @@
       <c r="F224" s="40"/>
       <c r="G224" s="38"/>
     </row>
-    <row r="225" spans="1:7">
+    <row r="225" spans="1:7" hidden="1">
       <c r="A225" s="38" t="s">
         <v>58</v>
       </c>
@@ -12613,7 +12613,7 @@
       <c r="F225" s="38"/>
       <c r="G225" s="38"/>
     </row>
-    <row r="226" spans="1:7">
+    <row r="226" spans="1:7" hidden="1">
       <c r="A226" s="38" t="s">
         <v>58</v>
       </c>
@@ -12632,7 +12632,7 @@
       <c r="F226" s="38"/>
       <c r="G226" s="38"/>
     </row>
-    <row r="227" spans="1:7" ht="30">
+    <row r="227" spans="1:7" ht="30" hidden="1">
       <c r="A227" s="38" t="s">
         <v>58</v>
       </c>
@@ -12651,7 +12651,7 @@
       <c r="F227" s="38"/>
       <c r="G227" s="38"/>
     </row>
-    <row r="228" spans="1:7">
+    <row r="228" spans="1:7" hidden="1">
       <c r="A228" s="38" t="s">
         <v>58</v>
       </c>
@@ -12668,7 +12668,7 @@
       <c r="F228" s="38"/>
       <c r="G228" s="38"/>
     </row>
-    <row r="229" spans="1:7">
+    <row r="229" spans="1:7" hidden="1">
       <c r="A229" s="38" t="s">
         <v>58</v>
       </c>
@@ -12685,7 +12685,7 @@
       <c r="F229" s="38"/>
       <c r="G229" s="38"/>
     </row>
-    <row r="230" spans="1:7">
+    <row r="230" spans="1:7" hidden="1">
       <c r="A230" s="38" t="s">
         <v>58</v>
       </c>
@@ -12702,7 +12702,7 @@
       <c r="F230" s="38"/>
       <c r="G230" s="38"/>
     </row>
-    <row r="231" spans="1:7">
+    <row r="231" spans="1:7" hidden="1">
       <c r="A231" s="38" t="s">
         <v>58</v>
       </c>
@@ -12717,7 +12717,7 @@
       <c r="F231" s="41"/>
       <c r="G231" s="41"/>
     </row>
-    <row r="232" spans="1:7">
+    <row r="232" spans="1:7" hidden="1">
       <c r="A232" s="38" t="s">
         <v>58</v>
       </c>
@@ -12736,7 +12736,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="233" spans="1:7">
+    <row r="233" spans="1:7" hidden="1">
       <c r="A233" s="38" t="s">
         <v>58</v>
       </c>
@@ -12753,7 +12753,7 @@
       <c r="F233" s="38"/>
       <c r="G233" s="38"/>
     </row>
-    <row r="234" spans="1:7">
+    <row r="234" spans="1:7" hidden="1">
       <c r="A234" s="38" t="s">
         <v>58</v>
       </c>
@@ -12770,7 +12770,7 @@
       <c r="F234" s="38"/>
       <c r="G234" s="38"/>
     </row>
-    <row r="235" spans="1:7">
+    <row r="235" spans="1:7" hidden="1">
       <c r="A235" s="38" t="s">
         <v>58</v>
       </c>
@@ -12787,7 +12787,7 @@
       <c r="F235" s="38"/>
       <c r="G235" s="38"/>
     </row>
-    <row r="236" spans="1:7">
+    <row r="236" spans="1:7" hidden="1">
       <c r="A236" s="38" t="s">
         <v>58</v>
       </c>
@@ -12806,7 +12806,7 @@
       <c r="F236" s="40"/>
       <c r="G236" s="38"/>
     </row>
-    <row r="237" spans="1:7">
+    <row r="237" spans="1:7" hidden="1">
       <c r="A237" s="38" t="s">
         <v>58</v>
       </c>
@@ -12823,7 +12823,7 @@
       <c r="F237" s="38"/>
       <c r="G237" s="38"/>
     </row>
-    <row r="238" spans="1:7">
+    <row r="238" spans="1:7" hidden="1">
       <c r="A238" s="38" t="s">
         <v>58</v>
       </c>
@@ -12840,7 +12840,7 @@
       <c r="F238" s="38"/>
       <c r="G238" s="38"/>
     </row>
-    <row r="239" spans="1:7">
+    <row r="239" spans="1:7" hidden="1">
       <c r="A239" s="38" t="s">
         <v>58</v>
       </c>
@@ -12857,7 +12857,7 @@
       <c r="F239" s="38"/>
       <c r="G239" s="38"/>
     </row>
-    <row r="240" spans="1:7">
+    <row r="240" spans="1:7" hidden="1">
       <c r="A240" s="38" t="s">
         <v>58</v>
       </c>
@@ -12874,7 +12874,7 @@
       <c r="F240" s="38"/>
       <c r="G240" s="38"/>
     </row>
-    <row r="241" spans="1:7">
+    <row r="241" spans="1:7" hidden="1">
       <c r="A241" s="38" t="s">
         <v>58</v>
       </c>
@@ -12891,7 +12891,7 @@
       <c r="F241" s="38"/>
       <c r="G241" s="38"/>
     </row>
-    <row r="242" spans="1:7">
+    <row r="242" spans="1:7" hidden="1">
       <c r="A242" s="38" t="s">
         <v>58</v>
       </c>
@@ -12908,7 +12908,7 @@
       <c r="F242" s="38"/>
       <c r="G242" s="38"/>
     </row>
-    <row r="243" spans="1:7">
+    <row r="243" spans="1:7" hidden="1">
       <c r="A243" s="38" t="s">
         <v>58</v>
       </c>
@@ -12923,7 +12923,7 @@
       <c r="F243" s="41"/>
       <c r="G243" s="41"/>
     </row>
-    <row r="244" spans="1:7">
+    <row r="244" spans="1:7" hidden="1">
       <c r="A244" s="38" t="s">
         <v>58</v>
       </c>
@@ -12942,7 +12942,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="245" spans="1:7">
+    <row r="245" spans="1:7" hidden="1">
       <c r="A245" s="38" t="s">
         <v>58</v>
       </c>
@@ -12959,7 +12959,7 @@
       <c r="F245" s="38"/>
       <c r="G245" s="38"/>
     </row>
-    <row r="246" spans="1:7">
+    <row r="246" spans="1:7" hidden="1">
       <c r="A246" s="38" t="s">
         <v>58</v>
       </c>
@@ -12974,7 +12974,7 @@
       <c r="F246" s="41"/>
       <c r="G246" s="41"/>
     </row>
-    <row r="247" spans="1:7">
+    <row r="247" spans="1:7" hidden="1">
       <c r="A247" s="38" t="s">
         <v>58</v>
       </c>
@@ -12991,7 +12991,7 @@
       <c r="F247" s="38"/>
       <c r="G247" s="38"/>
     </row>
-    <row r="248" spans="1:7">
+    <row r="248" spans="1:7" hidden="1">
       <c r="A248" s="38" t="s">
         <v>58</v>
       </c>
@@ -13006,7 +13006,7 @@
       <c r="F248" s="38"/>
       <c r="G248" s="43"/>
     </row>
-    <row r="249" spans="1:7">
+    <row r="249" spans="1:7" hidden="1">
       <c r="A249" s="38" t="s">
         <v>58</v>
       </c>
@@ -13023,7 +13023,7 @@
       <c r="F249" s="38"/>
       <c r="G249" s="38"/>
     </row>
-    <row r="250" spans="1:7">
+    <row r="250" spans="1:7" hidden="1">
       <c r="A250" s="38" t="s">
         <v>58</v>
       </c>
@@ -13040,7 +13040,7 @@
       <c r="F250" s="38"/>
       <c r="G250" s="38"/>
     </row>
-    <row r="251" spans="1:7">
+    <row r="251" spans="1:7" hidden="1">
       <c r="A251" s="38" t="s">
         <v>58</v>
       </c>
@@ -13055,7 +13055,7 @@
       <c r="F251" s="41"/>
       <c r="G251" s="41"/>
     </row>
-    <row r="252" spans="1:7">
+    <row r="252" spans="1:7" hidden="1">
       <c r="A252" s="38" t="s">
         <v>58</v>
       </c>
@@ -13072,7 +13072,7 @@
       <c r="F252" s="38"/>
       <c r="G252" s="38"/>
     </row>
-    <row r="253" spans="1:7">
+    <row r="253" spans="1:7" hidden="1">
       <c r="A253" s="38" t="s">
         <v>58</v>
       </c>
@@ -13089,7 +13089,7 @@
       <c r="F253" s="38"/>
       <c r="G253" s="38"/>
     </row>
-    <row r="254" spans="1:7" ht="15.6">
+    <row r="254" spans="1:7" ht="15.6" hidden="1">
       <c r="A254" s="38" t="s">
         <v>58</v>
       </c>
@@ -13104,7 +13104,7 @@
       <c r="F254" s="41"/>
       <c r="G254" s="45"/>
     </row>
-    <row r="255" spans="1:7">
+    <row r="255" spans="1:7" hidden="1">
       <c r="A255" s="38" t="s">
         <v>58</v>
       </c>
@@ -13119,7 +13119,7 @@
       <c r="F255" s="41"/>
       <c r="G255" s="41"/>
     </row>
-    <row r="256" spans="1:7">
+    <row r="256" spans="1:7" hidden="1">
       <c r="A256" s="38" t="s">
         <v>58</v>
       </c>
@@ -13134,7 +13134,7 @@
       <c r="F256" s="41"/>
       <c r="G256" s="41"/>
     </row>
-    <row r="257" spans="1:7" ht="30">
+    <row r="257" spans="1:7" ht="30" hidden="1">
       <c r="A257" s="38" t="s">
         <v>58</v>
       </c>
@@ -13153,7 +13153,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="258" spans="1:7">
+    <row r="258" spans="1:7" hidden="1">
       <c r="A258" s="38" t="s">
         <v>58</v>
       </c>
@@ -13170,7 +13170,7 @@
       <c r="F258" s="38"/>
       <c r="G258" s="44"/>
     </row>
-    <row r="259" spans="1:7">
+    <row r="259" spans="1:7" hidden="1">
       <c r="A259" s="38" t="s">
         <v>58</v>
       </c>
@@ -13189,7 +13189,7 @@
       <c r="F259" s="38"/>
       <c r="G259" s="44"/>
     </row>
-    <row r="260" spans="1:7" ht="30">
+    <row r="260" spans="1:7" ht="30" hidden="1">
       <c r="A260" s="38" t="s">
         <v>58</v>
       </c>
@@ -13206,7 +13206,7 @@
       <c r="F260" s="38"/>
       <c r="G260" s="44"/>
     </row>
-    <row r="261" spans="1:7">
+    <row r="261" spans="1:7" hidden="1">
       <c r="A261" s="38" t="s">
         <v>58</v>
       </c>
@@ -13223,7 +13223,7 @@
       <c r="F261" s="38"/>
       <c r="G261" s="44"/>
     </row>
-    <row r="262" spans="1:7">
+    <row r="262" spans="1:7" hidden="1">
       <c r="A262" s="38" t="s">
         <v>58</v>
       </c>
@@ -13240,7 +13240,7 @@
       <c r="F262" s="38"/>
       <c r="G262" s="44"/>
     </row>
-    <row r="263" spans="1:7" ht="30">
+    <row r="263" spans="1:7" ht="30" hidden="1">
       <c r="A263" s="38" t="s">
         <v>58</v>
       </c>
@@ -13257,7 +13257,7 @@
       <c r="F263" s="38"/>
       <c r="G263" s="44"/>
     </row>
-    <row r="264" spans="1:7">
+    <row r="264" spans="1:7" hidden="1">
       <c r="A264" s="38" t="s">
         <v>58</v>
       </c>
@@ -13276,7 +13276,7 @@
       <c r="F264" s="38"/>
       <c r="G264" s="44"/>
     </row>
-    <row r="265" spans="1:7" ht="30">
+    <row r="265" spans="1:7" ht="30" hidden="1">
       <c r="A265" s="38" t="s">
         <v>58</v>
       </c>
@@ -13293,7 +13293,7 @@
       <c r="F265" s="38"/>
       <c r="G265" s="44"/>
     </row>
-    <row r="266" spans="1:7" ht="45">
+    <row r="266" spans="1:7" ht="45" hidden="1">
       <c r="A266" s="38" t="s">
         <v>58</v>
       </c>
@@ -13310,7 +13310,7 @@
       <c r="F266" s="38"/>
       <c r="G266" s="44"/>
     </row>
-    <row r="267" spans="1:7" ht="30">
+    <row r="267" spans="1:7" ht="30" hidden="1">
       <c r="A267" s="38" t="s">
         <v>58</v>
       </c>
@@ -13327,7 +13327,7 @@
       <c r="F267" s="38"/>
       <c r="G267" s="44"/>
     </row>
-    <row r="268" spans="1:7" ht="45">
+    <row r="268" spans="1:7" ht="45" hidden="1">
       <c r="A268" s="38" t="s">
         <v>58</v>
       </c>
@@ -13346,7 +13346,7 @@
       <c r="F268" s="38"/>
       <c r="G268" s="44"/>
     </row>
-    <row r="269" spans="1:7">
+    <row r="269" spans="1:7" hidden="1">
       <c r="A269" s="38" t="s">
         <v>58</v>
       </c>
@@ -13363,7 +13363,7 @@
       <c r="F269" s="38"/>
       <c r="G269" s="44"/>
     </row>
-    <row r="270" spans="1:7">
+    <row r="270" spans="1:7" hidden="1">
       <c r="A270" s="38" t="s">
         <v>58</v>
       </c>
@@ -13378,7 +13378,7 @@
       <c r="F270" s="41"/>
       <c r="G270" s="41"/>
     </row>
-    <row r="271" spans="1:7">
+    <row r="271" spans="1:7" hidden="1">
       <c r="A271" s="38" t="s">
         <v>58</v>
       </c>
@@ -13393,7 +13393,7 @@
       <c r="F271" s="41"/>
       <c r="G271" s="41"/>
     </row>
-    <row r="272" spans="1:7" ht="30">
+    <row r="272" spans="1:7" ht="30" hidden="1">
       <c r="A272" s="38" t="s">
         <v>58</v>
       </c>
@@ -13412,7 +13412,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="273" spans="1:7">
+    <row r="273" spans="1:7" hidden="1">
       <c r="A273" s="38" t="s">
         <v>58</v>
       </c>
@@ -13429,7 +13429,7 @@
       <c r="F273" s="38"/>
       <c r="G273" s="44"/>
     </row>
-    <row r="274" spans="1:7">
+    <row r="274" spans="1:7" hidden="1">
       <c r="A274" s="38" t="s">
         <v>58</v>
       </c>
@@ -13446,7 +13446,7 @@
       <c r="F274" s="38"/>
       <c r="G274" s="44"/>
     </row>
-    <row r="275" spans="1:7" ht="30">
+    <row r="275" spans="1:7" ht="30" hidden="1">
       <c r="A275" s="38" t="s">
         <v>58</v>
       </c>
@@ -13463,7 +13463,7 @@
       <c r="F275" s="38"/>
       <c r="G275" s="44"/>
     </row>
-    <row r="276" spans="1:7">
+    <row r="276" spans="1:7" hidden="1">
       <c r="A276" s="38" t="s">
         <v>58</v>
       </c>
@@ -13480,7 +13480,7 @@
       <c r="F276" s="38"/>
       <c r="G276" s="44"/>
     </row>
-    <row r="277" spans="1:7">
+    <row r="277" spans="1:7" hidden="1">
       <c r="A277" s="38" t="s">
         <v>58</v>
       </c>
@@ -13497,7 +13497,7 @@
       <c r="F277" s="38"/>
       <c r="G277" s="44"/>
     </row>
-    <row r="278" spans="1:7">
+    <row r="278" spans="1:7" hidden="1">
       <c r="A278" s="38" t="s">
         <v>58</v>
       </c>
@@ -13514,7 +13514,7 @@
       <c r="F278" s="38"/>
       <c r="G278" s="44"/>
     </row>
-    <row r="279" spans="1:7" ht="30">
+    <row r="279" spans="1:7" ht="30" hidden="1">
       <c r="A279" s="38" t="s">
         <v>58</v>
       </c>
@@ -13531,7 +13531,7 @@
       <c r="F279" s="38"/>
       <c r="G279" s="44"/>
     </row>
-    <row r="280" spans="1:7">
+    <row r="280" spans="1:7" hidden="1">
       <c r="A280" s="38" t="s">
         <v>58</v>
       </c>
@@ -13548,7 +13548,7 @@
       <c r="F280" s="38"/>
       <c r="G280" s="44"/>
     </row>
-    <row r="281" spans="1:7" ht="30">
+    <row r="281" spans="1:7" ht="30" hidden="1">
       <c r="A281" s="38" t="s">
         <v>58</v>
       </c>
@@ -13565,7 +13565,7 @@
       <c r="F281" s="38"/>
       <c r="G281" s="44"/>
     </row>
-    <row r="282" spans="1:7" ht="30">
+    <row r="282" spans="1:7" ht="30" hidden="1">
       <c r="A282" s="38" t="s">
         <v>58</v>
       </c>
@@ -13582,7 +13582,7 @@
       <c r="F282" s="38"/>
       <c r="G282" s="44"/>
     </row>
-    <row r="283" spans="1:7" ht="30">
+    <row r="283" spans="1:7" ht="30" hidden="1">
       <c r="A283" s="38" t="s">
         <v>58</v>
       </c>
@@ -13599,7 +13599,7 @@
       <c r="F283" s="38"/>
       <c r="G283" s="38"/>
     </row>
-    <row r="284" spans="1:7" ht="45">
+    <row r="284" spans="1:7" ht="45" hidden="1">
       <c r="A284" s="38" t="s">
         <v>58</v>
       </c>
@@ -13616,7 +13616,7 @@
       <c r="F284" s="38"/>
       <c r="G284" s="44"/>
     </row>
-    <row r="285" spans="1:7" ht="45">
+    <row r="285" spans="1:7" ht="45" hidden="1">
       <c r="A285" s="38" t="s">
         <v>58</v>
       </c>
@@ -13633,7 +13633,7 @@
       <c r="F285" s="38"/>
       <c r="G285" s="38"/>
     </row>
-    <row r="286" spans="1:7" ht="45">
+    <row r="286" spans="1:7" ht="45" hidden="1">
       <c r="A286" s="38" t="s">
         <v>58</v>
       </c>
@@ -13650,7 +13650,7 @@
       <c r="F286" s="38"/>
       <c r="G286" s="44"/>
     </row>
-    <row r="287" spans="1:7" ht="30">
+    <row r="287" spans="1:7" ht="30" hidden="1">
       <c r="A287" s="38" t="s">
         <v>58</v>
       </c>
@@ -13669,7 +13669,7 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="288" spans="1:7">
+    <row r="288" spans="1:7" hidden="1">
       <c r="A288" s="38" t="s">
         <v>58</v>
       </c>
@@ -13684,7 +13684,7 @@
       <c r="F288" s="41"/>
       <c r="G288" s="41"/>
     </row>
-    <row r="289" spans="1:7">
+    <row r="289" spans="1:7" hidden="1">
       <c r="A289" s="38" t="s">
         <v>58</v>
       </c>
@@ -13699,7 +13699,7 @@
       <c r="F289" s="41"/>
       <c r="G289" s="41"/>
     </row>
-    <row r="290" spans="1:7" ht="30">
+    <row r="290" spans="1:7" ht="30" hidden="1">
       <c r="A290" s="38" t="s">
         <v>58</v>
       </c>
@@ -13718,7 +13718,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="291" spans="1:7">
+    <row r="291" spans="1:7" hidden="1">
       <c r="A291" s="38" t="s">
         <v>58</v>
       </c>
@@ -13735,7 +13735,7 @@
       <c r="F291" s="38"/>
       <c r="G291" s="44"/>
     </row>
-    <row r="292" spans="1:7">
+    <row r="292" spans="1:7" hidden="1">
       <c r="A292" s="38" t="s">
         <v>58</v>
       </c>
@@ -13752,7 +13752,7 @@
       <c r="F292" s="38"/>
       <c r="G292" s="44"/>
     </row>
-    <row r="293" spans="1:7" ht="30">
+    <row r="293" spans="1:7" ht="30" hidden="1">
       <c r="A293" s="38" t="s">
         <v>58</v>
       </c>
@@ -13769,7 +13769,7 @@
       <c r="F293" s="38"/>
       <c r="G293" s="44"/>
     </row>
-    <row r="294" spans="1:7">
+    <row r="294" spans="1:7" hidden="1">
       <c r="A294" s="38" t="s">
         <v>58</v>
       </c>
@@ -13786,7 +13786,7 @@
       <c r="F294" s="38"/>
       <c r="G294" s="44"/>
     </row>
-    <row r="295" spans="1:7">
+    <row r="295" spans="1:7" hidden="1">
       <c r="A295" s="38" t="s">
         <v>58</v>
       </c>
@@ -13803,7 +13803,7 @@
       <c r="F295" s="38"/>
       <c r="G295" s="44"/>
     </row>
-    <row r="296" spans="1:7">
+    <row r="296" spans="1:7" hidden="1">
       <c r="A296" s="38" t="s">
         <v>58</v>
       </c>
@@ -13820,7 +13820,7 @@
       <c r="F296" s="38"/>
       <c r="G296" s="44"/>
     </row>
-    <row r="297" spans="1:7" ht="30">
+    <row r="297" spans="1:7" ht="30" hidden="1">
       <c r="A297" s="38" t="s">
         <v>58</v>
       </c>
@@ -13837,7 +13837,7 @@
       <c r="F297" s="38"/>
       <c r="G297" s="44"/>
     </row>
-    <row r="298" spans="1:7">
+    <row r="298" spans="1:7" hidden="1">
       <c r="A298" s="38" t="s">
         <v>58</v>
       </c>
@@ -13854,7 +13854,7 @@
       <c r="F298" s="38"/>
       <c r="G298" s="44"/>
     </row>
-    <row r="299" spans="1:7" ht="30">
+    <row r="299" spans="1:7" ht="30" hidden="1">
       <c r="A299" s="38" t="s">
         <v>58</v>
       </c>
@@ -13871,7 +13871,7 @@
       <c r="F299" s="38"/>
       <c r="G299" s="44"/>
     </row>
-    <row r="300" spans="1:7" ht="30">
+    <row r="300" spans="1:7" ht="30" hidden="1">
       <c r="A300" s="38" t="s">
         <v>58</v>
       </c>
@@ -13888,7 +13888,7 @@
       <c r="F300" s="38"/>
       <c r="G300" s="44"/>
     </row>
-    <row r="301" spans="1:7" ht="30">
+    <row r="301" spans="1:7" ht="30" hidden="1">
       <c r="A301" s="38" t="s">
         <v>58</v>
       </c>
@@ -13905,7 +13905,7 @@
       <c r="F301" s="38"/>
       <c r="G301" s="38"/>
     </row>
-    <row r="302" spans="1:7" ht="45">
+    <row r="302" spans="1:7" ht="45" hidden="1">
       <c r="A302" s="38" t="s">
         <v>58</v>
       </c>
@@ -13922,7 +13922,7 @@
       <c r="F302" s="38"/>
       <c r="G302" s="44"/>
     </row>
-    <row r="303" spans="1:7" ht="45">
+    <row r="303" spans="1:7" ht="45" hidden="1">
       <c r="A303" s="38" t="s">
         <v>58</v>
       </c>
@@ -13939,7 +13939,7 @@
       <c r="F303" s="38"/>
       <c r="G303" s="38"/>
     </row>
-    <row r="304" spans="1:7" ht="45">
+    <row r="304" spans="1:7" ht="45" hidden="1">
       <c r="A304" s="38" t="s">
         <v>58</v>
       </c>
@@ -13956,7 +13956,7 @@
       <c r="F304" s="38"/>
       <c r="G304" s="44"/>
     </row>
-    <row r="305" spans="1:7" ht="30">
+    <row r="305" spans="1:7" ht="30" hidden="1">
       <c r="A305" s="38" t="s">
         <v>58</v>
       </c>
@@ -13975,7 +13975,7 @@
       </c>
       <c r="G305" s="44"/>
     </row>
-    <row r="306" spans="1:7">
+    <row r="306" spans="1:7" hidden="1">
       <c r="A306" s="38" t="s">
         <v>58</v>
       </c>
@@ -13990,7 +13990,7 @@
       <c r="F306" s="41"/>
       <c r="G306" s="41"/>
     </row>
-    <row r="307" spans="1:7">
+    <row r="307" spans="1:7" hidden="1">
       <c r="A307" s="38" t="s">
         <v>58</v>
       </c>
@@ -14005,7 +14005,7 @@
       <c r="F307" s="41"/>
       <c r="G307" s="41"/>
     </row>
-    <row r="308" spans="1:7" ht="30">
+    <row r="308" spans="1:7" ht="30" hidden="1">
       <c r="A308" s="38" t="s">
         <v>58</v>
       </c>
@@ -14022,7 +14022,7 @@
       <c r="F308" s="38"/>
       <c r="G308" s="44"/>
     </row>
-    <row r="309" spans="1:7">
+    <row r="309" spans="1:7" hidden="1">
       <c r="A309" s="38" t="s">
         <v>58</v>
       </c>
@@ -14037,7 +14037,7 @@
       <c r="F309" s="41"/>
       <c r="G309" s="41"/>
     </row>
-    <row r="310" spans="1:7" ht="30">
+    <row r="310" spans="1:7" ht="30" hidden="1">
       <c r="A310" s="38" t="s">
         <v>58</v>
       </c>
@@ -14056,7 +14056,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="311" spans="1:7">
+    <row r="311" spans="1:7" hidden="1">
       <c r="A311" s="38" t="s">
         <v>58</v>
       </c>
@@ -14073,7 +14073,7 @@
       <c r="F311" s="38"/>
       <c r="G311" s="44"/>
     </row>
-    <row r="312" spans="1:7">
+    <row r="312" spans="1:7" hidden="1">
       <c r="A312" s="38" t="s">
         <v>58</v>
       </c>
@@ -14090,7 +14090,7 @@
       <c r="F312" s="38"/>
       <c r="G312" s="44"/>
     </row>
-    <row r="313" spans="1:7" ht="30">
+    <row r="313" spans="1:7" ht="30" hidden="1">
       <c r="A313" s="38" t="s">
         <v>58</v>
       </c>
@@ -14107,7 +14107,7 @@
       <c r="F313" s="38"/>
       <c r="G313" s="44"/>
     </row>
-    <row r="314" spans="1:7">
+    <row r="314" spans="1:7" hidden="1">
       <c r="A314" s="38" t="s">
         <v>58</v>
       </c>
@@ -14124,7 +14124,7 @@
       <c r="F314" s="38"/>
       <c r="G314" s="44"/>
     </row>
-    <row r="315" spans="1:7">
+    <row r="315" spans="1:7" hidden="1">
       <c r="A315" s="38" t="s">
         <v>58</v>
       </c>
@@ -14141,7 +14141,7 @@
       <c r="F315" s="38"/>
       <c r="G315" s="44"/>
     </row>
-    <row r="316" spans="1:7" ht="45">
+    <row r="316" spans="1:7" ht="45" hidden="1">
       <c r="A316" s="38" t="s">
         <v>58</v>
       </c>
@@ -14158,7 +14158,7 @@
       <c r="F316" s="38"/>
       <c r="G316" s="44"/>
     </row>
-    <row r="317" spans="1:7">
+    <row r="317" spans="1:7" hidden="1">
       <c r="A317" s="38" t="s">
         <v>58</v>
       </c>
@@ -14173,7 +14173,7 @@
       <c r="F317" s="41"/>
       <c r="G317" s="48"/>
     </row>
-    <row r="318" spans="1:7">
+    <row r="318" spans="1:7" hidden="1">
       <c r="A318" s="38" t="s">
         <v>58</v>
       </c>
@@ -14188,7 +14188,7 @@
       <c r="F318" s="41"/>
       <c r="G318" s="48"/>
     </row>
-    <row r="319" spans="1:7" ht="30">
+    <row r="319" spans="1:7" ht="30" hidden="1">
       <c r="A319" s="38" t="s">
         <v>58</v>
       </c>
@@ -14207,7 +14207,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="320" spans="1:7">
+    <row r="320" spans="1:7" hidden="1">
       <c r="A320" s="38" t="s">
         <v>58</v>
       </c>
@@ -14224,7 +14224,7 @@
       <c r="F320" s="38"/>
       <c r="G320" s="38"/>
     </row>
-    <row r="321" spans="1:7">
+    <row r="321" spans="1:7" hidden="1">
       <c r="A321" s="38" t="s">
         <v>58</v>
       </c>
@@ -14241,7 +14241,7 @@
       <c r="F321" s="38"/>
       <c r="G321" s="38"/>
     </row>
-    <row r="322" spans="1:7" ht="30">
+    <row r="322" spans="1:7" ht="30" hidden="1">
       <c r="A322" s="38" t="s">
         <v>58</v>
       </c>
@@ -14258,7 +14258,7 @@
       <c r="F322" s="38"/>
       <c r="G322" s="38"/>
     </row>
-    <row r="323" spans="1:7">
+    <row r="323" spans="1:7" hidden="1">
       <c r="A323" s="38" t="s">
         <v>58</v>
       </c>
@@ -14275,7 +14275,7 @@
       <c r="F323" s="38"/>
       <c r="G323" s="38"/>
     </row>
-    <row r="324" spans="1:7">
+    <row r="324" spans="1:7" hidden="1">
       <c r="A324" s="38" t="s">
         <v>58</v>
       </c>
@@ -14292,7 +14292,7 @@
       <c r="F324" s="38"/>
       <c r="G324" s="38"/>
     </row>
-    <row r="325" spans="1:7">
+    <row r="325" spans="1:7" hidden="1">
       <c r="A325" s="38" t="s">
         <v>58</v>
       </c>
@@ -14309,7 +14309,7 @@
       <c r="F325" s="38"/>
       <c r="G325" s="38"/>
     </row>
-    <row r="326" spans="1:7" ht="30">
+    <row r="326" spans="1:7" ht="30" hidden="1">
       <c r="A326" s="38" t="s">
         <v>58</v>
       </c>
@@ -14326,7 +14326,7 @@
       <c r="F326" s="38"/>
       <c r="G326" s="38"/>
     </row>
-    <row r="327" spans="1:7">
+    <row r="327" spans="1:7" hidden="1">
       <c r="A327" s="38" t="s">
         <v>58</v>
       </c>
@@ -14343,7 +14343,7 @@
       <c r="F327" s="38"/>
       <c r="G327" s="38"/>
     </row>
-    <row r="328" spans="1:7" ht="30">
+    <row r="328" spans="1:7" ht="30" hidden="1">
       <c r="A328" s="38" t="s">
         <v>58</v>
       </c>
@@ -14360,7 +14360,7 @@
       <c r="F328" s="38"/>
       <c r="G328" s="38"/>
     </row>
-    <row r="329" spans="1:7" ht="30">
+    <row r="329" spans="1:7" ht="30" hidden="1">
       <c r="A329" s="38" t="s">
         <v>58</v>
       </c>
@@ -14377,7 +14377,7 @@
       <c r="F329" s="38"/>
       <c r="G329" s="38"/>
     </row>
-    <row r="330" spans="1:7" ht="30">
+    <row r="330" spans="1:7" ht="30" hidden="1">
       <c r="A330" s="38" t="s">
         <v>58</v>
       </c>
@@ -14394,7 +14394,7 @@
       <c r="F330" s="38"/>
       <c r="G330" s="38"/>
     </row>
-    <row r="331" spans="1:7" ht="45">
+    <row r="331" spans="1:7" ht="45" hidden="1">
       <c r="A331" s="38" t="s">
         <v>58</v>
       </c>
@@ -14411,7 +14411,7 @@
       <c r="F331" s="38"/>
       <c r="G331" s="38"/>
     </row>
-    <row r="332" spans="1:7" ht="45">
+    <row r="332" spans="1:7" ht="45" hidden="1">
       <c r="A332" s="38" t="s">
         <v>58</v>
       </c>
@@ -14428,7 +14428,7 @@
       <c r="F332" s="38"/>
       <c r="G332" s="38"/>
     </row>
-    <row r="333" spans="1:7" ht="45">
+    <row r="333" spans="1:7" ht="45" hidden="1">
       <c r="A333" s="38" t="s">
         <v>58</v>
       </c>
@@ -14447,7 +14447,7 @@
       </c>
       <c r="G333" s="38"/>
     </row>
-    <row r="334" spans="1:7" ht="30">
+    <row r="334" spans="1:7" ht="30" hidden="1">
       <c r="A334" s="38" t="s">
         <v>58</v>
       </c>
@@ -14466,7 +14466,7 @@
       </c>
       <c r="G334" s="38"/>
     </row>
-    <row r="335" spans="1:7" ht="15.6">
+    <row r="335" spans="1:7" ht="15.6" hidden="1">
       <c r="A335" s="38" t="s">
         <v>58</v>
       </c>
@@ -14481,7 +14481,7 @@
       <c r="F335" s="41"/>
       <c r="G335" s="49"/>
     </row>
-    <row r="336" spans="1:7">
+    <row r="336" spans="1:7" hidden="1">
       <c r="A336" s="38" t="s">
         <v>58</v>
       </c>
@@ -14496,7 +14496,7 @@
       <c r="F336" s="41"/>
       <c r="G336" s="48"/>
     </row>
-    <row r="337" spans="1:7">
+    <row r="337" spans="1:7" hidden="1">
       <c r="A337" s="38" t="s">
         <v>58</v>
       </c>
@@ -14511,7 +14511,7 @@
       <c r="F337" s="41"/>
       <c r="G337" s="48"/>
     </row>
-    <row r="338" spans="1:7" ht="60">
+    <row r="338" spans="1:7" ht="60" hidden="1">
       <c r="A338" s="38" t="s">
         <v>58</v>
       </c>
@@ -14534,7 +14534,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="339" spans="1:7">
+    <row r="339" spans="1:7" hidden="1">
       <c r="A339" s="38" t="s">
         <v>58</v>
       </c>
@@ -14555,7 +14555,7 @@
       </c>
       <c r="G339" s="44"/>
     </row>
-    <row r="340" spans="1:7">
+    <row r="340" spans="1:7" hidden="1">
       <c r="A340" s="38" t="s">
         <v>58</v>
       </c>
@@ -14574,7 +14574,7 @@
       </c>
       <c r="G340" s="44"/>
     </row>
-    <row r="341" spans="1:7">
+    <row r="341" spans="1:7" hidden="1">
       <c r="A341" s="38" t="s">
         <v>58</v>
       </c>
@@ -14589,7 +14589,7 @@
       <c r="F341" s="41"/>
       <c r="G341" s="41"/>
     </row>
-    <row r="342" spans="1:7">
+    <row r="342" spans="1:7" hidden="1">
       <c r="A342" s="38" t="s">
         <v>58</v>
       </c>
@@ -14610,7 +14610,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="343" spans="1:7">
+    <row r="343" spans="1:7" hidden="1">
       <c r="A343" s="38" t="s">
         <v>58</v>
       </c>
@@ -14629,7 +14629,7 @@
       </c>
       <c r="G343" s="44"/>
     </row>
-    <row r="344" spans="1:7">
+    <row r="344" spans="1:7" hidden="1">
       <c r="A344" s="38" t="s">
         <v>58</v>
       </c>
@@ -14648,7 +14648,7 @@
       </c>
       <c r="G344" s="38"/>
     </row>
-    <row r="345" spans="1:7">
+    <row r="345" spans="1:7" hidden="1">
       <c r="A345" s="38" t="s">
         <v>58</v>
       </c>
@@ -14667,7 +14667,7 @@
       </c>
       <c r="G345" s="44"/>
     </row>
-    <row r="346" spans="1:7">
+    <row r="346" spans="1:7" hidden="1">
       <c r="A346" s="38" t="s">
         <v>58</v>
       </c>
@@ -14682,7 +14682,7 @@
       <c r="F346" s="41"/>
       <c r="G346" s="41"/>
     </row>
-    <row r="347" spans="1:7">
+    <row r="347" spans="1:7" hidden="1">
       <c r="A347" s="38" t="s">
         <v>58</v>
       </c>
@@ -14703,7 +14703,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="348" spans="1:7">
+    <row r="348" spans="1:7" hidden="1">
       <c r="A348" s="38" t="s">
         <v>58</v>
       </c>
@@ -14722,7 +14722,7 @@
       </c>
       <c r="G348" s="44"/>
     </row>
-    <row r="349" spans="1:7">
+    <row r="349" spans="1:7" hidden="1">
       <c r="A349" s="38" t="s">
         <v>58</v>
       </c>
@@ -14741,7 +14741,7 @@
       </c>
       <c r="G349" s="44"/>
     </row>
-    <row r="350" spans="1:7">
+    <row r="350" spans="1:7" hidden="1">
       <c r="A350" s="38" t="s">
         <v>58</v>
       </c>
@@ -14760,7 +14760,7 @@
       </c>
       <c r="G350" s="44"/>
     </row>
-    <row r="351" spans="1:7">
+    <row r="351" spans="1:7" hidden="1">
       <c r="A351" s="38" t="s">
         <v>58</v>
       </c>
@@ -14779,7 +14779,7 @@
       </c>
       <c r="G351" s="44"/>
     </row>
-    <row r="352" spans="1:7">
+    <row r="352" spans="1:7" hidden="1">
       <c r="A352" s="38" t="s">
         <v>58</v>
       </c>
@@ -14794,7 +14794,7 @@
       <c r="F352" s="41"/>
       <c r="G352" s="41"/>
     </row>
-    <row r="353" spans="1:7" ht="45">
+    <row r="353" spans="1:7" ht="45" hidden="1">
       <c r="A353" s="38" t="s">
         <v>58</v>
       </c>
@@ -14815,7 +14815,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="354" spans="1:7" ht="30">
+    <row r="354" spans="1:7" ht="30" hidden="1">
       <c r="A354" s="38" t="s">
         <v>58</v>
       </c>
@@ -14834,7 +14834,7 @@
       </c>
       <c r="G354" s="44"/>
     </row>
-    <row r="355" spans="1:7" ht="37.5" customHeight="1">
+    <row r="355" spans="1:7" ht="37.5" hidden="1" customHeight="1">
       <c r="A355" s="38" t="s">
         <v>58</v>
       </c>
@@ -14853,7 +14853,7 @@
       </c>
       <c r="G355" s="38"/>
     </row>
-    <row r="356" spans="1:7" ht="30">
+    <row r="356" spans="1:7" ht="30" hidden="1">
       <c r="A356" s="38" t="s">
         <v>58</v>
       </c>
@@ -14872,7 +14872,7 @@
       </c>
       <c r="G356" s="44"/>
     </row>
-    <row r="357" spans="1:7">
+    <row r="357" spans="1:7" hidden="1">
       <c r="A357" s="38" t="s">
         <v>58</v>
       </c>
@@ -14891,7 +14891,7 @@
       </c>
       <c r="G357" s="44"/>
     </row>
-    <row r="358" spans="1:7">
+    <row r="358" spans="1:7" hidden="1">
       <c r="A358" s="38" t="s">
         <v>58</v>
       </c>
@@ -14906,7 +14906,7 @@
       <c r="F358" s="41"/>
       <c r="G358" s="41"/>
     </row>
-    <row r="359" spans="1:7">
+    <row r="359" spans="1:7" hidden="1">
       <c r="A359" s="38" t="s">
         <v>58</v>
       </c>
@@ -14927,7 +14927,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="360" spans="1:7">
+    <row r="360" spans="1:7" hidden="1">
       <c r="A360" s="38" t="s">
         <v>58</v>
       </c>
@@ -14946,7 +14946,7 @@
       </c>
       <c r="G360" s="38"/>
     </row>
-    <row r="361" spans="1:7">
+    <row r="361" spans="1:7" hidden="1">
       <c r="A361" s="38" t="s">
         <v>58</v>
       </c>
@@ -14961,7 +14961,7 @@
       <c r="F361" s="41"/>
       <c r="G361" s="41"/>
     </row>
-    <row r="362" spans="1:7">
+    <row r="362" spans="1:7" hidden="1">
       <c r="A362" s="38" t="s">
         <v>58</v>
       </c>
@@ -14982,7 +14982,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="363" spans="1:7">
+    <row r="363" spans="1:7" hidden="1">
       <c r="A363" s="38" t="s">
         <v>58</v>
       </c>
@@ -15001,7 +15001,7 @@
       </c>
       <c r="G363" s="44"/>
     </row>
-    <row r="364" spans="1:7">
+    <row r="364" spans="1:7" hidden="1">
       <c r="A364" s="38" t="s">
         <v>58</v>
       </c>
@@ -15020,7 +15020,7 @@
       </c>
       <c r="G364" s="44"/>
     </row>
-    <row r="365" spans="1:7">
+    <row r="365" spans="1:7" hidden="1">
       <c r="A365" s="38" t="s">
         <v>58</v>
       </c>
@@ -15039,7 +15039,7 @@
       </c>
       <c r="G365" s="44"/>
     </row>
-    <row r="366" spans="1:7">
+    <row r="366" spans="1:7" hidden="1">
       <c r="A366" s="38" t="s">
         <v>58</v>
       </c>
@@ -15060,7 +15060,7 @@
       </c>
       <c r="G366" s="38"/>
     </row>
-    <row r="367" spans="1:7">
+    <row r="367" spans="1:7" hidden="1">
       <c r="A367" s="38" t="s">
         <v>58</v>
       </c>
@@ -15075,7 +15075,7 @@
       <c r="F367" s="41"/>
       <c r="G367" s="41"/>
     </row>
-    <row r="368" spans="1:7">
+    <row r="368" spans="1:7" hidden="1">
       <c r="A368" s="38" t="s">
         <v>58</v>
       </c>
@@ -15090,7 +15090,7 @@
       <c r="F368" s="41"/>
       <c r="G368" s="41"/>
     </row>
-    <row r="369" spans="1:7" ht="60">
+    <row r="369" spans="1:7" ht="60" hidden="1">
       <c r="A369" s="38" t="s">
         <v>58</v>
       </c>
@@ -15113,7 +15113,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="370" spans="1:7" ht="30">
+    <row r="370" spans="1:7" ht="30" hidden="1">
       <c r="A370" s="38" t="s">
         <v>58</v>
       </c>
@@ -15134,7 +15134,7 @@
       </c>
       <c r="G370" s="44"/>
     </row>
-    <row r="371" spans="1:7">
+    <row r="371" spans="1:7" hidden="1">
       <c r="A371" s="38" t="s">
         <v>58</v>
       </c>
@@ -15155,7 +15155,7 @@
       </c>
       <c r="G371" s="44"/>
     </row>
-    <row r="372" spans="1:7">
+    <row r="372" spans="1:7" hidden="1">
       <c r="A372" s="38" t="s">
         <v>58</v>
       </c>
@@ -15170,7 +15170,7 @@
       <c r="F372" s="41"/>
       <c r="G372" s="41"/>
     </row>
-    <row r="373" spans="1:7">
+    <row r="373" spans="1:7" hidden="1">
       <c r="A373" s="38" t="s">
         <v>58</v>
       </c>
@@ -15185,7 +15185,7 @@
       <c r="F373" s="41"/>
       <c r="G373" s="41"/>
     </row>
-    <row r="374" spans="1:7">
+    <row r="374" spans="1:7" hidden="1">
       <c r="A374" s="38" t="s">
         <v>58</v>
       </c>
@@ -15206,7 +15206,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="375" spans="1:7">
+    <row r="375" spans="1:7" hidden="1">
       <c r="A375" s="38" t="s">
         <v>58</v>
       </c>
@@ -15225,7 +15225,7 @@
       </c>
       <c r="G375" s="44"/>
     </row>
-    <row r="376" spans="1:7" ht="30">
+    <row r="376" spans="1:7" ht="30" hidden="1">
       <c r="A376" s="38" t="s">
         <v>58</v>
       </c>
@@ -15244,7 +15244,7 @@
       </c>
       <c r="G376" s="44"/>
     </row>
-    <row r="377" spans="1:7" ht="30">
+    <row r="377" spans="1:7" ht="30" hidden="1">
       <c r="A377" s="38" t="s">
         <v>58</v>
       </c>
@@ -15263,7 +15263,7 @@
       </c>
       <c r="G377" s="44"/>
     </row>
-    <row r="378" spans="1:7">
+    <row r="378" spans="1:7" hidden="1">
       <c r="A378" s="38" t="s">
         <v>58</v>
       </c>
@@ -15282,7 +15282,7 @@
       </c>
       <c r="G378" s="44"/>
     </row>
-    <row r="379" spans="1:7" ht="30">
+    <row r="379" spans="1:7" ht="30" hidden="1">
       <c r="A379" s="38" t="s">
         <v>58</v>
       </c>
@@ -15301,7 +15301,7 @@
       </c>
       <c r="G379" s="44"/>
     </row>
-    <row r="380" spans="1:7">
+    <row r="380" spans="1:7" hidden="1">
       <c r="A380" s="38" t="s">
         <v>58</v>
       </c>
@@ -15316,7 +15316,7 @@
       <c r="F380" s="41"/>
       <c r="G380" s="41"/>
     </row>
-    <row r="381" spans="1:7">
+    <row r="381" spans="1:7" hidden="1">
       <c r="A381" s="38" t="s">
         <v>58</v>
       </c>
@@ -15337,7 +15337,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="382" spans="1:7">
+    <row r="382" spans="1:7" hidden="1">
       <c r="A382" s="38" t="s">
         <v>58</v>
       </c>
@@ -15358,7 +15358,7 @@
       </c>
       <c r="G382" s="38"/>
     </row>
-    <row r="383" spans="1:7">
+    <row r="383" spans="1:7" hidden="1">
       <c r="A383" s="38" t="s">
         <v>58</v>
       </c>
@@ -15373,7 +15373,7 @@
       <c r="F383" s="41"/>
       <c r="G383" s="41"/>
     </row>
-    <row r="384" spans="1:7">
+    <row r="384" spans="1:7" hidden="1">
       <c r="A384" s="38" t="s">
         <v>58</v>
       </c>
@@ -15394,7 +15394,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="385" spans="1:7">
+    <row r="385" spans="1:7" hidden="1">
       <c r="A385" s="38" t="s">
         <v>58</v>
       </c>
@@ -15413,7 +15413,7 @@
       </c>
       <c r="G385" s="44"/>
     </row>
-    <row r="386" spans="1:7">
+    <row r="386" spans="1:7" hidden="1">
       <c r="A386" s="38" t="s">
         <v>58</v>
       </c>
@@ -15432,7 +15432,7 @@
       </c>
       <c r="G386" s="44"/>
     </row>
-    <row r="387" spans="1:7">
+    <row r="387" spans="1:7" hidden="1">
       <c r="A387" s="38" t="s">
         <v>58</v>
       </c>
@@ -15451,7 +15451,7 @@
       </c>
       <c r="G387" s="38"/>
     </row>
-    <row r="388" spans="1:7">
+    <row r="388" spans="1:7" hidden="1">
       <c r="A388" s="38" t="s">
         <v>58</v>
       </c>
@@ -15472,7 +15472,7 @@
       </c>
       <c r="G388" s="38"/>
     </row>
-    <row r="389" spans="1:7">
+    <row r="389" spans="1:7" hidden="1">
       <c r="A389" s="38" t="s">
         <v>58</v>
       </c>
@@ -15487,7 +15487,7 @@
       <c r="F389" s="41"/>
       <c r="G389" s="41"/>
     </row>
-    <row r="390" spans="1:7">
+    <row r="390" spans="1:7" hidden="1">
       <c r="A390" s="38" t="s">
         <v>58</v>
       </c>
@@ -15502,7 +15502,7 @@
       <c r="F390" s="41"/>
       <c r="G390" s="41"/>
     </row>
-    <row r="391" spans="1:7" ht="45">
+    <row r="391" spans="1:7" ht="45" hidden="1">
       <c r="A391" s="38" t="s">
         <v>58</v>
       </c>
@@ -15525,7 +15525,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="392" spans="1:7" ht="30">
+    <row r="392" spans="1:7" ht="30" hidden="1">
       <c r="A392" s="38" t="s">
         <v>58</v>
       </c>
@@ -15546,7 +15546,7 @@
       </c>
       <c r="G392" s="38"/>
     </row>
-    <row r="393" spans="1:7">
+    <row r="393" spans="1:7" hidden="1">
       <c r="A393" s="38" t="s">
         <v>58</v>
       </c>
@@ -15567,7 +15567,7 @@
       </c>
       <c r="G393" s="44"/>
     </row>
-    <row r="394" spans="1:7">
+    <row r="394" spans="1:7" hidden="1">
       <c r="A394" s="38" t="s">
         <v>58</v>
       </c>
@@ -15582,7 +15582,7 @@
       <c r="F394" s="41"/>
       <c r="G394" s="41"/>
     </row>
-    <row r="395" spans="1:7">
+    <row r="395" spans="1:7" hidden="1">
       <c r="A395" s="38" t="s">
         <v>58</v>
       </c>
@@ -15597,7 +15597,7 @@
       <c r="F395" s="41"/>
       <c r="G395" s="41"/>
     </row>
-    <row r="396" spans="1:7">
+    <row r="396" spans="1:7" hidden="1">
       <c r="A396" s="38" t="s">
         <v>58</v>
       </c>
@@ -15618,7 +15618,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="397" spans="1:7">
+    <row r="397" spans="1:7" hidden="1">
       <c r="A397" s="38" t="s">
         <v>58</v>
       </c>
@@ -15637,7 +15637,7 @@
       </c>
       <c r="G397" s="44"/>
     </row>
-    <row r="398" spans="1:7">
+    <row r="398" spans="1:7" hidden="1">
       <c r="A398" s="38" t="s">
         <v>58</v>
       </c>
@@ -15656,7 +15656,7 @@
       </c>
       <c r="G398" s="44"/>
     </row>
-    <row r="399" spans="1:7" ht="30">
+    <row r="399" spans="1:7" ht="30" hidden="1">
       <c r="A399" s="38" t="s">
         <v>58</v>
       </c>
@@ -15675,7 +15675,7 @@
       </c>
       <c r="G399" s="44"/>
     </row>
-    <row r="400" spans="1:7">
+    <row r="400" spans="1:7" hidden="1">
       <c r="A400" s="38" t="s">
         <v>58</v>
       </c>
@@ -15694,7 +15694,7 @@
       </c>
       <c r="G400" s="44"/>
     </row>
-    <row r="401" spans="1:7" ht="30">
+    <row r="401" spans="1:7" ht="30" hidden="1">
       <c r="A401" s="38" t="s">
         <v>58</v>
       </c>
@@ -15713,7 +15713,7 @@
       </c>
       <c r="G401" s="44"/>
     </row>
-    <row r="402" spans="1:7">
+    <row r="402" spans="1:7" hidden="1">
       <c r="A402" s="38" t="s">
         <v>58</v>
       </c>
@@ -15728,7 +15728,7 @@
       <c r="F402" s="41"/>
       <c r="G402" s="41"/>
     </row>
-    <row r="403" spans="1:7">
+    <row r="403" spans="1:7" hidden="1">
       <c r="A403" s="38" t="s">
         <v>58</v>
       </c>
@@ -15749,7 +15749,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="404" spans="1:7">
+    <row r="404" spans="1:7" hidden="1">
       <c r="A404" s="38" t="s">
         <v>58</v>
       </c>
@@ -15770,7 +15770,7 @@
       </c>
       <c r="G404" s="38"/>
     </row>
-    <row r="405" spans="1:7">
+    <row r="405" spans="1:7" hidden="1">
       <c r="A405" s="38" t="s">
         <v>58</v>
       </c>
@@ -15785,7 +15785,7 @@
       <c r="F405" s="41"/>
       <c r="G405" s="41"/>
     </row>
-    <row r="406" spans="1:7">
+    <row r="406" spans="1:7" hidden="1">
       <c r="A406" s="38" t="s">
         <v>58</v>
       </c>
@@ -15806,7 +15806,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="407" spans="1:7">
+    <row r="407" spans="1:7" hidden="1">
       <c r="A407" s="38" t="s">
         <v>58</v>
       </c>
@@ -15825,7 +15825,7 @@
       </c>
       <c r="G407" s="44"/>
     </row>
-    <row r="408" spans="1:7">
+    <row r="408" spans="1:7" hidden="1">
       <c r="A408" s="38" t="s">
         <v>58</v>
       </c>
@@ -15844,7 +15844,7 @@
       </c>
       <c r="G408" s="44"/>
     </row>
-    <row r="409" spans="1:7">
+    <row r="409" spans="1:7" hidden="1">
       <c r="A409" s="38" t="s">
         <v>58</v>
       </c>
@@ -15863,7 +15863,7 @@
       </c>
       <c r="G409" s="38"/>
     </row>
-    <row r="410" spans="1:7">
+    <row r="410" spans="1:7" hidden="1">
       <c r="A410" s="38" t="s">
         <v>58</v>
       </c>
@@ -15884,7 +15884,7 @@
       </c>
       <c r="G410" s="38"/>
     </row>
-    <row r="411" spans="1:7">
+    <row r="411" spans="1:7" hidden="1">
       <c r="A411" s="38" t="s">
         <v>58</v>
       </c>
@@ -15899,7 +15899,7 @@
       <c r="F411" s="41"/>
       <c r="G411" s="41"/>
     </row>
-    <row r="412" spans="1:7">
+    <row r="412" spans="1:7" hidden="1">
       <c r="A412" s="38" t="s">
         <v>58</v>
       </c>
@@ -15914,7 +15914,7 @@
       <c r="F412" s="41"/>
       <c r="G412" s="41"/>
     </row>
-    <row r="413" spans="1:7" ht="45">
+    <row r="413" spans="1:7" ht="45" hidden="1">
       <c r="A413" s="38" t="s">
         <v>58</v>
       </c>
@@ -15937,7 +15937,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="414" spans="1:7">
+    <row r="414" spans="1:7" hidden="1">
       <c r="A414" s="38" t="s">
         <v>58</v>
       </c>
@@ -15958,7 +15958,7 @@
       </c>
       <c r="G414" s="44"/>
     </row>
-    <row r="415" spans="1:7">
+    <row r="415" spans="1:7" hidden="1">
       <c r="A415" s="38" t="s">
         <v>58</v>
       </c>
@@ -15979,7 +15979,7 @@
       </c>
       <c r="G415" s="44"/>
     </row>
-    <row r="416" spans="1:7">
+    <row r="416" spans="1:7" hidden="1">
       <c r="A416" s="38" t="s">
         <v>58</v>
       </c>
@@ -15994,7 +15994,7 @@
       <c r="F416" s="41"/>
       <c r="G416" s="41"/>
     </row>
-    <row r="417" spans="1:7">
+    <row r="417" spans="1:7" hidden="1">
       <c r="A417" s="38" t="s">
         <v>58</v>
       </c>
@@ -16009,7 +16009,7 @@
       <c r="F417" s="41"/>
       <c r="G417" s="41"/>
     </row>
-    <row r="418" spans="1:7">
+    <row r="418" spans="1:7" hidden="1">
       <c r="A418" s="38" t="s">
         <v>58</v>
       </c>
@@ -16030,7 +16030,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="419" spans="1:7">
+    <row r="419" spans="1:7" hidden="1">
       <c r="A419" s="38" t="s">
         <v>58</v>
       </c>
@@ -16049,7 +16049,7 @@
       </c>
       <c r="G419" s="44"/>
     </row>
-    <row r="420" spans="1:7">
+    <row r="420" spans="1:7" hidden="1">
       <c r="A420" s="38" t="s">
         <v>58</v>
       </c>
@@ -16068,7 +16068,7 @@
       </c>
       <c r="G420" s="44"/>
     </row>
-    <row r="421" spans="1:7">
+    <row r="421" spans="1:7" hidden="1">
       <c r="A421" s="38" t="s">
         <v>58</v>
       </c>
@@ -16134,7 +16134,7 @@
         <v>1297</v>
       </c>
       <c r="D424" s="40" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="E424" s="40"/>
       <c r="F424" s="38" t="s">
@@ -16161,7 +16161,7 @@
       </c>
       <c r="G425" s="38"/>
     </row>
-    <row r="426" spans="1:7">
+    <row r="426" spans="1:7" hidden="1">
       <c r="A426" s="38" t="s">
         <v>58</v>
       </c>
@@ -16176,7 +16176,7 @@
       <c r="F426" s="41"/>
       <c r="G426" s="41"/>
     </row>
-    <row r="427" spans="1:7">
+    <row r="427" spans="1:7" hidden="1">
       <c r="A427" s="38" t="s">
         <v>58</v>
       </c>
@@ -16197,7 +16197,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="428" spans="1:7">
+    <row r="428" spans="1:7" hidden="1">
       <c r="A428" s="38" t="s">
         <v>58</v>
       </c>
@@ -16216,7 +16216,7 @@
       </c>
       <c r="G428" s="44"/>
     </row>
-    <row r="429" spans="1:7">
+    <row r="429" spans="1:7" hidden="1">
       <c r="A429" s="38" t="s">
         <v>58</v>
       </c>
@@ -16235,7 +16235,7 @@
       </c>
       <c r="G429" s="44"/>
     </row>
-    <row r="430" spans="1:7">
+    <row r="430" spans="1:7" hidden="1">
       <c r="A430" s="38" t="s">
         <v>58</v>
       </c>
@@ -16254,7 +16254,7 @@
       </c>
       <c r="G430" s="38"/>
     </row>
-    <row r="431" spans="1:7">
+    <row r="431" spans="1:7" hidden="1">
       <c r="A431" s="38" t="s">
         <v>58</v>
       </c>
@@ -16273,7 +16273,7 @@
       </c>
       <c r="G431" s="44"/>
     </row>
-    <row r="432" spans="1:7" ht="30">
+    <row r="432" spans="1:7" ht="30" hidden="1">
       <c r="A432" s="38" t="s">
         <v>58</v>
       </c>
@@ -16292,7 +16292,7 @@
       </c>
       <c r="G432" s="44"/>
     </row>
-    <row r="433" spans="1:7">
+    <row r="433" spans="1:7" hidden="1">
       <c r="A433" s="38" t="s">
         <v>58</v>
       </c>
@@ -16309,7 +16309,7 @@
       </c>
       <c r="G433" s="41"/>
     </row>
-    <row r="434" spans="1:7" ht="45">
+    <row r="434" spans="1:7" ht="45" hidden="1">
       <c r="A434" s="38" t="s">
         <v>58</v>
       </c>
@@ -16330,7 +16330,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="435" spans="1:7" ht="30">
+    <row r="435" spans="1:7" ht="30" hidden="1">
       <c r="A435" s="38" t="s">
         <v>58</v>
       </c>
@@ -16349,7 +16349,7 @@
       </c>
       <c r="G435" s="44"/>
     </row>
-    <row r="436" spans="1:7">
+    <row r="436" spans="1:7" hidden="1">
       <c r="A436" s="38" t="s">
         <v>58</v>
       </c>
@@ -16370,7 +16370,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="437" spans="1:7">
+    <row r="437" spans="1:7" hidden="1">
       <c r="A437" s="38" t="s">
         <v>58</v>
       </c>
@@ -16389,7 +16389,7 @@
       </c>
       <c r="G437" s="44"/>
     </row>
-    <row r="438" spans="1:7">
+    <row r="438" spans="1:7" hidden="1">
       <c r="A438" s="38" t="s">
         <v>58</v>
       </c>
@@ -16406,7 +16406,7 @@
       </c>
       <c r="G438" s="41"/>
     </row>
-    <row r="439" spans="1:7">
+    <row r="439" spans="1:7" hidden="1">
       <c r="A439" s="38" t="s">
         <v>58</v>
       </c>
@@ -16427,7 +16427,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="440" spans="1:7">
+    <row r="440" spans="1:7" hidden="1">
       <c r="A440" s="38" t="s">
         <v>58</v>
       </c>
@@ -16448,7 +16448,7 @@
       </c>
       <c r="G440" s="38"/>
     </row>
-    <row r="441" spans="1:7">
+    <row r="441" spans="1:7" hidden="1">
       <c r="A441" s="38" t="s">
         <v>58</v>
       </c>
@@ -16465,7 +16465,7 @@
       </c>
       <c r="G441" s="41"/>
     </row>
-    <row r="442" spans="1:7">
+    <row r="442" spans="1:7" hidden="1">
       <c r="A442" s="38" t="s">
         <v>58</v>
       </c>
@@ -16486,7 +16486,7 @@
       </c>
       <c r="G442" s="38"/>
     </row>
-    <row r="443" spans="1:7">
+    <row r="443" spans="1:7" hidden="1">
       <c r="A443" s="38" t="s">
         <v>58</v>
       </c>
@@ -16503,7 +16503,7 @@
       </c>
       <c r="G443" s="37"/>
     </row>
-    <row r="444" spans="1:7">
+    <row r="444" spans="1:7" hidden="1">
       <c r="A444" s="38" t="s">
         <v>58</v>
       </c>
@@ -16522,7 +16522,7 @@
       </c>
       <c r="G444" s="44"/>
     </row>
-    <row r="445" spans="1:7">
+    <row r="445" spans="1:7" hidden="1">
       <c r="A445" s="38" t="s">
         <v>58</v>
       </c>
@@ -16541,7 +16541,7 @@
       </c>
       <c r="G445" s="44"/>
     </row>
-    <row r="446" spans="1:7">
+    <row r="446" spans="1:7" hidden="1">
       <c r="A446" s="38" t="s">
         <v>58</v>
       </c>
@@ -16560,7 +16560,7 @@
       </c>
       <c r="G446" s="44"/>
     </row>
-    <row r="447" spans="1:7">
+    <row r="447" spans="1:7" hidden="1">
       <c r="A447" s="38" t="s">
         <v>58</v>
       </c>
@@ -16577,7 +16577,7 @@
       </c>
       <c r="G447" s="37"/>
     </row>
-    <row r="448" spans="1:7">
+    <row r="448" spans="1:7" hidden="1">
       <c r="A448" s="38" t="s">
         <v>58</v>
       </c>
@@ -16596,7 +16596,7 @@
       </c>
       <c r="G448" s="44"/>
     </row>
-    <row r="449" spans="1:7">
+    <row r="449" spans="1:7" hidden="1">
       <c r="A449" s="38" t="s">
         <v>58</v>
       </c>
@@ -16615,7 +16615,7 @@
       </c>
       <c r="G449" s="44"/>
     </row>
-    <row r="450" spans="1:7">
+    <row r="450" spans="1:7" hidden="1">
       <c r="A450" s="38" t="s">
         <v>58</v>
       </c>
@@ -16632,7 +16632,7 @@
       </c>
       <c r="G450" s="37"/>
     </row>
-    <row r="451" spans="1:7">
+    <row r="451" spans="1:7" hidden="1">
       <c r="A451" s="38" t="s">
         <v>58</v>
       </c>
@@ -16649,7 +16649,7 @@
       </c>
       <c r="G451" s="41"/>
     </row>
-    <row r="452" spans="1:7" ht="45">
+    <row r="452" spans="1:7" ht="45" hidden="1">
       <c r="A452" s="38" t="s">
         <v>58</v>
       </c>
@@ -16670,7 +16670,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="453" spans="1:7">
+    <row r="453" spans="1:7" hidden="1">
       <c r="A453" s="38" t="s">
         <v>58</v>
       </c>
@@ -16689,7 +16689,7 @@
       </c>
       <c r="G453" s="44"/>
     </row>
-    <row r="454" spans="1:7">
+    <row r="454" spans="1:7" hidden="1">
       <c r="A454" s="38" t="s">
         <v>58</v>
       </c>
@@ -16708,7 +16708,7 @@
       </c>
       <c r="G454" s="44"/>
     </row>
-    <row r="455" spans="1:7">
+    <row r="455" spans="1:7" hidden="1">
       <c r="A455" s="38" t="s">
         <v>58</v>
       </c>
@@ -16725,7 +16725,7 @@
       </c>
       <c r="G455" s="41"/>
     </row>
-    <row r="456" spans="1:7">
+    <row r="456" spans="1:7" hidden="1">
       <c r="A456" s="38" t="s">
         <v>58</v>
       </c>
@@ -16742,7 +16742,7 @@
       </c>
       <c r="G456" s="41"/>
     </row>
-    <row r="457" spans="1:7">
+    <row r="457" spans="1:7" hidden="1">
       <c r="A457" s="38" t="s">
         <v>58</v>
       </c>
@@ -16763,7 +16763,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="458" spans="1:7">
+    <row r="458" spans="1:7" hidden="1">
       <c r="A458" s="38" t="s">
         <v>58</v>
       </c>
@@ -16782,7 +16782,7 @@
       </c>
       <c r="G458" s="44"/>
     </row>
-    <row r="459" spans="1:7">
+    <row r="459" spans="1:7" hidden="1">
       <c r="A459" s="38" t="s">
         <v>58</v>
       </c>
@@ -16801,7 +16801,7 @@
       </c>
       <c r="G459" s="38"/>
     </row>
-    <row r="460" spans="1:7">
+    <row r="460" spans="1:7" hidden="1">
       <c r="A460" s="38" t="s">
         <v>58</v>
       </c>
@@ -16820,7 +16820,7 @@
       </c>
       <c r="G460" s="38"/>
     </row>
-    <row r="461" spans="1:7">
+    <row r="461" spans="1:7" hidden="1">
       <c r="A461" s="38" t="s">
         <v>58</v>
       </c>
@@ -16837,7 +16837,7 @@
       </c>
       <c r="G461" s="38"/>
     </row>
-    <row r="462" spans="1:7" ht="30">
+    <row r="462" spans="1:7" ht="30" hidden="1">
       <c r="A462" s="38" t="s">
         <v>58</v>
       </c>
@@ -16856,7 +16856,7 @@
       </c>
       <c r="G462" s="38"/>
     </row>
-    <row r="463" spans="1:7">
+    <row r="463" spans="1:7" hidden="1">
       <c r="A463" s="38" t="s">
         <v>58</v>
       </c>
@@ -16875,7 +16875,7 @@
       </c>
       <c r="G463" s="38"/>
     </row>
-    <row r="464" spans="1:7">
+    <row r="464" spans="1:7" hidden="1">
       <c r="A464" s="38" t="s">
         <v>58</v>
       </c>
@@ -16892,7 +16892,7 @@
       </c>
       <c r="G464" s="41"/>
     </row>
-    <row r="465" spans="1:7">
+    <row r="465" spans="1:7" hidden="1">
       <c r="A465" s="38" t="s">
         <v>58</v>
       </c>
@@ -16913,7 +16913,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="466" spans="1:7">
+    <row r="466" spans="1:7" hidden="1">
       <c r="A466" s="38" t="s">
         <v>58</v>
       </c>
@@ -16932,7 +16932,7 @@
       </c>
       <c r="G466" s="38"/>
     </row>
-    <row r="467" spans="1:7">
+    <row r="467" spans="1:7" hidden="1">
       <c r="A467" s="38" t="s">
         <v>58</v>
       </c>
@@ -16949,7 +16949,7 @@
       </c>
       <c r="G467" s="41"/>
     </row>
-    <row r="468" spans="1:7">
+    <row r="468" spans="1:7" hidden="1">
       <c r="A468" s="38" t="s">
         <v>58</v>
       </c>
@@ -16970,7 +16970,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="469" spans="1:7">
+    <row r="469" spans="1:7" hidden="1">
       <c r="A469" s="38" t="s">
         <v>58</v>
       </c>
@@ -16989,7 +16989,7 @@
       </c>
       <c r="G469" s="44"/>
     </row>
-    <row r="470" spans="1:7">
+    <row r="470" spans="1:7" hidden="1">
       <c r="A470" s="38" t="s">
         <v>58</v>
       </c>
@@ -17008,7 +17008,7 @@
       </c>
       <c r="G470" s="44"/>
     </row>
-    <row r="471" spans="1:7">
+    <row r="471" spans="1:7" hidden="1">
       <c r="A471" s="38" t="s">
         <v>58</v>
       </c>
@@ -17027,7 +17027,7 @@
       </c>
       <c r="G471" s="38"/>
     </row>
-    <row r="472" spans="1:7">
+    <row r="472" spans="1:7" hidden="1">
       <c r="A472" s="38" t="s">
         <v>58</v>
       </c>
@@ -17047,7 +17047,16 @@
       <c r="G472" s="38"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B472" xr:uid="{7D022713-DD5E-432D-B8E4-1D5C596D7380}"/>
+  <autoFilter ref="B1:B472" xr:uid="{3DC38FAA-34B5-43EA-BCBF-EF3645E6BCF1}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="11.4.2.3"/>
+        <filter val="11.4.2.3.1"/>
+        <filter val="11.4.2.3.2"/>
+        <filter val="11.4.2.3.3"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -17203,8 +17212,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AMK55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView showGridLines="0" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -21980,7 +21989,7 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix parameters in prod sheet for pkix.13
</commit_message>
<xml_diff>
--- a/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
+++ b/conformancelib/testdata/85b_test_definitions_PIV_ICAM_Test_Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geoff\gsa-devel\piv-conformance\conformancelib\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68B8CDA-7D5A-49B3-85E9-6759BAC13686}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5CE77B-0329-4234-9432-AEFF2E701685}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP 800-85B Reference" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Placeholders" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Steps Overview'!$B$1:$B$472</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Steps Overview'!$D$1:$D$472</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -8518,8 +8518,8 @@
   <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:H472"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D424" sqref="D424"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -14853,7 +14853,7 @@
       </c>
       <c r="G355" s="38"/>
     </row>
-    <row r="356" spans="1:7" ht="30" hidden="1">
+    <row r="356" spans="1:7" ht="30">
       <c r="A356" s="38" t="s">
         <v>58</v>
       </c>
@@ -15244,7 +15244,7 @@
       </c>
       <c r="G376" s="44"/>
     </row>
-    <row r="377" spans="1:7" ht="30" hidden="1">
+    <row r="377" spans="1:7" ht="30">
       <c r="A377" s="38" t="s">
         <v>58</v>
       </c>
@@ -16087,7 +16087,7 @@
       </c>
       <c r="G421" s="38"/>
     </row>
-    <row r="422" spans="1:7">
+    <row r="422" spans="1:7" hidden="1">
       <c r="A422" s="38" t="s">
         <v>58</v>
       </c>
@@ -16102,7 +16102,7 @@
       <c r="F422" s="41"/>
       <c r="G422" s="41"/>
     </row>
-    <row r="423" spans="1:7">
+    <row r="423" spans="1:7" hidden="1">
       <c r="A423" s="38" t="s">
         <v>58</v>
       </c>
@@ -16123,7 +16123,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="424" spans="1:7">
+    <row r="424" spans="1:7" hidden="1">
       <c r="A424" s="38" t="s">
         <v>58</v>
       </c>
@@ -16142,7 +16142,7 @@
       </c>
       <c r="G424" s="38"/>
     </row>
-    <row r="425" spans="1:7">
+    <row r="425" spans="1:7" hidden="1">
       <c r="A425" s="38" t="s">
         <v>58</v>
       </c>
@@ -16801,7 +16801,7 @@
       </c>
       <c r="G459" s="38"/>
     </row>
-    <row r="460" spans="1:7" hidden="1">
+    <row r="460" spans="1:7" ht="30" hidden="1">
       <c r="A460" s="38" t="s">
         <v>58</v>
       </c>
@@ -17047,13 +17047,10 @@
       <c r="G472" s="38"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B472" xr:uid="{3DC38FAA-34B5-43EA-BCBF-EF3645E6BCF1}">
+  <autoFilter ref="D1:D472" xr:uid="{9979DB17-DD3C-4836-94F3-6ACDFC434949}">
     <filterColumn colId="0">
       <filters>
-        <filter val="11.4.2.3"/>
-        <filter val="11.4.2.3.1"/>
-        <filter val="11.4.2.3.2"/>
-        <filter val="11.4.2.3.3"/>
+        <filter val="PKIX.13"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -21989,8 +21986,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:IV27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>

</xml_diff>